<commit_message>
Add ResultsOrdering to template
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Projects/HMCTS/sscs-ccd-definitions/benefit/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jack/Development/hmcts/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4344B709-01A8-D147-B481-CAD4A73CFD1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E904E65E-4899-6B4C-B20A-58FEC4219E1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25800" windowHeight="10600" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25800" windowHeight="10600" tabRatio="500" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="177">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -676,6 +676,9 @@
   </si>
   <si>
     <t>RetriesTimeoutURLMidEvent</t>
+  </si>
+  <si>
+    <t>ResultsOrdering</t>
   </si>
 </sst>
 </file>
@@ -3882,10 +3885,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3900,7 +3903,7 @@
     <col min="8" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>146</v>
       </c>
@@ -3917,7 +3920,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="39" customHeight="1">
+    <row r="2" spans="1:8" ht="39" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -3938,7 +3941,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1">
+    <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -3960,62 +3963,65 @@
       <c r="G3" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1">
+      <c r="H3" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1">
+    <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1">
+    <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1">
+    <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1">
+    <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="22"/>
       <c r="B8" s="22"/>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1">
+    <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1">
+    <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="F10" s="57"/>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1">
+    <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="F11" s="146"/>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1">
+    <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="22"/>
       <c r="B12" s="22"/>
       <c r="F12" s="146"/>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1">
+    <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
       <c r="F13" s="146"/>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1">
+    <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" s="22"/>
       <c r="B14" s="22"/>
       <c r="F14" s="146"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1">
+    <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
       <c r="F15" s="146"/>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1">
+    <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="22"/>
       <c r="B16" s="22"/>
       <c r="F16" s="146"/>
@@ -42541,7 +42547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMK229"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added ResultsOrdering column to WorkBasketResult
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jack/Development/hmcts/sscs-ccd-definitions/benefit/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisdavidson/Documents/Dev/hmcts/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA465885-2A54-AF4E-9601-D964F8F6CDF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794F51C2-149C-C34B-BF55-3F012017F475}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25800" windowHeight="10600" tabRatio="500" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25800" windowHeight="12340" tabRatio="500" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="178">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -677,12 +677,18 @@
   <si>
     <t>RetriesTimeoutURLMidEvent</t>
   </si>
+  <si>
+    <t>ResultsOrdering</t>
+  </si>
+  <si>
+    <t>Field to use for the order of results</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="33">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -911,6 +917,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1196,7 +1207,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1455,6 +1466,8 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3882,10 +3895,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:G1048576"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3900,7 +3913,7 @@
     <col min="8" max="1024" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>146</v>
       </c>
@@ -3917,7 +3930,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="39" customHeight="1">
+    <row r="2" spans="1:8" ht="39" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -3937,8 +3950,11 @@
       <c r="G2" s="4" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1">
+      <c r="H2" s="194" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -3960,62 +3976,65 @@
       <c r="G3" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1">
+      <c r="H3" s="195" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1">
+    <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1">
+    <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1">
+    <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1">
+    <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="22"/>
       <c r="B8" s="22"/>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1">
+    <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1">
+    <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="F10" s="57"/>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1">
+    <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="F11" s="146"/>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1">
+    <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="22"/>
       <c r="B12" s="22"/>
       <c r="F12" s="146"/>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1">
+    <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
       <c r="F13" s="146"/>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1">
+    <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" s="22"/>
       <c r="B14" s="22"/>
       <c r="F14" s="146"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1">
+    <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
       <c r="F15" s="146"/>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1">
+    <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="22"/>
       <c r="B16" s="22"/>
       <c r="F16" s="146"/>
@@ -42542,7 +42561,7 @@
   <dimension ref="A1:AMK229"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -42556,7 +42575,8 @@
     <col min="8" max="8" width="8.83203125" style="18" customWidth="1"/>
     <col min="9" max="9" width="27.33203125" style="18" customWidth="1"/>
     <col min="10" max="15" width="8.83203125" style="18" customWidth="1"/>
-    <col min="16" max="17" width="8.83203125" style="45" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" style="45" customWidth="1"/>
+    <col min="17" max="17" width="24" style="45" customWidth="1"/>
     <col min="18" max="1025" width="8.83203125" style="18" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Update interloc label for work basket
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisdavidson/Documents/Dev/hmcts/sscs-ccd-definitions/benefit/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jack/Development/hmcts/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794F51C2-149C-C34B-BF55-3F012017F475}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3826F5-C4B7-3045-B496-CC1CB76AA001}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25800" windowHeight="12340" tabRatio="500" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25800" windowHeight="12340" tabRatio="500" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="178">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2746,23 +2746,24 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5" style="1" customWidth="1"/>
     <col min="2" max="3" width="8.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="1" customWidth="1"/>
-    <col min="7" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="32.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="1" customWidth="1"/>
+    <col min="8" max="1026" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1">
+    <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>136</v>
       </c>
@@ -2772,13 +2773,14 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="39" customHeight="1">
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" ht="39" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2788,17 +2790,18 @@
       <c r="C2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
+    <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2808,207 +2811,248 @@
       <c r="C3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
+    <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1">
       <c r="A8" s="22"/>
       <c r="B8" s="22"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="45"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1">
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1">
+      <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
+      <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1">
       <c r="A12" s="22"/>
       <c r="B12" s="22"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1">
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" s="144" customFormat="1" ht="15" customHeight="1">
+      <c r="F13" s="2"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" s="144" customFormat="1" ht="15" customHeight="1">
       <c r="A14" s="22"/>
       <c r="B14" s="22"/>
       <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="45"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1">
+      <c r="F14" s="12"/>
+      <c r="G14" s="45"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" s="24" customFormat="1" ht="15" customHeight="1">
+      <c r="F15" s="9"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="22"/>
       <c r="B16" s="22"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="63"/>
-    </row>
-    <row r="17" spans="1:2" ht="15" customHeight="1">
+      <c r="F16" s="6"/>
+      <c r="G16" s="63"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="22"/>
       <c r="B17" s="22"/>
-    </row>
-    <row r="18" spans="1:2" ht="15" customHeight="1">
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
-    </row>
-    <row r="19" spans="1:2" ht="15" customHeight="1">
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
-    </row>
-    <row r="20" spans="1:2" ht="15" customHeight="1">
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
-    </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1">
+      <c r="D20" s="15"/>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1">
       <c r="A21" s="22"/>
       <c r="B21" s="22"/>
-    </row>
-    <row r="22" spans="1:2" ht="15" customHeight="1">
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
-    </row>
-    <row r="23" spans="1:2" ht="15" customHeight="1">
+      <c r="D22" s="15"/>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1">
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
-    </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1">
+      <c r="D23" s="15"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1">
       <c r="A24" s="22"/>
       <c r="B24" s="22"/>
-    </row>
-    <row r="25" spans="1:2" ht="15" customHeight="1">
+      <c r="D24" s="15"/>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1">
       <c r="A25" s="22"/>
       <c r="B25" s="22"/>
-    </row>
-    <row r="26" spans="1:2" ht="15" customHeight="1">
+      <c r="D25" s="15"/>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1">
       <c r="A26" s="22"/>
       <c r="B26" s="22"/>
-    </row>
-    <row r="27" spans="1:2" ht="15" customHeight="1">
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1">
       <c r="A27" s="22"/>
       <c r="B27" s="22"/>
-    </row>
-    <row r="28" spans="1:2" ht="15" customHeight="1">
+      <c r="D27" s="15"/>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
-    </row>
-    <row r="29" spans="1:2" ht="15" customHeight="1">
+      <c r="D28" s="15"/>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1">
       <c r="A29" s="22"/>
       <c r="B29" s="22"/>
-    </row>
-    <row r="30" spans="1:2" ht="15" customHeight="1">
+      <c r="D29" s="15"/>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1">
       <c r="A30" s="22"/>
       <c r="B30" s="22"/>
-    </row>
-    <row r="31" spans="1:2" ht="15" customHeight="1">
+      <c r="D30" s="15"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1">
       <c r="A31" s="22"/>
       <c r="B31" s="22"/>
-    </row>
-    <row r="32" spans="1:2" ht="15" customHeight="1">
+      <c r="D31" s="18"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1">
       <c r="A32" s="22"/>
       <c r="B32" s="22"/>
-    </row>
-    <row r="33" spans="1:2" ht="15" customHeight="1">
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1">
       <c r="A33" s="22"/>
       <c r="B33" s="22"/>
-    </row>
-    <row r="34" spans="1:2" ht="15" customHeight="1">
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1">
       <c r="A34" s="22"/>
       <c r="B34" s="22"/>
-    </row>
-    <row r="35" spans="1:2" ht="15" customHeight="1">
+      <c r="D34" s="11"/>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1">
       <c r="A35" s="22"/>
       <c r="B35" s="22"/>
-    </row>
-    <row r="36" spans="1:2" ht="15" customHeight="1">
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1">
       <c r="A36" s="22"/>
       <c r="B36" s="22"/>
-    </row>
-    <row r="37" spans="1:2" ht="15" customHeight="1">
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" spans="1:4" ht="15" customHeight="1">
       <c r="A37" s="22"/>
       <c r="B37" s="22"/>
-    </row>
-    <row r="38" spans="1:2" ht="15" customHeight="1">
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" spans="1:4" ht="15" customHeight="1">
       <c r="A38" s="22"/>
       <c r="B38" s="22"/>
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="D39" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
@@ -3021,23 +3065,24 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D3" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
     <col min="2" max="3" width="8.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="1" customWidth="1"/>
-    <col min="7" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="32.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="1" customWidth="1"/>
+    <col min="8" max="1026" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1">
+    <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>140</v>
       </c>
@@ -3047,13 +3092,14 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="39" customHeight="1">
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" ht="39" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -3063,17 +3109,18 @@
       <c r="C2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
+    <row r="3" spans="1:7" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -3083,175 +3130,220 @@
       <c r="C3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
+    <row r="4" spans="1:7" ht="15" customHeight="1">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1">
       <c r="A8" s="22"/>
       <c r="B8" s="22"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="45"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" s="24" customFormat="1" ht="15" customHeight="1">
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" s="24" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
       <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="62"/>
-      <c r="F9" s="63"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1">
+      <c r="F9" s="62"/>
+      <c r="G9" s="63"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1">
       <c r="A12" s="22"/>
       <c r="B12" s="22"/>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1">
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1">
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1">
       <c r="A14" s="22"/>
       <c r="B14" s="22"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1">
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1">
+      <c r="D15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1">
       <c r="A16" s="22"/>
       <c r="B16" s="22"/>
-    </row>
-    <row r="17" spans="1:2" ht="15" customHeight="1">
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="22"/>
       <c r="B17" s="22"/>
-    </row>
-    <row r="18" spans="1:2" ht="15" customHeight="1">
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
-    </row>
-    <row r="19" spans="1:2" ht="15" customHeight="1">
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
-    </row>
-    <row r="20" spans="1:2" ht="15" customHeight="1">
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
-    </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1">
+      <c r="D20" s="15"/>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1">
       <c r="A21" s="22"/>
       <c r="B21" s="22"/>
-    </row>
-    <row r="22" spans="1:2" ht="15" customHeight="1">
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
-    </row>
-    <row r="23" spans="1:2" ht="15" customHeight="1">
+      <c r="D22" s="15"/>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1">
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
-    </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1">
+      <c r="D23" s="15"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1">
       <c r="A24" s="22"/>
       <c r="B24" s="22"/>
-    </row>
-    <row r="25" spans="1:2" ht="15" customHeight="1">
+      <c r="D24" s="15"/>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1">
       <c r="A25" s="22"/>
       <c r="B25" s="22"/>
-    </row>
-    <row r="26" spans="1:2" ht="15" customHeight="1">
+      <c r="D25" s="15"/>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1">
       <c r="A26" s="22"/>
       <c r="B26" s="22"/>
-    </row>
-    <row r="27" spans="1:2" ht="15" customHeight="1">
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1">
       <c r="A27" s="22"/>
       <c r="B27" s="22"/>
-    </row>
-    <row r="28" spans="1:2" ht="15" customHeight="1">
+      <c r="D27" s="15"/>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
-    </row>
-    <row r="29" spans="1:2" ht="15" customHeight="1">
+      <c r="D28" s="15"/>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1">
       <c r="A29" s="22"/>
       <c r="B29" s="22"/>
-    </row>
-    <row r="30" spans="1:2" ht="15" customHeight="1">
+      <c r="D29" s="15"/>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1">
       <c r="A30" s="22"/>
       <c r="B30" s="22"/>
-    </row>
-    <row r="31" spans="1:2" ht="15" customHeight="1">
+      <c r="D30" s="15"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1">
       <c r="A31" s="22"/>
       <c r="B31" s="22"/>
-    </row>
-    <row r="32" spans="1:2" ht="15" customHeight="1">
+      <c r="D31" s="18"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1">
       <c r="A32" s="22"/>
       <c r="B32" s="22"/>
-    </row>
-    <row r="33" spans="1:2" ht="15" customHeight="1">
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1">
       <c r="A33" s="22"/>
       <c r="B33" s="22"/>
-    </row>
-    <row r="34" spans="1:2" ht="15" customHeight="1">
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1">
       <c r="A34" s="22"/>
       <c r="B34" s="22"/>
-    </row>
-    <row r="35" spans="1:2" ht="15" customHeight="1">
+      <c r="D34" s="11"/>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1">
       <c r="A35" s="22"/>
       <c r="B35" s="22"/>
-    </row>
-    <row r="36" spans="1:2" ht="15" customHeight="1">
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1">
       <c r="A36" s="22"/>
       <c r="B36" s="22"/>
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="D39" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
@@ -3266,8 +3358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3897,7 +3989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Feature/sscs 7054 hide history tab and minise ccd bug (#155)
* extend format for new rows in the liveFrom column

* configure fine access for the history tab

* add tl1Form field in the dwpDocument tab

* bring it up to date with master

* bump up the version
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jack/Development/hmcts/sscs-ccd-definitions/benefit/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcrespo/data/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61149132-FA52-8440-B4EA-F2BC57165D17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64F0695-B4D0-A74D-BFF2-4E1EB8978FCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25800" windowHeight="12340" tabRatio="500" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="1540" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -2742,10 +2742,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:H91"/>
+  <dimension ref="A1:H573"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A5" sqref="A5:A573"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3360,6 +3360,1452 @@
     <row r="91" spans="1:2" ht="15" customHeight="1">
       <c r="A91" s="22"/>
       <c r="B91" s="22"/>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="22"/>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="22"/>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="22"/>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="22"/>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="22"/>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="22"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="22"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="22"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="22"/>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="22"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="22"/>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="22"/>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="22"/>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="22"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="22"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="22"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="22"/>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="22"/>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="22"/>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="22"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="22"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="22"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="22"/>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="22"/>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="22"/>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="22"/>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="22"/>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="22"/>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="22"/>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="22"/>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="22"/>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="22"/>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="22"/>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="22"/>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="22"/>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="22"/>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="22"/>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="22"/>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="22"/>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="22"/>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="22"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="22"/>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="22"/>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="22"/>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="22"/>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="22"/>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="22"/>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="22"/>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="22"/>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="22"/>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="22"/>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="22"/>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="22"/>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="22"/>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="22"/>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="22"/>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="22"/>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="22"/>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="22"/>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="22"/>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="22"/>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="22"/>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="22"/>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="22"/>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="22"/>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="22"/>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="22"/>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="22"/>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="22"/>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="22"/>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="22"/>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="22"/>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="22"/>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" s="22"/>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="22"/>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="22"/>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="22"/>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="22"/>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="22"/>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="22"/>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" s="22"/>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" s="22"/>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" s="22"/>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" s="22"/>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" s="22"/>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" s="22"/>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" s="22"/>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" s="22"/>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" s="22"/>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" s="22"/>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" s="22"/>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" s="22"/>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" s="22"/>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" s="22"/>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" s="22"/>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" s="22"/>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" s="22"/>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" s="22"/>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" s="22"/>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" s="22"/>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" s="22"/>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" s="22"/>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" s="22"/>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" s="22"/>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" s="22"/>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" s="22"/>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" s="22"/>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" s="22"/>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" s="22"/>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" s="22"/>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" s="22"/>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" s="22"/>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" s="22"/>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" s="22"/>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" s="22"/>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" s="22"/>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" s="22"/>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" s="22"/>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" s="22"/>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" s="22"/>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" s="22"/>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" s="22"/>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" s="22"/>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" s="22"/>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" s="22"/>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" s="22"/>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" s="22"/>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" s="22"/>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" s="22"/>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" s="22"/>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" s="22"/>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" s="22"/>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" s="22"/>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" s="22"/>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" s="22"/>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" s="22"/>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" s="22"/>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" s="22"/>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" s="22"/>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" s="22"/>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" s="22"/>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" s="22"/>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" s="22"/>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" s="22"/>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" s="22"/>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" s="22"/>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" s="22"/>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" s="22"/>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" s="22"/>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" s="22"/>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" s="22"/>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" s="22"/>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" s="22"/>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" s="22"/>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" s="22"/>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" s="22"/>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" s="22"/>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" s="22"/>
+    </row>
+    <row r="250" spans="1:1">
+      <c r="A250" s="22"/>
+    </row>
+    <row r="251" spans="1:1">
+      <c r="A251" s="22"/>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252" s="22"/>
+    </row>
+    <row r="253" spans="1:1">
+      <c r="A253" s="22"/>
+    </row>
+    <row r="254" spans="1:1">
+      <c r="A254" s="22"/>
+    </row>
+    <row r="255" spans="1:1">
+      <c r="A255" s="22"/>
+    </row>
+    <row r="256" spans="1:1">
+      <c r="A256" s="22"/>
+    </row>
+    <row r="257" spans="1:1">
+      <c r="A257" s="22"/>
+    </row>
+    <row r="258" spans="1:1">
+      <c r="A258" s="22"/>
+    </row>
+    <row r="259" spans="1:1">
+      <c r="A259" s="22"/>
+    </row>
+    <row r="260" spans="1:1">
+      <c r="A260" s="22"/>
+    </row>
+    <row r="261" spans="1:1">
+      <c r="A261" s="22"/>
+    </row>
+    <row r="262" spans="1:1">
+      <c r="A262" s="22"/>
+    </row>
+    <row r="263" spans="1:1">
+      <c r="A263" s="22"/>
+    </row>
+    <row r="264" spans="1:1">
+      <c r="A264" s="22"/>
+    </row>
+    <row r="265" spans="1:1">
+      <c r="A265" s="22"/>
+    </row>
+    <row r="266" spans="1:1">
+      <c r="A266" s="22"/>
+    </row>
+    <row r="267" spans="1:1">
+      <c r="A267" s="22"/>
+    </row>
+    <row r="268" spans="1:1">
+      <c r="A268" s="22"/>
+    </row>
+    <row r="269" spans="1:1">
+      <c r="A269" s="22"/>
+    </row>
+    <row r="270" spans="1:1">
+      <c r="A270" s="22"/>
+    </row>
+    <row r="271" spans="1:1">
+      <c r="A271" s="22"/>
+    </row>
+    <row r="272" spans="1:1">
+      <c r="A272" s="22"/>
+    </row>
+    <row r="273" spans="1:1">
+      <c r="A273" s="22"/>
+    </row>
+    <row r="274" spans="1:1">
+      <c r="A274" s="22"/>
+    </row>
+    <row r="275" spans="1:1">
+      <c r="A275" s="22"/>
+    </row>
+    <row r="276" spans="1:1">
+      <c r="A276" s="22"/>
+    </row>
+    <row r="277" spans="1:1">
+      <c r="A277" s="22"/>
+    </row>
+    <row r="278" spans="1:1">
+      <c r="A278" s="22"/>
+    </row>
+    <row r="279" spans="1:1">
+      <c r="A279" s="22"/>
+    </row>
+    <row r="280" spans="1:1">
+      <c r="A280" s="22"/>
+    </row>
+    <row r="281" spans="1:1">
+      <c r="A281" s="22"/>
+    </row>
+    <row r="282" spans="1:1">
+      <c r="A282" s="22"/>
+    </row>
+    <row r="283" spans="1:1">
+      <c r="A283" s="22"/>
+    </row>
+    <row r="284" spans="1:1">
+      <c r="A284" s="22"/>
+    </row>
+    <row r="285" spans="1:1">
+      <c r="A285" s="22"/>
+    </row>
+    <row r="286" spans="1:1">
+      <c r="A286" s="22"/>
+    </row>
+    <row r="287" spans="1:1">
+      <c r="A287" s="22"/>
+    </row>
+    <row r="288" spans="1:1">
+      <c r="A288" s="22"/>
+    </row>
+    <row r="289" spans="1:1">
+      <c r="A289" s="22"/>
+    </row>
+    <row r="290" spans="1:1">
+      <c r="A290" s="22"/>
+    </row>
+    <row r="291" spans="1:1">
+      <c r="A291" s="22"/>
+    </row>
+    <row r="292" spans="1:1">
+      <c r="A292" s="22"/>
+    </row>
+    <row r="293" spans="1:1">
+      <c r="A293" s="22"/>
+    </row>
+    <row r="294" spans="1:1">
+      <c r="A294" s="22"/>
+    </row>
+    <row r="295" spans="1:1">
+      <c r="A295" s="22"/>
+    </row>
+    <row r="296" spans="1:1">
+      <c r="A296" s="22"/>
+    </row>
+    <row r="297" spans="1:1">
+      <c r="A297" s="22"/>
+    </row>
+    <row r="298" spans="1:1">
+      <c r="A298" s="22"/>
+    </row>
+    <row r="299" spans="1:1">
+      <c r="A299" s="22"/>
+    </row>
+    <row r="300" spans="1:1">
+      <c r="A300" s="22"/>
+    </row>
+    <row r="301" spans="1:1">
+      <c r="A301" s="22"/>
+    </row>
+    <row r="302" spans="1:1">
+      <c r="A302" s="22"/>
+    </row>
+    <row r="303" spans="1:1">
+      <c r="A303" s="22"/>
+    </row>
+    <row r="304" spans="1:1">
+      <c r="A304" s="22"/>
+    </row>
+    <row r="305" spans="1:1">
+      <c r="A305" s="22"/>
+    </row>
+    <row r="306" spans="1:1">
+      <c r="A306" s="22"/>
+    </row>
+    <row r="307" spans="1:1">
+      <c r="A307" s="22"/>
+    </row>
+    <row r="308" spans="1:1">
+      <c r="A308" s="22"/>
+    </row>
+    <row r="309" spans="1:1">
+      <c r="A309" s="22"/>
+    </row>
+    <row r="310" spans="1:1">
+      <c r="A310" s="22"/>
+    </row>
+    <row r="311" spans="1:1">
+      <c r="A311" s="22"/>
+    </row>
+    <row r="312" spans="1:1">
+      <c r="A312" s="22"/>
+    </row>
+    <row r="313" spans="1:1">
+      <c r="A313" s="22"/>
+    </row>
+    <row r="314" spans="1:1">
+      <c r="A314" s="22"/>
+    </row>
+    <row r="315" spans="1:1">
+      <c r="A315" s="22"/>
+    </row>
+    <row r="316" spans="1:1">
+      <c r="A316" s="22"/>
+    </row>
+    <row r="317" spans="1:1">
+      <c r="A317" s="22"/>
+    </row>
+    <row r="318" spans="1:1">
+      <c r="A318" s="22"/>
+    </row>
+    <row r="319" spans="1:1">
+      <c r="A319" s="22"/>
+    </row>
+    <row r="320" spans="1:1">
+      <c r="A320" s="22"/>
+    </row>
+    <row r="321" spans="1:1">
+      <c r="A321" s="22"/>
+    </row>
+    <row r="322" spans="1:1">
+      <c r="A322" s="22"/>
+    </row>
+    <row r="323" spans="1:1">
+      <c r="A323" s="22"/>
+    </row>
+    <row r="324" spans="1:1">
+      <c r="A324" s="22"/>
+    </row>
+    <row r="325" spans="1:1">
+      <c r="A325" s="22"/>
+    </row>
+    <row r="326" spans="1:1">
+      <c r="A326" s="22"/>
+    </row>
+    <row r="327" spans="1:1">
+      <c r="A327" s="22"/>
+    </row>
+    <row r="328" spans="1:1">
+      <c r="A328" s="22"/>
+    </row>
+    <row r="329" spans="1:1">
+      <c r="A329" s="22"/>
+    </row>
+    <row r="330" spans="1:1">
+      <c r="A330" s="22"/>
+    </row>
+    <row r="331" spans="1:1">
+      <c r="A331" s="22"/>
+    </row>
+    <row r="332" spans="1:1">
+      <c r="A332" s="22"/>
+    </row>
+    <row r="333" spans="1:1">
+      <c r="A333" s="22"/>
+    </row>
+    <row r="334" spans="1:1">
+      <c r="A334" s="22"/>
+    </row>
+    <row r="335" spans="1:1">
+      <c r="A335" s="22"/>
+    </row>
+    <row r="336" spans="1:1">
+      <c r="A336" s="22"/>
+    </row>
+    <row r="337" spans="1:1">
+      <c r="A337" s="22"/>
+    </row>
+    <row r="338" spans="1:1">
+      <c r="A338" s="22"/>
+    </row>
+    <row r="339" spans="1:1">
+      <c r="A339" s="22"/>
+    </row>
+    <row r="340" spans="1:1">
+      <c r="A340" s="22"/>
+    </row>
+    <row r="341" spans="1:1">
+      <c r="A341" s="22"/>
+    </row>
+    <row r="342" spans="1:1">
+      <c r="A342" s="22"/>
+    </row>
+    <row r="343" spans="1:1">
+      <c r="A343" s="22"/>
+    </row>
+    <row r="344" spans="1:1">
+      <c r="A344" s="22"/>
+    </row>
+    <row r="345" spans="1:1">
+      <c r="A345" s="22"/>
+    </row>
+    <row r="346" spans="1:1">
+      <c r="A346" s="22"/>
+    </row>
+    <row r="347" spans="1:1">
+      <c r="A347" s="22"/>
+    </row>
+    <row r="348" spans="1:1">
+      <c r="A348" s="22"/>
+    </row>
+    <row r="349" spans="1:1">
+      <c r="A349" s="22"/>
+    </row>
+    <row r="350" spans="1:1">
+      <c r="A350" s="22"/>
+    </row>
+    <row r="351" spans="1:1">
+      <c r="A351" s="22"/>
+    </row>
+    <row r="352" spans="1:1">
+      <c r="A352" s="22"/>
+    </row>
+    <row r="353" spans="1:1">
+      <c r="A353" s="22"/>
+    </row>
+    <row r="354" spans="1:1">
+      <c r="A354" s="22"/>
+    </row>
+    <row r="355" spans="1:1">
+      <c r="A355" s="22"/>
+    </row>
+    <row r="356" spans="1:1">
+      <c r="A356" s="22"/>
+    </row>
+    <row r="357" spans="1:1">
+      <c r="A357" s="22"/>
+    </row>
+    <row r="358" spans="1:1">
+      <c r="A358" s="22"/>
+    </row>
+    <row r="359" spans="1:1">
+      <c r="A359" s="22"/>
+    </row>
+    <row r="360" spans="1:1">
+      <c r="A360" s="22"/>
+    </row>
+    <row r="361" spans="1:1">
+      <c r="A361" s="22"/>
+    </row>
+    <row r="362" spans="1:1">
+      <c r="A362" s="22"/>
+    </row>
+    <row r="363" spans="1:1">
+      <c r="A363" s="22"/>
+    </row>
+    <row r="364" spans="1:1">
+      <c r="A364" s="22"/>
+    </row>
+    <row r="365" spans="1:1">
+      <c r="A365" s="22"/>
+    </row>
+    <row r="366" spans="1:1">
+      <c r="A366" s="22"/>
+    </row>
+    <row r="367" spans="1:1">
+      <c r="A367" s="22"/>
+    </row>
+    <row r="368" spans="1:1">
+      <c r="A368" s="22"/>
+    </row>
+    <row r="369" spans="1:1">
+      <c r="A369" s="22"/>
+    </row>
+    <row r="370" spans="1:1">
+      <c r="A370" s="22"/>
+    </row>
+    <row r="371" spans="1:1">
+      <c r="A371" s="22"/>
+    </row>
+    <row r="372" spans="1:1">
+      <c r="A372" s="22"/>
+    </row>
+    <row r="373" spans="1:1">
+      <c r="A373" s="22"/>
+    </row>
+    <row r="374" spans="1:1">
+      <c r="A374" s="22"/>
+    </row>
+    <row r="375" spans="1:1">
+      <c r="A375" s="22"/>
+    </row>
+    <row r="376" spans="1:1">
+      <c r="A376" s="22"/>
+    </row>
+    <row r="377" spans="1:1">
+      <c r="A377" s="22"/>
+    </row>
+    <row r="378" spans="1:1">
+      <c r="A378" s="22"/>
+    </row>
+    <row r="379" spans="1:1">
+      <c r="A379" s="22"/>
+    </row>
+    <row r="380" spans="1:1">
+      <c r="A380" s="22"/>
+    </row>
+    <row r="381" spans="1:1">
+      <c r="A381" s="22"/>
+    </row>
+    <row r="382" spans="1:1">
+      <c r="A382" s="22"/>
+    </row>
+    <row r="383" spans="1:1">
+      <c r="A383" s="22"/>
+    </row>
+    <row r="384" spans="1:1">
+      <c r="A384" s="22"/>
+    </row>
+    <row r="385" spans="1:1">
+      <c r="A385" s="22"/>
+    </row>
+    <row r="386" spans="1:1">
+      <c r="A386" s="22"/>
+    </row>
+    <row r="387" spans="1:1">
+      <c r="A387" s="22"/>
+    </row>
+    <row r="388" spans="1:1">
+      <c r="A388" s="22"/>
+    </row>
+    <row r="389" spans="1:1">
+      <c r="A389" s="22"/>
+    </row>
+    <row r="390" spans="1:1">
+      <c r="A390" s="22"/>
+    </row>
+    <row r="391" spans="1:1">
+      <c r="A391" s="22"/>
+    </row>
+    <row r="392" spans="1:1">
+      <c r="A392" s="22"/>
+    </row>
+    <row r="393" spans="1:1">
+      <c r="A393" s="22"/>
+    </row>
+    <row r="394" spans="1:1">
+      <c r="A394" s="22"/>
+    </row>
+    <row r="395" spans="1:1">
+      <c r="A395" s="22"/>
+    </row>
+    <row r="396" spans="1:1">
+      <c r="A396" s="22"/>
+    </row>
+    <row r="397" spans="1:1">
+      <c r="A397" s="22"/>
+    </row>
+    <row r="398" spans="1:1">
+      <c r="A398" s="22"/>
+    </row>
+    <row r="399" spans="1:1">
+      <c r="A399" s="22"/>
+    </row>
+    <row r="400" spans="1:1">
+      <c r="A400" s="22"/>
+    </row>
+    <row r="401" spans="1:1">
+      <c r="A401" s="22"/>
+    </row>
+    <row r="402" spans="1:1">
+      <c r="A402" s="22"/>
+    </row>
+    <row r="403" spans="1:1">
+      <c r="A403" s="22"/>
+    </row>
+    <row r="404" spans="1:1">
+      <c r="A404" s="22"/>
+    </row>
+    <row r="405" spans="1:1">
+      <c r="A405" s="22"/>
+    </row>
+    <row r="406" spans="1:1">
+      <c r="A406" s="22"/>
+    </row>
+    <row r="407" spans="1:1">
+      <c r="A407" s="22"/>
+    </row>
+    <row r="408" spans="1:1">
+      <c r="A408" s="22"/>
+    </row>
+    <row r="409" spans="1:1">
+      <c r="A409" s="22"/>
+    </row>
+    <row r="410" spans="1:1">
+      <c r="A410" s="22"/>
+    </row>
+    <row r="411" spans="1:1">
+      <c r="A411" s="22"/>
+    </row>
+    <row r="412" spans="1:1">
+      <c r="A412" s="22"/>
+    </row>
+    <row r="413" spans="1:1">
+      <c r="A413" s="22"/>
+    </row>
+    <row r="414" spans="1:1">
+      <c r="A414" s="22"/>
+    </row>
+    <row r="415" spans="1:1">
+      <c r="A415" s="22"/>
+    </row>
+    <row r="416" spans="1:1">
+      <c r="A416" s="22"/>
+    </row>
+    <row r="417" spans="1:1">
+      <c r="A417" s="22"/>
+    </row>
+    <row r="418" spans="1:1">
+      <c r="A418" s="22"/>
+    </row>
+    <row r="419" spans="1:1">
+      <c r="A419" s="22"/>
+    </row>
+    <row r="420" spans="1:1">
+      <c r="A420" s="22"/>
+    </row>
+    <row r="421" spans="1:1">
+      <c r="A421" s="22"/>
+    </row>
+    <row r="422" spans="1:1">
+      <c r="A422" s="22"/>
+    </row>
+    <row r="423" spans="1:1">
+      <c r="A423" s="22"/>
+    </row>
+    <row r="424" spans="1:1">
+      <c r="A424" s="22"/>
+    </row>
+    <row r="425" spans="1:1">
+      <c r="A425" s="22"/>
+    </row>
+    <row r="426" spans="1:1">
+      <c r="A426" s="22"/>
+    </row>
+    <row r="427" spans="1:1">
+      <c r="A427" s="22"/>
+    </row>
+    <row r="428" spans="1:1">
+      <c r="A428" s="22"/>
+    </row>
+    <row r="429" spans="1:1">
+      <c r="A429" s="22"/>
+    </row>
+    <row r="430" spans="1:1">
+      <c r="A430" s="22"/>
+    </row>
+    <row r="431" spans="1:1">
+      <c r="A431" s="22"/>
+    </row>
+    <row r="432" spans="1:1">
+      <c r="A432" s="22"/>
+    </row>
+    <row r="433" spans="1:1">
+      <c r="A433" s="22"/>
+    </row>
+    <row r="434" spans="1:1">
+      <c r="A434" s="22"/>
+    </row>
+    <row r="435" spans="1:1">
+      <c r="A435" s="22"/>
+    </row>
+    <row r="436" spans="1:1">
+      <c r="A436" s="22"/>
+    </row>
+    <row r="437" spans="1:1">
+      <c r="A437" s="22"/>
+    </row>
+    <row r="438" spans="1:1">
+      <c r="A438" s="22"/>
+    </row>
+    <row r="439" spans="1:1">
+      <c r="A439" s="22"/>
+    </row>
+    <row r="440" spans="1:1">
+      <c r="A440" s="22"/>
+    </row>
+    <row r="441" spans="1:1">
+      <c r="A441" s="22"/>
+    </row>
+    <row r="442" spans="1:1">
+      <c r="A442" s="22"/>
+    </row>
+    <row r="443" spans="1:1">
+      <c r="A443" s="22"/>
+    </row>
+    <row r="444" spans="1:1">
+      <c r="A444" s="22"/>
+    </row>
+    <row r="445" spans="1:1">
+      <c r="A445" s="22"/>
+    </row>
+    <row r="446" spans="1:1">
+      <c r="A446" s="22"/>
+    </row>
+    <row r="447" spans="1:1">
+      <c r="A447" s="22"/>
+    </row>
+    <row r="448" spans="1:1">
+      <c r="A448" s="22"/>
+    </row>
+    <row r="449" spans="1:1">
+      <c r="A449" s="22"/>
+    </row>
+    <row r="450" spans="1:1">
+      <c r="A450" s="22"/>
+    </row>
+    <row r="451" spans="1:1">
+      <c r="A451" s="22"/>
+    </row>
+    <row r="452" spans="1:1">
+      <c r="A452" s="22"/>
+    </row>
+    <row r="453" spans="1:1">
+      <c r="A453" s="22"/>
+    </row>
+    <row r="454" spans="1:1">
+      <c r="A454" s="22"/>
+    </row>
+    <row r="455" spans="1:1">
+      <c r="A455" s="22"/>
+    </row>
+    <row r="456" spans="1:1">
+      <c r="A456" s="22"/>
+    </row>
+    <row r="457" spans="1:1">
+      <c r="A457" s="22"/>
+    </row>
+    <row r="458" spans="1:1">
+      <c r="A458" s="22"/>
+    </row>
+    <row r="459" spans="1:1">
+      <c r="A459" s="22"/>
+    </row>
+    <row r="460" spans="1:1">
+      <c r="A460" s="22"/>
+    </row>
+    <row r="461" spans="1:1">
+      <c r="A461" s="22"/>
+    </row>
+    <row r="462" spans="1:1">
+      <c r="A462" s="22"/>
+    </row>
+    <row r="463" spans="1:1">
+      <c r="A463" s="22"/>
+    </row>
+    <row r="464" spans="1:1">
+      <c r="A464" s="22"/>
+    </row>
+    <row r="465" spans="1:1">
+      <c r="A465" s="22"/>
+    </row>
+    <row r="466" spans="1:1">
+      <c r="A466" s="22"/>
+    </row>
+    <row r="467" spans="1:1">
+      <c r="A467" s="22"/>
+    </row>
+    <row r="468" spans="1:1">
+      <c r="A468" s="22"/>
+    </row>
+    <row r="469" spans="1:1">
+      <c r="A469" s="22"/>
+    </row>
+    <row r="470" spans="1:1">
+      <c r="A470" s="22"/>
+    </row>
+    <row r="471" spans="1:1">
+      <c r="A471" s="22"/>
+    </row>
+    <row r="472" spans="1:1">
+      <c r="A472" s="22"/>
+    </row>
+    <row r="473" spans="1:1">
+      <c r="A473" s="22"/>
+    </row>
+    <row r="474" spans="1:1">
+      <c r="A474" s="22"/>
+    </row>
+    <row r="475" spans="1:1">
+      <c r="A475" s="22"/>
+    </row>
+    <row r="476" spans="1:1">
+      <c r="A476" s="22"/>
+    </row>
+    <row r="477" spans="1:1">
+      <c r="A477" s="22"/>
+    </row>
+    <row r="478" spans="1:1">
+      <c r="A478" s="22"/>
+    </row>
+    <row r="479" spans="1:1">
+      <c r="A479" s="22"/>
+    </row>
+    <row r="480" spans="1:1">
+      <c r="A480" s="22"/>
+    </row>
+    <row r="481" spans="1:1">
+      <c r="A481" s="22"/>
+    </row>
+    <row r="482" spans="1:1">
+      <c r="A482" s="22"/>
+    </row>
+    <row r="483" spans="1:1">
+      <c r="A483" s="22"/>
+    </row>
+    <row r="484" spans="1:1">
+      <c r="A484" s="22"/>
+    </row>
+    <row r="485" spans="1:1">
+      <c r="A485" s="22"/>
+    </row>
+    <row r="486" spans="1:1">
+      <c r="A486" s="22"/>
+    </row>
+    <row r="487" spans="1:1">
+      <c r="A487" s="22"/>
+    </row>
+    <row r="488" spans="1:1">
+      <c r="A488" s="22"/>
+    </row>
+    <row r="489" spans="1:1">
+      <c r="A489" s="22"/>
+    </row>
+    <row r="490" spans="1:1">
+      <c r="A490" s="22"/>
+    </row>
+    <row r="491" spans="1:1">
+      <c r="A491" s="22"/>
+    </row>
+    <row r="492" spans="1:1">
+      <c r="A492" s="22"/>
+    </row>
+    <row r="493" spans="1:1">
+      <c r="A493" s="22"/>
+    </row>
+    <row r="494" spans="1:1">
+      <c r="A494" s="22"/>
+    </row>
+    <row r="495" spans="1:1">
+      <c r="A495" s="22"/>
+    </row>
+    <row r="496" spans="1:1">
+      <c r="A496" s="22"/>
+    </row>
+    <row r="497" spans="1:1">
+      <c r="A497" s="22"/>
+    </row>
+    <row r="498" spans="1:1">
+      <c r="A498" s="22"/>
+    </row>
+    <row r="499" spans="1:1">
+      <c r="A499" s="22"/>
+    </row>
+    <row r="500" spans="1:1">
+      <c r="A500" s="22"/>
+    </row>
+    <row r="501" spans="1:1">
+      <c r="A501" s="22"/>
+    </row>
+    <row r="502" spans="1:1">
+      <c r="A502" s="22"/>
+    </row>
+    <row r="503" spans="1:1">
+      <c r="A503" s="22"/>
+    </row>
+    <row r="504" spans="1:1">
+      <c r="A504" s="22"/>
+    </row>
+    <row r="505" spans="1:1">
+      <c r="A505" s="22"/>
+    </row>
+    <row r="506" spans="1:1">
+      <c r="A506" s="22"/>
+    </row>
+    <row r="507" spans="1:1">
+      <c r="A507" s="22"/>
+    </row>
+    <row r="508" spans="1:1">
+      <c r="A508" s="22"/>
+    </row>
+    <row r="509" spans="1:1">
+      <c r="A509" s="22"/>
+    </row>
+    <row r="510" spans="1:1">
+      <c r="A510" s="22"/>
+    </row>
+    <row r="511" spans="1:1">
+      <c r="A511" s="22"/>
+    </row>
+    <row r="512" spans="1:1">
+      <c r="A512" s="22"/>
+    </row>
+    <row r="513" spans="1:1">
+      <c r="A513" s="22"/>
+    </row>
+    <row r="514" spans="1:1">
+      <c r="A514" s="22"/>
+    </row>
+    <row r="515" spans="1:1">
+      <c r="A515" s="22"/>
+    </row>
+    <row r="516" spans="1:1">
+      <c r="A516" s="22"/>
+    </row>
+    <row r="517" spans="1:1">
+      <c r="A517" s="22"/>
+    </row>
+    <row r="518" spans="1:1">
+      <c r="A518" s="22"/>
+    </row>
+    <row r="519" spans="1:1">
+      <c r="A519" s="22"/>
+    </row>
+    <row r="520" spans="1:1">
+      <c r="A520" s="22"/>
+    </row>
+    <row r="521" spans="1:1">
+      <c r="A521" s="22"/>
+    </row>
+    <row r="522" spans="1:1">
+      <c r="A522" s="22"/>
+    </row>
+    <row r="523" spans="1:1">
+      <c r="A523" s="22"/>
+    </row>
+    <row r="524" spans="1:1">
+      <c r="A524" s="22"/>
+    </row>
+    <row r="525" spans="1:1">
+      <c r="A525" s="22"/>
+    </row>
+    <row r="526" spans="1:1">
+      <c r="A526" s="22"/>
+    </row>
+    <row r="527" spans="1:1">
+      <c r="A527" s="22"/>
+    </row>
+    <row r="528" spans="1:1">
+      <c r="A528" s="22"/>
+    </row>
+    <row r="529" spans="1:1">
+      <c r="A529" s="22"/>
+    </row>
+    <row r="530" spans="1:1">
+      <c r="A530" s="22"/>
+    </row>
+    <row r="531" spans="1:1">
+      <c r="A531" s="22"/>
+    </row>
+    <row r="532" spans="1:1">
+      <c r="A532" s="22"/>
+    </row>
+    <row r="533" spans="1:1">
+      <c r="A533" s="22"/>
+    </row>
+    <row r="534" spans="1:1">
+      <c r="A534" s="22"/>
+    </row>
+    <row r="535" spans="1:1">
+      <c r="A535" s="22"/>
+    </row>
+    <row r="536" spans="1:1">
+      <c r="A536" s="22"/>
+    </row>
+    <row r="537" spans="1:1">
+      <c r="A537" s="22"/>
+    </row>
+    <row r="538" spans="1:1">
+      <c r="A538" s="22"/>
+    </row>
+    <row r="539" spans="1:1">
+      <c r="A539" s="22"/>
+    </row>
+    <row r="540" spans="1:1">
+      <c r="A540" s="22"/>
+    </row>
+    <row r="541" spans="1:1">
+      <c r="A541" s="22"/>
+    </row>
+    <row r="542" spans="1:1">
+      <c r="A542" s="22"/>
+    </row>
+    <row r="543" spans="1:1">
+      <c r="A543" s="22"/>
+    </row>
+    <row r="544" spans="1:1">
+      <c r="A544" s="22"/>
+    </row>
+    <row r="545" spans="1:1">
+      <c r="A545" s="22"/>
+    </row>
+    <row r="546" spans="1:1">
+      <c r="A546" s="22"/>
+    </row>
+    <row r="547" spans="1:1">
+      <c r="A547" s="22"/>
+    </row>
+    <row r="548" spans="1:1">
+      <c r="A548" s="22"/>
+    </row>
+    <row r="549" spans="1:1">
+      <c r="A549" s="22"/>
+    </row>
+    <row r="550" spans="1:1">
+      <c r="A550" s="22"/>
+    </row>
+    <row r="551" spans="1:1">
+      <c r="A551" s="22"/>
+    </row>
+    <row r="552" spans="1:1">
+      <c r="A552" s="22"/>
+    </row>
+    <row r="553" spans="1:1">
+      <c r="A553" s="22"/>
+    </row>
+    <row r="554" spans="1:1">
+      <c r="A554" s="22"/>
+    </row>
+    <row r="555" spans="1:1">
+      <c r="A555" s="22"/>
+    </row>
+    <row r="556" spans="1:1">
+      <c r="A556" s="22"/>
+    </row>
+    <row r="557" spans="1:1">
+      <c r="A557" s="22"/>
+    </row>
+    <row r="558" spans="1:1">
+      <c r="A558" s="22"/>
+    </row>
+    <row r="559" spans="1:1">
+      <c r="A559" s="22"/>
+    </row>
+    <row r="560" spans="1:1">
+      <c r="A560" s="22"/>
+    </row>
+    <row r="561" spans="1:1">
+      <c r="A561" s="22"/>
+    </row>
+    <row r="562" spans="1:1">
+      <c r="A562" s="22"/>
+    </row>
+    <row r="563" spans="1:1">
+      <c r="A563" s="22"/>
+    </row>
+    <row r="564" spans="1:1">
+      <c r="A564" s="22"/>
+    </row>
+    <row r="565" spans="1:1">
+      <c r="A565" s="22"/>
+    </row>
+    <row r="566" spans="1:1">
+      <c r="A566" s="22"/>
+    </row>
+    <row r="567" spans="1:1">
+      <c r="A567" s="22"/>
+    </row>
+    <row r="568" spans="1:1">
+      <c r="A568" s="22"/>
+    </row>
+    <row r="569" spans="1:1">
+      <c r="A569" s="22"/>
+    </row>
+    <row r="570" spans="1:1">
+      <c r="A570" s="22"/>
+    </row>
+    <row r="571" spans="1:1">
+      <c r="A571" s="22"/>
+    </row>
+    <row r="572" spans="1:1">
+      <c r="A572" s="22"/>
+    </row>
+    <row r="573" spans="1:1">
+      <c r="A573" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>

</xml_diff>

<commit_message>
Add ListElementCode to search filters
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jack/Development/hmcts/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762C124F-70C8-A544-8C21-96AB0C210006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769796AE-53FE-3A46-B34E-EBEDBC0C4795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -22,22 +22,21 @@
     <sheet name="State" sheetId="7" r:id="rId7"/>
     <sheet name="CaseEvent" sheetId="8" r:id="rId8"/>
     <sheet name="CaseEventToFields" sheetId="9" r:id="rId9"/>
-    <sheet name="EventToComplexTypes" sheetId="21" r:id="rId10"/>
-    <sheet name="SearchInputFields" sheetId="10" r:id="rId11"/>
-    <sheet name="SearchResultFields" sheetId="11" r:id="rId12"/>
-    <sheet name="WorkBasketInputFields" sheetId="12" r:id="rId13"/>
-    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId14"/>
-    <sheet name="UserProfile" sheetId="14" r:id="rId15"/>
-    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId16"/>
-    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId17"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId18"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId19"/>
-    <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId20"/>
+    <sheet name="SearchInputFields" sheetId="10" r:id="rId10"/>
+    <sheet name="SearchResultFields" sheetId="11" r:id="rId11"/>
+    <sheet name="WorkBasketInputFields" sheetId="12" r:id="rId12"/>
+    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId13"/>
+    <sheet name="UserProfile" sheetId="14" r:id="rId14"/>
+    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId15"/>
+    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId16"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId17"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId18"/>
+    <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$T$110</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$2:$L$98</definedName>
@@ -45,9 +44,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ComplexTypes!$A$3:$M$232</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">FixedLists!$A$1:$E$702</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">State!$A$3:$H$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">WorkBasketInputFields!$A$3:$G$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">WorkBasketResultFields!$A$3:$G$3</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="16">AuthorisationCaseField!$J$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="15">AuthorisationCaseField!$J$5</definedName>
     <definedName name="_xlnm.Extract" localSheetId="5">CaseTypeTab!$K$61</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="177">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -680,57 +679,12 @@
   <si>
     <t>Field to use for the order of results</t>
   </si>
-  <si>
-    <t>EventToComplexTypes</t>
-  </si>
-  <si>
-    <t>New Override label</t>
-  </si>
-  <si>
-    <t>new Override Hint Text</t>
-  </si>
-  <si>
-    <t>Order of fields</t>
-  </si>
-  <si>
-    <t>MaxLength: 70</t>
-  </si>
-  <si>
-    <t>Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
-  </si>
-  <si>
-    <t>Always top level case field ID (from CaseField tab)</t>
-  </si>
-  <si>
-    <t>MaxLength:200</t>
-  </si>
-  <si>
-    <t>MaxLength: 300</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>Accepted Values: MANDATORY, READONLY, OPTIONAL for mandatory, readonly and optional data on UI</t>
-  </si>
-  <si>
-    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;</t>
-  </si>
-  <si>
-    <t>EventElementLabel</t>
-  </si>
-  <si>
-    <t>EventHintText</t>
-  </si>
-  <si>
-    <t>FieldDisplayOrder</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="39">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -965,45 +919,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1016,14 +933,8 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0432FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="28">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1284,54 +1195,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1340,7 +1203,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="211">
+  <cellXfs count="196">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1601,51 +1464,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="33" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2923,137 +2741,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C049F10D-F059-F941-9EA1-9C15C4FFCFC4}">
-  <dimension ref="A1:K4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="18">
-      <c r="A1" s="196" t="s">
-        <v>177</v>
-      </c>
-      <c r="B1" s="197" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="198" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="199" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="197" t="s">
-        <v>178</v>
-      </c>
-      <c r="H1" s="197" t="s">
-        <v>179</v>
-      </c>
-      <c r="I1" s="197" t="s">
-        <v>180</v>
-      </c>
-      <c r="J1" s="200"/>
-      <c r="K1" s="197"/>
-    </row>
-    <row r="2" spans="1:11" ht="122" customHeight="1">
-      <c r="A2" s="201"/>
-      <c r="B2" s="201"/>
-      <c r="C2" s="202" t="s">
-        <v>181</v>
-      </c>
-      <c r="D2" s="203" t="s">
-        <v>182</v>
-      </c>
-      <c r="E2" s="203" t="s">
-        <v>183</v>
-      </c>
-      <c r="F2" s="201" t="s">
-        <v>181</v>
-      </c>
-      <c r="G2" s="201" t="s">
-        <v>184</v>
-      </c>
-      <c r="H2" s="201" t="s">
-        <v>185</v>
-      </c>
-      <c r="I2" s="203" t="s">
-        <v>186</v>
-      </c>
-      <c r="J2" s="203" t="s">
-        <v>187</v>
-      </c>
-      <c r="K2" s="204" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1">
-      <c r="A3" s="205" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="206" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="206" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="206" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="206" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="206" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="206" t="s">
-        <v>189</v>
-      </c>
-      <c r="H3" s="206" t="s">
-        <v>190</v>
-      </c>
-      <c r="I3" s="206" t="s">
-        <v>191</v>
-      </c>
-      <c r="J3" s="206" t="s">
-        <v>128</v>
-      </c>
-      <c r="K3" s="207" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="208"/>
-      <c r="B4" s="200"/>
-      <c r="C4" s="200"/>
-      <c r="D4" s="209"/>
-      <c r="E4" s="209"/>
-      <c r="F4" s="209"/>
-      <c r="G4" s="200"/>
-      <c r="H4" s="200"/>
-      <c r="I4" s="200"/>
-      <c r="J4" s="209"/>
-      <c r="K4" s="210"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:H573"/>
+  <dimension ref="A1:I573"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A573"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3061,13 +2753,13 @@
     <col min="1" max="1" width="34" style="1" customWidth="1"/>
     <col min="2" max="3" width="8.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="32.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="1" customWidth="1"/>
-    <col min="8" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="5" max="6" width="36.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="1" customWidth="1"/>
+    <col min="9" max="1026" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="195" t="s">
         <v>136</v>
       </c>
@@ -3081,10 +2773,11 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="2"/>
       <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="39" customHeight="1">
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="39" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -3098,14 +2791,15 @@
       <c r="E2" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="59" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="59" t="s">
         <v>144</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1">
+    <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
@@ -3122,305 +2816,340 @@
         <v>77</v>
       </c>
       <c r="F3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1">
+    <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
       <c r="C4" s="9"/>
       <c r="D4" s="11"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1">
+      <c r="G4" s="9"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
       <c r="C5" s="12"/>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="45"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1">
+      <c r="G5" s="12"/>
+      <c r="H5" s="45"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="12"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="45"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1">
+      <c r="G6" s="12"/>
+      <c r="H6" s="45"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="12"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="45"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1">
+      <c r="G7" s="12"/>
+      <c r="H7" s="45"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="22"/>
       <c r="B8" s="22"/>
       <c r="C8" s="12"/>
       <c r="D8" s="45"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="45"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1">
+      <c r="G8" s="11"/>
+      <c r="H8" s="45"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="106"/>
-      <c r="G9" s="87"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1">
+      <c r="F9" s="19"/>
+      <c r="G9" s="106"/>
+      <c r="H9" s="87"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="12"/>
       <c r="D10" s="20"/>
       <c r="E10" s="17"/>
-      <c r="F10" s="106"/>
-      <c r="G10" s="45"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1">
+      <c r="F10" s="17"/>
+      <c r="G10" s="106"/>
+      <c r="H10" s="45"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="45"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1">
+      <c r="G11" s="12"/>
+      <c r="H11" s="45"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="22"/>
       <c r="B12" s="22"/>
       <c r="C12" s="9"/>
       <c r="D12" s="15"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="74"/>
-    </row>
-    <row r="13" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="G12" s="9"/>
+      <c r="H12" s="74"/>
+    </row>
+    <row r="13" spans="1:8" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
       <c r="C13" s="9"/>
       <c r="D13" s="11"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="74"/>
-    </row>
-    <row r="14" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="G13" s="9"/>
+      <c r="H13" s="74"/>
+    </row>
+    <row r="14" spans="1:8" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A14" s="22"/>
       <c r="B14" s="22"/>
       <c r="C14" s="9"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="74"/>
-    </row>
-    <row r="15" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="F14" s="11"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="74"/>
+    </row>
+    <row r="15" spans="1:8" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
       <c r="C15" s="9"/>
       <c r="D15" s="11"/>
       <c r="E15" s="16"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="74"/>
-    </row>
-    <row r="16" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="F15" s="16"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="74"/>
+    </row>
+    <row r="16" spans="1:8" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="22"/>
       <c r="B16" s="22"/>
       <c r="C16" s="12"/>
       <c r="D16" s="11"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="45"/>
-    </row>
-    <row r="17" spans="1:8" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="G16" s="9"/>
+      <c r="H16" s="45"/>
+    </row>
+    <row r="17" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="22"/>
       <c r="B17" s="22"/>
       <c r="C17" s="9"/>
       <c r="D17" s="15"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="87"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1">
+      <c r="F17" s="19"/>
+      <c r="G17" s="106"/>
+      <c r="H17" s="87"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
       <c r="C18" s="9"/>
       <c r="D18" s="15"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="87"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1">
+      <c r="G18" s="12"/>
+      <c r="H18" s="87"/>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="9"/>
       <c r="D19" s="15"/>
       <c r="E19" s="17"/>
-      <c r="F19" s="106"/>
-      <c r="G19" s="87"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1">
+      <c r="F19" s="17"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="87"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="9"/>
       <c r="D20" s="15"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="87"/>
-    </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1">
+      <c r="G20" s="9"/>
+      <c r="H20" s="87"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1">
       <c r="A21" s="22"/>
       <c r="B21" s="22"/>
       <c r="C21" s="12"/>
       <c r="D21" s="15"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="106"/>
-      <c r="G21" s="87"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1">
+      <c r="F21" s="19"/>
+      <c r="G21" s="106"/>
+      <c r="H21" s="87"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
       <c r="C22" s="12"/>
       <c r="D22" s="15"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="87"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1">
+      <c r="F22" s="14"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="87"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1">
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
       <c r="C23" s="12"/>
       <c r="D23" s="15"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="45"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1">
+      <c r="F23" s="9"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="45"/>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1">
       <c r="A24" s="22"/>
       <c r="B24" s="22"/>
       <c r="C24" s="12"/>
       <c r="D24" s="15"/>
       <c r="E24" s="33"/>
-      <c r="F24" s="106"/>
-      <c r="G24" s="87"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1">
+      <c r="F24" s="33"/>
+      <c r="G24" s="106"/>
+      <c r="H24" s="87"/>
+    </row>
+    <row r="25" spans="1:9" ht="15" customHeight="1">
       <c r="A25" s="22"/>
       <c r="B25" s="22"/>
       <c r="C25" s="9"/>
       <c r="D25" s="15"/>
       <c r="E25" s="17"/>
-      <c r="F25" s="106"/>
-      <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1">
+      <c r="F25" s="17"/>
+      <c r="G25" s="106"/>
+      <c r="H25" s="18"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" customHeight="1">
       <c r="A26" s="22"/>
       <c r="B26" s="22"/>
       <c r="C26" s="145"/>
       <c r="D26" s="11"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="106"/>
-      <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1">
+      <c r="F26" s="17"/>
+      <c r="G26" s="106"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="1:9" ht="15" customHeight="1">
       <c r="A27" s="22"/>
       <c r="B27" s="22"/>
       <c r="C27" s="9"/>
       <c r="D27" s="15"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="106"/>
-      <c r="G27" s="87"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1">
+      <c r="F27" s="17"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="87"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" customHeight="1">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="9"/>
       <c r="D28" s="15"/>
       <c r="E28" s="17"/>
-      <c r="F28" s="106"/>
-      <c r="G28" s="87"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1">
+      <c r="F28" s="17"/>
+      <c r="G28" s="106"/>
+      <c r="H28" s="87"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" customHeight="1">
       <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="9"/>
       <c r="D29" s="15"/>
       <c r="E29" s="17"/>
-      <c r="F29" s="106"/>
-      <c r="G29" s="87"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1">
+      <c r="F29" s="17"/>
+      <c r="G29" s="106"/>
+      <c r="H29" s="87"/>
+    </row>
+    <row r="30" spans="1:9" ht="15" customHeight="1">
       <c r="A30" s="22"/>
       <c r="B30" s="22"/>
       <c r="C30" s="16"/>
       <c r="D30" s="15"/>
       <c r="E30" s="17"/>
-      <c r="F30" s="106"/>
-      <c r="G30" s="87"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1">
+      <c r="F30" s="17"/>
+      <c r="G30" s="106"/>
+      <c r="H30" s="87"/>
+    </row>
+    <row r="31" spans="1:9" ht="15" customHeight="1">
       <c r="A31" s="22"/>
       <c r="B31" s="22"/>
       <c r="C31" s="16"/>
       <c r="D31" s="18"/>
       <c r="E31" s="17"/>
-      <c r="F31" s="106"/>
-      <c r="G31" s="18"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1">
+      <c r="F31" s="17"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32" spans="1:9" ht="15" customHeight="1">
       <c r="A32" s="22"/>
       <c r="B32" s="22"/>
       <c r="C32" s="9"/>
       <c r="D32" s="11"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="57"/>
-    </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1">
+      <c r="G32" s="9"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="57"/>
+    </row>
+    <row r="33" spans="1:9" ht="15" customHeight="1">
       <c r="A33" s="22"/>
       <c r="B33" s="22"/>
       <c r="C33" s="9"/>
       <c r="D33" s="11"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="57"/>
-    </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1">
+      <c r="G33" s="9"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="57"/>
+    </row>
+    <row r="34" spans="1:9" ht="15" customHeight="1">
       <c r="A34" s="22"/>
       <c r="B34" s="22"/>
       <c r="C34" s="9"/>
       <c r="D34" s="11"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="57"/>
-    </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1">
+      <c r="G34" s="9"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="57"/>
+    </row>
+    <row r="35" spans="1:9" ht="15" customHeight="1">
       <c r="A35" s="22"/>
       <c r="B35" s="22"/>
       <c r="C35" s="9"/>
       <c r="D35" s="11"/>
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="57"/>
-    </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1">
+      <c r="G35" s="9"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="57"/>
+    </row>
+    <row r="36" spans="1:9" ht="15" customHeight="1">
       <c r="A36" s="22"/>
       <c r="B36" s="22"/>
       <c r="C36" s="9"/>
@@ -3428,72 +3157,76 @@
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
-      <c r="H36" s="57"/>
-    </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1">
+      <c r="H36" s="11"/>
+      <c r="I36" s="57"/>
+    </row>
+    <row r="37" spans="1:9" ht="15" customHeight="1">
       <c r="A37" s="22"/>
       <c r="B37" s="22"/>
       <c r="C37" s="9"/>
       <c r="D37" s="11"/>
       <c r="E37" s="9"/>
       <c r="F37" s="19"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="57"/>
-    </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1">
+      <c r="G37" s="19"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="57"/>
+    </row>
+    <row r="38" spans="1:9" ht="15" customHeight="1">
       <c r="A38" s="22"/>
       <c r="B38" s="22"/>
       <c r="C38" s="16"/>
       <c r="D38" s="11"/>
       <c r="E38" s="14"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="57"/>
-    </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1">
+      <c r="F38" s="14"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="57"/>
+    </row>
+    <row r="39" spans="1:9" ht="15" customHeight="1">
       <c r="A39" s="22"/>
       <c r="B39" s="22"/>
       <c r="C39" s="16"/>
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
-      <c r="F39" s="106"/>
-      <c r="G39" s="15"/>
-    </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1">
+      <c r="F39" s="18"/>
+      <c r="G39" s="106"/>
+      <c r="H39" s="15"/>
+    </row>
+    <row r="40" spans="1:9" ht="15" customHeight="1">
       <c r="A40" s="22"/>
       <c r="B40" s="22"/>
-      <c r="G40" s="146"/>
-    </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1">
+      <c r="H40" s="146"/>
+    </row>
+    <row r="41" spans="1:9" ht="15" customHeight="1">
       <c r="A41" s="22"/>
       <c r="B41" s="22"/>
-      <c r="G41" s="146"/>
-    </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1">
+      <c r="H41" s="146"/>
+    </row>
+    <row r="42" spans="1:9" ht="15" customHeight="1">
       <c r="A42" s="22"/>
       <c r="B42" s="22"/>
     </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1">
+    <row r="43" spans="1:9" ht="15" customHeight="1">
       <c r="A43" s="22"/>
       <c r="B43" s="22"/>
     </row>
-    <row r="44" spans="1:8" ht="15" customHeight="1">
+    <row r="44" spans="1:9" ht="15" customHeight="1">
       <c r="A44" s="22"/>
       <c r="B44" s="22"/>
     </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1">
+    <row r="45" spans="1:9" ht="15" customHeight="1">
       <c r="A45" s="22"/>
       <c r="B45" s="22"/>
     </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1">
+    <row r="46" spans="1:9" ht="15" customHeight="1">
       <c r="A46" s="22"/>
       <c r="B46" s="22"/>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1">
+    <row r="47" spans="1:9" ht="15" customHeight="1">
       <c r="A47" s="22"/>
       <c r="B47" s="22"/>
     </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1">
+    <row r="48" spans="1:9" ht="15" customHeight="1">
       <c r="A48" s="22"/>
       <c r="B48" s="22"/>
     </row>
@@ -5124,12 +4857,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D1:D1048576"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5137,13 +4870,13 @@
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
     <col min="2" max="3" width="8.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="32.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="1" customWidth="1"/>
-    <col min="8" max="1026" width="8.83203125" customWidth="1"/>
+    <col min="5" max="6" width="41.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="1" customWidth="1"/>
+    <col min="9" max="1027" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>139</v>
       </c>
@@ -5157,10 +4890,11 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="2"/>
       <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="39" customHeight="1">
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="39" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -5174,14 +4908,994 @@
       <c r="E2" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1">
+    <row r="3" spans="1:8" ht="15" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" s="24" customFormat="1" ht="15" customHeight="1">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="63"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="D15" s="11"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1">
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="D20" s="15"/>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1">
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="D22" s="15"/>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="D23" s="15"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="D24" s="15"/>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="D25" s="15"/>
+    </row>
+    <row r="26" spans="1:4" ht="15" customHeight="1">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="D27" s="15"/>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="D28" s="15"/>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="D29" s="15"/>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="D30" s="15"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="D31" s="18"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1">
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1">
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="D34" s="11"/>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:4" ht="15" customHeight="1">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="D39" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:I91"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34" style="1" customWidth="1"/>
+    <col min="2" max="3" width="8.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5" style="1" customWidth="1"/>
+    <col min="5" max="6" width="36.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="1" customWidth="1"/>
+    <col min="9" max="1026" width="8.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="39" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="59" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1">
+      <c r="A3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="45"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="45"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="45"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="45"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="106"/>
+      <c r="H9" s="87"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="106"/>
+      <c r="H10" s="45"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="45"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="74"/>
+    </row>
+    <row r="13" spans="1:8" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="74"/>
+    </row>
+    <row r="14" spans="1:8" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="74"/>
+    </row>
+    <row r="15" spans="1:8" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="74"/>
+    </row>
+    <row r="16" spans="1:8" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="45"/>
+    </row>
+    <row r="17" spans="1:9" s="29" customFormat="1" ht="15" customHeight="1">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="106"/>
+      <c r="H17" s="87"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="87"/>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1">
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="87"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="87"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1">
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="106"/>
+      <c r="H21" s="87"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="87"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="45"/>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="106"/>
+      <c r="H24" s="87"/>
+    </row>
+    <row r="25" spans="1:9" ht="15" customHeight="1">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="106"/>
+      <c r="H25" s="18"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" customHeight="1">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="145"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="106"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="1:9" ht="15" customHeight="1">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="87"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" customHeight="1">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="106"/>
+      <c r="H28" s="87"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" customHeight="1">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="106"/>
+      <c r="H29" s="87"/>
+    </row>
+    <row r="30" spans="1:9" ht="15" customHeight="1">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="106"/>
+      <c r="H30" s="87"/>
+    </row>
+    <row r="31" spans="1:9" ht="15" customHeight="1">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32" spans="1:9" ht="15" customHeight="1">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="57"/>
+    </row>
+    <row r="33" spans="1:9" ht="15" customHeight="1">
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="57"/>
+    </row>
+    <row r="34" spans="1:9" ht="15" customHeight="1">
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="57"/>
+    </row>
+    <row r="35" spans="1:9" ht="15" customHeight="1">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="57"/>
+    </row>
+    <row r="36" spans="1:9" ht="15" customHeight="1">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="57"/>
+    </row>
+    <row r="37" spans="1:9" ht="15" customHeight="1">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="57"/>
+    </row>
+    <row r="38" spans="1:9" ht="15" customHeight="1">
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="57"/>
+    </row>
+    <row r="39" spans="1:9" ht="15" customHeight="1">
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="106"/>
+      <c r="H39" s="15"/>
+    </row>
+    <row r="40" spans="1:9" ht="15" customHeight="1">
+      <c r="A40" s="22"/>
+      <c r="B40" s="22"/>
+      <c r="H40" s="146"/>
+    </row>
+    <row r="41" spans="1:9" ht="15" customHeight="1">
+      <c r="A41" s="22"/>
+      <c r="B41" s="22"/>
+      <c r="H41" s="146"/>
+    </row>
+    <row r="42" spans="1:9" ht="15" customHeight="1">
+      <c r="A42" s="22"/>
+      <c r="B42" s="22"/>
+    </row>
+    <row r="43" spans="1:9" ht="15" customHeight="1">
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+    </row>
+    <row r="44" spans="1:9" ht="15" customHeight="1">
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
+    </row>
+    <row r="45" spans="1:9" ht="15" customHeight="1">
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
+    </row>
+    <row r="46" spans="1:9" ht="15" customHeight="1">
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
+    </row>
+    <row r="47" spans="1:9" ht="15" customHeight="1">
+      <c r="A47" s="22"/>
+      <c r="B47" s="22"/>
+    </row>
+    <row r="48" spans="1:9" ht="15" customHeight="1">
+      <c r="A48" s="22"/>
+      <c r="B48" s="22"/>
+    </row>
+    <row r="49" spans="1:2" ht="15" customHeight="1">
+      <c r="A49" s="22"/>
+      <c r="B49" s="22"/>
+    </row>
+    <row r="50" spans="1:2" ht="15" customHeight="1">
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
+    </row>
+    <row r="51" spans="1:2" ht="15" customHeight="1">
+      <c r="A51" s="22"/>
+      <c r="B51" s="22"/>
+    </row>
+    <row r="52" spans="1:2" ht="15" customHeight="1">
+      <c r="A52" s="22"/>
+      <c r="B52" s="22"/>
+    </row>
+    <row r="53" spans="1:2" ht="15" customHeight="1">
+      <c r="A53" s="22"/>
+      <c r="B53" s="22"/>
+    </row>
+    <row r="54" spans="1:2" ht="15" customHeight="1">
+      <c r="A54" s="22"/>
+      <c r="B54" s="22"/>
+    </row>
+    <row r="55" spans="1:2" ht="15" customHeight="1">
+      <c r="A55" s="22"/>
+      <c r="B55" s="22"/>
+    </row>
+    <row r="56" spans="1:2" ht="15" customHeight="1">
+      <c r="A56" s="22"/>
+      <c r="B56" s="22"/>
+    </row>
+    <row r="57" spans="1:2" ht="15" customHeight="1">
+      <c r="A57" s="22"/>
+      <c r="B57" s="22"/>
+    </row>
+    <row r="58" spans="1:2" ht="15" customHeight="1">
+      <c r="A58" s="22"/>
+      <c r="B58" s="22"/>
+    </row>
+    <row r="59" spans="1:2" ht="15" customHeight="1">
+      <c r="A59" s="22"/>
+      <c r="B59" s="22"/>
+    </row>
+    <row r="60" spans="1:2" ht="15" customHeight="1">
+      <c r="A60" s="22"/>
+      <c r="B60" s="22"/>
+    </row>
+    <row r="61" spans="1:2" ht="15" customHeight="1">
+      <c r="A61" s="22"/>
+      <c r="B61" s="22"/>
+    </row>
+    <row r="62" spans="1:2" ht="15" customHeight="1">
+      <c r="A62" s="22"/>
+      <c r="B62" s="22"/>
+    </row>
+    <row r="63" spans="1:2" ht="15" customHeight="1">
+      <c r="A63" s="22"/>
+      <c r="B63" s="22"/>
+    </row>
+    <row r="64" spans="1:2" ht="15" customHeight="1">
+      <c r="A64" s="22"/>
+      <c r="B64" s="22"/>
+    </row>
+    <row r="65" spans="1:2" ht="15" customHeight="1">
+      <c r="A65" s="22"/>
+      <c r="B65" s="22"/>
+    </row>
+    <row r="66" spans="1:2" ht="15" customHeight="1">
+      <c r="A66" s="22"/>
+      <c r="B66" s="22"/>
+    </row>
+    <row r="67" spans="1:2" ht="15" customHeight="1">
+      <c r="A67" s="22"/>
+      <c r="B67" s="22"/>
+    </row>
+    <row r="68" spans="1:2" ht="15" customHeight="1">
+      <c r="A68" s="22"/>
+      <c r="B68" s="22"/>
+    </row>
+    <row r="69" spans="1:2" ht="15" customHeight="1">
+      <c r="A69" s="22"/>
+      <c r="B69" s="22"/>
+    </row>
+    <row r="70" spans="1:2" ht="15" customHeight="1">
+      <c r="A70" s="22"/>
+      <c r="B70" s="22"/>
+    </row>
+    <row r="71" spans="1:2" ht="15" customHeight="1">
+      <c r="A71" s="22"/>
+      <c r="B71" s="22"/>
+    </row>
+    <row r="72" spans="1:2" ht="15" customHeight="1">
+      <c r="A72" s="22"/>
+      <c r="B72" s="22"/>
+    </row>
+    <row r="73" spans="1:2" ht="15" customHeight="1">
+      <c r="A73" s="22"/>
+      <c r="B73" s="22"/>
+    </row>
+    <row r="74" spans="1:2" ht="15" customHeight="1">
+      <c r="A74" s="22"/>
+      <c r="B74" s="22"/>
+    </row>
+    <row r="75" spans="1:2" ht="15" customHeight="1">
+      <c r="A75" s="22"/>
+      <c r="B75" s="22"/>
+    </row>
+    <row r="76" spans="1:2" ht="15" customHeight="1">
+      <c r="A76" s="22"/>
+      <c r="B76" s="22"/>
+    </row>
+    <row r="77" spans="1:2" ht="15" customHeight="1">
+      <c r="A77" s="22"/>
+      <c r="B77" s="22"/>
+    </row>
+    <row r="78" spans="1:2" ht="15" customHeight="1">
+      <c r="A78" s="22"/>
+      <c r="B78" s="22"/>
+    </row>
+    <row r="79" spans="1:2" ht="15" customHeight="1">
+      <c r="A79" s="22"/>
+      <c r="B79" s="22"/>
+    </row>
+    <row r="80" spans="1:2" ht="15" customHeight="1">
+      <c r="A80" s="22"/>
+      <c r="B80" s="22"/>
+    </row>
+    <row r="81" spans="1:2" ht="15" customHeight="1">
+      <c r="A81" s="22"/>
+      <c r="B81" s="22"/>
+    </row>
+    <row r="82" spans="1:2" ht="15" customHeight="1">
+      <c r="A82" s="22"/>
+      <c r="B82" s="22"/>
+    </row>
+    <row r="83" spans="1:2" ht="15" customHeight="1">
+      <c r="A83" s="22"/>
+      <c r="B83" s="22"/>
+    </row>
+    <row r="84" spans="1:2" ht="15" customHeight="1">
+      <c r="A84" s="22"/>
+      <c r="B84" s="22"/>
+    </row>
+    <row r="85" spans="1:2" ht="15" customHeight="1">
+      <c r="A85" s="22"/>
+      <c r="B85" s="22"/>
+    </row>
+    <row r="86" spans="1:2" ht="15" customHeight="1">
+      <c r="A86" s="22"/>
+      <c r="B86" s="22"/>
+    </row>
+    <row r="87" spans="1:2" ht="15" customHeight="1">
+      <c r="A87" s="22"/>
+      <c r="B87" s="22"/>
+    </row>
+    <row r="88" spans="1:2" ht="15" customHeight="1">
+      <c r="A88" s="22"/>
+      <c r="B88" s="22"/>
+    </row>
+    <row r="89" spans="1:2" ht="15" customHeight="1">
+      <c r="A89" s="22"/>
+      <c r="B89" s="22"/>
+    </row>
+    <row r="90" spans="1:2" ht="15" customHeight="1">
+      <c r="A90" s="22"/>
+      <c r="B90" s="22"/>
+    </row>
+    <row r="91" spans="1:2" ht="15" customHeight="1">
+      <c r="A91" s="22"/>
+      <c r="B91" s="22"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A3:H30" xr:uid="{00000000-0009-0000-0000-00000B000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:I1048576"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="54" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" ht="39" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="194" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -5198,999 +5912,76 @@
         <v>77</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1">
+      <c r="I3" s="195" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1">
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1">
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1">
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1">
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1">
       <c r="A8" s="22"/>
       <c r="B8" s="22"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" s="24" customFormat="1" ht="15" customHeight="1">
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1">
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="63"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1">
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1">
+      <c r="G10" s="57"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1">
+      <c r="G11" s="146"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1">
       <c r="A12" s="22"/>
       <c r="B12" s="22"/>
-      <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1">
+      <c r="G12" s="146"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1">
+      <c r="G13" s="146"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1">
       <c r="A14" s="22"/>
       <c r="B14" s="22"/>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1">
+      <c r="G14" s="146"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
-      <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1">
+      <c r="G15" s="146"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1">
       <c r="A16" s="22"/>
       <c r="B16" s="22"/>
-      <c r="D16" s="11"/>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="D18" s="15"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="D20" s="15"/>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="D21" s="15"/>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="D22" s="15"/>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="D23" s="15"/>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="D24" s="15"/>
-    </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="D25" s="15"/>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="D26" s="11"/>
-    </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="D27" s="15"/>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="D28" s="15"/>
-    </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="D29" s="15"/>
-    </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="D30" s="15"/>
-    </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="D31" s="18"/>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-      <c r="D32" s="11"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-      <c r="D33" s="11"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1">
-      <c r="A34" s="22"/>
-      <c r="B34" s="22"/>
-      <c r="D34" s="11"/>
-    </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
-      <c r="D35" s="11"/>
-    </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
-      <c r="D36" s="11"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="D37" s="11"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="D38" s="11"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="D39" s="18"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:H91"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="34" style="1" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="1" customWidth="1"/>
-    <col min="8" max="1025" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="39" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1">
-      <c r="A3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="45"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="45"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="45"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="45"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="106"/>
-      <c r="G9" s="87"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="106"/>
-      <c r="G10" s="45"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="45"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="74"/>
-    </row>
-    <row r="13" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="74"/>
-    </row>
-    <row r="14" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="74"/>
-    </row>
-    <row r="15" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="74"/>
-    </row>
-    <row r="16" spans="1:7" s="29" customFormat="1" ht="15" customHeight="1">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="45"/>
-    </row>
-    <row r="17" spans="1:8" s="29" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="87"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="87"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="106"/>
-      <c r="G19" s="87"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="87"/>
-    </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="106"/>
-      <c r="G21" s="87"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="87"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="45"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="106"/>
-      <c r="G24" s="87"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="106"/>
-      <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="145"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="106"/>
-      <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="106"/>
-      <c r="G27" s="87"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="106"/>
-      <c r="G28" s="87"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="106"/>
-      <c r="G29" s="87"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="106"/>
-      <c r="G30" s="87"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="106"/>
-      <c r="G31" s="18"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="57"/>
-    </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="57"/>
-    </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1">
-      <c r="A34" s="22"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="57"/>
-    </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="57"/>
-    </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="57"/>
-    </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="57"/>
-    </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="57"/>
-    </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1">
-      <c r="A39" s="22"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="106"/>
-      <c r="G39" s="15"/>
-    </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1">
-      <c r="A40" s="22"/>
-      <c r="B40" s="22"/>
-      <c r="G40" s="146"/>
-    </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1">
-      <c r="A41" s="22"/>
-      <c r="B41" s="22"/>
-      <c r="G41" s="146"/>
-    </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
-    </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
-    </row>
-    <row r="44" spans="1:8" ht="15" customHeight="1">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
-    </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
-    </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
-    </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1">
-      <c r="A47" s="22"/>
-      <c r="B47" s="22"/>
-    </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1">
-      <c r="A48" s="22"/>
-      <c r="B48" s="22"/>
-    </row>
-    <row r="49" spans="1:2" ht="15" customHeight="1">
-      <c r="A49" s="22"/>
-      <c r="B49" s="22"/>
-    </row>
-    <row r="50" spans="1:2" ht="15" customHeight="1">
-      <c r="A50" s="22"/>
-      <c r="B50" s="22"/>
-    </row>
-    <row r="51" spans="1:2" ht="15" customHeight="1">
-      <c r="A51" s="22"/>
-      <c r="B51" s="22"/>
-    </row>
-    <row r="52" spans="1:2" ht="15" customHeight="1">
-      <c r="A52" s="22"/>
-      <c r="B52" s="22"/>
-    </row>
-    <row r="53" spans="1:2" ht="15" customHeight="1">
-      <c r="A53" s="22"/>
-      <c r="B53" s="22"/>
-    </row>
-    <row r="54" spans="1:2" ht="15" customHeight="1">
-      <c r="A54" s="22"/>
-      <c r="B54" s="22"/>
-    </row>
-    <row r="55" spans="1:2" ht="15" customHeight="1">
-      <c r="A55" s="22"/>
-      <c r="B55" s="22"/>
-    </row>
-    <row r="56" spans="1:2" ht="15" customHeight="1">
-      <c r="A56" s="22"/>
-      <c r="B56" s="22"/>
-    </row>
-    <row r="57" spans="1:2" ht="15" customHeight="1">
-      <c r="A57" s="22"/>
-      <c r="B57" s="22"/>
-    </row>
-    <row r="58" spans="1:2" ht="15" customHeight="1">
-      <c r="A58" s="22"/>
-      <c r="B58" s="22"/>
-    </row>
-    <row r="59" spans="1:2" ht="15" customHeight="1">
-      <c r="A59" s="22"/>
-      <c r="B59" s="22"/>
-    </row>
-    <row r="60" spans="1:2" ht="15" customHeight="1">
-      <c r="A60" s="22"/>
-      <c r="B60" s="22"/>
-    </row>
-    <row r="61" spans="1:2" ht="15" customHeight="1">
-      <c r="A61" s="22"/>
-      <c r="B61" s="22"/>
-    </row>
-    <row r="62" spans="1:2" ht="15" customHeight="1">
-      <c r="A62" s="22"/>
-      <c r="B62" s="22"/>
-    </row>
-    <row r="63" spans="1:2" ht="15" customHeight="1">
-      <c r="A63" s="22"/>
-      <c r="B63" s="22"/>
-    </row>
-    <row r="64" spans="1:2" ht="15" customHeight="1">
-      <c r="A64" s="22"/>
-      <c r="B64" s="22"/>
-    </row>
-    <row r="65" spans="1:2" ht="15" customHeight="1">
-      <c r="A65" s="22"/>
-      <c r="B65" s="22"/>
-    </row>
-    <row r="66" spans="1:2" ht="15" customHeight="1">
-      <c r="A66" s="22"/>
-      <c r="B66" s="22"/>
-    </row>
-    <row r="67" spans="1:2" ht="15" customHeight="1">
-      <c r="A67" s="22"/>
-      <c r="B67" s="22"/>
-    </row>
-    <row r="68" spans="1:2" ht="15" customHeight="1">
-      <c r="A68" s="22"/>
-      <c r="B68" s="22"/>
-    </row>
-    <row r="69" spans="1:2" ht="15" customHeight="1">
-      <c r="A69" s="22"/>
-      <c r="B69" s="22"/>
-    </row>
-    <row r="70" spans="1:2" ht="15" customHeight="1">
-      <c r="A70" s="22"/>
-      <c r="B70" s="22"/>
-    </row>
-    <row r="71" spans="1:2" ht="15" customHeight="1">
-      <c r="A71" s="22"/>
-      <c r="B71" s="22"/>
-    </row>
-    <row r="72" spans="1:2" ht="15" customHeight="1">
-      <c r="A72" s="22"/>
-      <c r="B72" s="22"/>
-    </row>
-    <row r="73" spans="1:2" ht="15" customHeight="1">
-      <c r="A73" s="22"/>
-      <c r="B73" s="22"/>
-    </row>
-    <row r="74" spans="1:2" ht="15" customHeight="1">
-      <c r="A74" s="22"/>
-      <c r="B74" s="22"/>
-    </row>
-    <row r="75" spans="1:2" ht="15" customHeight="1">
-      <c r="A75" s="22"/>
-      <c r="B75" s="22"/>
-    </row>
-    <row r="76" spans="1:2" ht="15" customHeight="1">
-      <c r="A76" s="22"/>
-      <c r="B76" s="22"/>
-    </row>
-    <row r="77" spans="1:2" ht="15" customHeight="1">
-      <c r="A77" s="22"/>
-      <c r="B77" s="22"/>
-    </row>
-    <row r="78" spans="1:2" ht="15" customHeight="1">
-      <c r="A78" s="22"/>
-      <c r="B78" s="22"/>
-    </row>
-    <row r="79" spans="1:2" ht="15" customHeight="1">
-      <c r="A79" s="22"/>
-      <c r="B79" s="22"/>
-    </row>
-    <row r="80" spans="1:2" ht="15" customHeight="1">
-      <c r="A80" s="22"/>
-      <c r="B80" s="22"/>
-    </row>
-    <row r="81" spans="1:2" ht="15" customHeight="1">
-      <c r="A81" s="22"/>
-      <c r="B81" s="22"/>
-    </row>
-    <row r="82" spans="1:2" ht="15" customHeight="1">
-      <c r="A82" s="22"/>
-      <c r="B82" s="22"/>
-    </row>
-    <row r="83" spans="1:2" ht="15" customHeight="1">
-      <c r="A83" s="22"/>
-      <c r="B83" s="22"/>
-    </row>
-    <row r="84" spans="1:2" ht="15" customHeight="1">
-      <c r="A84" s="22"/>
-      <c r="B84" s="22"/>
-    </row>
-    <row r="85" spans="1:2" ht="15" customHeight="1">
-      <c r="A85" s="22"/>
-      <c r="B85" s="22"/>
-    </row>
-    <row r="86" spans="1:2" ht="15" customHeight="1">
-      <c r="A86" s="22"/>
-      <c r="B86" s="22"/>
-    </row>
-    <row r="87" spans="1:2" ht="15" customHeight="1">
-      <c r="A87" s="22"/>
-      <c r="B87" s="22"/>
-    </row>
-    <row r="88" spans="1:2" ht="15" customHeight="1">
-      <c r="A88" s="22"/>
-      <c r="B88" s="22"/>
-    </row>
-    <row r="89" spans="1:2" ht="15" customHeight="1">
-      <c r="A89" s="22"/>
-      <c r="B89" s="22"/>
-    </row>
-    <row r="90" spans="1:2" ht="15" customHeight="1">
-      <c r="A90" s="22"/>
-      <c r="B90" s="22"/>
-    </row>
-    <row r="91" spans="1:2" ht="15" customHeight="1">
-      <c r="A91" s="22"/>
-      <c r="B91" s="22"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A3:G30" xr:uid="{00000000-0009-0000-0000-00000B000000}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:H1048576"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="54" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="1" customWidth="1"/>
-    <col min="8" max="1024" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" ht="39" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H2" s="194" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" s="195" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-    </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="F10" s="57"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="F11" s="146"/>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="F12" s="146"/>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="F13" s="146"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="F14" s="146"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="F15" s="146"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="F16" s="146"/>
+      <c r="G16" s="146"/>
     </row>
     <row r="17" spans="1:2" ht="15" customHeight="1">
       <c r="A17" s="22"/>
@@ -6503,7 +6294,7 @@
     <row r="1048575" ht="12.75" customHeight="1"/>
     <row r="1048576" ht="12.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A3:G3" xr:uid="{00000000-0009-0000-0000-00000C000000}"/>
+  <autoFilter ref="A3:H3" xr:uid="{00000000-0009-0000-0000-00000C000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -6512,7 +6303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
@@ -7180,7 +6971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:IV35"/>
   <sheetViews>
@@ -7405,7 +7196,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AMK1015"/>
   <sheetViews>
@@ -21425,7 +21216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMK696"/>
   <sheetViews>
@@ -27472,7 +27263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IV151"/>
   <sheetViews>
@@ -28520,6 +28311,311 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:AMK38"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="173" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="173" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="173" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="173" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="173" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="173" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="173" customWidth="1"/>
+    <col min="8" max="1025" width="10.83203125" style="173" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18">
+      <c r="A1" s="174" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="175" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="176" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="177" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+    </row>
+    <row r="2" spans="1:7" ht="71">
+      <c r="A2" s="179"/>
+      <c r="B2" s="179"/>
+      <c r="C2" s="180" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="180" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="180" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="180" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="180" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="181" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="181" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="182" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="182" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="182" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="181" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="181" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="178"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="184"/>
+      <c r="F4" s="184"/>
+      <c r="G4" s="178"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="178"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="184"/>
+      <c r="F5" s="184"/>
+      <c r="G5" s="178"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="178"/>
+      <c r="D6" s="183"/>
+      <c r="E6" s="184"/>
+      <c r="F6" s="184"/>
+      <c r="G6" s="178"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="178"/>
+      <c r="D7" s="183"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="178"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="178"/>
+      <c r="D8" s="183"/>
+      <c r="E8" s="184"/>
+      <c r="F8" s="184"/>
+      <c r="G8" s="178"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="183"/>
+      <c r="E9" s="184"/>
+      <c r="F9" s="184"/>
+      <c r="G9" s="178"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="178"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="178"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="178"/>
+      <c r="D11" s="178"/>
+      <c r="E11" s="178"/>
+      <c r="F11" s="184"/>
+      <c r="G11" s="178"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="178"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="178"/>
+      <c r="F12" s="184"/>
+      <c r="G12" s="178"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="178"/>
+      <c r="D13" s="178"/>
+      <c r="E13" s="184"/>
+      <c r="F13" s="184"/>
+      <c r="G13" s="178"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="178"/>
+      <c r="D14" s="178"/>
+      <c r="E14" s="184"/>
+      <c r="F14" s="184"/>
+      <c r="G14" s="178"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="178"/>
+      <c r="D15" s="178"/>
+      <c r="E15" s="184"/>
+      <c r="F15" s="184"/>
+      <c r="G15" s="178"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="178"/>
+      <c r="D16" s="178"/>
+      <c r="E16" s="184"/>
+      <c r="F16" s="184"/>
+      <c r="G16" s="178"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="178"/>
+      <c r="D17" s="178"/>
+      <c r="E17" s="184"/>
+      <c r="F17" s="184"/>
+      <c r="G17" s="178"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="178"/>
+      <c r="D18" s="178"/>
+      <c r="E18" s="178"/>
+      <c r="F18" s="184"/>
+      <c r="G18" s="178"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="178"/>
+      <c r="D19" s="178"/>
+      <c r="E19" s="178"/>
+      <c r="F19" s="184"/>
+      <c r="G19" s="178"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -28705,317 +28801,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:AMK38"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="33.1640625" style="173" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="173" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="173" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="173" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="173" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="173" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="173" customWidth="1"/>
-    <col min="8" max="1025" width="10.83203125" style="173" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="174" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="175" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="176" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="177" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-    </row>
-    <row r="2" spans="1:7" ht="71">
-      <c r="A2" s="179"/>
-      <c r="B2" s="179"/>
-      <c r="C2" s="180" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="180" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" s="180" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="180" t="s">
-        <v>156</v>
-      </c>
-      <c r="G2" s="180" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="181" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="181" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="182" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="182" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="182" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="181" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="181" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="178"/>
-      <c r="D4" s="183"/>
-      <c r="E4" s="184"/>
-      <c r="F4" s="184"/>
-      <c r="G4" s="178"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="178"/>
-      <c r="D5" s="183"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="184"/>
-      <c r="G5" s="178"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="178"/>
-      <c r="D6" s="183"/>
-      <c r="E6" s="184"/>
-      <c r="F6" s="184"/>
-      <c r="G6" s="178"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="178"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="184"/>
-      <c r="F7" s="184"/>
-      <c r="G7" s="178"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="178"/>
-      <c r="D8" s="183"/>
-      <c r="E8" s="184"/>
-      <c r="F8" s="184"/>
-      <c r="G8" s="178"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="178"/>
-      <c r="D9" s="183"/>
-      <c r="E9" s="184"/>
-      <c r="F9" s="184"/>
-      <c r="G9" s="178"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="178"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="184"/>
-      <c r="F10" s="184"/>
-      <c r="G10" s="178"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="178"/>
-      <c r="D11" s="178"/>
-      <c r="E11" s="178"/>
-      <c r="F11" s="184"/>
-      <c r="G11" s="178"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="178"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="178"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="178"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="178"/>
-      <c r="D13" s="178"/>
-      <c r="E13" s="184"/>
-      <c r="F13" s="184"/>
-      <c r="G13" s="178"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="178"/>
-      <c r="D14" s="178"/>
-      <c r="E14" s="184"/>
-      <c r="F14" s="184"/>
-      <c r="G14" s="178"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="178"/>
-      <c r="D15" s="178"/>
-      <c r="E15" s="184"/>
-      <c r="F15" s="184"/>
-      <c r="G15" s="178"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="178"/>
-      <c r="D16" s="178"/>
-      <c r="E16" s="184"/>
-      <c r="F16" s="184"/>
-      <c r="G16" s="178"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="178"/>
-      <c r="D17" s="178"/>
-      <c r="E17" s="184"/>
-      <c r="F17" s="184"/>
-      <c r="G17" s="178"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="178"/>
-      <c r="D18" s="178"/>
-      <c r="E18" s="178"/>
-      <c r="F18" s="184"/>
-      <c r="G18" s="178"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="178"/>
-      <c r="D19" s="178"/>
-      <c r="E19" s="178"/>
-      <c r="F19" s="184"/>
-      <c r="G19" s="178"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="22"/>
-      <c r="B34" s="22"/>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV225"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A190" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E210" sqref="E210"/>
+    <sheetView showGridLines="0" topLeftCell="A190" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
SSCS-7497 Removing decisionType dropdown and working around issues with conditional fields.  Implementing type of award options
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jack/Development/hmcts/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B95BF7-81B8-7142-9A1E-2B5415E27146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762C124F-70C8-A544-8C21-96AB0C210006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,21 +22,22 @@
     <sheet name="State" sheetId="7" r:id="rId7"/>
     <sheet name="CaseEvent" sheetId="8" r:id="rId8"/>
     <sheet name="CaseEventToFields" sheetId="9" r:id="rId9"/>
-    <sheet name="SearchInputFields" sheetId="10" r:id="rId10"/>
-    <sheet name="SearchResultFields" sheetId="11" r:id="rId11"/>
-    <sheet name="WorkBasketInputFields" sheetId="12" r:id="rId12"/>
-    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId13"/>
-    <sheet name="UserProfile" sheetId="14" r:id="rId14"/>
-    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId15"/>
-    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId16"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId17"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId18"/>
-    <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
+    <sheet name="EventToComplexTypes" sheetId="21" r:id="rId10"/>
+    <sheet name="SearchInputFields" sheetId="10" r:id="rId11"/>
+    <sheet name="SearchResultFields" sheetId="11" r:id="rId12"/>
+    <sheet name="WorkBasketInputFields" sheetId="12" r:id="rId13"/>
+    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId14"/>
+    <sheet name="UserProfile" sheetId="14" r:id="rId15"/>
+    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId16"/>
+    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId17"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId18"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId19"/>
+    <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId20"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$T$110</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$2:$L$98</definedName>
@@ -44,9 +45,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ComplexTypes!$A$3:$M$232</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">FixedLists!$A$1:$E$702</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">State!$A$3:$H$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">WorkBasketInputFields!$A$3:$G$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">WorkBasketResultFields!$A$3:$G$3</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="15">AuthorisationCaseField!$J$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">WorkBasketInputFields!$A$3:$G$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">WorkBasketResultFields!$A$3:$G$3</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="16">AuthorisationCaseField!$J$5</definedName>
     <definedName name="_xlnm.Extract" localSheetId="5">CaseTypeTab!$K$61</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="192">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -679,12 +680,57 @@
   <si>
     <t>Field to use for the order of results</t>
   </si>
+  <si>
+    <t>EventToComplexTypes</t>
+  </si>
+  <si>
+    <t>New Override label</t>
+  </si>
+  <si>
+    <t>new Override Hint Text</t>
+  </si>
+  <si>
+    <t>Order of fields</t>
+  </si>
+  <si>
+    <t>MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Always top level case field ID (from CaseField tab)</t>
+  </si>
+  <si>
+    <t>MaxLength:200</t>
+  </si>
+  <si>
+    <t>MaxLength: 300</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Accepted Values: MANDATORY, READONLY, OPTIONAL for mandatory, readonly and optional data on UI</t>
+  </si>
+  <si>
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;</t>
+  </si>
+  <si>
+    <t>EventElementLabel</t>
+  </si>
+  <si>
+    <t>EventHintText</t>
+  </si>
+  <si>
+    <t>FieldDisplayOrder</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="34">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -919,8 +965,45 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -933,8 +1016,14 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0432FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1195,6 +1284,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1203,7 +1340,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="196">
+  <cellXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1464,6 +1601,51 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="33" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2741,6 +2923,132 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C049F10D-F059-F941-9EA1-9C15C4FFCFC4}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18">
+      <c r="A1" s="196" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="198" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="199" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="197" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="197" t="s">
+        <v>179</v>
+      </c>
+      <c r="I1" s="197" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" s="200"/>
+      <c r="K1" s="197"/>
+    </row>
+    <row r="2" spans="1:11" ht="122" customHeight="1">
+      <c r="A2" s="201"/>
+      <c r="B2" s="201"/>
+      <c r="C2" s="202" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="203" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="203" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" s="201" t="s">
+        <v>181</v>
+      </c>
+      <c r="G2" s="201" t="s">
+        <v>184</v>
+      </c>
+      <c r="H2" s="201" t="s">
+        <v>185</v>
+      </c>
+      <c r="I2" s="203" t="s">
+        <v>186</v>
+      </c>
+      <c r="J2" s="203" t="s">
+        <v>187</v>
+      </c>
+      <c r="K2" s="204" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1">
+      <c r="A3" s="205" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="206" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="206" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="206" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="206" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="206" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="206" t="s">
+        <v>189</v>
+      </c>
+      <c r="H3" s="206" t="s">
+        <v>190</v>
+      </c>
+      <c r="I3" s="206" t="s">
+        <v>191</v>
+      </c>
+      <c r="J3" s="206" t="s">
+        <v>128</v>
+      </c>
+      <c r="K3" s="207" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1">
+      <c r="A4" s="208"/>
+      <c r="B4" s="200"/>
+      <c r="C4" s="200"/>
+      <c r="D4" s="209"/>
+      <c r="E4" s="209"/>
+      <c r="F4" s="209"/>
+      <c r="G4" s="200"/>
+      <c r="H4" s="200"/>
+      <c r="I4" s="200"/>
+      <c r="J4" s="209"/>
+      <c r="K4" s="210"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H573"/>
   <sheetViews>
@@ -4816,7 +5124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G39"/>
   <sheetViews>
@@ -5107,7 +5415,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H91"/>
   <sheetViews>
@@ -5738,7 +6046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H1048576"/>
   <sheetViews>
@@ -6204,7 +6512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
@@ -6872,7 +7180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:IV35"/>
   <sheetViews>
@@ -7097,7 +7405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AMK1015"/>
   <sheetViews>
@@ -21117,7 +21425,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMK696"/>
   <sheetViews>
@@ -27164,7 +27472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IV151"/>
   <sheetViews>
@@ -28212,311 +28520,6 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:AMK38"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="33.1640625" style="173" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="173" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="173" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="173" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="173" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="173" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="173" customWidth="1"/>
-    <col min="8" max="1025" width="10.83203125" style="173" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="174" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="175" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="176" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="177" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-    </row>
-    <row r="2" spans="1:7" ht="71">
-      <c r="A2" s="179"/>
-      <c r="B2" s="179"/>
-      <c r="C2" s="180" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="180" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" s="180" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="180" t="s">
-        <v>156</v>
-      </c>
-      <c r="G2" s="180" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="181" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="181" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="182" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="182" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="182" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="181" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="181" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="178"/>
-      <c r="D4" s="183"/>
-      <c r="E4" s="184"/>
-      <c r="F4" s="184"/>
-      <c r="G4" s="178"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="178"/>
-      <c r="D5" s="183"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="184"/>
-      <c r="G5" s="178"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="178"/>
-      <c r="D6" s="183"/>
-      <c r="E6" s="184"/>
-      <c r="F6" s="184"/>
-      <c r="G6" s="178"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="178"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="184"/>
-      <c r="F7" s="184"/>
-      <c r="G7" s="178"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="178"/>
-      <c r="D8" s="183"/>
-      <c r="E8" s="184"/>
-      <c r="F8" s="184"/>
-      <c r="G8" s="178"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="178"/>
-      <c r="D9" s="183"/>
-      <c r="E9" s="184"/>
-      <c r="F9" s="184"/>
-      <c r="G9" s="178"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="178"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="184"/>
-      <c r="F10" s="184"/>
-      <c r="G10" s="178"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="178"/>
-      <c r="D11" s="178"/>
-      <c r="E11" s="178"/>
-      <c r="F11" s="184"/>
-      <c r="G11" s="178"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="178"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="178"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="178"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="178"/>
-      <c r="D13" s="178"/>
-      <c r="E13" s="184"/>
-      <c r="F13" s="184"/>
-      <c r="G13" s="178"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="178"/>
-      <c r="D14" s="178"/>
-      <c r="E14" s="184"/>
-      <c r="F14" s="184"/>
-      <c r="G14" s="178"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="178"/>
-      <c r="D15" s="178"/>
-      <c r="E15" s="184"/>
-      <c r="F15" s="184"/>
-      <c r="G15" s="178"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="178"/>
-      <c r="D16" s="178"/>
-      <c r="E16" s="184"/>
-      <c r="F16" s="184"/>
-      <c r="G16" s="178"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="178"/>
-      <c r="D17" s="178"/>
-      <c r="E17" s="184"/>
-      <c r="F17" s="184"/>
-      <c r="G17" s="178"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="178"/>
-      <c r="D18" s="178"/>
-      <c r="E18" s="178"/>
-      <c r="F18" s="184"/>
-      <c r="G18" s="178"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="178"/>
-      <c r="D19" s="178"/>
-      <c r="E19" s="178"/>
-      <c r="F19" s="184"/>
-      <c r="G19" s="178"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="22"/>
-      <c r="B34" s="22"/>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -28702,12 +28705,317 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:AMK38"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="173" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="173" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="173" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="173" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="173" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="173" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="173" customWidth="1"/>
+    <col min="8" max="1025" width="10.83203125" style="173" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18">
+      <c r="A1" s="174" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="175" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="176" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="177" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+    </row>
+    <row r="2" spans="1:7" ht="71">
+      <c r="A2" s="179"/>
+      <c r="B2" s="179"/>
+      <c r="C2" s="180" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="180" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="180" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="180" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="180" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="181" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="181" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="182" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="182" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="182" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="181" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="181" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="178"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="184"/>
+      <c r="F4" s="184"/>
+      <c r="G4" s="178"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="178"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="184"/>
+      <c r="F5" s="184"/>
+      <c r="G5" s="178"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="178"/>
+      <c r="D6" s="183"/>
+      <c r="E6" s="184"/>
+      <c r="F6" s="184"/>
+      <c r="G6" s="178"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="178"/>
+      <c r="D7" s="183"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="178"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="178"/>
+      <c r="D8" s="183"/>
+      <c r="E8" s="184"/>
+      <c r="F8" s="184"/>
+      <c r="G8" s="178"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="183"/>
+      <c r="E9" s="184"/>
+      <c r="F9" s="184"/>
+      <c r="G9" s="178"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="178"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="178"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="178"/>
+      <c r="D11" s="178"/>
+      <c r="E11" s="178"/>
+      <c r="F11" s="184"/>
+      <c r="G11" s="178"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="178"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="178"/>
+      <c r="F12" s="184"/>
+      <c r="G12" s="178"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="178"/>
+      <c r="D13" s="178"/>
+      <c r="E13" s="184"/>
+      <c r="F13" s="184"/>
+      <c r="G13" s="178"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="178"/>
+      <c r="D14" s="178"/>
+      <c r="E14" s="184"/>
+      <c r="F14" s="184"/>
+      <c r="G14" s="178"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="178"/>
+      <c r="D15" s="178"/>
+      <c r="E15" s="184"/>
+      <c r="F15" s="184"/>
+      <c r="G15" s="178"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="178"/>
+      <c r="D16" s="178"/>
+      <c r="E16" s="184"/>
+      <c r="F16" s="184"/>
+      <c r="G16" s="178"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="178"/>
+      <c r="D17" s="178"/>
+      <c r="E17" s="184"/>
+      <c r="F17" s="184"/>
+      <c r="G17" s="178"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="178"/>
+      <c r="D18" s="178"/>
+      <c r="E18" s="178"/>
+      <c r="F18" s="184"/>
+      <c r="G18" s="178"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="178"/>
+      <c r="D19" s="178"/>
+      <c r="E19" s="178"/>
+      <c r="F19" s="184"/>
+      <c r="G19" s="178"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV225"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A190" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F212" sqref="F212"/>
+      <selection activeCell="E210" sqref="E210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Bring 7187 up to scratch with master
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jack/Development/hmcts/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769796AE-53FE-3A46-B34E-EBEDBC0C4795}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17544AC-1E2C-9049-BBB5-53BB8938929A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -22,21 +22,22 @@
     <sheet name="State" sheetId="7" r:id="rId7"/>
     <sheet name="CaseEvent" sheetId="8" r:id="rId8"/>
     <sheet name="CaseEventToFields" sheetId="9" r:id="rId9"/>
-    <sheet name="SearchInputFields" sheetId="10" r:id="rId10"/>
-    <sheet name="SearchResultFields" sheetId="11" r:id="rId11"/>
-    <sheet name="WorkBasketInputFields" sheetId="12" r:id="rId12"/>
-    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId13"/>
-    <sheet name="UserProfile" sheetId="14" r:id="rId14"/>
-    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId15"/>
-    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId16"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId17"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId18"/>
-    <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
+    <sheet name="EventToComplexTypes" sheetId="20" r:id="rId10"/>
+    <sheet name="SearchInputFields" sheetId="10" r:id="rId11"/>
+    <sheet name="SearchResultFields" sheetId="11" r:id="rId12"/>
+    <sheet name="WorkBasketInputFields" sheetId="12" r:id="rId13"/>
+    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId14"/>
+    <sheet name="UserProfile" sheetId="14" r:id="rId15"/>
+    <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId16"/>
+    <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId17"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId18"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId19"/>
+    <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId20"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$T$110</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$2:$L$98</definedName>
@@ -44,9 +45,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ComplexTypes!$A$3:$M$232</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">FixedLists!$A$1:$E$702</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">State!$A$3:$H$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="15">AuthorisationCaseField!$J$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="16">AuthorisationCaseField!$J$5</definedName>
     <definedName name="_xlnm.Extract" localSheetId="5">CaseTypeTab!$K$61</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="192">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -679,12 +680,57 @@
   <si>
     <t>Field to use for the order of results</t>
   </si>
+  <si>
+    <t>EventToComplexTypes</t>
+  </si>
+  <si>
+    <t>New Override label</t>
+  </si>
+  <si>
+    <t>new Override Hint Text</t>
+  </si>
+  <si>
+    <t>Order of fields</t>
+  </si>
+  <si>
+    <t>MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Always top level case field ID (from CaseField tab)</t>
+  </si>
+  <si>
+    <t>MaxLength:200</t>
+  </si>
+  <si>
+    <t>MaxLength: 300</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Accepted Values: MANDATORY, READONLY, OPTIONAL for mandatory, readonly and optional data on UI</t>
+  </si>
+  <si>
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;</t>
+  </si>
+  <si>
+    <t>EventElementLabel</t>
+  </si>
+  <si>
+    <t>EventHintText</t>
+  </si>
+  <si>
+    <t>FieldDisplayOrder</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="34">
+  <fonts count="38">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -919,8 +965,39 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -933,8 +1010,14 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0432FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1195,6 +1278,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1203,7 +1321,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="196">
+  <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1464,6 +1582,42 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="33" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2741,6 +2895,119 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A9C771-3461-1047-9C92-C326BE0E36D7}">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18">
+      <c r="A1" s="196" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="197" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="198" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="199" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="199"/>
+      <c r="F1" s="199" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="197" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="197" t="s">
+        <v>179</v>
+      </c>
+      <c r="I1" s="197" t="s">
+        <v>180</v>
+      </c>
+      <c r="J1" s="200"/>
+      <c r="K1" s="197"/>
+    </row>
+    <row r="2" spans="1:11" ht="182">
+      <c r="A2" s="201"/>
+      <c r="B2" s="201"/>
+      <c r="C2" s="202" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="203" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="203" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" s="201" t="s">
+        <v>181</v>
+      </c>
+      <c r="G2" s="201" t="s">
+        <v>184</v>
+      </c>
+      <c r="H2" s="201" t="s">
+        <v>185</v>
+      </c>
+      <c r="I2" s="203" t="s">
+        <v>186</v>
+      </c>
+      <c r="J2" s="203" t="s">
+        <v>187</v>
+      </c>
+      <c r="K2" s="204" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="205" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="206" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="206" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="206" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="206" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="206" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="206" t="s">
+        <v>189</v>
+      </c>
+      <c r="H3" s="206" t="s">
+        <v>190</v>
+      </c>
+      <c r="I3" s="206" t="s">
+        <v>191</v>
+      </c>
+      <c r="J3" s="206" t="s">
+        <v>128</v>
+      </c>
+      <c r="K3" s="207" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I573"/>
   <sheetViews>
@@ -4857,7 +5124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
@@ -5160,7 +5427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I91"/>
   <sheetViews>
@@ -5832,12 +6099,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6303,7 +6570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
@@ -6971,7 +7238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:IV35"/>
   <sheetViews>
@@ -7196,7 +7463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AMK1015"/>
   <sheetViews>
@@ -21216,7 +21483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMK696"/>
   <sheetViews>
@@ -27263,7 +27530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:IV151"/>
   <sheetViews>
@@ -28311,311 +28578,6 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:AMK38"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="33.1640625" style="173" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="173" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="173" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="173" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="173" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="173" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="173" customWidth="1"/>
-    <col min="8" max="1025" width="10.83203125" style="173" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18">
-      <c r="A1" s="174" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="175" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="176" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="177" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-    </row>
-    <row r="2" spans="1:7" ht="71">
-      <c r="A2" s="179"/>
-      <c r="B2" s="179"/>
-      <c r="C2" s="180" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="180" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" s="180" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="180" t="s">
-        <v>156</v>
-      </c>
-      <c r="G2" s="180" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="181" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="181" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="182" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="182" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="182" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="181" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="181" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="178"/>
-      <c r="D4" s="183"/>
-      <c r="E4" s="184"/>
-      <c r="F4" s="184"/>
-      <c r="G4" s="178"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="178"/>
-      <c r="D5" s="183"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="184"/>
-      <c r="G5" s="178"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="178"/>
-      <c r="D6" s="183"/>
-      <c r="E6" s="184"/>
-      <c r="F6" s="184"/>
-      <c r="G6" s="178"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="178"/>
-      <c r="D7" s="183"/>
-      <c r="E7" s="184"/>
-      <c r="F7" s="184"/>
-      <c r="G7" s="178"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="178"/>
-      <c r="D8" s="183"/>
-      <c r="E8" s="184"/>
-      <c r="F8" s="184"/>
-      <c r="G8" s="178"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="178"/>
-      <c r="D9" s="183"/>
-      <c r="E9" s="184"/>
-      <c r="F9" s="184"/>
-      <c r="G9" s="178"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="178"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="184"/>
-      <c r="F10" s="184"/>
-      <c r="G10" s="178"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="178"/>
-      <c r="D11" s="178"/>
-      <c r="E11" s="178"/>
-      <c r="F11" s="184"/>
-      <c r="G11" s="178"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="178"/>
-      <c r="D12" s="178"/>
-      <c r="E12" s="178"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="178"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="178"/>
-      <c r="D13" s="178"/>
-      <c r="E13" s="184"/>
-      <c r="F13" s="184"/>
-      <c r="G13" s="178"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="178"/>
-      <c r="D14" s="178"/>
-      <c r="E14" s="184"/>
-      <c r="F14" s="184"/>
-      <c r="G14" s="178"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="178"/>
-      <c r="D15" s="178"/>
-      <c r="E15" s="184"/>
-      <c r="F15" s="184"/>
-      <c r="G15" s="178"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="178"/>
-      <c r="D16" s="178"/>
-      <c r="E16" s="184"/>
-      <c r="F16" s="184"/>
-      <c r="G16" s="178"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="178"/>
-      <c r="D17" s="178"/>
-      <c r="E17" s="184"/>
-      <c r="F17" s="184"/>
-      <c r="G17" s="178"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="178"/>
-      <c r="D18" s="178"/>
-      <c r="E18" s="178"/>
-      <c r="F18" s="184"/>
-      <c r="G18" s="178"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="178"/>
-      <c r="D19" s="178"/>
-      <c r="E19" s="178"/>
-      <c r="F19" s="184"/>
-      <c r="G19" s="178"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="22"/>
-      <c r="B32" s="22"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="22"/>
-      <c r="B33" s="22"/>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="22"/>
-      <c r="B34" s="22"/>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="22"/>
-      <c r="B35" s="22"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="22"/>
-      <c r="B36" s="22"/>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="22"/>
-      <c r="B37" s="22"/>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="22"/>
-      <c r="B38" s="22"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -28798,6 +28760,311 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:AMK38"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.1640625" style="173" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="173" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="173" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="173" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="173" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="173" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="173" customWidth="1"/>
+    <col min="8" max="1025" width="10.83203125" style="173" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18">
+      <c r="A1" s="174" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="175" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="176" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="177" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+    </row>
+    <row r="2" spans="1:7" ht="71">
+      <c r="A2" s="179"/>
+      <c r="B2" s="179"/>
+      <c r="C2" s="180" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="180" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="180" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="180" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="180" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="181" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="181" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="182" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="182" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="182" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="181" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="181" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="178"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="184"/>
+      <c r="F4" s="184"/>
+      <c r="G4" s="178"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="178"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="184"/>
+      <c r="F5" s="184"/>
+      <c r="G5" s="178"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="178"/>
+      <c r="D6" s="183"/>
+      <c r="E6" s="184"/>
+      <c r="F6" s="184"/>
+      <c r="G6" s="178"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="178"/>
+      <c r="D7" s="183"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="184"/>
+      <c r="G7" s="178"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="178"/>
+      <c r="D8" s="183"/>
+      <c r="E8" s="184"/>
+      <c r="F8" s="184"/>
+      <c r="G8" s="178"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="183"/>
+      <c r="E9" s="184"/>
+      <c r="F9" s="184"/>
+      <c r="G9" s="178"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="178"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="178"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="178"/>
+      <c r="D11" s="178"/>
+      <c r="E11" s="178"/>
+      <c r="F11" s="184"/>
+      <c r="G11" s="178"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="178"/>
+      <c r="D12" s="178"/>
+      <c r="E12" s="178"/>
+      <c r="F12" s="184"/>
+      <c r="G12" s="178"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="178"/>
+      <c r="D13" s="178"/>
+      <c r="E13" s="184"/>
+      <c r="F13" s="184"/>
+      <c r="G13" s="178"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="178"/>
+      <c r="D14" s="178"/>
+      <c r="E14" s="184"/>
+      <c r="F14" s="184"/>
+      <c r="G14" s="178"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="178"/>
+      <c r="D15" s="178"/>
+      <c r="E15" s="184"/>
+      <c r="F15" s="184"/>
+      <c r="G15" s="178"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="178"/>
+      <c r="D16" s="178"/>
+      <c r="E16" s="184"/>
+      <c r="F16" s="184"/>
+      <c r="G16" s="178"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="178"/>
+      <c r="D17" s="178"/>
+      <c r="E17" s="184"/>
+      <c r="F17" s="184"/>
+      <c r="G17" s="178"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="178"/>
+      <c r="D18" s="178"/>
+      <c r="E18" s="178"/>
+      <c r="F18" s="184"/>
+      <c r="G18" s="178"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="178"/>
+      <c r="D19" s="178"/>
+      <c r="E19" s="178"/>
+      <c r="F19" s="184"/>
+      <c r="G19" s="178"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Set all rows for liveFrom and liveTo to datetimes
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jack/Development/hmcts/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762C124F-70C8-A544-8C21-96AB0C210006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E912A974-825B-3F4F-B336-17D190620029}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -29014,7 +29014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV225"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A190" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A174" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E210" sqref="E210"/>
     </sheetView>
   </sheetViews>
@@ -44713,14 +44713,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMK229"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A294" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D177" sqref="D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="18" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="22" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="18" customWidth="1"/>
     <col min="4" max="4" width="77.1640625" style="18" customWidth="1"/>
     <col min="5" max="5" width="66" style="18" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" style="18" customWidth="1"/>
@@ -44734,10 +44735,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
@@ -44761,10 +44762,10 @@
       <c r="Q1" s="185"/>
     </row>
     <row r="2" spans="1:17" ht="160" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="46" t="s">
@@ -44814,10 +44815,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="22" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -44867,8 +44868,8 @@
       </c>
     </row>
     <row r="4" spans="1:17" s="57" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="13"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="9"/>
       <c r="D4" s="13"/>
       <c r="E4" s="11"/>
@@ -44886,8 +44887,8 @@
       <c r="Q4" s="58"/>
     </row>
     <row r="5" spans="1:17" s="57" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="13"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="9"/>
       <c r="D5" s="13"/>
       <c r="E5" s="11"/>
@@ -44905,8 +44906,8 @@
       <c r="Q5" s="58"/>
     </row>
     <row r="6" spans="1:17" s="57" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="9"/>
       <c r="D6" s="13"/>
       <c r="E6" s="11"/>
@@ -44924,8 +44925,6 @@
       <c r="Q6" s="58"/>
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1">
-      <c r="A7" s="22"/>
-      <c r="B7" s="45"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -44941,8 +44940,6 @@
       <c r="O7" s="189"/>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1">
-      <c r="A8" s="22"/>
-      <c r="B8" s="45"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
@@ -44958,8 +44955,6 @@
       <c r="O8" s="189"/>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1">
-      <c r="A9" s="22"/>
-      <c r="B9" s="45"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -44975,8 +44970,6 @@
       <c r="O9" s="189"/>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1">
-      <c r="A10" s="22"/>
-      <c r="B10" s="45"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -44992,8 +44985,6 @@
       <c r="O10" s="189"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1">
-      <c r="A11" s="22"/>
-      <c r="B11" s="45"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
@@ -45009,8 +45000,6 @@
       <c r="O11" s="189"/>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1">
-      <c r="A12" s="22"/>
-      <c r="B12" s="45"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
@@ -45026,8 +45015,6 @@
       <c r="O12" s="189"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1">
-      <c r="A13" s="22"/>
-      <c r="B13" s="45"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
@@ -45043,8 +45030,6 @@
       <c r="O13" s="189"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1">
-      <c r="A14" s="22"/>
-      <c r="B14" s="45"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
@@ -45060,8 +45045,6 @@
       <c r="O14" s="189"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1">
-      <c r="A15" s="22"/>
-      <c r="B15" s="45"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
@@ -45077,8 +45060,6 @@
       <c r="O15" s="189"/>
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1">
-      <c r="A16" s="22"/>
-      <c r="B16" s="45"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
@@ -45093,9 +45074,7 @@
       <c r="N16" s="45"/>
       <c r="O16" s="189"/>
     </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1">
-      <c r="A17" s="22"/>
-      <c r="B17" s="45"/>
+    <row r="17" spans="3:15" ht="15" customHeight="1">
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
@@ -45110,9 +45089,7 @@
       <c r="N17" s="45"/>
       <c r="O17" s="189"/>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1">
-      <c r="A18" s="22"/>
-      <c r="B18" s="45"/>
+    <row r="18" spans="3:15" ht="15" customHeight="1">
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
@@ -45127,9 +45104,7 @@
       <c r="N18" s="45"/>
       <c r="O18" s="189"/>
     </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1">
-      <c r="A19" s="13"/>
-      <c r="B19" s="11"/>
+    <row r="19" spans="3:15" ht="15" customHeight="1">
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -45144,9 +45119,7 @@
       <c r="N19" s="11"/>
       <c r="O19" s="192"/>
     </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1">
-      <c r="A20" s="13"/>
-      <c r="B20" s="130"/>
+    <row r="20" spans="3:15" ht="15" customHeight="1">
       <c r="C20" s="9"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
@@ -45161,9 +45134,7 @@
       <c r="N20" s="130"/>
       <c r="O20" s="192"/>
     </row>
-    <row r="21" spans="1:15" ht="15" customHeight="1">
-      <c r="A21" s="13"/>
-      <c r="B21" s="130"/>
+    <row r="21" spans="3:15" ht="15" customHeight="1">
       <c r="C21" s="9"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
@@ -45178,9 +45149,7 @@
       <c r="N21" s="130"/>
       <c r="O21" s="192"/>
     </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1">
-      <c r="A22" s="22"/>
-      <c r="B22" s="45"/>
+    <row r="22" spans="3:15" ht="15" customHeight="1">
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -45195,9 +45164,7 @@
       <c r="N22" s="45"/>
       <c r="O22" s="189"/>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1">
-      <c r="A23" s="22"/>
-      <c r="B23" s="45"/>
+    <row r="23" spans="3:15" ht="15" customHeight="1">
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
@@ -45212,9 +45179,7 @@
       <c r="N23" s="45"/>
       <c r="O23" s="189"/>
     </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1">
-      <c r="A24" s="22"/>
-      <c r="B24" s="45"/>
+    <row r="24" spans="3:15" ht="15" customHeight="1">
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
@@ -45229,9 +45194,7 @@
       <c r="N24" s="45"/>
       <c r="O24" s="189"/>
     </row>
-    <row r="25" spans="1:15" ht="15" customHeight="1">
-      <c r="A25" s="22"/>
-      <c r="B25" s="45"/>
+    <row r="25" spans="3:15" ht="15" customHeight="1">
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
@@ -45246,9 +45209,7 @@
       <c r="N25" s="45"/>
       <c r="O25" s="189"/>
     </row>
-    <row r="26" spans="1:15" ht="15" customHeight="1">
-      <c r="A26" s="22"/>
-      <c r="B26" s="45"/>
+    <row r="26" spans="3:15" ht="15" customHeight="1">
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
@@ -45263,9 +45224,7 @@
       <c r="N26" s="45"/>
       <c r="O26" s="189"/>
     </row>
-    <row r="27" spans="1:15" ht="15" customHeight="1">
-      <c r="A27" s="22"/>
-      <c r="B27" s="45"/>
+    <row r="27" spans="3:15" ht="15" customHeight="1">
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
@@ -45280,9 +45239,7 @@
       <c r="N27" s="45"/>
       <c r="O27" s="189"/>
     </row>
-    <row r="28" spans="1:15" ht="15" customHeight="1">
-      <c r="A28" s="22"/>
-      <c r="B28" s="45"/>
+    <row r="28" spans="3:15" ht="15" customHeight="1">
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
@@ -45297,9 +45254,7 @@
       <c r="N28" s="45"/>
       <c r="O28" s="189"/>
     </row>
-    <row r="29" spans="1:15" ht="15" customHeight="1">
-      <c r="A29" s="22"/>
-      <c r="B29" s="45"/>
+    <row r="29" spans="3:15" ht="15" customHeight="1">
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
@@ -45314,9 +45269,7 @@
       <c r="N29" s="45"/>
       <c r="O29" s="189"/>
     </row>
-    <row r="30" spans="1:15" ht="15" customHeight="1">
-      <c r="A30" s="22"/>
-      <c r="B30" s="45"/>
+    <row r="30" spans="3:15" ht="15" customHeight="1">
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
@@ -45331,9 +45284,7 @@
       <c r="N30" s="45"/>
       <c r="O30" s="189"/>
     </row>
-    <row r="31" spans="1:15" ht="15" customHeight="1">
-      <c r="A31" s="22"/>
-      <c r="B31" s="45"/>
+    <row r="31" spans="3:15" ht="15" customHeight="1">
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
@@ -45348,9 +45299,7 @@
       <c r="N31" s="45"/>
       <c r="O31" s="189"/>
     </row>
-    <row r="32" spans="1:15" ht="15" customHeight="1">
-      <c r="A32" s="22"/>
-      <c r="B32" s="45"/>
+    <row r="32" spans="3:15" ht="15" customHeight="1">
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
@@ -45366,8 +45315,6 @@
       <c r="O32" s="189"/>
     </row>
     <row r="33" spans="1:17" ht="15" customHeight="1">
-      <c r="A33" s="22"/>
-      <c r="B33" s="45"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
@@ -45383,8 +45330,6 @@
       <c r="O33" s="189"/>
     </row>
     <row r="34" spans="1:17" ht="15" customHeight="1">
-      <c r="A34" s="22"/>
-      <c r="B34" s="45"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
@@ -45400,8 +45345,6 @@
       <c r="O34" s="189"/>
     </row>
     <row r="35" spans="1:17" ht="15" customHeight="1">
-      <c r="A35" s="13"/>
-      <c r="B35" s="11"/>
       <c r="C35" s="9"/>
       <c r="D35" s="36"/>
       <c r="E35" s="36"/>
@@ -45417,8 +45360,6 @@
       <c r="O35" s="192"/>
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1">
-      <c r="A36" s="13"/>
-      <c r="B36" s="11"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="11"/>
@@ -45434,8 +45375,6 @@
       <c r="O36" s="192"/>
     </row>
     <row r="37" spans="1:17" ht="15" customHeight="1">
-      <c r="A37" s="13"/>
-      <c r="B37" s="11"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -45451,8 +45390,6 @@
       <c r="O37" s="192"/>
     </row>
     <row r="38" spans="1:17" ht="15" customHeight="1">
-      <c r="A38" s="13"/>
-      <c r="B38" s="11"/>
       <c r="C38" s="9"/>
       <c r="D38" s="45"/>
       <c r="E38" s="11"/>
@@ -45468,8 +45405,6 @@
       <c r="O38" s="189"/>
     </row>
     <row r="39" spans="1:17" ht="15" customHeight="1">
-      <c r="A39" s="13"/>
-      <c r="B39" s="11"/>
       <c r="C39" s="9"/>
       <c r="D39" s="45"/>
       <c r="E39" s="45"/>
@@ -45485,8 +45420,6 @@
       <c r="O39" s="189"/>
     </row>
     <row r="40" spans="1:17" ht="15" customHeight="1">
-      <c r="A40" s="13"/>
-      <c r="B40" s="11"/>
       <c r="C40" s="9"/>
       <c r="D40" s="12"/>
       <c r="E40" s="11"/>
@@ -45502,8 +45435,6 @@
       <c r="O40" s="189"/>
     </row>
     <row r="41" spans="1:17" ht="15" customHeight="1">
-      <c r="A41" s="13"/>
-      <c r="B41" s="11"/>
       <c r="C41" s="9"/>
       <c r="D41" s="12"/>
       <c r="E41" s="9"/>
@@ -45519,8 +45450,6 @@
       <c r="O41" s="192"/>
     </row>
     <row r="42" spans="1:17" ht="15" customHeight="1">
-      <c r="A42" s="13"/>
-      <c r="B42" s="11"/>
       <c r="C42" s="9"/>
       <c r="D42" s="12"/>
       <c r="E42" s="9"/>
@@ -45536,8 +45465,8 @@
       <c r="O42" s="192"/>
     </row>
     <row r="43" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A43" s="13"/>
-      <c r="B43" s="11"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -45555,8 +45484,8 @@
       <c r="Q43" s="11"/>
     </row>
     <row r="44" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A44" s="13"/>
-      <c r="B44" s="11"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="11"/>
@@ -45574,8 +45503,6 @@
       <c r="Q44" s="11"/>
     </row>
     <row r="45" spans="1:17" ht="15" customHeight="1">
-      <c r="A45" s="13"/>
-      <c r="B45" s="11"/>
       <c r="C45" s="9"/>
       <c r="D45" s="11"/>
       <c r="E45" s="9"/>
@@ -45591,8 +45518,6 @@
       <c r="O45" s="192"/>
     </row>
     <row r="46" spans="1:17" ht="15" customHeight="1">
-      <c r="A46" s="13"/>
-      <c r="B46" s="11"/>
       <c r="C46" s="9"/>
       <c r="D46" s="11"/>
       <c r="E46" s="9"/>
@@ -45608,8 +45533,8 @@
       <c r="O46" s="192"/>
     </row>
     <row r="47" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A47" s="13"/>
-      <c r="B47" s="11"/>
+      <c r="A47" s="22"/>
+      <c r="B47" s="22"/>
       <c r="C47" s="9"/>
       <c r="D47" s="11"/>
       <c r="E47" s="9"/>
@@ -45627,8 +45552,8 @@
       <c r="Q47" s="11"/>
     </row>
     <row r="48" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A48" s="13"/>
-      <c r="B48" s="11"/>
+      <c r="A48" s="22"/>
+      <c r="B48" s="22"/>
       <c r="C48" s="9"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -45646,8 +45571,6 @@
       <c r="Q48" s="11"/>
     </row>
     <row r="49" spans="1:17" ht="15" customHeight="1">
-      <c r="A49" s="13"/>
-      <c r="B49" s="11"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
       <c r="E49" s="45"/>
@@ -45663,8 +45586,6 @@
       <c r="O49" s="189"/>
     </row>
     <row r="50" spans="1:17" ht="15" customHeight="1">
-      <c r="A50" s="13"/>
-      <c r="B50" s="11"/>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
       <c r="E50" s="33"/>
@@ -45680,8 +45601,6 @@
       <c r="O50" s="15"/>
     </row>
     <row r="51" spans="1:17" ht="15" customHeight="1">
-      <c r="A51" s="13"/>
-      <c r="B51" s="11"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="14"/>
@@ -45697,8 +45616,8 @@
       <c r="O51" s="15"/>
     </row>
     <row r="52" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A52" s="13"/>
-      <c r="B52" s="11"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="22"/>
       <c r="C52" s="9"/>
       <c r="D52" s="33"/>
       <c r="E52" s="33"/>
@@ -45709,8 +45628,8 @@
       <c r="Q52" s="11"/>
     </row>
     <row r="53" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A53" s="13"/>
-      <c r="B53" s="11"/>
+      <c r="A53" s="22"/>
+      <c r="B53" s="22"/>
       <c r="C53" s="9"/>
       <c r="D53" s="33"/>
       <c r="E53" s="14"/>
@@ -45721,8 +45640,8 @@
       <c r="Q53" s="11"/>
     </row>
     <row r="54" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A54" s="13"/>
-      <c r="B54" s="11"/>
+      <c r="A54" s="22"/>
+      <c r="B54" s="22"/>
       <c r="C54" s="9"/>
       <c r="D54" s="33"/>
       <c r="E54" s="14"/>
@@ -45734,8 +45653,8 @@
       <c r="Q54" s="11"/>
     </row>
     <row r="55" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A55" s="13"/>
-      <c r="B55" s="11"/>
+      <c r="A55" s="22"/>
+      <c r="B55" s="22"/>
       <c r="C55" s="9"/>
       <c r="D55" s="33"/>
       <c r="E55" s="9"/>
@@ -45747,8 +45666,8 @@
       <c r="Q55" s="11"/>
     </row>
     <row r="56" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A56" s="13"/>
-      <c r="B56" s="11"/>
+      <c r="A56" s="22"/>
+      <c r="B56" s="22"/>
       <c r="C56" s="9"/>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
@@ -45759,8 +45678,8 @@
       <c r="Q56" s="11"/>
     </row>
     <row r="57" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A57" s="13"/>
-      <c r="B57" s="11"/>
+      <c r="A57" s="22"/>
+      <c r="B57" s="22"/>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="14"/>
@@ -45770,7 +45689,8 @@
       <c r="Q57" s="11"/>
     </row>
     <row r="58" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A58" s="13"/>
+      <c r="A58" s="22"/>
+      <c r="B58" s="22"/>
       <c r="C58" s="9"/>
       <c r="D58" s="132"/>
       <c r="E58" s="132"/>
@@ -45780,7 +45700,8 @@
       <c r="Q58" s="11"/>
     </row>
     <row r="59" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A59" s="13"/>
+      <c r="A59" s="22"/>
+      <c r="B59" s="22"/>
       <c r="C59" s="9"/>
       <c r="D59" s="132"/>
       <c r="E59" s="133"/>
@@ -45790,7 +45711,8 @@
       <c r="Q59" s="11"/>
     </row>
     <row r="60" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A60" s="13"/>
+      <c r="A60" s="22"/>
+      <c r="B60" s="22"/>
       <c r="C60" s="9"/>
       <c r="D60" s="114"/>
       <c r="E60" s="132"/>
@@ -45800,8 +45722,6 @@
       <c r="Q60" s="11"/>
     </row>
     <row r="61" spans="1:17" ht="15" customHeight="1">
-      <c r="A61" s="13"/>
-      <c r="B61" s="11"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
       <c r="E61" s="45"/>
@@ -45817,8 +45737,6 @@
       <c r="O61" s="15"/>
     </row>
     <row r="62" spans="1:17" ht="15" customHeight="1">
-      <c r="A62" s="13"/>
-      <c r="B62" s="11"/>
       <c r="C62" s="9"/>
       <c r="D62" s="134"/>
       <c r="E62" s="123"/>
@@ -45834,8 +45752,6 @@
       <c r="O62" s="15"/>
     </row>
     <row r="63" spans="1:17" ht="15" customHeight="1">
-      <c r="A63" s="22"/>
-      <c r="B63" s="45"/>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
@@ -45851,8 +45767,6 @@
       <c r="O63" s="189"/>
     </row>
     <row r="64" spans="1:17" ht="15" customHeight="1">
-      <c r="A64" s="13"/>
-      <c r="B64" s="11"/>
       <c r="C64" s="12"/>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
@@ -45867,9 +45781,7 @@
       <c r="N64" s="11"/>
       <c r="O64" s="192"/>
     </row>
-    <row r="65" spans="1:15" ht="15" customHeight="1">
-      <c r="A65" s="13"/>
-      <c r="B65" s="11"/>
+    <row r="65" spans="3:15" ht="15" customHeight="1">
       <c r="C65" s="9"/>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
@@ -45884,9 +45796,7 @@
       <c r="N65" s="11"/>
       <c r="O65" s="192"/>
     </row>
-    <row r="66" spans="1:15" ht="15" customHeight="1">
-      <c r="A66" s="22"/>
-      <c r="B66" s="45"/>
+    <row r="66" spans="3:15" ht="15" customHeight="1">
       <c r="C66" s="12"/>
       <c r="D66" s="12"/>
       <c r="E66" s="12"/>
@@ -45901,9 +45811,7 @@
       <c r="N66" s="45"/>
       <c r="O66" s="189"/>
     </row>
-    <row r="67" spans="1:15" ht="15" customHeight="1">
-      <c r="A67" s="22"/>
-      <c r="B67" s="45"/>
+    <row r="67" spans="3:15" ht="15" customHeight="1">
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
@@ -45918,9 +45826,7 @@
       <c r="N67" s="45"/>
       <c r="O67" s="189"/>
     </row>
-    <row r="68" spans="1:15" ht="15" customHeight="1">
-      <c r="A68" s="22"/>
-      <c r="B68" s="45"/>
+    <row r="68" spans="3:15" ht="15" customHeight="1">
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
@@ -45935,9 +45841,7 @@
       <c r="N68" s="45"/>
       <c r="O68" s="189"/>
     </row>
-    <row r="69" spans="1:15" ht="15" customHeight="1">
-      <c r="A69" s="22"/>
-      <c r="B69" s="45"/>
+    <row r="69" spans="3:15" ht="15" customHeight="1">
       <c r="C69" s="12"/>
       <c r="D69" s="20"/>
       <c r="E69" s="17"/>
@@ -45946,9 +45850,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="20"/>
     </row>
-    <row r="70" spans="1:15" ht="15" customHeight="1">
-      <c r="A70" s="13"/>
-      <c r="B70" s="11"/>
+    <row r="70" spans="3:15" ht="15" customHeight="1">
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
       <c r="E70" s="14"/>
@@ -45963,9 +45865,7 @@
       <c r="N70" s="45"/>
       <c r="O70" s="189"/>
     </row>
-    <row r="71" spans="1:15" ht="15" customHeight="1">
-      <c r="A71" s="13"/>
-      <c r="B71" s="11"/>
+    <row r="71" spans="3:15" ht="15" customHeight="1">
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
       <c r="E71" s="14"/>
@@ -45980,9 +45880,7 @@
       <c r="N71" s="45"/>
       <c r="O71" s="189"/>
     </row>
-    <row r="72" spans="1:15" ht="15" customHeight="1">
-      <c r="A72" s="13"/>
-      <c r="B72" s="11"/>
+    <row r="72" spans="3:15" ht="15" customHeight="1">
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
       <c r="E72" s="12"/>
@@ -45997,9 +45895,7 @@
       <c r="N72" s="45"/>
       <c r="O72" s="189"/>
     </row>
-    <row r="73" spans="1:15" ht="15" customHeight="1">
-      <c r="A73" s="13"/>
-      <c r="B73" s="11"/>
+    <row r="73" spans="3:15" ht="15" customHeight="1">
       <c r="C73" s="9"/>
       <c r="D73" s="11"/>
       <c r="E73" s="14"/>
@@ -46014,9 +45910,7 @@
       <c r="N73" s="11"/>
       <c r="O73" s="189"/>
     </row>
-    <row r="74" spans="1:15" ht="15" customHeight="1">
-      <c r="A74" s="13"/>
-      <c r="B74" s="11"/>
+    <row r="74" spans="3:15" ht="15" customHeight="1">
       <c r="C74" s="9"/>
       <c r="D74" s="11"/>
       <c r="E74" s="9"/>
@@ -46031,9 +45925,7 @@
       <c r="N74" s="11"/>
       <c r="O74" s="189"/>
     </row>
-    <row r="75" spans="1:15" ht="15" customHeight="1">
-      <c r="A75" s="13"/>
-      <c r="B75" s="11"/>
+    <row r="75" spans="3:15" ht="15" customHeight="1">
       <c r="C75" s="9"/>
       <c r="D75" s="11"/>
       <c r="E75" s="14"/>
@@ -46048,9 +45940,7 @@
       <c r="N75" s="11"/>
       <c r="O75" s="189"/>
     </row>
-    <row r="76" spans="1:15" ht="15" customHeight="1">
-      <c r="A76" s="13"/>
-      <c r="B76" s="11"/>
+    <row r="76" spans="3:15" ht="15" customHeight="1">
       <c r="C76" s="9"/>
       <c r="D76" s="11"/>
       <c r="E76" s="14"/>
@@ -46065,9 +45955,7 @@
       <c r="N76" s="11"/>
       <c r="O76" s="189"/>
     </row>
-    <row r="77" spans="1:15" ht="15" customHeight="1">
-      <c r="A77" s="13"/>
-      <c r="B77" s="11"/>
+    <row r="77" spans="3:15" ht="15" customHeight="1">
       <c r="C77" s="9"/>
       <c r="D77" s="11"/>
       <c r="E77" s="14"/>
@@ -46081,9 +45969,7 @@
       <c r="M77" s="15"/>
       <c r="N77" s="15"/>
     </row>
-    <row r="78" spans="1:15" ht="15" customHeight="1">
-      <c r="A78" s="13"/>
-      <c r="B78" s="11"/>
+    <row r="78" spans="3:15" ht="15" customHeight="1">
       <c r="C78" s="9"/>
       <c r="D78" s="11"/>
       <c r="E78" s="14"/>
@@ -46097,9 +45983,7 @@
       <c r="M78" s="15"/>
       <c r="N78" s="15"/>
     </row>
-    <row r="79" spans="1:15" ht="15" customHeight="1">
-      <c r="A79" s="13"/>
-      <c r="B79" s="11"/>
+    <row r="79" spans="3:15" ht="15" customHeight="1">
       <c r="C79" s="9"/>
       <c r="D79" s="33"/>
       <c r="E79" s="14"/>
@@ -46113,9 +45997,7 @@
       <c r="M79" s="15"/>
       <c r="N79" s="15"/>
     </row>
-    <row r="80" spans="1:15" ht="15" customHeight="1">
-      <c r="A80" s="13"/>
-      <c r="B80" s="11"/>
+    <row r="80" spans="3:15" ht="15" customHeight="1">
       <c r="C80" s="9"/>
       <c r="D80" s="33"/>
       <c r="E80" s="14"/>
@@ -46131,8 +46013,6 @@
       <c r="O80" s="189"/>
     </row>
     <row r="81" spans="1:17" ht="15" customHeight="1">
-      <c r="A81" s="13"/>
-      <c r="B81" s="11"/>
       <c r="C81" s="9"/>
       <c r="D81" s="11"/>
       <c r="E81" s="14"/>
@@ -46148,8 +46028,6 @@
       <c r="O81" s="189"/>
     </row>
     <row r="82" spans="1:17" ht="15" customHeight="1">
-      <c r="A82" s="13"/>
-      <c r="B82" s="11"/>
       <c r="C82" s="12"/>
       <c r="D82" s="9"/>
       <c r="E82" s="14"/>
@@ -46165,8 +46043,6 @@
       <c r="O82" s="15"/>
     </row>
     <row r="83" spans="1:17" ht="15" customHeight="1">
-      <c r="A83" s="13"/>
-      <c r="B83" s="11"/>
       <c r="C83" s="9"/>
       <c r="D83" s="9"/>
       <c r="E83" s="14"/>
@@ -46182,8 +46058,8 @@
       <c r="O83" s="189"/>
     </row>
     <row r="84" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A84" s="13"/>
-      <c r="B84" s="16"/>
+      <c r="A84" s="22"/>
+      <c r="B84" s="22"/>
       <c r="C84" s="9"/>
       <c r="D84" s="16"/>
       <c r="E84" s="16"/>
@@ -46194,7 +46070,8 @@
       <c r="Q84" s="11"/>
     </row>
     <row r="85" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A85" s="13"/>
+      <c r="A85" s="22"/>
+      <c r="B85" s="22"/>
       <c r="C85" s="9"/>
       <c r="E85" s="16"/>
       <c r="F85" s="138"/>
@@ -46205,8 +46082,8 @@
       <c r="Q85" s="11"/>
     </row>
     <row r="86" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A86" s="13"/>
-      <c r="B86" s="16"/>
+      <c r="A86" s="22"/>
+      <c r="B86" s="22"/>
       <c r="C86" s="9"/>
       <c r="D86" s="16"/>
       <c r="E86" s="16"/>
@@ -46217,7 +46094,8 @@
       <c r="Q86" s="11"/>
     </row>
     <row r="87" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A87" s="13"/>
+      <c r="A87" s="22"/>
+      <c r="B87" s="22"/>
       <c r="C87" s="12"/>
       <c r="D87" s="16"/>
       <c r="E87" s="16"/>
@@ -46227,8 +46105,6 @@
       <c r="Q87" s="11"/>
     </row>
     <row r="88" spans="1:17" ht="15" customHeight="1">
-      <c r="A88" s="13"/>
-      <c r="B88" s="9"/>
       <c r="C88" s="9"/>
       <c r="D88" s="12"/>
       <c r="E88" s="12"/>
@@ -46244,8 +46120,6 @@
       <c r="O88" s="189"/>
     </row>
     <row r="89" spans="1:17" ht="15" customHeight="1">
-      <c r="A89" s="22"/>
-      <c r="B89" s="45"/>
       <c r="C89" s="12"/>
       <c r="D89" s="12"/>
       <c r="E89" s="17"/>
@@ -46261,8 +46135,6 @@
       <c r="O89" s="189"/>
     </row>
     <row r="90" spans="1:17" ht="15" customHeight="1">
-      <c r="A90" s="22"/>
-      <c r="B90" s="45"/>
       <c r="C90" s="12"/>
       <c r="D90" s="12"/>
       <c r="E90" s="9"/>
@@ -46273,7 +46145,7 @@
     </row>
     <row r="91" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
       <c r="A91" s="22"/>
-      <c r="B91" s="45"/>
+      <c r="B91" s="22"/>
       <c r="C91" s="12"/>
       <c r="D91" s="17"/>
       <c r="E91" s="9"/>
@@ -46291,8 +46163,8 @@
       <c r="Q91" s="11"/>
     </row>
     <row r="92" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A92" s="13"/>
-      <c r="B92" s="11"/>
+      <c r="A92" s="22"/>
+      <c r="B92" s="22"/>
       <c r="C92" s="9"/>
       <c r="D92" s="139"/>
       <c r="E92" s="103"/>
@@ -46310,8 +46182,8 @@
       <c r="Q92" s="11"/>
     </row>
     <row r="93" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A93" s="13"/>
-      <c r="B93" s="11"/>
+      <c r="A93" s="22"/>
+      <c r="B93" s="22"/>
       <c r="C93" s="9"/>
       <c r="D93" s="14"/>
       <c r="G93" s="87"/>
@@ -46320,8 +46192,8 @@
       <c r="Q93" s="11"/>
     </row>
     <row r="94" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A94" s="13"/>
-      <c r="B94" s="11"/>
+      <c r="A94" s="22"/>
+      <c r="B94" s="22"/>
       <c r="C94" s="9"/>
       <c r="D94" s="14"/>
       <c r="E94" s="16"/>
@@ -46331,8 +46203,8 @@
       <c r="Q94" s="11"/>
     </row>
     <row r="95" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A95" s="13"/>
-      <c r="B95" s="11"/>
+      <c r="A95" s="22"/>
+      <c r="B95" s="22"/>
       <c r="C95" s="9"/>
       <c r="D95" s="14"/>
       <c r="E95" s="16"/>
@@ -46342,7 +46214,8 @@
       <c r="Q95" s="11"/>
     </row>
     <row r="96" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A96" s="13"/>
+      <c r="A96" s="22"/>
+      <c r="B96" s="22"/>
       <c r="C96" s="9"/>
       <c r="D96" s="134"/>
       <c r="E96" s="123"/>
@@ -46356,7 +46229,7 @@
     </row>
     <row r="97" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
       <c r="A97" s="22"/>
-      <c r="B97" s="45"/>
+      <c r="B97" s="22"/>
       <c r="C97" s="12"/>
       <c r="D97" s="17"/>
       <c r="E97" s="20"/>
@@ -46374,8 +46247,8 @@
       <c r="Q97" s="11"/>
     </row>
     <row r="98" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A98" s="13"/>
-      <c r="B98" s="11"/>
+      <c r="A98" s="22"/>
+      <c r="B98" s="22"/>
       <c r="C98" s="12"/>
       <c r="D98" s="14"/>
       <c r="E98" s="16"/>
@@ -46385,8 +46258,8 @@
       <c r="Q98" s="11"/>
     </row>
     <row r="99" spans="1:17" s="15" customFormat="1" ht="15" customHeight="1">
-      <c r="A99" s="13"/>
-      <c r="B99" s="11"/>
+      <c r="A99" s="22"/>
+      <c r="B99" s="22"/>
       <c r="C99" s="9"/>
       <c r="D99" s="14"/>
       <c r="E99" s="16"/>
@@ -46404,8 +46277,6 @@
       <c r="Q99" s="11"/>
     </row>
     <row r="100" spans="1:17" ht="15" customHeight="1">
-      <c r="A100" s="13"/>
-      <c r="B100" s="11"/>
       <c r="C100" s="12"/>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
@@ -46421,8 +46292,6 @@
       <c r="O100" s="15"/>
     </row>
     <row r="101" spans="1:17" ht="15" customHeight="1">
-      <c r="A101" s="13"/>
-      <c r="B101" s="11"/>
       <c r="C101" s="9"/>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
@@ -46430,8 +46299,6 @@
       <c r="I101" s="45"/>
     </row>
     <row r="102" spans="1:17" ht="15" customHeight="1">
-      <c r="A102" s="22"/>
-      <c r="B102" s="45"/>
       <c r="C102" s="12"/>
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
@@ -46440,8 +46307,6 @@
       <c r="I102" s="12"/>
     </row>
     <row r="103" spans="1:17" ht="15" customHeight="1">
-      <c r="A103" s="13"/>
-      <c r="B103" s="11"/>
       <c r="C103" s="9"/>
       <c r="D103" s="9"/>
       <c r="E103" s="9"/>
@@ -46451,8 +46316,6 @@
       <c r="I103" s="9"/>
     </row>
     <row r="104" spans="1:17" ht="15" customHeight="1">
-      <c r="A104" s="22"/>
-      <c r="B104" s="45"/>
       <c r="C104" s="12"/>
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
@@ -46461,8 +46324,6 @@
       <c r="I104" s="12"/>
     </row>
     <row r="105" spans="1:17" ht="15" customHeight="1">
-      <c r="A105" s="22"/>
-      <c r="B105" s="45"/>
       <c r="C105" s="12"/>
       <c r="D105" s="12"/>
       <c r="E105" s="12"/>
@@ -46471,8 +46332,6 @@
       <c r="I105" s="12"/>
     </row>
     <row r="106" spans="1:17" ht="15" customHeight="1">
-      <c r="A106" s="22"/>
-      <c r="B106" s="45"/>
       <c r="C106" s="12"/>
       <c r="D106" s="12"/>
       <c r="E106" s="12"/>
@@ -46481,8 +46340,6 @@
       <c r="I106" s="12"/>
     </row>
     <row r="107" spans="1:17" ht="15" customHeight="1">
-      <c r="A107" s="22"/>
-      <c r="B107" s="45"/>
       <c r="C107" s="12"/>
       <c r="D107" s="12"/>
       <c r="E107" s="12"/>
@@ -46491,7 +46348,6 @@
       <c r="I107" s="12"/>
     </row>
     <row r="108" spans="1:17" ht="15" customHeight="1">
-      <c r="A108" s="22"/>
       <c r="C108" s="12"/>
       <c r="D108" s="20"/>
       <c r="E108" s="12"/>
@@ -46505,7 +46361,6 @@
       <c r="M108" s="45"/>
     </row>
     <row r="109" spans="1:17" ht="15" customHeight="1">
-      <c r="A109" s="22"/>
       <c r="C109" s="12"/>
       <c r="D109" s="20"/>
       <c r="E109" s="12"/>
@@ -46514,7 +46369,6 @@
       <c r="I109" s="12"/>
     </row>
     <row r="110" spans="1:17" ht="15" customHeight="1">
-      <c r="A110" s="22"/>
       <c r="C110" s="12"/>
       <c r="D110" s="20"/>
       <c r="E110" s="12"/>
@@ -46523,7 +46377,6 @@
       <c r="I110" s="12"/>
     </row>
     <row r="111" spans="1:17" ht="15" customHeight="1">
-      <c r="A111" s="22"/>
       <c r="C111" s="12"/>
       <c r="D111" s="20"/>
       <c r="E111" s="12"/>
@@ -46532,24 +46385,18 @@
       <c r="I111" s="12"/>
     </row>
     <row r="112" spans="1:17" ht="15" customHeight="1">
-      <c r="A112" s="13"/>
-      <c r="B112" s="15"/>
       <c r="C112" s="9"/>
       <c r="E112" s="17"/>
       <c r="H112" s="9"/>
       <c r="I112" s="45"/>
     </row>
-    <row r="113" spans="1:14" ht="14" customHeight="1">
-      <c r="A113" s="13"/>
-      <c r="B113" s="15"/>
+    <row r="113" spans="3:14" ht="14" customHeight="1">
       <c r="C113" s="9"/>
       <c r="E113" s="16"/>
       <c r="H113" s="9"/>
       <c r="I113" s="45"/>
     </row>
-    <row r="114" spans="1:14" ht="15" customHeight="1">
-      <c r="A114" s="13"/>
-      <c r="B114" s="15"/>
+    <row r="114" spans="3:14" ht="15" customHeight="1">
       <c r="C114" s="9"/>
       <c r="D114" s="16"/>
       <c r="E114" s="9"/>
@@ -46563,9 +46410,7 @@
       <c r="M114" s="15"/>
       <c r="N114" s="15"/>
     </row>
-    <row r="115" spans="1:14" ht="15" customHeight="1">
-      <c r="A115" s="13"/>
-      <c r="B115" s="15"/>
+    <row r="115" spans="3:14" ht="15" customHeight="1">
       <c r="C115" s="9"/>
       <c r="D115" s="16"/>
       <c r="E115" s="9"/>
@@ -46579,9 +46424,7 @@
       <c r="M115" s="15"/>
       <c r="N115" s="15"/>
     </row>
-    <row r="116" spans="1:14" ht="15" customHeight="1">
-      <c r="A116" s="13"/>
-      <c r="B116" s="15"/>
+    <row r="116" spans="3:14" ht="15" customHeight="1">
       <c r="C116" s="9"/>
       <c r="D116" s="16"/>
       <c r="E116" s="9"/>
@@ -46595,9 +46438,7 @@
       <c r="M116" s="15"/>
       <c r="N116" s="15"/>
     </row>
-    <row r="117" spans="1:14" ht="15" customHeight="1">
-      <c r="A117" s="13"/>
-      <c r="B117" s="15"/>
+    <row r="117" spans="3:14" ht="15" customHeight="1">
       <c r="C117" s="9"/>
       <c r="D117" s="16"/>
       <c r="E117" s="16"/>
@@ -46611,9 +46452,7 @@
       <c r="M117" s="15"/>
       <c r="N117" s="15"/>
     </row>
-    <row r="118" spans="1:14" ht="15" customHeight="1">
-      <c r="A118" s="13"/>
-      <c r="B118" s="15"/>
+    <row r="118" spans="3:14" ht="15" customHeight="1">
       <c r="C118" s="9"/>
       <c r="D118" s="16"/>
       <c r="E118" s="16"/>
@@ -46627,9 +46466,7 @@
       <c r="M118" s="15"/>
       <c r="N118" s="15"/>
     </row>
-    <row r="119" spans="1:14" ht="15" customHeight="1">
-      <c r="A119" s="13"/>
-      <c r="B119" s="15"/>
+    <row r="119" spans="3:14" ht="15" customHeight="1">
       <c r="C119" s="9"/>
       <c r="D119" s="16"/>
       <c r="E119" s="16"/>
@@ -46643,9 +46480,7 @@
       <c r="M119" s="15"/>
       <c r="N119" s="15"/>
     </row>
-    <row r="120" spans="1:14" ht="15" customHeight="1">
-      <c r="A120" s="13"/>
-      <c r="B120" s="15"/>
+    <row r="120" spans="3:14" ht="15" customHeight="1">
       <c r="C120" s="9"/>
       <c r="D120" s="14"/>
       <c r="E120" s="14"/>
@@ -46659,9 +46494,7 @@
       <c r="M120" s="15"/>
       <c r="N120" s="15"/>
     </row>
-    <row r="121" spans="1:14" ht="15" customHeight="1">
-      <c r="A121" s="13"/>
-      <c r="B121" s="15"/>
+    <row r="121" spans="3:14" ht="15" customHeight="1">
       <c r="C121" s="9"/>
       <c r="D121" s="14"/>
       <c r="E121" s="14"/>
@@ -46675,9 +46508,7 @@
       <c r="M121" s="15"/>
       <c r="N121" s="15"/>
     </row>
-    <row r="122" spans="1:14" ht="15" customHeight="1">
-      <c r="A122" s="13"/>
-      <c r="B122" s="15"/>
+    <row r="122" spans="3:14" ht="15" customHeight="1">
       <c r="C122" s="9"/>
       <c r="D122" s="14"/>
       <c r="E122" s="14"/>
@@ -46691,8 +46522,7 @@
       <c r="M122" s="15"/>
       <c r="N122" s="15"/>
     </row>
-    <row r="123" spans="1:14" ht="15" customHeight="1">
-      <c r="A123" s="22"/>
+    <row r="123" spans="3:14" ht="15" customHeight="1">
       <c r="C123" s="12"/>
       <c r="D123" s="17"/>
       <c r="E123" s="17"/>
@@ -46700,8 +46530,7 @@
       <c r="H123" s="12"/>
       <c r="I123" s="20"/>
     </row>
-    <row r="124" spans="1:14" ht="15" customHeight="1">
-      <c r="A124" s="22"/>
+    <row r="124" spans="3:14" ht="15" customHeight="1">
       <c r="C124" s="12"/>
       <c r="D124" s="17"/>
       <c r="E124" s="17"/>
@@ -46709,8 +46538,7 @@
       <c r="H124" s="12"/>
       <c r="I124" s="20"/>
     </row>
-    <row r="125" spans="1:14" ht="15" customHeight="1">
-      <c r="A125" s="22"/>
+    <row r="125" spans="3:14" ht="15" customHeight="1">
       <c r="C125" s="12"/>
       <c r="D125" s="17"/>
       <c r="E125" s="17"/>
@@ -46718,9 +46546,7 @@
       <c r="H125" s="12"/>
       <c r="I125" s="20"/>
     </row>
-    <row r="126" spans="1:14" ht="15" customHeight="1">
-      <c r="A126" s="22"/>
-      <c r="B126" s="22"/>
+    <row r="126" spans="3:14" ht="15" customHeight="1">
       <c r="C126" s="12"/>
       <c r="D126" s="17"/>
       <c r="E126" s="17"/>
@@ -46728,9 +46554,7 @@
       <c r="H126" s="12"/>
       <c r="I126" s="20"/>
     </row>
-    <row r="127" spans="1:14" ht="15" customHeight="1">
-      <c r="A127" s="22"/>
-      <c r="B127" s="22"/>
+    <row r="127" spans="3:14" ht="15" customHeight="1">
       <c r="C127" s="12"/>
       <c r="D127" s="17"/>
       <c r="E127" s="17"/>
@@ -46738,9 +46562,7 @@
       <c r="H127" s="12"/>
       <c r="I127" s="20"/>
     </row>
-    <row r="128" spans="1:14" ht="15" customHeight="1">
-      <c r="A128" s="22"/>
-      <c r="B128" s="22"/>
+    <row r="128" spans="3:14" ht="15" customHeight="1">
       <c r="C128" s="12"/>
       <c r="D128" s="17"/>
       <c r="E128" s="17"/>
@@ -46768,8 +46590,6 @@
       <c r="Q129" s="11"/>
     </row>
     <row r="130" spans="1:17" ht="15" customHeight="1">
-      <c r="A130" s="22"/>
-      <c r="B130" s="22"/>
       <c r="C130" s="12"/>
       <c r="D130" s="12"/>
       <c r="E130" s="9"/>
@@ -46784,8 +46604,6 @@
       <c r="N130" s="11"/>
     </row>
     <row r="131" spans="1:17" ht="15" customHeight="1">
-      <c r="A131" s="22"/>
-      <c r="B131" s="22"/>
       <c r="C131" s="12"/>
       <c r="D131" s="12"/>
       <c r="E131" s="14"/>
@@ -46800,8 +46618,6 @@
       <c r="N131" s="15"/>
     </row>
     <row r="132" spans="1:17" ht="15" customHeight="1">
-      <c r="A132" s="22"/>
-      <c r="B132" s="22"/>
       <c r="C132" s="12"/>
       <c r="D132" s="12"/>
       <c r="E132" s="14"/>
@@ -46816,8 +46632,6 @@
       <c r="N132" s="15"/>
     </row>
     <row r="133" spans="1:17" ht="15" customHeight="1">
-      <c r="A133" s="22"/>
-      <c r="B133" s="22"/>
       <c r="C133" s="12"/>
       <c r="D133" s="12"/>
       <c r="E133" s="16"/>
@@ -47160,8 +46974,6 @@
       <c r="Q156" s="11"/>
     </row>
     <row r="157" spans="1:17" ht="15" customHeight="1">
-      <c r="A157" s="22"/>
-      <c r="B157" s="22"/>
       <c r="C157" s="12"/>
       <c r="D157" s="17"/>
       <c r="E157" s="14"/>
@@ -47177,8 +46989,6 @@
       <c r="O157" s="192"/>
     </row>
     <row r="158" spans="1:17" ht="15" customHeight="1">
-      <c r="A158" s="22"/>
-      <c r="B158" s="22"/>
       <c r="C158" s="12"/>
       <c r="D158" s="17"/>
       <c r="E158" s="14"/>
@@ -47212,15 +47022,11 @@
       <c r="Q159" s="11"/>
     </row>
     <row r="160" spans="1:17" ht="15" customHeight="1">
-      <c r="A160" s="22"/>
-      <c r="B160" s="22"/>
       <c r="C160" s="9"/>
       <c r="G160" s="9"/>
       <c r="H160" s="9"/>
     </row>
     <row r="161" spans="1:17" ht="15" customHeight="1">
-      <c r="A161" s="22"/>
-      <c r="B161" s="22"/>
       <c r="C161" s="9"/>
       <c r="G161" s="9"/>
       <c r="H161" s="9"/>
@@ -47301,262 +47107,70 @@
       <c r="P165" s="27"/>
       <c r="Q165" s="27"/>
     </row>
-    <row r="166" spans="1:17" ht="15" customHeight="1">
-      <c r="A166" s="22"/>
-      <c r="B166" s="22"/>
-    </row>
-    <row r="167" spans="1:17" ht="15" customHeight="1">
-      <c r="A167" s="22"/>
-      <c r="B167" s="22"/>
-    </row>
-    <row r="168" spans="1:17" ht="15" customHeight="1">
-      <c r="A168" s="22"/>
-      <c r="B168" s="22"/>
-    </row>
-    <row r="169" spans="1:17" ht="15" customHeight="1">
-      <c r="A169" s="22"/>
-      <c r="B169" s="22"/>
-    </row>
-    <row r="170" spans="1:17" ht="15" customHeight="1">
-      <c r="A170" s="22"/>
-      <c r="B170" s="22"/>
-    </row>
-    <row r="171" spans="1:17" ht="15" customHeight="1">
-      <c r="A171" s="22"/>
-      <c r="B171" s="22"/>
-    </row>
-    <row r="172" spans="1:17" ht="15" customHeight="1">
-      <c r="A172" s="22"/>
-      <c r="B172" s="22"/>
-    </row>
-    <row r="173" spans="1:17" ht="15" customHeight="1">
-      <c r="A173" s="22"/>
-      <c r="B173" s="22"/>
-    </row>
-    <row r="174" spans="1:17" ht="15" customHeight="1">
-      <c r="A174" s="22"/>
-      <c r="B174" s="22"/>
-    </row>
-    <row r="175" spans="1:17" ht="15" customHeight="1">
-      <c r="A175" s="22"/>
-      <c r="B175" s="22"/>
-    </row>
-    <row r="176" spans="1:17" ht="15" customHeight="1">
-      <c r="A176" s="22"/>
-      <c r="B176" s="22"/>
-    </row>
-    <row r="177" spans="1:2" ht="15" customHeight="1">
-      <c r="A177" s="22"/>
-      <c r="B177" s="22"/>
-    </row>
-    <row r="178" spans="1:2" ht="15" customHeight="1">
-      <c r="A178" s="22"/>
-      <c r="B178" s="22"/>
-    </row>
-    <row r="179" spans="1:2" ht="15" customHeight="1">
-      <c r="A179" s="22"/>
-      <c r="B179" s="22"/>
-    </row>
-    <row r="180" spans="1:2" ht="15" customHeight="1">
-      <c r="A180" s="22"/>
-      <c r="B180" s="22"/>
-    </row>
-    <row r="181" spans="1:2" ht="15" customHeight="1">
-      <c r="A181" s="22"/>
-      <c r="B181" s="22"/>
-    </row>
-    <row r="182" spans="1:2" ht="15" customHeight="1">
-      <c r="A182" s="22"/>
-      <c r="B182" s="22"/>
-    </row>
-    <row r="183" spans="1:2" ht="15" customHeight="1">
-      <c r="A183" s="22"/>
-      <c r="B183" s="22"/>
-    </row>
-    <row r="184" spans="1:2" ht="15" customHeight="1">
-      <c r="A184" s="22"/>
-      <c r="B184" s="22"/>
-    </row>
-    <row r="185" spans="1:2" ht="15" customHeight="1">
-      <c r="A185" s="22"/>
-      <c r="B185" s="22"/>
-    </row>
-    <row r="186" spans="1:2" ht="15" customHeight="1">
-      <c r="A186" s="22"/>
-      <c r="B186" s="22"/>
-    </row>
-    <row r="187" spans="1:2" ht="15" customHeight="1">
-      <c r="A187" s="22"/>
-      <c r="B187" s="22"/>
-    </row>
-    <row r="188" spans="1:2" ht="15" customHeight="1">
-      <c r="A188" s="22"/>
-      <c r="B188" s="22"/>
-    </row>
-    <row r="189" spans="1:2" ht="15" customHeight="1">
-      <c r="A189" s="22"/>
-      <c r="B189" s="22"/>
-    </row>
-    <row r="190" spans="1:2" ht="15" customHeight="1">
-      <c r="A190" s="22"/>
-      <c r="B190" s="22"/>
-    </row>
-    <row r="191" spans="1:2" ht="15" customHeight="1">
-      <c r="A191" s="22"/>
-      <c r="B191" s="22"/>
-    </row>
-    <row r="192" spans="1:2" ht="15" customHeight="1">
-      <c r="A192" s="22"/>
-      <c r="B192" s="22"/>
-    </row>
-    <row r="193" spans="1:2" ht="15" customHeight="1">
-      <c r="A193" s="22"/>
-      <c r="B193" s="22"/>
-    </row>
-    <row r="194" spans="1:2" ht="15" customHeight="1">
-      <c r="A194" s="22"/>
-      <c r="B194" s="22"/>
-    </row>
-    <row r="195" spans="1:2" ht="15" customHeight="1">
-      <c r="A195" s="22"/>
-      <c r="B195" s="22"/>
-    </row>
-    <row r="196" spans="1:2" ht="15" customHeight="1">
-      <c r="A196" s="22"/>
-      <c r="B196" s="22"/>
-    </row>
-    <row r="197" spans="1:2" ht="15" customHeight="1">
-      <c r="A197" s="22"/>
-      <c r="B197" s="22"/>
-    </row>
-    <row r="198" spans="1:2" ht="15" customHeight="1">
-      <c r="A198" s="22"/>
-      <c r="B198" s="22"/>
-    </row>
-    <row r="199" spans="1:2" ht="15" customHeight="1">
-      <c r="A199" s="22"/>
-      <c r="B199" s="22"/>
-    </row>
-    <row r="200" spans="1:2" ht="15" customHeight="1">
-      <c r="A200" s="22"/>
-      <c r="B200" s="22"/>
-    </row>
-    <row r="201" spans="1:2" ht="15" customHeight="1">
-      <c r="A201" s="22"/>
-      <c r="B201" s="22"/>
-    </row>
-    <row r="202" spans="1:2" ht="15" customHeight="1">
-      <c r="A202" s="22"/>
-      <c r="B202" s="22"/>
-    </row>
-    <row r="203" spans="1:2" ht="15" customHeight="1">
-      <c r="A203" s="22"/>
-      <c r="B203" s="22"/>
-    </row>
-    <row r="204" spans="1:2" ht="15" customHeight="1">
-      <c r="A204" s="22"/>
-      <c r="B204" s="22"/>
-    </row>
-    <row r="205" spans="1:2" ht="15" customHeight="1">
-      <c r="A205" s="22"/>
-      <c r="B205" s="22"/>
-    </row>
-    <row r="206" spans="1:2" ht="15" customHeight="1">
-      <c r="A206" s="22"/>
-      <c r="B206" s="22"/>
-    </row>
-    <row r="207" spans="1:2" ht="15" customHeight="1">
-      <c r="A207" s="22"/>
-      <c r="B207" s="22"/>
-    </row>
-    <row r="208" spans="1:2" ht="15" customHeight="1">
-      <c r="A208" s="22"/>
-      <c r="B208" s="22"/>
-    </row>
-    <row r="209" spans="1:2" ht="15" customHeight="1">
-      <c r="A209" s="22"/>
-      <c r="B209" s="22"/>
-    </row>
-    <row r="210" spans="1:2" ht="15" customHeight="1">
-      <c r="A210" s="22"/>
-      <c r="B210" s="22"/>
-    </row>
-    <row r="211" spans="1:2" ht="15" customHeight="1">
-      <c r="A211" s="22"/>
-      <c r="B211" s="22"/>
-    </row>
-    <row r="212" spans="1:2" ht="15" customHeight="1">
-      <c r="A212" s="22"/>
-      <c r="B212" s="22"/>
-    </row>
-    <row r="213" spans="1:2" ht="15" customHeight="1">
-      <c r="A213" s="22"/>
-      <c r="B213" s="22"/>
-    </row>
-    <row r="214" spans="1:2" ht="15" customHeight="1">
-      <c r="A214" s="22"/>
-      <c r="B214" s="22"/>
-    </row>
-    <row r="215" spans="1:2" ht="15" customHeight="1">
-      <c r="A215" s="22"/>
-      <c r="B215" s="22"/>
-    </row>
-    <row r="216" spans="1:2" ht="15" customHeight="1">
-      <c r="A216" s="22"/>
-      <c r="B216" s="22"/>
-    </row>
-    <row r="217" spans="1:2" ht="15" customHeight="1">
-      <c r="A217" s="22"/>
-      <c r="B217" s="22"/>
-    </row>
-    <row r="218" spans="1:2" ht="15" customHeight="1">
-      <c r="A218" s="22"/>
-      <c r="B218" s="22"/>
-    </row>
-    <row r="219" spans="1:2" ht="15" customHeight="1">
-      <c r="A219" s="22"/>
-      <c r="B219" s="22"/>
-    </row>
-    <row r="220" spans="1:2" ht="15" customHeight="1">
-      <c r="A220" s="22"/>
-      <c r="B220" s="22"/>
-    </row>
-    <row r="221" spans="1:2" ht="15" customHeight="1">
-      <c r="A221" s="22"/>
-      <c r="B221" s="22"/>
-    </row>
-    <row r="222" spans="1:2" ht="15" customHeight="1">
-      <c r="A222" s="22"/>
-      <c r="B222" s="22"/>
-    </row>
-    <row r="223" spans="1:2" ht="15" customHeight="1">
-      <c r="A223" s="22"/>
-      <c r="B223" s="22"/>
-    </row>
-    <row r="224" spans="1:2" ht="15" customHeight="1">
-      <c r="A224" s="22"/>
-      <c r="B224" s="22"/>
-    </row>
-    <row r="225" spans="1:2" ht="15" customHeight="1">
-      <c r="A225" s="22"/>
-      <c r="B225" s="22"/>
-    </row>
-    <row r="226" spans="1:2" ht="15" customHeight="1">
-      <c r="A226" s="22"/>
-      <c r="B226" s="22"/>
-    </row>
-    <row r="227" spans="1:2" ht="15" customHeight="1">
-      <c r="A227" s="22"/>
-      <c r="B227" s="22"/>
-    </row>
-    <row r="228" spans="1:2" ht="15" customHeight="1">
-      <c r="A228" s="22"/>
-      <c r="B228" s="22"/>
-    </row>
-    <row r="229" spans="1:2" ht="15" customHeight="1">
-      <c r="A229" s="22"/>
-      <c r="B229" s="22"/>
-    </row>
+    <row r="166" spans="1:17" ht="15" customHeight="1"/>
+    <row r="167" spans="1:17" ht="15" customHeight="1"/>
+    <row r="168" spans="1:17" ht="15" customHeight="1"/>
+    <row r="169" spans="1:17" ht="15" customHeight="1"/>
+    <row r="170" spans="1:17" ht="15" customHeight="1"/>
+    <row r="171" spans="1:17" ht="15" customHeight="1"/>
+    <row r="172" spans="1:17" ht="15" customHeight="1"/>
+    <row r="173" spans="1:17" ht="15" customHeight="1"/>
+    <row r="174" spans="1:17" ht="15" customHeight="1"/>
+    <row r="175" spans="1:17" ht="15" customHeight="1"/>
+    <row r="176" spans="1:17" ht="15" customHeight="1"/>
+    <row r="177" ht="15" customHeight="1"/>
+    <row r="178" ht="15" customHeight="1"/>
+    <row r="179" ht="15" customHeight="1"/>
+    <row r="180" ht="15" customHeight="1"/>
+    <row r="181" ht="15" customHeight="1"/>
+    <row r="182" ht="15" customHeight="1"/>
+    <row r="183" ht="15" customHeight="1"/>
+    <row r="184" ht="15" customHeight="1"/>
+    <row r="185" ht="15" customHeight="1"/>
+    <row r="186" ht="15" customHeight="1"/>
+    <row r="187" ht="15" customHeight="1"/>
+    <row r="188" ht="15" customHeight="1"/>
+    <row r="189" ht="15" customHeight="1"/>
+    <row r="190" ht="15" customHeight="1"/>
+    <row r="191" ht="15" customHeight="1"/>
+    <row r="192" ht="15" customHeight="1"/>
+    <row r="193" ht="15" customHeight="1"/>
+    <row r="194" ht="15" customHeight="1"/>
+    <row r="195" ht="15" customHeight="1"/>
+    <row r="196" ht="15" customHeight="1"/>
+    <row r="197" ht="15" customHeight="1"/>
+    <row r="198" ht="15" customHeight="1"/>
+    <row r="199" ht="15" customHeight="1"/>
+    <row r="200" ht="15" customHeight="1"/>
+    <row r="201" ht="15" customHeight="1"/>
+    <row r="202" ht="15" customHeight="1"/>
+    <row r="203" ht="15" customHeight="1"/>
+    <row r="204" ht="15" customHeight="1"/>
+    <row r="205" ht="15" customHeight="1"/>
+    <row r="206" ht="15" customHeight="1"/>
+    <row r="207" ht="15" customHeight="1"/>
+    <row r="208" ht="15" customHeight="1"/>
+    <row r="209" ht="15" customHeight="1"/>
+    <row r="210" ht="15" customHeight="1"/>
+    <row r="211" ht="15" customHeight="1"/>
+    <row r="212" ht="15" customHeight="1"/>
+    <row r="213" ht="15" customHeight="1"/>
+    <row r="214" ht="15" customHeight="1"/>
+    <row r="215" ht="15" customHeight="1"/>
+    <row r="216" ht="15" customHeight="1"/>
+    <row r="217" ht="15" customHeight="1"/>
+    <row r="218" ht="15" customHeight="1"/>
+    <row r="219" ht="15" customHeight="1"/>
+    <row r="220" ht="15" customHeight="1"/>
+    <row r="221" ht="15" customHeight="1"/>
+    <row r="222" ht="15" customHeight="1"/>
+    <row r="223" ht="15" customHeight="1"/>
+    <row r="224" ht="15" customHeight="1"/>
+    <row r="225" ht="15" customHeight="1"/>
+    <row r="226" ht="15" customHeight="1"/>
+    <row r="227" ht="15" customHeight="1"/>
+    <row r="228" ht="15" customHeight="1"/>
+    <row r="229" ht="15" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A3:O161" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <conditionalFormatting sqref="E120">

</xml_diff>

<commit_message>
SSCS-7828 Elements and issues for UC
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jack/Development/hmcts/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31908D2D-5030-F842-937C-F2E231EDB684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB694CE-81E6-C24F-91A1-73A7F4A07542}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -730,7 +730,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="39">
+  <fonts count="38">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -966,14 +966,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Arial"/>
@@ -1023,7 +1015,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1298,17 +1290,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1340,7 +1321,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="220">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1601,13 +1582,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="33" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1619,7 +1597,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1628,19 +1606,16 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2937,122 +2912,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C049F10D-F059-F941-9EA1-9C15C4FFCFC4}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="10.83203125" style="206"/>
+    <col min="2" max="2" width="10.83203125" style="199"/>
     <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18">
-      <c r="A1" s="196" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="206" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="197" t="s">
+      <c r="B1" s="199" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="198" t="s">
+      <c r="C1" s="197" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="199" t="s">
+      <c r="D1" s="198" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="199"/>
-      <c r="F1" s="199" t="s">
+      <c r="E1" s="198"/>
+      <c r="F1" s="198" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="197" t="s">
+      <c r="G1" s="196" t="s">
         <v>178</v>
       </c>
-      <c r="H1" s="197" t="s">
+      <c r="H1" s="196" t="s">
         <v>179</v>
       </c>
-      <c r="I1" s="197" t="s">
+      <c r="I1" s="196" t="s">
         <v>180</v>
       </c>
-      <c r="J1" s="200"/>
-      <c r="K1" s="197"/>
+      <c r="J1" s="199"/>
+      <c r="K1" s="196"/>
     </row>
     <row r="2" spans="1:11" ht="122" customHeight="1">
-      <c r="A2" s="201"/>
-      <c r="B2" s="201"/>
-      <c r="C2" s="202" t="s">
+      <c r="C2" s="201" t="s">
         <v>181</v>
       </c>
-      <c r="D2" s="203" t="s">
+      <c r="D2" s="202" t="s">
         <v>182</v>
       </c>
-      <c r="E2" s="203" t="s">
+      <c r="E2" s="202" t="s">
         <v>183</v>
       </c>
-      <c r="F2" s="201" t="s">
+      <c r="F2" s="200" t="s">
         <v>181</v>
       </c>
-      <c r="G2" s="201" t="s">
+      <c r="G2" s="200" t="s">
         <v>184</v>
       </c>
-      <c r="H2" s="201" t="s">
+      <c r="H2" s="200" t="s">
         <v>185</v>
       </c>
-      <c r="I2" s="203" t="s">
+      <c r="I2" s="202" t="s">
         <v>186</v>
       </c>
-      <c r="J2" s="203" t="s">
+      <c r="J2" s="202" t="s">
         <v>187</v>
       </c>
-      <c r="K2" s="204" t="s">
+      <c r="K2" s="203" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1">
-      <c r="A3" s="205" t="s">
+      <c r="A3" s="204" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="206" t="s">
+      <c r="B3" s="204" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="206" t="s">
+      <c r="C3" s="204" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="206" t="s">
+      <c r="D3" s="204" t="s">
         <v>126</v>
       </c>
-      <c r="E3" s="206" t="s">
+      <c r="E3" s="204" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="206" t="s">
+      <c r="F3" s="204" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="206" t="s">
+      <c r="G3" s="204" t="s">
         <v>189</v>
       </c>
-      <c r="H3" s="206" t="s">
+      <c r="H3" s="204" t="s">
         <v>190</v>
       </c>
-      <c r="I3" s="206" t="s">
+      <c r="I3" s="204" t="s">
         <v>191</v>
       </c>
-      <c r="J3" s="206" t="s">
+      <c r="J3" s="204" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="207" t="s">
+      <c r="K3" s="205" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="208"/>
-      <c r="B4" s="200"/>
-      <c r="C4" s="200"/>
-      <c r="D4" s="209"/>
-      <c r="E4" s="209"/>
-      <c r="F4" s="209"/>
-      <c r="G4" s="200"/>
-      <c r="H4" s="200"/>
-      <c r="I4" s="200"/>
-      <c r="J4" s="209"/>
-      <c r="K4" s="210"/>
+      <c r="C4" s="199"/>
+      <c r="D4" s="207"/>
+      <c r="E4" s="207"/>
+      <c r="F4" s="207"/>
+      <c r="G4" s="199"/>
+      <c r="H4" s="199"/>
+      <c r="I4" s="199"/>
+      <c r="J4" s="207"/>
+      <c r="K4" s="208"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3093,7 +3066,7 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="211"/>
+      <c r="F1" s="209"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
@@ -3111,7 +3084,7 @@
       <c r="E2" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="211"/>
+      <c r="F2" s="209"/>
       <c r="G2" s="59" t="s">
         <v>144</v>
       </c>
@@ -3135,7 +3108,7 @@
       <c r="E3" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="212" t="s">
+      <c r="F3" s="210" t="s">
         <v>56</v>
       </c>
       <c r="G3" s="12" t="s">
@@ -3151,7 +3124,7 @@
       <c r="C4" s="9"/>
       <c r="D4" s="11"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="212"/>
+      <c r="F4" s="210"/>
       <c r="G4" s="9"/>
       <c r="H4" s="11"/>
     </row>
@@ -3161,7 +3134,7 @@
       <c r="C5" s="12"/>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="212"/>
+      <c r="F5" s="210"/>
       <c r="G5" s="12"/>
       <c r="H5" s="45"/>
     </row>
@@ -3171,7 +3144,7 @@
       <c r="C6" s="12"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
-      <c r="F6" s="212"/>
+      <c r="F6" s="210"/>
       <c r="G6" s="12"/>
       <c r="H6" s="45"/>
     </row>
@@ -3181,7 +3154,7 @@
       <c r="C7" s="12"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
-      <c r="F7" s="212"/>
+      <c r="F7" s="210"/>
       <c r="G7" s="12"/>
       <c r="H7" s="45"/>
     </row>
@@ -3191,7 +3164,7 @@
       <c r="C8" s="12"/>
       <c r="D8" s="45"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="213"/>
+      <c r="F8" s="211"/>
       <c r="G8" s="11"/>
       <c r="H8" s="45"/>
     </row>
@@ -3201,7 +3174,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="214"/>
+      <c r="F9" s="212"/>
       <c r="G9" s="106"/>
       <c r="H9" s="87"/>
     </row>
@@ -3211,7 +3184,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="20"/>
       <c r="E10" s="17"/>
-      <c r="F10" s="215"/>
+      <c r="F10" s="213"/>
       <c r="G10" s="106"/>
       <c r="H10" s="45"/>
     </row>
@@ -3221,7 +3194,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="212"/>
+      <c r="F11" s="210"/>
       <c r="G11" s="12"/>
       <c r="H11" s="45"/>
     </row>
@@ -3231,7 +3204,7 @@
       <c r="C12" s="9"/>
       <c r="D12" s="15"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="212"/>
+      <c r="F12" s="210"/>
       <c r="G12" s="9"/>
       <c r="H12" s="74"/>
     </row>
@@ -3241,7 +3214,7 @@
       <c r="C13" s="9"/>
       <c r="D13" s="11"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="212"/>
+      <c r="F13" s="210"/>
       <c r="G13" s="9"/>
       <c r="H13" s="74"/>
     </row>
@@ -3251,7 +3224,7 @@
       <c r="C14" s="9"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="213"/>
+      <c r="F14" s="211"/>
       <c r="G14" s="9"/>
       <c r="H14" s="74"/>
     </row>
@@ -3261,7 +3234,7 @@
       <c r="C15" s="9"/>
       <c r="D15" s="11"/>
       <c r="E15" s="16"/>
-      <c r="F15" s="216"/>
+      <c r="F15" s="214"/>
       <c r="G15" s="19"/>
       <c r="H15" s="74"/>
     </row>
@@ -3271,7 +3244,7 @@
       <c r="C16" s="12"/>
       <c r="D16" s="11"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="212"/>
+      <c r="F16" s="210"/>
       <c r="G16" s="9"/>
       <c r="H16" s="45"/>
     </row>
@@ -3281,7 +3254,7 @@
       <c r="C17" s="9"/>
       <c r="D17" s="15"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="214"/>
+      <c r="F17" s="212"/>
       <c r="G17" s="106"/>
       <c r="H17" s="87"/>
     </row>
@@ -3291,7 +3264,7 @@
       <c r="C18" s="9"/>
       <c r="D18" s="15"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="212"/>
+      <c r="F18" s="210"/>
       <c r="G18" s="12"/>
       <c r="H18" s="87"/>
     </row>
@@ -3301,7 +3274,7 @@
       <c r="C19" s="9"/>
       <c r="D19" s="15"/>
       <c r="E19" s="17"/>
-      <c r="F19" s="215"/>
+      <c r="F19" s="213"/>
       <c r="G19" s="106"/>
       <c r="H19" s="87"/>
     </row>
@@ -3311,7 +3284,7 @@
       <c r="C20" s="9"/>
       <c r="D20" s="15"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="212"/>
+      <c r="F20" s="210"/>
       <c r="G20" s="9"/>
       <c r="H20" s="87"/>
     </row>
@@ -3321,7 +3294,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="15"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="214"/>
+      <c r="F21" s="212"/>
       <c r="G21" s="106"/>
       <c r="H21" s="87"/>
     </row>
@@ -3331,7 +3304,7 @@
       <c r="C22" s="12"/>
       <c r="D22" s="15"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="215"/>
+      <c r="F22" s="213"/>
       <c r="G22" s="19"/>
       <c r="H22" s="87"/>
     </row>
@@ -3341,7 +3314,7 @@
       <c r="C23" s="12"/>
       <c r="D23" s="15"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="212"/>
+      <c r="F23" s="210"/>
       <c r="G23" s="12"/>
       <c r="H23" s="45"/>
     </row>
@@ -3351,7 +3324,7 @@
       <c r="C24" s="12"/>
       <c r="D24" s="15"/>
       <c r="E24" s="33"/>
-      <c r="F24" s="217"/>
+      <c r="F24" s="215"/>
       <c r="G24" s="106"/>
       <c r="H24" s="87"/>
     </row>
@@ -3361,7 +3334,7 @@
       <c r="C25" s="9"/>
       <c r="D25" s="15"/>
       <c r="E25" s="17"/>
-      <c r="F25" s="215"/>
+      <c r="F25" s="213"/>
       <c r="G25" s="106"/>
       <c r="H25" s="18"/>
     </row>
@@ -3371,7 +3344,7 @@
       <c r="C26" s="145"/>
       <c r="D26" s="11"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="215"/>
+      <c r="F26" s="213"/>
       <c r="G26" s="106"/>
       <c r="H26" s="18"/>
     </row>
@@ -3381,7 +3354,7 @@
       <c r="C27" s="9"/>
       <c r="D27" s="15"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="215"/>
+      <c r="F27" s="213"/>
       <c r="G27" s="106"/>
       <c r="H27" s="87"/>
     </row>
@@ -3391,7 +3364,7 @@
       <c r="C28" s="9"/>
       <c r="D28" s="15"/>
       <c r="E28" s="17"/>
-      <c r="F28" s="215"/>
+      <c r="F28" s="213"/>
       <c r="G28" s="106"/>
       <c r="H28" s="87"/>
     </row>
@@ -3401,7 +3374,7 @@
       <c r="C29" s="9"/>
       <c r="D29" s="15"/>
       <c r="E29" s="17"/>
-      <c r="F29" s="215"/>
+      <c r="F29" s="213"/>
       <c r="G29" s="106"/>
       <c r="H29" s="87"/>
     </row>
@@ -3411,7 +3384,7 @@
       <c r="C30" s="16"/>
       <c r="D30" s="15"/>
       <c r="E30" s="17"/>
-      <c r="F30" s="215"/>
+      <c r="F30" s="213"/>
       <c r="G30" s="106"/>
       <c r="H30" s="87"/>
     </row>
@@ -3421,7 +3394,7 @@
       <c r="C31" s="16"/>
       <c r="D31" s="18"/>
       <c r="E31" s="17"/>
-      <c r="F31" s="215"/>
+      <c r="F31" s="213"/>
       <c r="G31" s="106"/>
       <c r="H31" s="18"/>
     </row>
@@ -3431,7 +3404,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="11"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="212"/>
+      <c r="F32" s="210"/>
       <c r="G32" s="9"/>
       <c r="H32" s="11"/>
       <c r="I32" s="57"/>
@@ -3442,7 +3415,7 @@
       <c r="C33" s="9"/>
       <c r="D33" s="11"/>
       <c r="E33" s="9"/>
-      <c r="F33" s="212"/>
+      <c r="F33" s="210"/>
       <c r="G33" s="9"/>
       <c r="H33" s="11"/>
       <c r="I33" s="57"/>
@@ -3453,7 +3426,7 @@
       <c r="C34" s="9"/>
       <c r="D34" s="11"/>
       <c r="E34" s="9"/>
-      <c r="F34" s="212"/>
+      <c r="F34" s="210"/>
       <c r="G34" s="9"/>
       <c r="H34" s="11"/>
       <c r="I34" s="57"/>
@@ -3464,7 +3437,7 @@
       <c r="C35" s="9"/>
       <c r="D35" s="11"/>
       <c r="E35" s="9"/>
-      <c r="F35" s="212"/>
+      <c r="F35" s="210"/>
       <c r="G35" s="9"/>
       <c r="H35" s="11"/>
       <c r="I35" s="57"/>
@@ -3475,7 +3448,7 @@
       <c r="C36" s="9"/>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
-      <c r="F36" s="213"/>
+      <c r="F36" s="211"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="57"/>
@@ -3486,7 +3459,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="11"/>
       <c r="E37" s="9"/>
-      <c r="F37" s="214"/>
+      <c r="F37" s="212"/>
       <c r="G37" s="19"/>
       <c r="H37" s="74"/>
       <c r="I37" s="57"/>
@@ -3497,7 +3470,7 @@
       <c r="C38" s="16"/>
       <c r="D38" s="11"/>
       <c r="E38" s="14"/>
-      <c r="F38" s="215"/>
+      <c r="F38" s="213"/>
       <c r="G38" s="19"/>
       <c r="H38" s="15"/>
       <c r="I38" s="57"/>
@@ -3508,7 +3481,7 @@
       <c r="C39" s="16"/>
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
-      <c r="F39" s="218"/>
+      <c r="F39" s="216"/>
       <c r="G39" s="106"/>
       <c r="H39" s="15"/>
     </row>
@@ -5211,7 +5184,7 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="211"/>
+      <c r="F1" s="209"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
@@ -5229,7 +5202,7 @@
       <c r="E2" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="211"/>
+      <c r="F2" s="209"/>
       <c r="G2" s="4" t="s">
         <v>141</v>
       </c>
@@ -5253,7 +5226,7 @@
       <c r="E3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="212" t="s">
+      <c r="F3" s="210" t="s">
         <v>56</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -5269,7 +5242,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="11"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="211"/>
+      <c r="F4" s="209"/>
       <c r="G4" s="2"/>
       <c r="H4" s="3"/>
     </row>
@@ -5279,7 +5252,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="11"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="211"/>
+      <c r="F5" s="209"/>
       <c r="G5" s="2"/>
       <c r="H5" s="3"/>
     </row>
@@ -5289,7 +5262,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="11"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="211"/>
+      <c r="F6" s="209"/>
       <c r="G6" s="2"/>
       <c r="H6" s="3"/>
     </row>
@@ -5299,7 +5272,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="11"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="211"/>
+      <c r="F7" s="209"/>
       <c r="G7" s="2"/>
       <c r="H7" s="3"/>
     </row>
@@ -5309,7 +5282,7 @@
       <c r="C8" s="2"/>
       <c r="D8" s="45"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="211"/>
+      <c r="F8" s="209"/>
       <c r="G8" s="2"/>
       <c r="H8" s="3"/>
     </row>
@@ -5319,7 +5292,7 @@
       <c r="C9" s="62"/>
       <c r="D9" s="11"/>
       <c r="E9" s="62"/>
-      <c r="F9" s="219"/>
+      <c r="F9" s="217"/>
       <c r="G9" s="62"/>
       <c r="H9" s="63"/>
     </row>
@@ -5329,7 +5302,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="20"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="220"/>
+      <c r="F10" s="218"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
@@ -5515,7 +5488,7 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="211"/>
+      <c r="F1" s="209"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
@@ -5533,7 +5506,7 @@
       <c r="E2" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="211"/>
+      <c r="F2" s="209"/>
       <c r="G2" s="59" t="s">
         <v>144</v>
       </c>
@@ -5557,7 +5530,7 @@
       <c r="E3" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="212" t="s">
+      <c r="F3" s="210" t="s">
         <v>56</v>
       </c>
       <c r="G3" s="12" t="s">
@@ -5573,7 +5546,7 @@
       <c r="C4" s="9"/>
       <c r="D4" s="11"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="212"/>
+      <c r="F4" s="210"/>
       <c r="G4" s="9"/>
       <c r="H4" s="11"/>
     </row>
@@ -5583,7 +5556,7 @@
       <c r="C5" s="12"/>
       <c r="D5" s="11"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="212"/>
+      <c r="F5" s="210"/>
       <c r="G5" s="12"/>
       <c r="H5" s="45"/>
     </row>
@@ -5593,7 +5566,7 @@
       <c r="C6" s="12"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
-      <c r="F6" s="212"/>
+      <c r="F6" s="210"/>
       <c r="G6" s="12"/>
       <c r="H6" s="45"/>
     </row>
@@ -5603,7 +5576,7 @@
       <c r="C7" s="12"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
-      <c r="F7" s="212"/>
+      <c r="F7" s="210"/>
       <c r="G7" s="12"/>
       <c r="H7" s="45"/>
     </row>
@@ -5613,7 +5586,7 @@
       <c r="C8" s="12"/>
       <c r="D8" s="45"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="213"/>
+      <c r="F8" s="211"/>
       <c r="G8" s="11"/>
       <c r="H8" s="45"/>
     </row>
@@ -5623,7 +5596,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="214"/>
+      <c r="F9" s="212"/>
       <c r="G9" s="106"/>
       <c r="H9" s="87"/>
     </row>
@@ -5633,7 +5606,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="20"/>
       <c r="E10" s="17"/>
-      <c r="F10" s="215"/>
+      <c r="F10" s="213"/>
       <c r="G10" s="106"/>
       <c r="H10" s="45"/>
     </row>
@@ -5643,7 +5616,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="212"/>
+      <c r="F11" s="210"/>
       <c r="G11" s="12"/>
       <c r="H11" s="45"/>
     </row>
@@ -5653,7 +5626,7 @@
       <c r="C12" s="9"/>
       <c r="D12" s="15"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="212"/>
+      <c r="F12" s="210"/>
       <c r="G12" s="9"/>
       <c r="H12" s="74"/>
     </row>
@@ -5663,7 +5636,7 @@
       <c r="C13" s="9"/>
       <c r="D13" s="11"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="212"/>
+      <c r="F13" s="210"/>
       <c r="G13" s="9"/>
       <c r="H13" s="74"/>
     </row>
@@ -5673,7 +5646,7 @@
       <c r="C14" s="9"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="213"/>
+      <c r="F14" s="211"/>
       <c r="G14" s="9"/>
       <c r="H14" s="74"/>
     </row>
@@ -5683,7 +5656,7 @@
       <c r="C15" s="9"/>
       <c r="D15" s="11"/>
       <c r="E15" s="16"/>
-      <c r="F15" s="216"/>
+      <c r="F15" s="214"/>
       <c r="G15" s="19"/>
       <c r="H15" s="74"/>
     </row>
@@ -5693,7 +5666,7 @@
       <c r="C16" s="12"/>
       <c r="D16" s="11"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="212"/>
+      <c r="F16" s="210"/>
       <c r="G16" s="9"/>
       <c r="H16" s="45"/>
     </row>
@@ -5703,7 +5676,7 @@
       <c r="C17" s="9"/>
       <c r="D17" s="15"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="214"/>
+      <c r="F17" s="212"/>
       <c r="G17" s="106"/>
       <c r="H17" s="87"/>
     </row>
@@ -5713,7 +5686,7 @@
       <c r="C18" s="9"/>
       <c r="D18" s="15"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="212"/>
+      <c r="F18" s="210"/>
       <c r="G18" s="12"/>
       <c r="H18" s="87"/>
     </row>
@@ -5723,7 +5696,7 @@
       <c r="C19" s="9"/>
       <c r="D19" s="15"/>
       <c r="E19" s="17"/>
-      <c r="F19" s="215"/>
+      <c r="F19" s="213"/>
       <c r="G19" s="106"/>
       <c r="H19" s="87"/>
     </row>
@@ -5733,7 +5706,7 @@
       <c r="C20" s="9"/>
       <c r="D20" s="15"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="212"/>
+      <c r="F20" s="210"/>
       <c r="G20" s="9"/>
       <c r="H20" s="87"/>
     </row>
@@ -5743,7 +5716,7 @@
       <c r="C21" s="12"/>
       <c r="D21" s="15"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="214"/>
+      <c r="F21" s="212"/>
       <c r="G21" s="106"/>
       <c r="H21" s="87"/>
     </row>
@@ -5753,7 +5726,7 @@
       <c r="C22" s="12"/>
       <c r="D22" s="15"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="215"/>
+      <c r="F22" s="213"/>
       <c r="G22" s="19"/>
       <c r="H22" s="87"/>
     </row>
@@ -5763,7 +5736,7 @@
       <c r="C23" s="12"/>
       <c r="D23" s="15"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="212"/>
+      <c r="F23" s="210"/>
       <c r="G23" s="12"/>
       <c r="H23" s="45"/>
     </row>
@@ -5773,7 +5746,7 @@
       <c r="C24" s="12"/>
       <c r="D24" s="15"/>
       <c r="E24" s="33"/>
-      <c r="F24" s="217"/>
+      <c r="F24" s="215"/>
       <c r="G24" s="106"/>
       <c r="H24" s="87"/>
     </row>
@@ -5783,7 +5756,7 @@
       <c r="C25" s="9"/>
       <c r="D25" s="15"/>
       <c r="E25" s="17"/>
-      <c r="F25" s="215"/>
+      <c r="F25" s="213"/>
       <c r="G25" s="106"/>
       <c r="H25" s="18"/>
     </row>
@@ -5793,7 +5766,7 @@
       <c r="C26" s="145"/>
       <c r="D26" s="11"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="215"/>
+      <c r="F26" s="213"/>
       <c r="G26" s="106"/>
       <c r="H26" s="18"/>
     </row>
@@ -5803,7 +5776,7 @@
       <c r="C27" s="9"/>
       <c r="D27" s="15"/>
       <c r="E27" s="17"/>
-      <c r="F27" s="215"/>
+      <c r="F27" s="213"/>
       <c r="G27" s="106"/>
       <c r="H27" s="87"/>
     </row>
@@ -5813,7 +5786,7 @@
       <c r="C28" s="9"/>
       <c r="D28" s="15"/>
       <c r="E28" s="17"/>
-      <c r="F28" s="215"/>
+      <c r="F28" s="213"/>
       <c r="G28" s="106"/>
       <c r="H28" s="87"/>
     </row>
@@ -5823,7 +5796,7 @@
       <c r="C29" s="9"/>
       <c r="D29" s="15"/>
       <c r="E29" s="17"/>
-      <c r="F29" s="215"/>
+      <c r="F29" s="213"/>
       <c r="G29" s="106"/>
       <c r="H29" s="87"/>
     </row>
@@ -5833,7 +5806,7 @@
       <c r="C30" s="16"/>
       <c r="D30" s="15"/>
       <c r="E30" s="17"/>
-      <c r="F30" s="215"/>
+      <c r="F30" s="213"/>
       <c r="G30" s="106"/>
       <c r="H30" s="87"/>
     </row>
@@ -5843,7 +5816,7 @@
       <c r="C31" s="16"/>
       <c r="D31" s="18"/>
       <c r="E31" s="17"/>
-      <c r="F31" s="215"/>
+      <c r="F31" s="213"/>
       <c r="G31" s="106"/>
       <c r="H31" s="18"/>
     </row>
@@ -5853,7 +5826,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="11"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="212"/>
+      <c r="F32" s="210"/>
       <c r="G32" s="9"/>
       <c r="H32" s="11"/>
       <c r="I32" s="57"/>
@@ -5864,7 +5837,7 @@
       <c r="C33" s="9"/>
       <c r="D33" s="11"/>
       <c r="E33" s="9"/>
-      <c r="F33" s="212"/>
+      <c r="F33" s="210"/>
       <c r="G33" s="9"/>
       <c r="H33" s="11"/>
       <c r="I33" s="57"/>
@@ -5875,7 +5848,7 @@
       <c r="C34" s="9"/>
       <c r="D34" s="11"/>
       <c r="E34" s="9"/>
-      <c r="F34" s="212"/>
+      <c r="F34" s="210"/>
       <c r="G34" s="9"/>
       <c r="H34" s="11"/>
       <c r="I34" s="57"/>
@@ -5886,7 +5859,7 @@
       <c r="C35" s="9"/>
       <c r="D35" s="11"/>
       <c r="E35" s="9"/>
-      <c r="F35" s="212"/>
+      <c r="F35" s="210"/>
       <c r="G35" s="9"/>
       <c r="H35" s="11"/>
       <c r="I35" s="57"/>
@@ -5897,7 +5870,7 @@
       <c r="C36" s="9"/>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
-      <c r="F36" s="213"/>
+      <c r="F36" s="211"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="57"/>
@@ -5908,7 +5881,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="11"/>
       <c r="E37" s="9"/>
-      <c r="F37" s="214"/>
+      <c r="F37" s="212"/>
       <c r="G37" s="19"/>
       <c r="H37" s="74"/>
       <c r="I37" s="57"/>
@@ -5919,7 +5892,7 @@
       <c r="C38" s="16"/>
       <c r="D38" s="11"/>
       <c r="E38" s="14"/>
-      <c r="F38" s="215"/>
+      <c r="F38" s="213"/>
       <c r="G38" s="19"/>
       <c r="H38" s="15"/>
       <c r="I38" s="57"/>
@@ -5930,7 +5903,7 @@
       <c r="C39" s="16"/>
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
-      <c r="F39" s="218"/>
+      <c r="F39" s="216"/>
       <c r="G39" s="106"/>
       <c r="H39" s="15"/>
     </row>
@@ -6189,7 +6162,7 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="211"/>
+      <c r="F1" s="209"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
@@ -6207,7 +6180,7 @@
       <c r="E2" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="211"/>
+      <c r="F2" s="209"/>
       <c r="G2" s="4" t="s">
         <v>141</v>
       </c>
@@ -6234,7 +6207,7 @@
       <c r="E3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="211" t="s">
+      <c r="F3" s="209" t="s">
         <v>56</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -29128,14 +29101,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV225"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="221" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="219" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="219" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="30.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="46.1640625" style="1" customWidth="1"/>
@@ -29146,10 +29120,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -29168,10 +29142,10 @@
       <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:12" ht="224" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -29206,10 +29180,10 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -29245,7 +29219,7 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -29259,7 +29233,7 @@
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
       <c r="A5" s="5"/>
-      <c r="B5" s="3"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -29273,7 +29247,7 @@
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1">
       <c r="A6" s="5"/>
-      <c r="B6" s="3"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -29287,7 +29261,7 @@
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1">
       <c r="A7" s="5"/>
-      <c r="B7" s="3"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -29301,7 +29275,7 @@
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1">
       <c r="A8" s="5"/>
-      <c r="B8" s="3"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -29315,7 +29289,7 @@
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1">
       <c r="A9" s="5"/>
-      <c r="B9" s="3"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -29329,7 +29303,7 @@
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1">
       <c r="A10" s="5"/>
-      <c r="B10" s="3"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -29343,7 +29317,7 @@
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="3"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -29357,7 +29331,7 @@
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1">
       <c r="A12" s="5"/>
-      <c r="B12" s="3"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -29371,7 +29345,7 @@
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1">
       <c r="A13" s="5"/>
-      <c r="B13" s="3"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -29385,7 +29359,7 @@
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1">
       <c r="A14" s="5"/>
-      <c r="B14" s="3"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="2"/>
       <c r="D14" s="8"/>
       <c r="E14" s="2"/>
@@ -29399,7 +29373,7 @@
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
       <c r="A15" s="5"/>
-      <c r="B15" s="3"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -29413,7 +29387,7 @@
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
       <c r="A16" s="5"/>
-      <c r="B16" s="3"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -29427,7 +29401,7 @@
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1">
       <c r="A17" s="5"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -29441,7 +29415,7 @@
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1">
       <c r="A18" s="5"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -29455,7 +29429,7 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1">
       <c r="A19" s="5"/>
-      <c r="B19" s="3"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -29469,7 +29443,7 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1">
       <c r="A20" s="5"/>
-      <c r="B20" s="3"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -29483,7 +29457,7 @@
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1">
       <c r="A21" s="5"/>
-      <c r="B21" s="3"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -29497,7 +29471,7 @@
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1">
       <c r="A22" s="5"/>
-      <c r="B22" s="3"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -29511,7 +29485,7 @@
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1">
       <c r="A23" s="5"/>
-      <c r="B23" s="3"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -29525,7 +29499,7 @@
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1">
       <c r="A24" s="5"/>
-      <c r="B24" s="3"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -29539,7 +29513,7 @@
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1">
       <c r="A25" s="5"/>
-      <c r="B25" s="3"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -29553,7 +29527,7 @@
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1">
       <c r="A26" s="5"/>
-      <c r="B26" s="3"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -29567,7 +29541,7 @@
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1">
       <c r="A27" s="5"/>
-      <c r="B27" s="3"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -29581,7 +29555,7 @@
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1">
       <c r="A28" s="5"/>
-      <c r="B28" s="3"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -29595,7 +29569,7 @@
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1">
       <c r="A29" s="5"/>
-      <c r="B29" s="3"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -29609,7 +29583,7 @@
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1">
       <c r="A30" s="5"/>
-      <c r="B30" s="3"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -29623,7 +29597,7 @@
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1">
       <c r="A31" s="5"/>
-      <c r="B31" s="3"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -29637,7 +29611,7 @@
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1">
       <c r="A32" s="5"/>
-      <c r="B32" s="3"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -29651,7 +29625,7 @@
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1">
       <c r="A33" s="5"/>
-      <c r="B33" s="3"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -29665,7 +29639,7 @@
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1">
       <c r="A34" s="5"/>
-      <c r="B34" s="3"/>
+      <c r="B34" s="5"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -29679,7 +29653,7 @@
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1">
       <c r="A35" s="5"/>
-      <c r="B35" s="3"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -29693,7 +29667,7 @@
     </row>
     <row r="36" spans="1:12" ht="15" customHeight="1">
       <c r="A36" s="5"/>
-      <c r="B36" s="3"/>
+      <c r="B36" s="5"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -29707,7 +29681,7 @@
     </row>
     <row r="37" spans="1:12" ht="15" customHeight="1">
       <c r="A37" s="5"/>
-      <c r="B37" s="3"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -29721,7 +29695,7 @@
     </row>
     <row r="38" spans="1:12" ht="15" customHeight="1">
       <c r="A38" s="5"/>
-      <c r="B38" s="3"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -29735,7 +29709,7 @@
     </row>
     <row r="39" spans="1:12" ht="15" customHeight="1">
       <c r="A39" s="5"/>
-      <c r="B39" s="3"/>
+      <c r="B39" s="5"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -29749,7 +29723,7 @@
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1">
       <c r="A40" s="5"/>
-      <c r="B40" s="3"/>
+      <c r="B40" s="5"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -29763,7 +29737,7 @@
     </row>
     <row r="41" spans="1:12" ht="15" customHeight="1">
       <c r="A41" s="5"/>
-      <c r="B41" s="3"/>
+      <c r="B41" s="5"/>
       <c r="C41" s="2"/>
       <c r="D41" s="8"/>
       <c r="E41" s="2"/>
@@ -29777,7 +29751,7 @@
     </row>
     <row r="42" spans="1:12" ht="15" customHeight="1">
       <c r="A42" s="5"/>
-      <c r="B42" s="3"/>
+      <c r="B42" s="5"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -29791,7 +29765,7 @@
     </row>
     <row r="43" spans="1:12" s="15" customFormat="1" ht="15" customHeight="1">
       <c r="A43" s="13"/>
-      <c r="B43" s="11"/>
+      <c r="B43" s="13"/>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
@@ -29800,7 +29774,7 @@
     </row>
     <row r="44" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1">
       <c r="A44" s="13"/>
-      <c r="B44" s="11"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
       <c r="E44" s="17"/>
@@ -29809,7 +29783,7 @@
     </row>
     <row r="45" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1">
       <c r="A45" s="13"/>
-      <c r="B45" s="11"/>
+      <c r="B45" s="13"/>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
       <c r="E45" s="17"/>
@@ -29818,7 +29792,7 @@
     </row>
     <row r="46" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1">
       <c r="A46" s="13"/>
-      <c r="B46" s="11"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="14"/>
       <c r="D46" s="14"/>
       <c r="E46" s="17"/>
@@ -29827,7 +29801,7 @@
     </row>
     <row r="47" spans="1:12" s="15" customFormat="1" ht="15" customHeight="1">
       <c r="A47" s="13"/>
-      <c r="B47" s="11"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="14"/>
       <c r="D47" s="14"/>
       <c r="E47" s="19"/>
@@ -29836,7 +29810,7 @@
     </row>
     <row r="48" spans="1:12" s="15" customFormat="1" ht="15" customHeight="1">
       <c r="A48" s="13"/>
-      <c r="B48" s="11"/>
+      <c r="B48" s="13"/>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
       <c r="E48" s="19"/>
@@ -29845,7 +29819,7 @@
     </row>
     <row r="49" spans="1:12" s="15" customFormat="1" ht="15" customHeight="1">
       <c r="A49" s="13"/>
-      <c r="B49" s="11"/>
+      <c r="B49" s="13"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
@@ -29854,7 +29828,7 @@
     </row>
     <row r="50" spans="1:12" s="15" customFormat="1" ht="15" customHeight="1">
       <c r="A50" s="13"/>
-      <c r="B50" s="11"/>
+      <c r="B50" s="13"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="19"/>
@@ -29863,7 +29837,7 @@
     </row>
     <row r="51" spans="1:12" s="15" customFormat="1" ht="15" customHeight="1">
       <c r="A51" s="13"/>
-      <c r="B51" s="11"/>
+      <c r="B51" s="13"/>
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
@@ -29872,7 +29846,7 @@
     </row>
     <row r="52" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1">
       <c r="A52" s="13"/>
-      <c r="B52" s="11"/>
+      <c r="B52" s="13"/>
       <c r="C52" s="14"/>
       <c r="D52" s="16"/>
       <c r="E52" s="17"/>
@@ -29899,7 +29873,7 @@
     </row>
     <row r="55" spans="1:12" ht="15" customHeight="1">
       <c r="A55" s="23"/>
-      <c r="B55" s="24"/>
+      <c r="B55" s="23"/>
       <c r="C55" s="25"/>
       <c r="D55" s="24"/>
       <c r="E55" s="24"/>
@@ -29918,7 +29892,7 @@
     </row>
     <row r="57" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A57" s="13"/>
-      <c r="B57" s="11"/>
+      <c r="B57" s="13"/>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
       <c r="E57" s="19"/>
@@ -29958,7 +29932,7 @@
     </row>
     <row r="60" spans="1:12" ht="15" customHeight="1">
       <c r="A60" s="13"/>
-      <c r="B60" s="11"/>
+      <c r="B60" s="13"/>
       <c r="C60" s="9"/>
       <c r="D60" s="19"/>
       <c r="E60" s="19"/>
@@ -29970,7 +29944,7 @@
     </row>
     <row r="61" spans="1:12" ht="15" customHeight="1">
       <c r="A61" s="13"/>
-      <c r="B61" s="11"/>
+      <c r="B61" s="13"/>
       <c r="C61" s="9"/>
       <c r="D61" s="19"/>
       <c r="E61" s="19"/>
@@ -29982,7 +29956,7 @@
     </row>
     <row r="62" spans="1:12" ht="15" customHeight="1">
       <c r="A62" s="13"/>
-      <c r="B62" s="11"/>
+      <c r="B62" s="13"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
@@ -29994,7 +29968,7 @@
     </row>
     <row r="63" spans="1:12" ht="15" customHeight="1">
       <c r="A63" s="13"/>
-      <c r="B63" s="11"/>
+      <c r="B63" s="13"/>
       <c r="C63" s="9"/>
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
@@ -30006,7 +29980,7 @@
     </row>
     <row r="64" spans="1:12" ht="15" customHeight="1">
       <c r="A64" s="13"/>
-      <c r="B64" s="11"/>
+      <c r="B64" s="13"/>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
@@ -30054,7 +30028,7 @@
     </row>
     <row r="68" spans="1:10" ht="15" customHeight="1">
       <c r="A68" s="13"/>
-      <c r="B68" s="11"/>
+      <c r="B68" s="13"/>
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
@@ -30078,6 +30052,7 @@
     </row>
     <row r="70" spans="1:10" s="15" customFormat="1" ht="15" customHeight="1">
       <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
       <c r="C70" s="14"/>
       <c r="D70" s="16"/>
       <c r="E70" s="16"/>
@@ -30110,7 +30085,7 @@
     </row>
     <row r="73" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A73" s="21"/>
-      <c r="B73" s="15"/>
+      <c r="B73" s="21"/>
       <c r="C73" s="21"/>
       <c r="D73" s="15"/>
       <c r="E73" s="15"/>
@@ -30122,7 +30097,7 @@
     </row>
     <row r="74" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A74" s="21"/>
-      <c r="B74" s="15"/>
+      <c r="B74" s="21"/>
       <c r="C74" s="21"/>
       <c r="D74" s="15"/>
       <c r="E74" s="15"/>
@@ -30134,7 +30109,7 @@
     </row>
     <row r="75" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A75" s="21"/>
-      <c r="B75" s="15"/>
+      <c r="B75" s="21"/>
       <c r="C75" s="21"/>
       <c r="D75" s="15"/>
       <c r="E75" s="15"/>
@@ -30146,7 +30121,7 @@
     </row>
     <row r="76" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A76" s="13"/>
-      <c r="B76" s="11"/>
+      <c r="B76" s="13"/>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
       <c r="E76" s="14"/>
@@ -30158,7 +30133,7 @@
     </row>
     <row r="77" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A77" s="13"/>
-      <c r="B77" s="11"/>
+      <c r="B77" s="13"/>
       <c r="C77" s="9"/>
       <c r="D77" s="14"/>
       <c r="E77" s="14"/>
@@ -30170,7 +30145,7 @@
     </row>
     <row r="78" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A78" s="13"/>
-      <c r="B78" s="11"/>
+      <c r="B78" s="13"/>
       <c r="C78" s="9"/>
       <c r="D78" s="16"/>
       <c r="E78" s="14"/>
@@ -30182,7 +30157,7 @@
     </row>
     <row r="79" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A79" s="13"/>
-      <c r="B79" s="15"/>
+      <c r="B79" s="21"/>
       <c r="C79" s="9"/>
       <c r="D79" s="16"/>
       <c r="E79" s="14"/>
@@ -30194,7 +30169,7 @@
     </row>
     <row r="80" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A80" s="13"/>
-      <c r="B80" s="15"/>
+      <c r="B80" s="21"/>
       <c r="C80" s="9"/>
       <c r="D80" s="16"/>
       <c r="E80" s="14"/>
@@ -30206,7 +30181,7 @@
     </row>
     <row r="81" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A81" s="13"/>
-      <c r="B81" s="15"/>
+      <c r="B81" s="21"/>
       <c r="C81" s="9"/>
       <c r="D81" s="16"/>
       <c r="E81" s="14"/>
@@ -30218,7 +30193,7 @@
     </row>
     <row r="82" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A82" s="13"/>
-      <c r="B82" s="15"/>
+      <c r="B82" s="21"/>
       <c r="C82" s="9"/>
       <c r="D82" s="15"/>
       <c r="E82" s="14"/>
@@ -30230,7 +30205,7 @@
     </row>
     <row r="83" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A83" s="13"/>
-      <c r="B83" s="15"/>
+      <c r="B83" s="21"/>
       <c r="C83" s="19"/>
       <c r="D83" s="16"/>
       <c r="E83" s="14"/>
@@ -30242,7 +30217,7 @@
     </row>
     <row r="84" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A84" s="13"/>
-      <c r="B84" s="15"/>
+      <c r="B84" s="21"/>
       <c r="C84" s="19"/>
       <c r="D84" s="16"/>
       <c r="E84" s="14"/>
@@ -30254,7 +30229,7 @@
     </row>
     <row r="85" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A85" s="13"/>
-      <c r="B85" s="15"/>
+      <c r="B85" s="21"/>
       <c r="C85" s="19"/>
       <c r="D85" s="16"/>
       <c r="E85" s="14"/>
@@ -30266,7 +30241,7 @@
     </row>
     <row r="86" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A86" s="13"/>
-      <c r="B86" s="15"/>
+      <c r="B86" s="21"/>
       <c r="C86" s="19"/>
       <c r="D86" s="16"/>
       <c r="E86" s="14"/>
@@ -30278,7 +30253,7 @@
     </row>
     <row r="87" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A87" s="13"/>
-      <c r="B87" s="15"/>
+      <c r="B87" s="21"/>
       <c r="C87" s="19"/>
       <c r="D87" s="16"/>
       <c r="E87" s="14"/>
@@ -30290,7 +30265,7 @@
     </row>
     <row r="88" spans="1:10" ht="15" customHeight="1">
       <c r="A88" s="13"/>
-      <c r="B88" s="11"/>
+      <c r="B88" s="13"/>
       <c r="C88" s="9"/>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
@@ -30302,7 +30277,7 @@
     </row>
     <row r="89" spans="1:10" ht="15" customHeight="1">
       <c r="A89" s="13"/>
-      <c r="B89" s="11"/>
+      <c r="B89" s="13"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
@@ -30314,7 +30289,7 @@
     </row>
     <row r="90" spans="1:10" ht="15" customHeight="1">
       <c r="A90" s="13"/>
-      <c r="B90" s="11"/>
+      <c r="B90" s="13"/>
       <c r="C90" s="9"/>
       <c r="D90" s="9"/>
       <c r="E90" s="35"/>
@@ -30326,7 +30301,7 @@
     </row>
     <row r="91" spans="1:10" ht="15" customHeight="1">
       <c r="A91" s="13"/>
-      <c r="B91" s="11"/>
+      <c r="B91" s="13"/>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
@@ -30338,7 +30313,7 @@
     </row>
     <row r="92" spans="1:10" ht="15" customHeight="1">
       <c r="A92" s="13"/>
-      <c r="B92" s="11"/>
+      <c r="B92" s="13"/>
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
@@ -30350,7 +30325,7 @@
     </row>
     <row r="93" spans="1:10" ht="15" customHeight="1">
       <c r="A93" s="13"/>
-      <c r="B93" s="11"/>
+      <c r="B93" s="13"/>
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
@@ -30362,7 +30337,7 @@
     </row>
     <row r="94" spans="1:10" ht="15" customHeight="1">
       <c r="A94" s="13"/>
-      <c r="B94" s="11"/>
+      <c r="B94" s="13"/>
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
@@ -30374,7 +30349,7 @@
     </row>
     <row r="95" spans="1:10" ht="15" customHeight="1">
       <c r="A95" s="13"/>
-      <c r="B95" s="11"/>
+      <c r="B95" s="13"/>
       <c r="C95" s="9"/>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
@@ -30386,7 +30361,7 @@
     </row>
     <row r="96" spans="1:10" ht="15" customHeight="1">
       <c r="A96" s="13"/>
-      <c r="B96" s="11"/>
+      <c r="B96" s="13"/>
       <c r="C96" s="9"/>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
@@ -30398,7 +30373,7 @@
     </row>
     <row r="97" spans="1:12" s="18" customFormat="1" ht="15" customHeight="1">
       <c r="A97" s="13"/>
-      <c r="B97" s="11"/>
+      <c r="B97" s="13"/>
       <c r="C97" s="9"/>
       <c r="D97" s="17"/>
       <c r="E97" s="37"/>
@@ -30407,7 +30382,7 @@
     </row>
     <row r="98" spans="1:12" s="15" customFormat="1" ht="15" customHeight="1">
       <c r="A98" s="13"/>
-      <c r="B98" s="11"/>
+      <c r="B98" s="13"/>
       <c r="C98" s="9"/>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
@@ -30421,7 +30396,7 @@
     </row>
     <row r="99" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A99" s="13"/>
-      <c r="B99" s="11"/>
+      <c r="B99" s="13"/>
       <c r="C99" s="13"/>
       <c r="D99" s="13"/>
       <c r="E99" s="13"/>
@@ -30433,7 +30408,7 @@
     </row>
     <row r="100" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A100" s="13"/>
-      <c r="B100" s="11"/>
+      <c r="B100" s="13"/>
       <c r="C100" s="13"/>
       <c r="D100" s="13"/>
       <c r="E100" s="13"/>
@@ -30445,7 +30420,7 @@
     </row>
     <row r="101" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A101" s="13"/>
-      <c r="B101" s="11"/>
+      <c r="B101" s="13"/>
       <c r="C101" s="13"/>
       <c r="D101" s="13"/>
       <c r="E101" s="13"/>
@@ -30457,7 +30432,7 @@
     </row>
     <row r="102" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A102" s="13"/>
-      <c r="B102" s="11"/>
+      <c r="B102" s="13"/>
       <c r="C102" s="13"/>
       <c r="D102" s="13"/>
       <c r="E102" s="13"/>
@@ -30469,7 +30444,7 @@
     </row>
     <row r="103" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A103" s="13"/>
-      <c r="B103" s="11"/>
+      <c r="B103" s="13"/>
       <c r="C103" s="13"/>
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
@@ -30481,7 +30456,7 @@
     </row>
     <row r="104" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A104" s="13"/>
-      <c r="B104" s="11"/>
+      <c r="B104" s="13"/>
       <c r="C104" s="13"/>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
@@ -30493,7 +30468,7 @@
     </row>
     <row r="105" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A105" s="13"/>
-      <c r="B105" s="11"/>
+      <c r="B105" s="13"/>
       <c r="C105" s="13"/>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
@@ -30505,7 +30480,7 @@
     </row>
     <row r="106" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A106" s="13"/>
-      <c r="B106" s="11"/>
+      <c r="B106" s="13"/>
       <c r="C106" s="13"/>
       <c r="D106" s="13"/>
       <c r="E106" s="13"/>
@@ -30517,7 +30492,7 @@
     </row>
     <row r="107" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A107" s="13"/>
-      <c r="B107" s="11"/>
+      <c r="B107" s="13"/>
       <c r="C107" s="13"/>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
@@ -30529,7 +30504,7 @@
     </row>
     <row r="108" spans="1:12" s="18" customFormat="1" ht="65" customHeight="1">
       <c r="A108" s="21"/>
-      <c r="B108" s="15"/>
+      <c r="B108" s="21"/>
       <c r="C108" s="10"/>
       <c r="D108" s="38"/>
       <c r="E108" s="39"/>
@@ -30541,7 +30516,7 @@
     </row>
     <row r="109" spans="1:12" s="18" customFormat="1" ht="84" customHeight="1">
       <c r="A109" s="21"/>
-      <c r="B109" s="15"/>
+      <c r="B109" s="21"/>
       <c r="C109" s="10"/>
       <c r="D109" s="38"/>
       <c r="E109" s="39"/>
@@ -30553,7 +30528,7 @@
     </row>
     <row r="110" spans="1:12" s="18" customFormat="1" ht="46" customHeight="1">
       <c r="A110" s="21"/>
-      <c r="B110" s="15"/>
+      <c r="B110" s="21"/>
       <c r="C110" s="10"/>
       <c r="D110" s="38"/>
       <c r="E110" s="41"/>
@@ -30565,7 +30540,7 @@
     </row>
     <row r="111" spans="1:12" s="18" customFormat="1" ht="45" customHeight="1">
       <c r="A111" s="21"/>
-      <c r="B111" s="15"/>
+      <c r="B111" s="21"/>
       <c r="C111" s="10"/>
       <c r="D111" s="38"/>
       <c r="E111" s="41"/>
@@ -30577,7 +30552,7 @@
     </row>
     <row r="112" spans="1:12" s="18" customFormat="1" ht="62" customHeight="1">
       <c r="A112" s="21"/>
-      <c r="B112" s="15"/>
+      <c r="B112" s="21"/>
       <c r="C112" s="10"/>
       <c r="D112" s="38"/>
       <c r="E112" s="41"/>
@@ -30589,7 +30564,7 @@
     </row>
     <row r="113" spans="1:10" s="18" customFormat="1" ht="49" customHeight="1">
       <c r="A113" s="21"/>
-      <c r="B113" s="15"/>
+      <c r="B113" s="21"/>
       <c r="C113" s="10"/>
       <c r="D113" s="38"/>
       <c r="E113" s="41"/>
@@ -30601,7 +30576,7 @@
     </row>
     <row r="114" spans="1:10" s="18" customFormat="1" ht="47" customHeight="1">
       <c r="A114" s="21"/>
-      <c r="B114" s="15"/>
+      <c r="B114" s="21"/>
       <c r="C114" s="10"/>
       <c r="D114" s="38"/>
       <c r="E114" s="41"/>
@@ -30613,7 +30588,7 @@
     </row>
     <row r="115" spans="1:10" s="18" customFormat="1" ht="50" customHeight="1">
       <c r="A115" s="21"/>
-      <c r="B115" s="15"/>
+      <c r="B115" s="21"/>
       <c r="C115" s="10"/>
       <c r="D115" s="38"/>
       <c r="E115" s="41"/>
@@ -30625,7 +30600,7 @@
     </row>
     <row r="116" spans="1:10" s="18" customFormat="1" ht="44" customHeight="1">
       <c r="A116" s="21"/>
-      <c r="B116" s="15"/>
+      <c r="B116" s="21"/>
       <c r="C116" s="10"/>
       <c r="D116" s="38"/>
       <c r="E116" s="41"/>
@@ -30637,7 +30612,7 @@
     </row>
     <row r="117" spans="1:10" s="18" customFormat="1" ht="55" customHeight="1">
       <c r="A117" s="21"/>
-      <c r="B117" s="15"/>
+      <c r="B117" s="21"/>
       <c r="C117" s="10"/>
       <c r="D117" s="38"/>
       <c r="E117" s="41"/>
@@ -30649,7 +30624,7 @@
     </row>
     <row r="118" spans="1:10" s="18" customFormat="1" ht="49" customHeight="1">
       <c r="A118" s="21"/>
-      <c r="B118" s="15"/>
+      <c r="B118" s="21"/>
       <c r="C118" s="10"/>
       <c r="D118" s="38"/>
       <c r="E118" s="41"/>
@@ -30661,7 +30636,7 @@
     </row>
     <row r="119" spans="1:10" s="18" customFormat="1" ht="119" customHeight="1">
       <c r="A119" s="21"/>
-      <c r="B119" s="15"/>
+      <c r="B119" s="21"/>
       <c r="C119" s="10"/>
       <c r="D119" s="38"/>
       <c r="E119" s="41"/>
@@ -30673,6 +30648,7 @@
     </row>
     <row r="120" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1">
       <c r="A120" s="43"/>
+      <c r="B120" s="34"/>
       <c r="C120" s="44"/>
       <c r="D120" s="27"/>
       <c r="H120" s="9"/>
@@ -30680,7 +30656,7 @@
     </row>
     <row r="121" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A121" s="43"/>
-      <c r="B121" s="26"/>
+      <c r="B121" s="34"/>
       <c r="C121" s="44"/>
       <c r="D121" s="26"/>
       <c r="E121" s="26"/>
@@ -30691,7 +30667,7 @@
     </row>
     <row r="122" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A122" s="43"/>
-      <c r="B122" s="26"/>
+      <c r="B122" s="34"/>
       <c r="C122" s="44"/>
       <c r="D122" s="26"/>
       <c r="E122" s="26"/>
@@ -30702,7 +30678,7 @@
     </row>
     <row r="123" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1">
       <c r="A123" s="43"/>
-      <c r="B123" s="26"/>
+      <c r="B123" s="34"/>
       <c r="C123" s="44"/>
       <c r="D123" s="26"/>
       <c r="E123" s="26"/>
@@ -30713,411 +30689,411 @@
     </row>
     <row r="124" spans="1:10" ht="15" customHeight="1">
       <c r="A124" s="43"/>
-      <c r="B124" s="26"/>
+      <c r="B124" s="34"/>
     </row>
     <row r="125" spans="1:10" ht="15" customHeight="1">
       <c r="A125" s="43"/>
-      <c r="B125" s="26"/>
+      <c r="B125" s="34"/>
     </row>
     <row r="126" spans="1:10" ht="15" customHeight="1">
       <c r="A126" s="43"/>
-      <c r="B126" s="26"/>
+      <c r="B126" s="34"/>
     </row>
     <row r="127" spans="1:10" ht="15" customHeight="1">
       <c r="A127" s="43"/>
-      <c r="B127" s="26"/>
+      <c r="B127" s="34"/>
     </row>
     <row r="128" spans="1:10" ht="15" customHeight="1">
       <c r="A128" s="43"/>
-      <c r="B128" s="26"/>
+      <c r="B128" s="34"/>
     </row>
     <row r="129" spans="1:2" ht="15" customHeight="1">
       <c r="A129" s="43"/>
-      <c r="B129" s="26"/>
+      <c r="B129" s="34"/>
     </row>
     <row r="130" spans="1:2" ht="15" customHeight="1">
       <c r="A130" s="43"/>
-      <c r="B130" s="26"/>
+      <c r="B130" s="34"/>
     </row>
     <row r="131" spans="1:2" ht="15" customHeight="1">
       <c r="A131" s="43"/>
-      <c r="B131" s="26"/>
+      <c r="B131" s="34"/>
     </row>
     <row r="132" spans="1:2" ht="15" customHeight="1">
       <c r="A132" s="43"/>
-      <c r="B132" s="26"/>
+      <c r="B132" s="34"/>
     </row>
     <row r="133" spans="1:2" ht="15" customHeight="1">
       <c r="A133" s="43"/>
-      <c r="B133" s="26"/>
+      <c r="B133" s="34"/>
     </row>
     <row r="134" spans="1:2" ht="15" customHeight="1">
       <c r="A134" s="43"/>
-      <c r="B134" s="26"/>
+      <c r="B134" s="34"/>
     </row>
     <row r="135" spans="1:2" ht="15" customHeight="1">
       <c r="A135" s="43"/>
-      <c r="B135" s="26"/>
+      <c r="B135" s="34"/>
     </row>
     <row r="136" spans="1:2" ht="15" customHeight="1">
       <c r="A136" s="43"/>
-      <c r="B136" s="26"/>
+      <c r="B136" s="34"/>
     </row>
     <row r="137" spans="1:2" ht="15" customHeight="1">
       <c r="A137" s="43"/>
-      <c r="B137" s="26"/>
+      <c r="B137" s="34"/>
     </row>
     <row r="138" spans="1:2" ht="15" customHeight="1">
       <c r="A138" s="43"/>
-      <c r="B138" s="26"/>
+      <c r="B138" s="34"/>
     </row>
     <row r="139" spans="1:2" ht="15" customHeight="1">
       <c r="A139" s="43"/>
-      <c r="B139" s="26"/>
+      <c r="B139" s="34"/>
     </row>
     <row r="140" spans="1:2" ht="15" customHeight="1">
       <c r="A140" s="43"/>
-      <c r="B140" s="26"/>
+      <c r="B140" s="34"/>
     </row>
     <row r="141" spans="1:2" ht="15" customHeight="1">
       <c r="A141" s="43"/>
-      <c r="B141" s="26"/>
+      <c r="B141" s="34"/>
     </row>
     <row r="142" spans="1:2" ht="15" customHeight="1">
       <c r="A142" s="43"/>
-      <c r="B142" s="26"/>
+      <c r="B142" s="34"/>
     </row>
     <row r="143" spans="1:2" ht="15" customHeight="1">
       <c r="A143" s="43"/>
-      <c r="B143" s="26"/>
+      <c r="B143" s="34"/>
     </row>
     <row r="144" spans="1:2" ht="15" customHeight="1">
       <c r="A144" s="43"/>
-      <c r="B144" s="26"/>
+      <c r="B144" s="34"/>
     </row>
     <row r="145" spans="1:2" ht="15" customHeight="1">
       <c r="A145" s="43"/>
-      <c r="B145" s="26"/>
+      <c r="B145" s="34"/>
     </row>
     <row r="146" spans="1:2" ht="15" customHeight="1">
       <c r="A146" s="43"/>
-      <c r="B146" s="26"/>
+      <c r="B146" s="34"/>
     </row>
     <row r="147" spans="1:2" ht="15" customHeight="1">
       <c r="A147" s="43"/>
-      <c r="B147" s="26"/>
+      <c r="B147" s="34"/>
     </row>
     <row r="148" spans="1:2" ht="15" customHeight="1">
       <c r="A148" s="43"/>
-      <c r="B148" s="26"/>
+      <c r="B148" s="34"/>
     </row>
     <row r="149" spans="1:2" ht="15" customHeight="1">
       <c r="A149" s="43"/>
-      <c r="B149" s="26"/>
+      <c r="B149" s="34"/>
     </row>
     <row r="150" spans="1:2" ht="15" customHeight="1">
       <c r="A150" s="43"/>
-      <c r="B150" s="26"/>
+      <c r="B150" s="34"/>
     </row>
     <row r="151" spans="1:2" ht="15" customHeight="1">
       <c r="A151" s="43"/>
-      <c r="B151" s="26"/>
+      <c r="B151" s="34"/>
     </row>
     <row r="152" spans="1:2" ht="15" customHeight="1">
       <c r="A152" s="43"/>
-      <c r="B152" s="26"/>
+      <c r="B152" s="34"/>
     </row>
     <row r="153" spans="1:2" ht="15" customHeight="1">
       <c r="A153" s="43"/>
-      <c r="B153" s="26"/>
+      <c r="B153" s="34"/>
     </row>
     <row r="154" spans="1:2" ht="15" customHeight="1">
       <c r="A154" s="43"/>
-      <c r="B154" s="26"/>
+      <c r="B154" s="34"/>
     </row>
     <row r="155" spans="1:2" ht="15" customHeight="1">
       <c r="A155" s="43"/>
-      <c r="B155" s="26"/>
+      <c r="B155" s="34"/>
     </row>
     <row r="156" spans="1:2" ht="15" customHeight="1">
       <c r="A156" s="43"/>
-      <c r="B156" s="26"/>
+      <c r="B156" s="34"/>
     </row>
     <row r="157" spans="1:2" ht="15" customHeight="1">
       <c r="A157" s="43"/>
-      <c r="B157" s="26"/>
+      <c r="B157" s="34"/>
     </row>
     <row r="158" spans="1:2" ht="15" customHeight="1">
       <c r="A158" s="43"/>
-      <c r="B158" s="26"/>
+      <c r="B158" s="34"/>
     </row>
     <row r="159" spans="1:2" ht="15" customHeight="1">
       <c r="A159" s="43"/>
-      <c r="B159" s="26"/>
+      <c r="B159" s="34"/>
     </row>
     <row r="160" spans="1:2" ht="15" customHeight="1">
       <c r="A160" s="43"/>
-      <c r="B160" s="26"/>
+      <c r="B160" s="34"/>
     </row>
     <row r="161" spans="1:2" ht="15" customHeight="1">
       <c r="A161" s="43"/>
-      <c r="B161" s="26"/>
+      <c r="B161" s="34"/>
     </row>
     <row r="162" spans="1:2" ht="15" customHeight="1">
       <c r="A162" s="43"/>
-      <c r="B162" s="26"/>
+      <c r="B162" s="34"/>
     </row>
     <row r="163" spans="1:2" ht="15" customHeight="1">
       <c r="A163" s="43"/>
-      <c r="B163" s="26"/>
+      <c r="B163" s="34"/>
     </row>
     <row r="164" spans="1:2" ht="15" customHeight="1">
       <c r="A164" s="43"/>
-      <c r="B164" s="26"/>
+      <c r="B164" s="34"/>
     </row>
     <row r="165" spans="1:2" ht="15" customHeight="1">
       <c r="A165" s="43"/>
-      <c r="B165" s="26"/>
+      <c r="B165" s="34"/>
     </row>
     <row r="166" spans="1:2" ht="15" customHeight="1">
       <c r="A166" s="43"/>
-      <c r="B166" s="26"/>
+      <c r="B166" s="34"/>
     </row>
     <row r="167" spans="1:2" ht="15" customHeight="1">
       <c r="A167" s="43"/>
-      <c r="B167" s="26"/>
+      <c r="B167" s="34"/>
     </row>
     <row r="168" spans="1:2" ht="15" customHeight="1">
       <c r="A168" s="43"/>
-      <c r="B168" s="26"/>
+      <c r="B168" s="34"/>
     </row>
     <row r="169" spans="1:2" ht="15" customHeight="1">
       <c r="A169" s="43"/>
-      <c r="B169" s="26"/>
+      <c r="B169" s="34"/>
     </row>
     <row r="170" spans="1:2" ht="15" customHeight="1">
       <c r="A170" s="43"/>
-      <c r="B170" s="26"/>
+      <c r="B170" s="34"/>
     </row>
     <row r="171" spans="1:2" ht="15" customHeight="1">
       <c r="A171" s="43"/>
-      <c r="B171" s="26"/>
+      <c r="B171" s="34"/>
     </row>
     <row r="172" spans="1:2" ht="15" customHeight="1">
       <c r="A172" s="43"/>
-      <c r="B172" s="26"/>
+      <c r="B172" s="34"/>
     </row>
     <row r="173" spans="1:2" ht="15" customHeight="1">
       <c r="A173" s="43"/>
-      <c r="B173" s="26"/>
+      <c r="B173" s="34"/>
     </row>
     <row r="174" spans="1:2" ht="15" customHeight="1">
       <c r="A174" s="43"/>
-      <c r="B174" s="26"/>
+      <c r="B174" s="34"/>
     </row>
     <row r="175" spans="1:2" ht="15" customHeight="1">
       <c r="A175" s="43"/>
-      <c r="B175" s="26"/>
+      <c r="B175" s="34"/>
     </row>
     <row r="176" spans="1:2" ht="15" customHeight="1">
       <c r="A176" s="43"/>
-      <c r="B176" s="26"/>
+      <c r="B176" s="34"/>
     </row>
     <row r="177" spans="1:2" ht="15" customHeight="1">
       <c r="A177" s="43"/>
-      <c r="B177" s="26"/>
+      <c r="B177" s="34"/>
     </row>
     <row r="178" spans="1:2" ht="15" customHeight="1">
       <c r="A178" s="43"/>
-      <c r="B178" s="26"/>
+      <c r="B178" s="34"/>
     </row>
     <row r="179" spans="1:2" ht="15" customHeight="1">
       <c r="A179" s="43"/>
-      <c r="B179" s="26"/>
+      <c r="B179" s="34"/>
     </row>
     <row r="180" spans="1:2" ht="15" customHeight="1">
       <c r="A180" s="43"/>
-      <c r="B180" s="26"/>
+      <c r="B180" s="34"/>
     </row>
     <row r="181" spans="1:2" ht="15" customHeight="1">
       <c r="A181" s="43"/>
-      <c r="B181" s="26"/>
+      <c r="B181" s="34"/>
     </row>
     <row r="182" spans="1:2" ht="15" customHeight="1">
       <c r="A182" s="43"/>
-      <c r="B182" s="26"/>
+      <c r="B182" s="34"/>
     </row>
     <row r="183" spans="1:2" ht="15" customHeight="1">
       <c r="A183" s="43"/>
-      <c r="B183" s="26"/>
+      <c r="B183" s="34"/>
     </row>
     <row r="184" spans="1:2" ht="15" customHeight="1">
       <c r="A184" s="43"/>
-      <c r="B184" s="26"/>
+      <c r="B184" s="34"/>
     </row>
     <row r="185" spans="1:2" ht="15" customHeight="1">
       <c r="A185" s="43"/>
-      <c r="B185" s="26"/>
+      <c r="B185" s="34"/>
     </row>
     <row r="186" spans="1:2" ht="15" customHeight="1">
       <c r="A186" s="43"/>
-      <c r="B186" s="26"/>
+      <c r="B186" s="34"/>
     </row>
     <row r="187" spans="1:2" ht="15" customHeight="1">
       <c r="A187" s="43"/>
-      <c r="B187" s="26"/>
+      <c r="B187" s="34"/>
     </row>
     <row r="188" spans="1:2" ht="15" customHeight="1">
       <c r="A188" s="43"/>
-      <c r="B188" s="26"/>
+      <c r="B188" s="34"/>
     </row>
     <row r="189" spans="1:2" ht="15" customHeight="1">
       <c r="A189" s="43"/>
-      <c r="B189" s="26"/>
+      <c r="B189" s="34"/>
     </row>
     <row r="190" spans="1:2" ht="15" customHeight="1">
       <c r="A190" s="43"/>
-      <c r="B190" s="26"/>
+      <c r="B190" s="34"/>
     </row>
     <row r="191" spans="1:2" ht="15" customHeight="1">
       <c r="A191" s="43"/>
-      <c r="B191" s="26"/>
+      <c r="B191" s="34"/>
     </row>
     <row r="192" spans="1:2" ht="15" customHeight="1">
       <c r="A192" s="43"/>
-      <c r="B192" s="26"/>
+      <c r="B192" s="34"/>
     </row>
     <row r="193" spans="1:2" ht="15" customHeight="1">
       <c r="A193" s="43"/>
-      <c r="B193" s="26"/>
+      <c r="B193" s="34"/>
     </row>
     <row r="194" spans="1:2" ht="15" customHeight="1">
       <c r="A194" s="43"/>
-      <c r="B194" s="26"/>
+      <c r="B194" s="34"/>
     </row>
     <row r="195" spans="1:2" ht="15" customHeight="1">
       <c r="A195" s="43"/>
-      <c r="B195" s="26"/>
+      <c r="B195" s="34"/>
     </row>
     <row r="196" spans="1:2" ht="15" customHeight="1">
       <c r="A196" s="43"/>
-      <c r="B196" s="26"/>
+      <c r="B196" s="34"/>
     </row>
     <row r="197" spans="1:2" ht="15" customHeight="1">
       <c r="A197" s="43"/>
-      <c r="B197" s="26"/>
+      <c r="B197" s="34"/>
     </row>
     <row r="198" spans="1:2" ht="15" customHeight="1">
       <c r="A198" s="43"/>
-      <c r="B198" s="26"/>
+      <c r="B198" s="34"/>
     </row>
     <row r="199" spans="1:2" ht="15" customHeight="1">
       <c r="A199" s="43"/>
-      <c r="B199" s="26"/>
+      <c r="B199" s="34"/>
     </row>
     <row r="200" spans="1:2" ht="15" customHeight="1">
       <c r="A200" s="43"/>
-      <c r="B200" s="26"/>
+      <c r="B200" s="34"/>
     </row>
     <row r="201" spans="1:2" ht="15" customHeight="1">
       <c r="A201" s="43"/>
-      <c r="B201" s="26"/>
+      <c r="B201" s="34"/>
     </row>
     <row r="202" spans="1:2" ht="15" customHeight="1">
       <c r="A202" s="43"/>
-      <c r="B202" s="26"/>
+      <c r="B202" s="34"/>
     </row>
     <row r="203" spans="1:2" ht="15" customHeight="1">
       <c r="A203" s="43"/>
-      <c r="B203" s="26"/>
+      <c r="B203" s="34"/>
     </row>
     <row r="204" spans="1:2" ht="15" customHeight="1">
       <c r="A204" s="43"/>
-      <c r="B204" s="26"/>
+      <c r="B204" s="34"/>
     </row>
     <row r="205" spans="1:2" ht="15" customHeight="1">
       <c r="A205" s="43"/>
-      <c r="B205" s="26"/>
+      <c r="B205" s="34"/>
     </row>
     <row r="206" spans="1:2" ht="15" customHeight="1">
       <c r="A206" s="43"/>
-      <c r="B206" s="26"/>
+      <c r="B206" s="34"/>
     </row>
     <row r="207" spans="1:2" ht="15" customHeight="1">
       <c r="A207" s="43"/>
-      <c r="B207" s="26"/>
+      <c r="B207" s="34"/>
     </row>
     <row r="208" spans="1:2" ht="15" customHeight="1">
       <c r="A208" s="43"/>
-      <c r="B208" s="26"/>
+      <c r="B208" s="34"/>
     </row>
     <row r="209" spans="1:2" ht="15" customHeight="1">
       <c r="A209" s="43"/>
-      <c r="B209" s="26"/>
+      <c r="B209" s="34"/>
     </row>
     <row r="210" spans="1:2" ht="15" customHeight="1">
       <c r="A210" s="43"/>
-      <c r="B210" s="26"/>
+      <c r="B210" s="34"/>
     </row>
     <row r="211" spans="1:2" ht="15" customHeight="1">
       <c r="A211" s="43"/>
-      <c r="B211" s="26"/>
+      <c r="B211" s="34"/>
     </row>
     <row r="212" spans="1:2" ht="15" customHeight="1">
       <c r="A212" s="43"/>
-      <c r="B212" s="26"/>
+      <c r="B212" s="34"/>
     </row>
     <row r="213" spans="1:2" ht="15" customHeight="1">
       <c r="A213" s="43"/>
-      <c r="B213" s="26"/>
+      <c r="B213" s="34"/>
     </row>
     <row r="214" spans="1:2" ht="15" customHeight="1">
       <c r="A214" s="43"/>
-      <c r="B214" s="26"/>
+      <c r="B214" s="34"/>
     </row>
     <row r="215" spans="1:2" ht="15" customHeight="1">
       <c r="A215" s="43"/>
-      <c r="B215" s="26"/>
+      <c r="B215" s="34"/>
     </row>
     <row r="216" spans="1:2" ht="15" customHeight="1">
       <c r="A216" s="43"/>
-      <c r="B216" s="26"/>
+      <c r="B216" s="34"/>
     </row>
     <row r="217" spans="1:2" ht="15" customHeight="1">
       <c r="A217" s="43"/>
-      <c r="B217" s="26"/>
+      <c r="B217" s="34"/>
     </row>
     <row r="218" spans="1:2" ht="15" customHeight="1">
       <c r="A218" s="43"/>
-      <c r="B218" s="26"/>
+      <c r="B218" s="34"/>
     </row>
     <row r="219" spans="1:2" ht="15" customHeight="1">
       <c r="A219" s="43"/>
-      <c r="B219" s="26"/>
+      <c r="B219" s="34"/>
     </row>
     <row r="220" spans="1:2" ht="15" customHeight="1">
       <c r="A220" s="43"/>
-      <c r="B220" s="26"/>
+      <c r="B220" s="34"/>
     </row>
     <row r="221" spans="1:2" ht="15" customHeight="1">
       <c r="A221" s="43"/>
-      <c r="B221" s="26"/>
+      <c r="B221" s="34"/>
     </row>
     <row r="222" spans="1:2" ht="15" customHeight="1">
       <c r="A222" s="43"/>
-      <c r="B222" s="26"/>
+      <c r="B222" s="34"/>
     </row>
     <row r="223" spans="1:2" ht="15" customHeight="1">
       <c r="A223" s="43"/>
-      <c r="B223" s="26"/>
+      <c r="B223" s="34"/>
     </row>
     <row r="224" spans="1:2" ht="15" customHeight="1">
       <c r="A224" s="43"/>
-      <c r="B224" s="26"/>
+      <c r="B224" s="34"/>
     </row>
     <row r="225" spans="1:2" ht="15" customHeight="1">
       <c r="A225" s="43"/>
-      <c r="B225" s="26"/>
+      <c r="B225" s="34"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:L98" xr:uid="{00000000-0009-0000-0000-000002000000}"/>

</xml_diff>

<commit_message>
SSCS-8723 Event enabling condition
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jason.Hart/Downloads/projects/sscs-ccd-definitions/benefit/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jack/Development/hmcts/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D2BA38-A676-7046-A52C-F763C0BF16A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6098BD92-D215-BC40-873A-A883185823F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$T$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$U$110</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$2:$L$98</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">CaseTypeTab!$H$58:$H$70</definedName>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="195">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -727,6 +727,12 @@
   </si>
   <si>
     <t>Shuttered</t>
+  </si>
+  <si>
+    <t>EventEnablingCondition</t>
+  </si>
+  <si>
+    <t>Hide or show condition for an event based on case data</t>
   </si>
 </sst>
 </file>
@@ -2795,7 +2801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -41679,10 +41685,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AMK208"/>
+  <dimension ref="A1:AML208"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41699,11 +41705,11 @@
     <col min="11" max="11" width="8.83203125" style="24" customWidth="1"/>
     <col min="12" max="12" width="59.5" style="15" customWidth="1"/>
     <col min="13" max="13" width="8.83203125" style="24" customWidth="1"/>
-    <col min="14" max="14" width="65.33203125" style="15" customWidth="1"/>
-    <col min="15" max="1025" width="8.83203125" style="57" customWidth="1"/>
+    <col min="14" max="15" width="65.33203125" style="15" customWidth="1"/>
+    <col min="16" max="1026" width="8.83203125" style="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>89</v>
       </c>
@@ -41726,14 +41732,15 @@
       <c r="L1" s="11"/>
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
-      <c r="O1" s="45"/>
+      <c r="O1" s="11"/>
       <c r="P1" s="45"/>
       <c r="Q1" s="45"/>
       <c r="R1" s="45"/>
       <c r="S1" s="45"/>
       <c r="T1" s="45"/>
-    </row>
-    <row r="2" spans="1:21" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U1" s="45"/>
+    </row>
+    <row r="2" spans="1:22" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -41777,25 +41784,28 @@
         <v>96</v>
       </c>
       <c r="O2" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="P2" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="P2" s="46" t="s">
+      <c r="Q2" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="46" t="s">
+      <c r="R2" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="R2" s="46" t="s">
+      <c r="S2" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="S2" s="46" t="s">
+      <c r="T2" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="T2" s="46" t="s">
+      <c r="U2" s="46" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
@@ -41838,27 +41848,30 @@
       <c r="N3" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="P3" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="Q3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="R3" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="S3" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="T3" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="U3" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="U3" s="89"/>
-    </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V3" s="89"/>
+    </row>
+    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="B4" s="45"/>
       <c r="C4" s="12"/>
@@ -41873,14 +41886,15 @@
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="45"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="12"/>
       <c r="R4" s="45"/>
       <c r="S4" s="45"/>
       <c r="T4" s="45"/>
-    </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U4" s="45"/>
+    </row>
+    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
       <c r="B5" s="45"/>
       <c r="C5" s="12"/>
@@ -41895,14 +41909,15 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="45"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="12"/>
       <c r="R5" s="45"/>
       <c r="S5" s="45"/>
       <c r="T5" s="45"/>
-    </row>
-    <row r="6" spans="1:21" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U5" s="45"/>
+    </row>
+    <row r="6" spans="1:22" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -41917,14 +41932,15 @@
       <c r="L6" s="90"/>
       <c r="M6" s="13"/>
       <c r="N6" s="90"/>
-      <c r="O6" s="13"/>
+      <c r="O6" s="90"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
       <c r="S6" s="13"/>
       <c r="T6" s="13"/>
-    </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U6" s="13"/>
+    </row>
+    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
       <c r="B7" s="45"/>
       <c r="C7" s="12"/>
@@ -41939,14 +41955,15 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="45"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="12"/>
       <c r="R7" s="45"/>
       <c r="S7" s="45"/>
       <c r="T7" s="45"/>
-    </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U7" s="45"/>
+    </row>
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="B8" s="45"/>
       <c r="C8" s="12"/>
@@ -41961,14 +41978,15 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="45"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="12"/>
       <c r="R8" s="45"/>
       <c r="S8" s="45"/>
       <c r="T8" s="45"/>
-    </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U8" s="45"/>
+    </row>
+    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="22"/>
       <c r="B9" s="45"/>
       <c r="C9" s="12"/>
@@ -41983,14 +42001,15 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
-      <c r="O9" s="45"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="45"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="12"/>
       <c r="R9" s="45"/>
       <c r="S9" s="45"/>
       <c r="T9" s="45"/>
-    </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U9" s="45"/>
+    </row>
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="22"/>
       <c r="B10" s="91"/>
       <c r="C10" s="12"/>
@@ -42006,13 +42025,14 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
-      <c r="P10" s="91"/>
-      <c r="Q10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="91"/>
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
-    </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U10" s="11"/>
+    </row>
+    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="22"/>
       <c r="B11" s="91"/>
       <c r="C11" s="12"/>
@@ -42028,13 +42048,14 @@
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
-      <c r="P11" s="91"/>
-      <c r="Q11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="91"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
       <c r="T11" s="11"/>
-    </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U11" s="11"/>
+    </row>
+    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="93"/>
       <c r="B12" s="36"/>
       <c r="C12" s="94"/>
@@ -42050,13 +42071,14 @@
       <c r="M12" s="36"/>
       <c r="N12" s="36"/>
       <c r="O12" s="36"/>
-      <c r="P12" s="95"/>
-      <c r="Q12" s="96"/>
-      <c r="R12" s="97"/>
-      <c r="S12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="95"/>
+      <c r="R12" s="96"/>
+      <c r="S12" s="97"/>
       <c r="T12" s="36"/>
-    </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U12" s="36"/>
+    </row>
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22"/>
       <c r="B13" s="45"/>
       <c r="C13" s="12"/>
@@ -42071,14 +42093,15 @@
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
       <c r="N13" s="90"/>
-      <c r="O13" s="12"/>
+      <c r="O13" s="90"/>
       <c r="P13" s="12"/>
-      <c r="Q13" s="45"/>
+      <c r="Q13" s="12"/>
       <c r="R13" s="45"/>
       <c r="S13" s="45"/>
       <c r="T13" s="45"/>
-    </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U13" s="45"/>
+    </row>
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22"/>
       <c r="B14" s="45"/>
       <c r="C14" s="12"/>
@@ -42093,14 +42116,15 @@
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
       <c r="N14" s="90"/>
-      <c r="O14" s="12"/>
+      <c r="O14" s="90"/>
       <c r="P14" s="12"/>
-      <c r="Q14" s="45"/>
+      <c r="Q14" s="12"/>
       <c r="R14" s="45"/>
       <c r="S14" s="45"/>
       <c r="T14" s="45"/>
-    </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U14" s="45"/>
+    </row>
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22"/>
       <c r="B15" s="45"/>
       <c r="C15" s="12"/>
@@ -42115,14 +42139,15 @@
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
       <c r="N15" s="90"/>
-      <c r="O15" s="12"/>
+      <c r="O15" s="90"/>
       <c r="P15" s="12"/>
-      <c r="Q15" s="45"/>
+      <c r="Q15" s="12"/>
       <c r="R15" s="45"/>
       <c r="S15" s="45"/>
       <c r="T15" s="45"/>
-    </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U15" s="45"/>
+    </row>
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22"/>
       <c r="B16" s="45"/>
       <c r="C16" s="12"/>
@@ -42137,14 +42162,15 @@
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
       <c r="N16" s="90"/>
-      <c r="O16" s="12"/>
+      <c r="O16" s="90"/>
       <c r="P16" s="12"/>
-      <c r="Q16" s="45"/>
+      <c r="Q16" s="12"/>
       <c r="R16" s="45"/>
       <c r="S16" s="45"/>
       <c r="T16" s="45"/>
-    </row>
-    <row r="17" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U16" s="45"/>
+    </row>
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="98"/>
       <c r="B17" s="91"/>
       <c r="C17" s="9"/>
@@ -42160,13 +42186,14 @@
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
-      <c r="P17" s="91"/>
-      <c r="Q17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="91"/>
       <c r="R17" s="11"/>
       <c r="S17" s="11"/>
       <c r="T17" s="11"/>
-    </row>
-    <row r="18" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U17" s="11"/>
+    </row>
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="98"/>
       <c r="B18" s="91"/>
       <c r="C18" s="9"/>
@@ -42181,14 +42208,15 @@
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
       <c r="N18" s="9"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="91"/>
-      <c r="Q18" s="11"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="91"/>
       <c r="R18" s="11"/>
       <c r="S18" s="11"/>
       <c r="T18" s="11"/>
-    </row>
-    <row r="19" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U18" s="11"/>
+    </row>
+    <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="98"/>
       <c r="B19" s="91"/>
       <c r="C19" s="9"/>
@@ -42203,14 +42231,15 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
       <c r="N19" s="9"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="91"/>
-      <c r="Q19" s="11"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="91"/>
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
       <c r="T19" s="11"/>
-    </row>
-    <row r="20" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U19" s="11"/>
+    </row>
+    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="22"/>
       <c r="B20" s="45"/>
       <c r="C20" s="12"/>
@@ -42225,14 +42254,15 @@
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
       <c r="N20" s="90"/>
-      <c r="O20" s="12"/>
+      <c r="O20" s="90"/>
       <c r="P20" s="12"/>
-      <c r="Q20" s="45"/>
+      <c r="Q20" s="12"/>
       <c r="R20" s="45"/>
       <c r="S20" s="45"/>
       <c r="T20" s="45"/>
-    </row>
-    <row r="21" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U20" s="45"/>
+    </row>
+    <row r="21" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="11"/>
       <c r="C21" s="9"/>
@@ -42249,12 +42279,13 @@
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="97"/>
-      <c r="S21" s="11"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="97"/>
       <c r="T21" s="11"/>
-    </row>
-    <row r="22" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U21" s="11"/>
+    </row>
+    <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="22"/>
       <c r="B22" s="45"/>
       <c r="C22" s="12"/>
@@ -42269,14 +42300,15 @@
       <c r="L22" s="11"/>
       <c r="M22" s="11"/>
       <c r="N22" s="90"/>
-      <c r="O22" s="12"/>
+      <c r="O22" s="90"/>
       <c r="P22" s="12"/>
-      <c r="Q22" s="45"/>
+      <c r="Q22" s="12"/>
       <c r="R22" s="45"/>
       <c r="S22" s="45"/>
       <c r="T22" s="45"/>
-    </row>
-    <row r="23" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U22" s="45"/>
+    </row>
+    <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="98"/>
       <c r="B23" s="91"/>
       <c r="C23" s="9"/>
@@ -42292,13 +42324,14 @@
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
       <c r="O23" s="11"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="9"/>
       <c r="R23" s="11"/>
       <c r="S23" s="11"/>
       <c r="T23" s="11"/>
-    </row>
-    <row r="24" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U23" s="11"/>
+    </row>
+    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="22"/>
       <c r="B24" s="45"/>
       <c r="C24" s="12"/>
@@ -42313,14 +42346,15 @@
       <c r="L24" s="11"/>
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
-      <c r="O24" s="45"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="45"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="12"/>
       <c r="R24" s="45"/>
       <c r="S24" s="45"/>
       <c r="T24" s="45"/>
-    </row>
-    <row r="25" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U24" s="45"/>
+    </row>
+    <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -42341,8 +42375,9 @@
       <c r="R25" s="13"/>
       <c r="S25" s="13"/>
       <c r="T25" s="13"/>
-    </row>
-    <row r="26" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U25" s="13"/>
+    </row>
+    <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="22"/>
       <c r="B26" s="45"/>
       <c r="C26" s="11"/>
@@ -42357,14 +42392,15 @@
       <c r="L26" s="11"/>
       <c r="M26" s="11"/>
       <c r="N26" s="11"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="99"/>
-      <c r="Q26" s="45"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="45"/>
+      <c r="Q26" s="99"/>
       <c r="R26" s="45"/>
       <c r="S26" s="45"/>
       <c r="T26" s="45"/>
-    </row>
-    <row r="27" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U26" s="45"/>
+    </row>
+    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="22"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -42379,14 +42415,15 @@
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
-      <c r="O27" s="12"/>
+      <c r="O27" s="9"/>
       <c r="P27" s="12"/>
       <c r="Q27" s="12"/>
       <c r="R27" s="12"/>
       <c r="S27" s="12"/>
       <c r="T27" s="12"/>
-    </row>
-    <row r="28" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U27" s="12"/>
+    </row>
+    <row r="28" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="22"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -42401,14 +42438,15 @@
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
-      <c r="O28" s="12"/>
+      <c r="O28" s="9"/>
       <c r="P28" s="12"/>
       <c r="Q28" s="12"/>
       <c r="R28" s="12"/>
       <c r="S28" s="12"/>
       <c r="T28" s="12"/>
-    </row>
-    <row r="29" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U28" s="12"/>
+    </row>
+    <row r="29" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="22"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -42423,14 +42461,15 @@
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
-      <c r="O29" s="12"/>
+      <c r="O29" s="9"/>
       <c r="P29" s="12"/>
       <c r="Q29" s="12"/>
       <c r="R29" s="12"/>
       <c r="S29" s="12"/>
       <c r="T29" s="12"/>
-    </row>
-    <row r="30" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U29" s="12"/>
+    </row>
+    <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="22"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -42445,14 +42484,15 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
-      <c r="O30" s="12"/>
+      <c r="O30" s="9"/>
       <c r="P30" s="12"/>
       <c r="Q30" s="12"/>
       <c r="R30" s="12"/>
       <c r="S30" s="12"/>
       <c r="T30" s="12"/>
-    </row>
-    <row r="31" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U30" s="12"/>
+    </row>
+    <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="22"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -42467,14 +42507,15 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
-      <c r="O31" s="12"/>
+      <c r="O31" s="9"/>
       <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
       <c r="R31" s="12"/>
       <c r="S31" s="12"/>
       <c r="T31" s="12"/>
-    </row>
-    <row r="32" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U31" s="12"/>
+    </row>
+    <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -42495,8 +42536,9 @@
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
       <c r="T32" s="9"/>
-    </row>
-    <row r="33" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U32" s="9"/>
+    </row>
+    <row r="33" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="22"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -42511,14 +42553,15 @@
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
-      <c r="O33" s="12"/>
+      <c r="O33" s="9"/>
       <c r="P33" s="12"/>
       <c r="Q33" s="12"/>
       <c r="R33" s="12"/>
       <c r="S33" s="12"/>
       <c r="T33" s="12"/>
-    </row>
-    <row r="34" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U33" s="12"/>
+    </row>
+    <row r="34" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="22"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -42533,14 +42576,15 @@
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
-      <c r="O34" s="12"/>
+      <c r="O34" s="9"/>
       <c r="P34" s="12"/>
       <c r="Q34" s="12"/>
       <c r="R34" s="12"/>
       <c r="S34" s="12"/>
       <c r="T34" s="12"/>
-    </row>
-    <row r="35" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U34" s="12"/>
+    </row>
+    <row r="35" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="22"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -42555,14 +42599,15 @@
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="16"/>
-      <c r="O35" s="12"/>
+      <c r="O35" s="16"/>
       <c r="P35" s="12"/>
       <c r="Q35" s="12"/>
       <c r="R35" s="12"/>
       <c r="S35" s="12"/>
       <c r="T35" s="12"/>
-    </row>
-    <row r="36" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U35" s="12"/>
+    </row>
+    <row r="36" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="22"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -42577,14 +42622,15 @@
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
-      <c r="O36" s="12"/>
+      <c r="O36" s="9"/>
       <c r="P36" s="12"/>
       <c r="Q36" s="12"/>
       <c r="R36" s="12"/>
       <c r="S36" s="12"/>
       <c r="T36" s="12"/>
-    </row>
-    <row r="37" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U36" s="12"/>
+    </row>
+    <row r="37" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="93"/>
       <c r="B37" s="36"/>
       <c r="C37" s="94"/>
@@ -42600,13 +42646,14 @@
       <c r="M37" s="36"/>
       <c r="N37" s="36"/>
       <c r="O37" s="36"/>
-      <c r="P37" s="95"/>
-      <c r="Q37" s="96"/>
-      <c r="R37" s="97"/>
-      <c r="S37" s="36"/>
+      <c r="P37" s="36"/>
+      <c r="Q37" s="95"/>
+      <c r="R37" s="96"/>
+      <c r="S37" s="97"/>
       <c r="T37" s="36"/>
-    </row>
-    <row r="38" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U37" s="36"/>
+    </row>
+    <row r="38" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="13"/>
       <c r="B38" s="11"/>
       <c r="C38" s="9"/>
@@ -42621,14 +42668,15 @@
       <c r="L38" s="11"/>
       <c r="M38" s="11"/>
       <c r="N38" s="16"/>
-      <c r="O38" s="9"/>
+      <c r="O38" s="16"/>
       <c r="P38" s="9"/>
-      <c r="Q38" s="11"/>
+      <c r="Q38" s="9"/>
       <c r="R38" s="11"/>
       <c r="S38" s="11"/>
       <c r="T38" s="11"/>
-    </row>
-    <row r="39" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U38" s="11"/>
+    </row>
+    <row r="39" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="22"/>
       <c r="B39" s="45"/>
       <c r="C39" s="12"/>
@@ -42642,14 +42690,14 @@
       <c r="K39" s="11"/>
       <c r="L39" s="11"/>
       <c r="M39" s="11"/>
-      <c r="O39" s="45"/>
-      <c r="P39" s="12"/>
-      <c r="Q39" s="45"/>
+      <c r="P39" s="45"/>
+      <c r="Q39" s="12"/>
       <c r="R39" s="45"/>
       <c r="S39" s="45"/>
       <c r="T39" s="45"/>
-    </row>
-    <row r="40" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U39" s="45"/>
+    </row>
+    <row r="40" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="13"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -42663,14 +42711,14 @@
       <c r="K40" s="11"/>
       <c r="L40" s="11"/>
       <c r="M40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="9"/>
       <c r="R40" s="11"/>
       <c r="S40" s="11"/>
       <c r="T40" s="11"/>
-    </row>
-    <row r="41" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U40" s="11"/>
+    </row>
+    <row r="41" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="98"/>
       <c r="B41" s="11"/>
       <c r="C41" s="9"/>
@@ -42686,13 +42734,14 @@
       <c r="M41" s="11"/>
       <c r="N41" s="11"/>
       <c r="O41" s="11"/>
-      <c r="P41" s="91"/>
-      <c r="Q41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="91"/>
       <c r="R41" s="11"/>
       <c r="S41" s="11"/>
       <c r="T41" s="11"/>
-    </row>
-    <row r="42" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U41" s="11"/>
+    </row>
+    <row r="42" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="22"/>
       <c r="B42" s="45"/>
       <c r="C42" s="12"/>
@@ -42707,14 +42756,15 @@
       <c r="L42" s="11"/>
       <c r="M42" s="11"/>
       <c r="N42" s="11"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="12"/>
-      <c r="Q42" s="45"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="45"/>
+      <c r="Q42" s="12"/>
       <c r="R42" s="45"/>
       <c r="S42" s="45"/>
       <c r="T42" s="45"/>
-    </row>
-    <row r="43" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U42" s="45"/>
+    </row>
+    <row r="43" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="22"/>
       <c r="B43" s="45"/>
       <c r="C43" s="12"/>
@@ -42729,14 +42779,15 @@
       <c r="L43" s="11"/>
       <c r="M43" s="11"/>
       <c r="N43" s="90"/>
-      <c r="O43" s="12"/>
+      <c r="O43" s="90"/>
       <c r="P43" s="12"/>
-      <c r="Q43" s="45"/>
+      <c r="Q43" s="12"/>
       <c r="R43" s="45"/>
       <c r="S43" s="45"/>
       <c r="T43" s="45"/>
-    </row>
-    <row r="44" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U43" s="45"/>
+    </row>
+    <row r="44" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="22"/>
       <c r="B44" s="45"/>
       <c r="C44" s="12"/>
@@ -42751,14 +42802,15 @@
       <c r="L44" s="11"/>
       <c r="M44" s="11"/>
       <c r="N44" s="11"/>
-      <c r="O44" s="45"/>
-      <c r="P44" s="12"/>
-      <c r="Q44" s="45"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="45"/>
+      <c r="Q44" s="12"/>
       <c r="R44" s="45"/>
       <c r="S44" s="45"/>
       <c r="T44" s="45"/>
-    </row>
-    <row r="45" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U44" s="45"/>
+    </row>
+    <row r="45" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="22"/>
       <c r="B45" s="45"/>
       <c r="C45" s="12"/>
@@ -42773,14 +42825,15 @@
       <c r="L45" s="11"/>
       <c r="M45" s="11"/>
       <c r="N45" s="11"/>
-      <c r="O45" s="45"/>
-      <c r="P45" s="12"/>
-      <c r="Q45" s="45"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="45"/>
+      <c r="Q45" s="12"/>
       <c r="R45" s="45"/>
       <c r="S45" s="45"/>
       <c r="T45" s="45"/>
-    </row>
-    <row r="46" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U45" s="45"/>
+    </row>
+    <row r="46" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="22"/>
       <c r="B46" s="45"/>
       <c r="C46" s="11"/>
@@ -42795,14 +42848,15 @@
       <c r="L46" s="11"/>
       <c r="M46" s="11"/>
       <c r="N46" s="11"/>
-      <c r="O46" s="45"/>
-      <c r="P46" s="91"/>
-      <c r="Q46" s="45"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="45"/>
+      <c r="Q46" s="91"/>
       <c r="R46" s="45"/>
       <c r="S46" s="45"/>
       <c r="T46" s="45"/>
-    </row>
-    <row r="47" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U46" s="45"/>
+    </row>
+    <row r="47" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="22"/>
       <c r="B47" s="45"/>
       <c r="C47" s="12"/>
@@ -42817,14 +42871,15 @@
       <c r="L47" s="100"/>
       <c r="M47" s="11"/>
       <c r="N47" s="90"/>
-      <c r="O47" s="12"/>
+      <c r="O47" s="90"/>
       <c r="P47" s="12"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="45"/>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="18"/>
       <c r="S47" s="45"/>
       <c r="T47" s="45"/>
-    </row>
-    <row r="48" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U47" s="45"/>
+    </row>
+    <row r="48" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
@@ -42845,8 +42900,9 @@
       <c r="R48" s="13"/>
       <c r="S48" s="13"/>
       <c r="T48" s="13"/>
-    </row>
-    <row r="49" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U48" s="13"/>
+    </row>
+    <row r="49" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="22"/>
       <c r="B49" s="45"/>
       <c r="C49" s="12"/>
@@ -42861,14 +42917,15 @@
       <c r="L49" s="11"/>
       <c r="M49" s="11"/>
       <c r="N49" s="90"/>
-      <c r="O49" s="12"/>
+      <c r="O49" s="90"/>
       <c r="P49" s="12"/>
-      <c r="Q49" s="45"/>
+      <c r="Q49" s="12"/>
       <c r="R49" s="45"/>
       <c r="S49" s="45"/>
       <c r="T49" s="45"/>
-    </row>
-    <row r="50" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U49" s="45"/>
+    </row>
+    <row r="50" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="22"/>
       <c r="B50" s="45"/>
       <c r="C50" s="12"/>
@@ -42883,14 +42940,15 @@
       <c r="L50" s="11"/>
       <c r="M50" s="11"/>
       <c r="N50" s="90"/>
-      <c r="O50" s="12"/>
+      <c r="O50" s="90"/>
       <c r="P50" s="12"/>
-      <c r="Q50" s="45"/>
+      <c r="Q50" s="12"/>
       <c r="R50" s="45"/>
       <c r="S50" s="45"/>
       <c r="T50" s="45"/>
-    </row>
-    <row r="51" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U50" s="45"/>
+    </row>
+    <row r="51" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="22"/>
       <c r="B51" s="45"/>
       <c r="C51" s="12"/>
@@ -42905,14 +42963,15 @@
       <c r="L51" s="11"/>
       <c r="M51" s="11"/>
       <c r="N51" s="11"/>
-      <c r="O51" s="45"/>
-      <c r="P51" s="12"/>
-      <c r="Q51" s="45"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="45"/>
+      <c r="Q51" s="12"/>
       <c r="R51" s="45"/>
       <c r="S51" s="45"/>
       <c r="T51" s="45"/>
-    </row>
-    <row r="52" spans="1:21" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U51" s="45"/>
+    </row>
+    <row r="52" spans="1:22" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="22"/>
       <c r="B52" s="45"/>
       <c r="C52" s="12"/>
@@ -42927,15 +42986,16 @@
       <c r="L52" s="11"/>
       <c r="M52" s="11"/>
       <c r="N52" s="90"/>
-      <c r="O52" s="12"/>
+      <c r="O52" s="90"/>
       <c r="P52" s="12"/>
-      <c r="Q52" s="45"/>
+      <c r="Q52" s="12"/>
       <c r="R52" s="45"/>
       <c r="S52" s="45"/>
       <c r="T52" s="45"/>
-      <c r="U52" s="57"/>
-    </row>
-    <row r="53" spans="1:21" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U52" s="45"/>
+      <c r="V52" s="57"/>
+    </row>
+    <row r="53" spans="1:22" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="22"/>
       <c r="B53" s="45"/>
       <c r="C53" s="12"/>
@@ -42950,15 +43010,16 @@
       <c r="L53" s="11"/>
       <c r="M53" s="11"/>
       <c r="N53" s="11"/>
-      <c r="O53" s="45"/>
-      <c r="P53" s="12"/>
-      <c r="Q53" s="45"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="45"/>
+      <c r="Q53" s="12"/>
       <c r="R53" s="45"/>
       <c r="S53" s="45"/>
       <c r="T53" s="45"/>
-      <c r="U53" s="57"/>
-    </row>
-    <row r="54" spans="1:21" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U53" s="45"/>
+      <c r="V53" s="57"/>
+    </row>
+    <row r="54" spans="1:22" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="22"/>
       <c r="B54" s="45"/>
       <c r="C54" s="12"/>
@@ -42973,15 +43034,16 @@
       <c r="L54" s="11"/>
       <c r="M54" s="11"/>
       <c r="N54" s="11"/>
-      <c r="O54" s="45"/>
-      <c r="P54" s="12"/>
-      <c r="Q54" s="45"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="45"/>
+      <c r="Q54" s="12"/>
       <c r="R54" s="45"/>
       <c r="S54" s="45"/>
       <c r="T54" s="45"/>
-      <c r="U54" s="57"/>
-    </row>
-    <row r="55" spans="1:21" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U54" s="45"/>
+      <c r="V54" s="57"/>
+    </row>
+    <row r="55" spans="1:22" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="22"/>
       <c r="B55" s="91"/>
       <c r="C55" s="12"/>
@@ -42997,14 +43059,15 @@
       <c r="M55" s="11"/>
       <c r="N55" s="11"/>
       <c r="O55" s="11"/>
-      <c r="P55" s="91"/>
-      <c r="Q55" s="11"/>
+      <c r="P55" s="11"/>
+      <c r="Q55" s="91"/>
       <c r="R55" s="11"/>
       <c r="S55" s="11"/>
       <c r="T55" s="11"/>
-      <c r="U55" s="57"/>
-    </row>
-    <row r="56" spans="1:21" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U55" s="11"/>
+      <c r="V55" s="57"/>
+    </row>
+    <row r="56" spans="1:22" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="22"/>
       <c r="B56" s="45"/>
       <c r="C56" s="12"/>
@@ -43019,15 +43082,16 @@
       <c r="L56" s="11"/>
       <c r="M56" s="11"/>
       <c r="N56" s="9"/>
-      <c r="O56" s="45"/>
-      <c r="P56" s="12"/>
-      <c r="Q56" s="45"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="45"/>
+      <c r="Q56" s="12"/>
       <c r="R56" s="45"/>
       <c r="S56" s="45"/>
       <c r="T56" s="45"/>
-      <c r="U56" s="57"/>
-    </row>
-    <row r="57" spans="1:21" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U56" s="45"/>
+      <c r="V56" s="57"/>
+    </row>
+    <row r="57" spans="1:22" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="22"/>
       <c r="B57" s="91"/>
       <c r="C57" s="12"/>
@@ -43042,15 +43106,16 @@
       <c r="L57" s="90"/>
       <c r="M57" s="11"/>
       <c r="N57" s="9"/>
-      <c r="O57" s="11"/>
-      <c r="P57" s="91"/>
-      <c r="Q57" s="11"/>
+      <c r="O57" s="9"/>
+      <c r="P57" s="11"/>
+      <c r="Q57" s="91"/>
       <c r="R57" s="11"/>
       <c r="S57" s="11"/>
       <c r="T57" s="11"/>
-      <c r="U57" s="57"/>
-    </row>
-    <row r="58" spans="1:21" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U57" s="11"/>
+      <c r="V57" s="57"/>
+    </row>
+    <row r="58" spans="1:22" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="22"/>
       <c r="B58" s="91"/>
       <c r="C58" s="12"/>
@@ -43065,15 +43130,16 @@
       <c r="L58" s="90"/>
       <c r="M58" s="11"/>
       <c r="N58" s="9"/>
-      <c r="O58" s="11"/>
-      <c r="P58" s="91"/>
-      <c r="Q58" s="11"/>
+      <c r="O58" s="9"/>
+      <c r="P58" s="11"/>
+      <c r="Q58" s="91"/>
       <c r="R58" s="11"/>
       <c r="S58" s="11"/>
       <c r="T58" s="11"/>
-      <c r="U58" s="57"/>
-    </row>
-    <row r="59" spans="1:21" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U58" s="11"/>
+      <c r="V58" s="57"/>
+    </row>
+    <row r="59" spans="1:22" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
@@ -43088,15 +43154,16 @@
       <c r="L59" s="90"/>
       <c r="M59" s="13"/>
       <c r="N59" s="101"/>
-      <c r="O59" s="13"/>
+      <c r="O59" s="101"/>
       <c r="P59" s="13"/>
       <c r="Q59" s="13"/>
       <c r="R59" s="13"/>
       <c r="S59" s="13"/>
       <c r="T59" s="13"/>
-      <c r="U59" s="57"/>
-    </row>
-    <row r="60" spans="1:21" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U59" s="13"/>
+      <c r="V59" s="57"/>
+    </row>
+    <row r="60" spans="1:22" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="22"/>
       <c r="B60" s="45"/>
       <c r="C60" s="11"/>
@@ -43111,15 +43178,16 @@
       <c r="L60" s="11"/>
       <c r="M60" s="11"/>
       <c r="N60" s="11"/>
-      <c r="O60" s="45"/>
-      <c r="P60" s="99"/>
-      <c r="Q60" s="45"/>
+      <c r="O60" s="11"/>
+      <c r="P60" s="45"/>
+      <c r="Q60" s="99"/>
       <c r="R60" s="45"/>
       <c r="S60" s="45"/>
       <c r="T60" s="45"/>
-      <c r="U60" s="57"/>
-    </row>
-    <row r="61" spans="1:21" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U60" s="45"/>
+      <c r="V60" s="57"/>
+    </row>
+    <row r="61" spans="1:22" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="22"/>
       <c r="B61" s="45"/>
       <c r="C61" s="11"/>
@@ -43134,15 +43202,16 @@
       <c r="L61" s="11"/>
       <c r="M61" s="11"/>
       <c r="N61" s="11"/>
-      <c r="O61" s="45"/>
-      <c r="P61" s="99"/>
-      <c r="Q61" s="45"/>
+      <c r="O61" s="11"/>
+      <c r="P61" s="45"/>
+      <c r="Q61" s="99"/>
       <c r="R61" s="45"/>
       <c r="S61" s="45"/>
       <c r="T61" s="45"/>
-      <c r="U61" s="57"/>
-    </row>
-    <row r="62" spans="1:21" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U61" s="45"/>
+      <c r="V61" s="57"/>
+    </row>
+    <row r="62" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="13"/>
       <c r="B62" s="11"/>
       <c r="C62" s="9"/>
@@ -43163,9 +43232,10 @@
       <c r="R62" s="11"/>
       <c r="S62" s="11"/>
       <c r="T62" s="11"/>
-      <c r="U62" s="57"/>
-    </row>
-    <row r="63" spans="1:21" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U62" s="11"/>
+      <c r="V62" s="57"/>
+    </row>
+    <row r="63" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="22"/>
       <c r="B63" s="18"/>
       <c r="C63" s="12"/>
@@ -43180,15 +43250,16 @@
       <c r="L63" s="11"/>
       <c r="M63" s="15"/>
       <c r="N63" s="15"/>
-      <c r="O63" s="18"/>
-      <c r="P63" s="20"/>
-      <c r="Q63" s="18"/>
+      <c r="O63" s="15"/>
+      <c r="P63" s="18"/>
+      <c r="Q63" s="20"/>
       <c r="R63" s="18"/>
       <c r="S63" s="18"/>
       <c r="T63" s="18"/>
-      <c r="U63" s="57"/>
-    </row>
-    <row r="64" spans="1:21" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U63" s="18"/>
+      <c r="V63" s="57"/>
+    </row>
+    <row r="64" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="98"/>
       <c r="B64" s="15"/>
       <c r="C64" s="9"/>
@@ -43209,9 +43280,10 @@
       <c r="R64" s="15"/>
       <c r="S64" s="15"/>
       <c r="T64" s="15"/>
-      <c r="U64" s="57"/>
-    </row>
-    <row r="65" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U64" s="15"/>
+      <c r="V64" s="57"/>
+    </row>
+    <row r="65" spans="1:23" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="13"/>
       <c r="B65" s="15"/>
       <c r="C65" s="9"/>
@@ -43226,15 +43298,16 @@
       <c r="L65" s="11"/>
       <c r="M65" s="15"/>
       <c r="N65" s="15"/>
-      <c r="O65" s="18"/>
+      <c r="O65" s="15"/>
       <c r="P65" s="18"/>
       <c r="Q65" s="18"/>
       <c r="R65" s="18"/>
       <c r="S65" s="18"/>
       <c r="T65" s="18"/>
-      <c r="U65" s="57"/>
-    </row>
-    <row r="66" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U65" s="18"/>
+      <c r="V65" s="57"/>
+    </row>
+    <row r="66" spans="1:23" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="98"/>
       <c r="B66" s="15"/>
       <c r="C66" s="11"/>
@@ -43250,14 +43323,15 @@
       <c r="M66" s="15"/>
       <c r="N66" s="15"/>
       <c r="O66" s="15"/>
-      <c r="P66" s="104"/>
-      <c r="Q66" s="15"/>
+      <c r="P66" s="15"/>
+      <c r="Q66" s="104"/>
       <c r="R66" s="15"/>
       <c r="S66" s="15"/>
       <c r="T66" s="15"/>
-      <c r="U66" s="57"/>
-    </row>
-    <row r="67" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U66" s="15"/>
+      <c r="V66" s="57"/>
+    </row>
+    <row r="67" spans="1:23" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="22"/>
       <c r="B67" s="18"/>
       <c r="C67" s="12"/>
@@ -43272,15 +43346,16 @@
       <c r="L67" s="100"/>
       <c r="M67" s="15"/>
       <c r="N67" s="16"/>
-      <c r="O67" s="18"/>
-      <c r="P67" s="20"/>
-      <c r="Q67" s="18"/>
+      <c r="O67" s="16"/>
+      <c r="P67" s="18"/>
+      <c r="Q67" s="20"/>
       <c r="R67" s="18"/>
       <c r="S67" s="18"/>
       <c r="T67" s="18"/>
-      <c r="U67" s="57"/>
-    </row>
-    <row r="68" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U67" s="18"/>
+      <c r="V67" s="57"/>
+    </row>
+    <row r="68" spans="1:23" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="98"/>
       <c r="B68" s="15"/>
       <c r="C68" s="9"/>
@@ -43296,14 +43371,15 @@
       <c r="M68" s="15"/>
       <c r="N68" s="15"/>
       <c r="O68" s="15"/>
-      <c r="P68" s="104"/>
-      <c r="Q68" s="15"/>
+      <c r="P68" s="15"/>
+      <c r="Q68" s="104"/>
       <c r="R68" s="15"/>
       <c r="S68" s="15"/>
       <c r="T68" s="15"/>
-      <c r="U68" s="57"/>
-    </row>
-    <row r="69" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U68" s="15"/>
+      <c r="V68" s="57"/>
+    </row>
+    <row r="69" spans="1:23" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="22"/>
       <c r="B69" s="18"/>
       <c r="C69" s="12"/>
@@ -43318,15 +43394,16 @@
       <c r="L69" s="11"/>
       <c r="M69" s="15"/>
       <c r="N69" s="9"/>
-      <c r="O69" s="20"/>
+      <c r="O69" s="16"/>
       <c r="P69" s="20"/>
-      <c r="Q69" s="18"/>
+      <c r="Q69" s="20"/>
       <c r="R69" s="18"/>
       <c r="S69" s="18"/>
       <c r="T69" s="18"/>
-      <c r="U69" s="57"/>
-    </row>
-    <row r="70" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U69" s="18"/>
+      <c r="V69" s="57"/>
+    </row>
+    <row r="70" spans="1:23" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="22"/>
       <c r="B70" s="18"/>
       <c r="C70" s="12"/>
@@ -43341,15 +43418,16 @@
       <c r="L70" s="100"/>
       <c r="M70" s="15"/>
       <c r="N70" s="15"/>
-      <c r="O70" s="18"/>
-      <c r="P70" s="20"/>
-      <c r="Q70" s="18"/>
+      <c r="O70" s="15"/>
+      <c r="P70" s="18"/>
+      <c r="Q70" s="20"/>
       <c r="R70" s="18"/>
       <c r="S70" s="18"/>
       <c r="T70" s="18"/>
-      <c r="U70" s="57"/>
-    </row>
-    <row r="71" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U70" s="18"/>
+      <c r="V70" s="57"/>
+    </row>
+    <row r="71" spans="1:23" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="22"/>
       <c r="B71" s="18"/>
       <c r="C71" s="12"/>
@@ -43364,15 +43442,16 @@
       <c r="L71" s="11"/>
       <c r="M71" s="15"/>
       <c r="N71" s="15"/>
-      <c r="O71" s="18"/>
-      <c r="P71" s="20"/>
-      <c r="Q71" s="18"/>
+      <c r="O71" s="15"/>
+      <c r="P71" s="18"/>
+      <c r="Q71" s="20"/>
       <c r="R71" s="18"/>
       <c r="S71" s="18"/>
       <c r="T71" s="18"/>
-      <c r="U71" s="57"/>
-    </row>
-    <row r="72" spans="1:22" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U71" s="18"/>
+      <c r="V71" s="57"/>
+    </row>
+    <row r="72" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
@@ -43387,7 +43466,7 @@
       <c r="L72" s="11"/>
       <c r="M72" s="11"/>
       <c r="N72" s="105"/>
-      <c r="O72" s="13"/>
+      <c r="O72" s="105"/>
       <c r="P72" s="13"/>
       <c r="Q72" s="13"/>
       <c r="R72" s="13"/>
@@ -43395,8 +43474,9 @@
       <c r="T72" s="13"/>
       <c r="U72" s="13"/>
       <c r="V72" s="13"/>
-    </row>
-    <row r="73" spans="1:22" s="107" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W72" s="13"/>
+    </row>
+    <row r="73" spans="1:23" s="107" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="22"/>
       <c r="B73" s="45"/>
       <c r="C73" s="12"/>
@@ -43411,15 +43491,16 @@
       <c r="L73" s="15"/>
       <c r="M73" s="15"/>
       <c r="N73" s="16"/>
-      <c r="O73" s="18"/>
-      <c r="P73" s="12"/>
-      <c r="Q73" s="18"/>
+      <c r="O73" s="16"/>
+      <c r="P73" s="18"/>
+      <c r="Q73" s="12"/>
       <c r="R73" s="18"/>
       <c r="S73" s="18"/>
       <c r="T73" s="18"/>
-      <c r="U73" s="57"/>
-    </row>
-    <row r="74" spans="1:22" s="107" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U73" s="18"/>
+      <c r="V73" s="57"/>
+    </row>
+    <row r="74" spans="1:23" s="107" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="22"/>
       <c r="B74" s="45"/>
       <c r="C74" s="12"/>
@@ -43434,15 +43515,16 @@
       <c r="L74" s="15"/>
       <c r="M74" s="15"/>
       <c r="N74" s="16"/>
-      <c r="O74" s="20"/>
-      <c r="P74" s="12"/>
-      <c r="Q74" s="18"/>
+      <c r="O74" s="16"/>
+      <c r="P74" s="20"/>
+      <c r="Q74" s="12"/>
       <c r="R74" s="18"/>
       <c r="S74" s="18"/>
       <c r="T74" s="18"/>
-      <c r="U74" s="57"/>
-    </row>
-    <row r="75" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U74" s="18"/>
+      <c r="V74" s="57"/>
+    </row>
+    <row r="75" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="22"/>
       <c r="B75" s="45"/>
       <c r="C75" s="12"/>
@@ -43456,14 +43538,15 @@
       <c r="K75" s="15"/>
       <c r="M75" s="15"/>
       <c r="N75" s="101"/>
-      <c r="O75" s="18"/>
-      <c r="P75" s="20"/>
-      <c r="Q75" s="18"/>
+      <c r="O75" s="105"/>
+      <c r="P75" s="18"/>
+      <c r="Q75" s="20"/>
       <c r="R75" s="18"/>
       <c r="S75" s="18"/>
       <c r="T75" s="18"/>
-    </row>
-    <row r="76" spans="1:22" s="111" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U75" s="18"/>
+    </row>
+    <row r="76" spans="1:23" s="111" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="22"/>
       <c r="B76" s="18"/>
       <c r="C76" s="12"/>
@@ -43478,15 +43561,16 @@
       <c r="L76" s="109"/>
       <c r="M76" s="15"/>
       <c r="N76" s="110"/>
-      <c r="O76" s="20"/>
+      <c r="O76" s="100"/>
       <c r="P76" s="20"/>
-      <c r="Q76" s="18"/>
+      <c r="Q76" s="20"/>
       <c r="R76" s="18"/>
       <c r="S76" s="18"/>
       <c r="T76" s="18"/>
-      <c r="U76" s="57"/>
-    </row>
-    <row r="77" spans="1:22" s="111" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U76" s="18"/>
+      <c r="V76" s="57"/>
+    </row>
+    <row r="77" spans="1:23" s="111" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="22"/>
       <c r="B77" s="18"/>
       <c r="C77" s="11"/>
@@ -43501,15 +43585,16 @@
       <c r="L77" s="109"/>
       <c r="M77" s="15"/>
       <c r="N77" s="109"/>
-      <c r="O77" s="18"/>
-      <c r="P77" s="113"/>
-      <c r="Q77" s="18"/>
+      <c r="O77" s="15"/>
+      <c r="P77" s="18"/>
+      <c r="Q77" s="113"/>
       <c r="R77" s="18"/>
       <c r="S77" s="18"/>
       <c r="T77" s="18"/>
-      <c r="U77" s="57"/>
-    </row>
-    <row r="78" spans="1:22" s="111" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U77" s="18"/>
+      <c r="V77" s="57"/>
+    </row>
+    <row r="78" spans="1:23" s="111" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="22"/>
       <c r="B78" s="104"/>
       <c r="C78" s="12"/>
@@ -43525,14 +43610,15 @@
       <c r="M78" s="15"/>
       <c r="N78" s="109"/>
       <c r="O78" s="15"/>
-      <c r="P78" s="104"/>
-      <c r="Q78" s="15"/>
+      <c r="P78" s="15"/>
+      <c r="Q78" s="104"/>
       <c r="R78" s="15"/>
       <c r="S78" s="15"/>
       <c r="T78" s="15"/>
-      <c r="U78" s="57"/>
-    </row>
-    <row r="79" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U78" s="15"/>
+      <c r="V78" s="57"/>
+    </row>
+    <row r="79" spans="1:23" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="115"/>
       <c r="B79" s="116"/>
       <c r="C79" s="117"/>
@@ -43547,15 +43633,16 @@
       <c r="L79" s="116"/>
       <c r="M79" s="116"/>
       <c r="N79" s="101"/>
-      <c r="O79" s="116"/>
-      <c r="P79" s="117"/>
-      <c r="Q79" s="116"/>
+      <c r="O79" s="101"/>
+      <c r="P79" s="116"/>
+      <c r="Q79" s="117"/>
       <c r="R79" s="116"/>
       <c r="S79" s="116"/>
       <c r="T79" s="116"/>
-      <c r="U79" s="57"/>
-    </row>
-    <row r="80" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U79" s="116"/>
+      <c r="V79" s="57"/>
+    </row>
+    <row r="80" spans="1:23" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="115"/>
       <c r="B80" s="116"/>
       <c r="C80" s="117"/>
@@ -43571,14 +43658,15 @@
       <c r="M80" s="116"/>
       <c r="N80" s="116"/>
       <c r="O80" s="116"/>
-      <c r="P80" s="117"/>
-      <c r="Q80" s="116"/>
+      <c r="P80" s="116"/>
+      <c r="Q80" s="117"/>
       <c r="R80" s="116"/>
       <c r="S80" s="116"/>
       <c r="T80" s="116"/>
-      <c r="U80" s="57"/>
-    </row>
-    <row r="81" spans="1:21" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U80" s="116"/>
+      <c r="V80" s="57"/>
+    </row>
+    <row r="81" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13"/>
       <c r="B81" s="11"/>
       <c r="C81" s="9"/>
@@ -43593,15 +43681,16 @@
       <c r="L81" s="119"/>
       <c r="M81" s="11"/>
       <c r="N81" s="11"/>
-      <c r="O81" s="45"/>
+      <c r="O81" s="11"/>
       <c r="P81" s="45"/>
       <c r="Q81" s="45"/>
-      <c r="R81" s="18"/>
-      <c r="S81" s="45"/>
+      <c r="R81" s="45"/>
+      <c r="S81" s="18"/>
       <c r="T81" s="45"/>
-      <c r="U81" s="57"/>
-    </row>
-    <row r="82" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U81" s="45"/>
+      <c r="V81" s="57"/>
+    </row>
+    <row r="82" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="22"/>
       <c r="B82" s="45"/>
       <c r="C82" s="12"/>
@@ -43615,14 +43704,14 @@
       <c r="K82" s="15"/>
       <c r="L82" s="100"/>
       <c r="M82" s="15"/>
-      <c r="O82" s="18"/>
-      <c r="P82" s="20"/>
-      <c r="Q82" s="18"/>
+      <c r="P82" s="18"/>
+      <c r="Q82" s="20"/>
       <c r="R82" s="18"/>
       <c r="S82" s="18"/>
       <c r="T82" s="18"/>
-    </row>
-    <row r="83" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U82" s="18"/>
+    </row>
+    <row r="83" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="22"/>
       <c r="B83" s="91"/>
       <c r="C83" s="12"/>
@@ -43637,14 +43726,14 @@
       <c r="L83" s="100"/>
       <c r="M83" s="15"/>
       <c r="N83" s="11"/>
-      <c r="O83" s="15"/>
-      <c r="P83" s="104"/>
-      <c r="Q83" s="15"/>
+      <c r="P83" s="15"/>
+      <c r="Q83" s="104"/>
       <c r="R83" s="15"/>
       <c r="S83" s="15"/>
       <c r="T83" s="15"/>
-    </row>
-    <row r="84" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U83" s="15"/>
+    </row>
+    <row r="84" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="13"/>
       <c r="B84" s="11"/>
       <c r="C84" s="9"/>
@@ -43657,14 +43746,14 @@
       <c r="J84" s="15"/>
       <c r="K84" s="15"/>
       <c r="M84" s="15"/>
-      <c r="O84" s="18"/>
-      <c r="P84" s="113"/>
-      <c r="Q84" s="18"/>
+      <c r="P84" s="18"/>
+      <c r="Q84" s="113"/>
       <c r="R84" s="18"/>
       <c r="S84" s="18"/>
       <c r="T84" s="18"/>
-    </row>
-    <row r="85" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U84" s="18"/>
+    </row>
+    <row r="85" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="93"/>
       <c r="B85" s="36"/>
       <c r="C85" s="94"/>
@@ -43680,13 +43769,14 @@
       <c r="M85" s="36"/>
       <c r="N85" s="36"/>
       <c r="O85" s="36"/>
-      <c r="P85" s="95"/>
-      <c r="Q85" s="121"/>
-      <c r="R85" s="122"/>
-      <c r="S85" s="123"/>
+      <c r="P85" s="36"/>
+      <c r="Q85" s="95"/>
+      <c r="R85" s="121"/>
+      <c r="S85" s="122"/>
       <c r="T85" s="123"/>
-    </row>
-    <row r="86" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U85" s="123"/>
+    </row>
+    <row r="86" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="13"/>
       <c r="B86" s="91"/>
       <c r="C86" s="9"/>
@@ -43702,13 +43792,14 @@
       <c r="M86" s="11"/>
       <c r="N86" s="11"/>
       <c r="O86" s="11"/>
-      <c r="P86" s="91"/>
-      <c r="Q86" s="15"/>
+      <c r="P86" s="11"/>
+      <c r="Q86" s="91"/>
       <c r="R86" s="15"/>
       <c r="S86" s="15"/>
       <c r="T86" s="15"/>
-    </row>
-    <row r="87" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U86" s="15"/>
+    </row>
+    <row r="87" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="13"/>
       <c r="B87" s="91"/>
       <c r="C87" s="9"/>
@@ -43724,13 +43815,14 @@
       <c r="M87" s="11"/>
       <c r="N87" s="11"/>
       <c r="O87" s="11"/>
-      <c r="P87" s="91"/>
-      <c r="Q87" s="11"/>
+      <c r="P87" s="11"/>
+      <c r="Q87" s="91"/>
       <c r="R87" s="11"/>
       <c r="S87" s="11"/>
       <c r="T87" s="11"/>
-    </row>
-    <row r="88" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U87" s="11"/>
+    </row>
+    <row r="88" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="22"/>
       <c r="B88" s="18"/>
       <c r="C88" s="12"/>
@@ -43744,14 +43836,15 @@
       <c r="K88" s="15"/>
       <c r="M88" s="15"/>
       <c r="N88" s="16"/>
-      <c r="O88" s="20"/>
+      <c r="O88" s="16"/>
       <c r="P88" s="20"/>
-      <c r="Q88" s="18"/>
+      <c r="Q88" s="20"/>
       <c r="R88" s="18"/>
       <c r="S88" s="18"/>
       <c r="T88" s="18"/>
-    </row>
-    <row r="89" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U88" s="18"/>
+    </row>
+    <row r="89" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="125"/>
       <c r="B89" s="15"/>
       <c r="C89" s="15"/>
@@ -43764,14 +43857,14 @@
       <c r="J89" s="15"/>
       <c r="K89" s="15"/>
       <c r="M89" s="15"/>
-      <c r="O89" s="15"/>
-      <c r="P89" s="104"/>
-      <c r="Q89" s="15"/>
+      <c r="P89" s="15"/>
+      <c r="Q89" s="104"/>
       <c r="R89" s="15"/>
       <c r="S89" s="15"/>
       <c r="T89" s="15"/>
-    </row>
-    <row r="90" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U89" s="15"/>
+    </row>
+    <row r="90" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="22"/>
       <c r="B90" s="45"/>
       <c r="C90" s="12"/>
@@ -43786,14 +43879,15 @@
       <c r="L90" s="11"/>
       <c r="M90" s="11"/>
       <c r="N90" s="11"/>
-      <c r="O90" s="45"/>
-      <c r="P90" s="12"/>
-      <c r="Q90" s="45"/>
+      <c r="O90" s="11"/>
+      <c r="P90" s="45"/>
+      <c r="Q90" s="12"/>
       <c r="R90" s="45"/>
       <c r="S90" s="45"/>
       <c r="T90" s="45"/>
-    </row>
-    <row r="91" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U90" s="45"/>
+    </row>
+    <row r="91" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
@@ -43808,14 +43902,15 @@
       <c r="L91" s="90"/>
       <c r="M91" s="13"/>
       <c r="N91" s="101"/>
-      <c r="O91" s="13"/>
+      <c r="O91" s="101"/>
       <c r="P91" s="13"/>
       <c r="Q91" s="13"/>
       <c r="R91" s="13"/>
       <c r="S91" s="13"/>
       <c r="T91" s="13"/>
-    </row>
-    <row r="92" spans="1:21" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U91" s="13"/>
+    </row>
+    <row r="92" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="13"/>
       <c r="B92" s="15"/>
       <c r="C92" s="9"/>
@@ -43832,13 +43927,14 @@
       <c r="N92" s="16"/>
       <c r="O92" s="16"/>
       <c r="P92" s="16"/>
-      <c r="Q92" s="15"/>
+      <c r="Q92" s="16"/>
       <c r="R92" s="15"/>
       <c r="S92" s="15"/>
       <c r="T92" s="15"/>
-      <c r="U92" s="57"/>
-    </row>
-    <row r="93" spans="1:21" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U92" s="15"/>
+      <c r="V92" s="57"/>
+    </row>
+    <row r="93" spans="1:22" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="126"/>
       <c r="B93" s="18"/>
       <c r="C93" s="20"/>
@@ -43853,15 +43949,16 @@
       <c r="L93" s="15"/>
       <c r="M93" s="15"/>
       <c r="N93" s="15"/>
-      <c r="O93" s="18"/>
-      <c r="P93" s="20"/>
-      <c r="Q93" s="18"/>
+      <c r="O93" s="15"/>
+      <c r="P93" s="18"/>
+      <c r="Q93" s="20"/>
       <c r="R93" s="18"/>
       <c r="S93" s="18"/>
       <c r="T93" s="18"/>
-      <c r="U93" s="57"/>
-    </row>
-    <row r="94" spans="1:21" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U93" s="18"/>
+      <c r="V93" s="57"/>
+    </row>
+    <row r="94" spans="1:22" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="126"/>
       <c r="B94" s="18"/>
       <c r="C94" s="20"/>
@@ -43876,15 +43973,16 @@
       <c r="L94" s="11"/>
       <c r="M94" s="15"/>
       <c r="N94" s="15"/>
-      <c r="O94" s="18"/>
-      <c r="P94" s="20"/>
-      <c r="Q94" s="18"/>
+      <c r="O94" s="15"/>
+      <c r="P94" s="18"/>
+      <c r="Q94" s="20"/>
       <c r="R94" s="18"/>
       <c r="S94" s="18"/>
       <c r="T94" s="18"/>
-      <c r="U94" s="57"/>
-    </row>
-    <row r="95" spans="1:21" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U94" s="18"/>
+      <c r="V94" s="57"/>
+    </row>
+    <row r="95" spans="1:22" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="126"/>
       <c r="B95" s="18"/>
       <c r="C95" s="20"/>
@@ -43899,15 +43997,16 @@
       <c r="L95" s="11"/>
       <c r="M95" s="15"/>
       <c r="N95" s="15"/>
-      <c r="O95" s="18"/>
-      <c r="P95" s="20"/>
-      <c r="Q95" s="18"/>
+      <c r="O95" s="15"/>
+      <c r="P95" s="18"/>
+      <c r="Q95" s="20"/>
       <c r="R95" s="18"/>
       <c r="S95" s="18"/>
       <c r="T95" s="18"/>
-      <c r="U95" s="24"/>
-    </row>
-    <row r="96" spans="1:21" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U95" s="18"/>
+      <c r="V95" s="24"/>
+    </row>
+    <row r="96" spans="1:22" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="126"/>
       <c r="B96" s="18"/>
       <c r="C96" s="20"/>
@@ -43922,15 +44021,16 @@
       <c r="L96" s="11"/>
       <c r="M96" s="15"/>
       <c r="N96" s="16"/>
-      <c r="O96" s="20"/>
+      <c r="O96" s="16"/>
       <c r="P96" s="20"/>
-      <c r="Q96" s="18"/>
+      <c r="Q96" s="20"/>
       <c r="R96" s="18"/>
       <c r="S96" s="18"/>
       <c r="T96" s="18"/>
-      <c r="U96" s="24"/>
-    </row>
-    <row r="97" spans="1:21" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U96" s="18"/>
+      <c r="V96" s="24"/>
+    </row>
+    <row r="97" spans="1:22" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="126"/>
       <c r="B97" s="18"/>
       <c r="C97" s="20"/>
@@ -43945,15 +44045,16 @@
       <c r="L97" s="11"/>
       <c r="M97" s="15"/>
       <c r="N97" s="90"/>
-      <c r="O97" s="20"/>
+      <c r="O97" s="100"/>
       <c r="P97" s="20"/>
-      <c r="Q97" s="18"/>
+      <c r="Q97" s="20"/>
       <c r="R97" s="18"/>
       <c r="S97" s="18"/>
       <c r="T97" s="18"/>
-      <c r="U97" s="57"/>
-    </row>
-    <row r="98" spans="1:21" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U97" s="18"/>
+      <c r="V97" s="57"/>
+    </row>
+    <row r="98" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="22"/>
       <c r="B98" s="45"/>
       <c r="C98" s="12"/>
@@ -43968,15 +44069,16 @@
       <c r="L98" s="11"/>
       <c r="M98" s="11"/>
       <c r="N98" s="11"/>
-      <c r="O98" s="45"/>
-      <c r="P98" s="12"/>
-      <c r="Q98" s="45"/>
+      <c r="O98" s="11"/>
+      <c r="P98" s="45"/>
+      <c r="Q98" s="12"/>
       <c r="R98" s="45"/>
       <c r="S98" s="45"/>
       <c r="T98" s="45"/>
-      <c r="U98" s="57"/>
-    </row>
-    <row r="99" spans="1:21" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U98" s="45"/>
+      <c r="V98" s="57"/>
+    </row>
+    <row r="99" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="22"/>
       <c r="B99" s="45"/>
       <c r="C99" s="12"/>
@@ -43991,15 +44093,16 @@
       <c r="L99" s="11"/>
       <c r="M99" s="11"/>
       <c r="N99" s="11"/>
-      <c r="O99" s="45"/>
-      <c r="P99" s="12"/>
-      <c r="Q99" s="45"/>
+      <c r="O99" s="11"/>
+      <c r="P99" s="45"/>
+      <c r="Q99" s="12"/>
       <c r="R99" s="45"/>
       <c r="S99" s="45"/>
       <c r="T99" s="45"/>
-      <c r="U99" s="57"/>
-    </row>
-    <row r="100" spans="1:21" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U99" s="45"/>
+      <c r="V99" s="57"/>
+    </row>
+    <row r="100" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="22"/>
       <c r="B100" s="22"/>
       <c r="C100" s="9"/>
@@ -44015,14 +44118,15 @@
       <c r="M100" s="15"/>
       <c r="N100" s="15"/>
       <c r="O100" s="15"/>
-      <c r="P100" s="16"/>
-      <c r="Q100" s="18"/>
+      <c r="P100" s="15"/>
+      <c r="Q100" s="16"/>
       <c r="R100" s="18"/>
       <c r="S100" s="18"/>
       <c r="T100" s="18"/>
-      <c r="U100" s="57"/>
-    </row>
-    <row r="101" spans="1:21" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U100" s="18"/>
+      <c r="V100" s="57"/>
+    </row>
+    <row r="101" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="22"/>
       <c r="B101" s="22"/>
       <c r="C101" s="9"/>
@@ -44038,14 +44142,15 @@
       <c r="M101" s="11"/>
       <c r="N101" s="11"/>
       <c r="O101" s="11"/>
-      <c r="P101" s="9"/>
-      <c r="Q101" s="45"/>
+      <c r="P101" s="11"/>
+      <c r="Q101" s="9"/>
       <c r="R101" s="45"/>
       <c r="S101" s="45"/>
       <c r="T101" s="45"/>
-      <c r="U101" s="57"/>
-    </row>
-    <row r="102" spans="1:21" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U101" s="45"/>
+      <c r="V101" s="57"/>
+    </row>
+    <row r="102" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="22"/>
       <c r="B102" s="22"/>
       <c r="C102" s="15"/>
@@ -44060,15 +44165,16 @@
       <c r="L102" s="15"/>
       <c r="M102" s="15"/>
       <c r="N102" s="15"/>
-      <c r="O102" s="18"/>
-      <c r="P102" s="113"/>
-      <c r="Q102" s="18"/>
+      <c r="O102" s="15"/>
+      <c r="P102" s="18"/>
+      <c r="Q102" s="113"/>
       <c r="R102" s="18"/>
       <c r="S102" s="18"/>
       <c r="T102" s="18"/>
-      <c r="U102" s="57"/>
-    </row>
-    <row r="103" spans="1:21" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U102" s="18"/>
+      <c r="V102" s="57"/>
+    </row>
+    <row r="103" spans="1:22" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="22"/>
       <c r="B103" s="22"/>
       <c r="C103" s="16"/>
@@ -44084,14 +44190,15 @@
       <c r="M103" s="15"/>
       <c r="N103" s="15"/>
       <c r="O103" s="15"/>
-      <c r="P103" s="104"/>
-      <c r="Q103" s="15"/>
+      <c r="P103" s="15"/>
+      <c r="Q103" s="104"/>
       <c r="R103" s="15"/>
       <c r="S103" s="15"/>
       <c r="T103" s="15"/>
-      <c r="U103" s="57"/>
-    </row>
-    <row r="104" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U103" s="15"/>
+      <c r="V103" s="57"/>
+    </row>
+    <row r="104" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="22"/>
       <c r="B104" s="22"/>
       <c r="C104" s="16"/>
@@ -44105,14 +44212,15 @@
       <c r="K104" s="15"/>
       <c r="M104" s="15"/>
       <c r="N104" s="100"/>
-      <c r="O104" s="18"/>
+      <c r="O104" s="100"/>
       <c r="P104" s="18"/>
       <c r="Q104" s="18"/>
       <c r="R104" s="18"/>
       <c r="S104" s="18"/>
       <c r="T104" s="18"/>
-    </row>
-    <row r="105" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U104" s="18"/>
+    </row>
+    <row r="105" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="22"/>
       <c r="B105" s="22"/>
       <c r="C105" s="20"/>
@@ -44127,14 +44235,15 @@
       <c r="L105" s="16"/>
       <c r="M105" s="16"/>
       <c r="N105" s="105"/>
-      <c r="O105" s="20"/>
+      <c r="O105" s="105"/>
       <c r="P105" s="20"/>
       <c r="Q105" s="20"/>
-      <c r="R105" s="18"/>
+      <c r="R105" s="20"/>
       <c r="S105" s="18"/>
       <c r="T105" s="18"/>
-    </row>
-    <row r="106" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U105" s="18"/>
+    </row>
+    <row r="106" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="22"/>
       <c r="B106" s="22"/>
       <c r="C106" s="20"/>
@@ -44149,14 +44258,15 @@
       <c r="L106" s="16"/>
       <c r="M106" s="16"/>
       <c r="N106" s="105"/>
-      <c r="O106" s="20"/>
+      <c r="O106" s="105"/>
       <c r="P106" s="20"/>
-      <c r="Q106" s="18"/>
+      <c r="Q106" s="20"/>
       <c r="R106" s="18"/>
       <c r="S106" s="18"/>
       <c r="T106" s="18"/>
-    </row>
-    <row r="107" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U106" s="18"/>
+    </row>
+    <row r="107" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="22"/>
       <c r="B107" s="22"/>
       <c r="C107" s="20"/>
@@ -44169,14 +44279,14 @@
       <c r="J107" s="15"/>
       <c r="K107" s="15"/>
       <c r="M107" s="15"/>
-      <c r="O107" s="18"/>
-      <c r="P107" s="20"/>
-      <c r="Q107" s="18"/>
+      <c r="P107" s="18"/>
+      <c r="Q107" s="20"/>
       <c r="R107" s="18"/>
       <c r="S107" s="18"/>
       <c r="T107" s="18"/>
-    </row>
-    <row r="108" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U107" s="18"/>
+    </row>
+    <row r="108" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="22"/>
       <c r="B108" s="22"/>
       <c r="C108" s="20"/>
@@ -44189,14 +44299,14 @@
       <c r="J108" s="15"/>
       <c r="K108" s="15"/>
       <c r="M108" s="15"/>
-      <c r="O108" s="18"/>
-      <c r="P108" s="20"/>
-      <c r="Q108" s="18"/>
+      <c r="P108" s="18"/>
+      <c r="Q108" s="20"/>
       <c r="R108" s="18"/>
       <c r="S108" s="18"/>
       <c r="T108" s="18"/>
-    </row>
-    <row r="109" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U108" s="18"/>
+    </row>
+    <row r="109" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="22"/>
       <c r="B109" s="22"/>
       <c r="C109" s="20"/>
@@ -44211,14 +44321,15 @@
       <c r="L109" s="16"/>
       <c r="M109" s="16"/>
       <c r="N109" s="16"/>
-      <c r="O109" s="20"/>
+      <c r="O109" s="16"/>
       <c r="P109" s="20"/>
       <c r="Q109" s="20"/>
       <c r="R109" s="20"/>
       <c r="S109" s="20"/>
       <c r="T109" s="20"/>
-    </row>
-    <row r="110" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U109" s="20"/>
+    </row>
+    <row r="110" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="22"/>
       <c r="B110" s="22"/>
       <c r="C110" s="20"/>
@@ -44231,14 +44342,14 @@
       <c r="J110" s="15"/>
       <c r="K110" s="15"/>
       <c r="M110" s="15"/>
-      <c r="O110" s="18"/>
-      <c r="P110" s="20"/>
-      <c r="Q110" s="18"/>
+      <c r="P110" s="18"/>
+      <c r="Q110" s="20"/>
       <c r="R110" s="18"/>
       <c r="S110" s="18"/>
       <c r="T110" s="18"/>
-    </row>
-    <row r="111" spans="1:21" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U110" s="18"/>
+    </row>
+    <row r="111" spans="1:22" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="22"/>
       <c r="B111" s="22"/>
       <c r="C111" s="20"/>
@@ -44250,9 +44361,10 @@
       <c r="L111" s="15"/>
       <c r="M111" s="15"/>
       <c r="N111" s="15"/>
-      <c r="P111" s="20"/>
-    </row>
-    <row r="112" spans="1:21" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O111" s="15"/>
+      <c r="Q111" s="20"/>
+    </row>
+    <row r="112" spans="1:22" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="22"/>
       <c r="B112" s="22"/>
       <c r="C112" s="20"/>
@@ -44264,9 +44376,10 @@
       <c r="L112" s="15"/>
       <c r="M112" s="15"/>
       <c r="N112" s="15"/>
-      <c r="P112" s="20"/>
-    </row>
-    <row r="113" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O112" s="15"/>
+      <c r="Q112" s="20"/>
+    </row>
+    <row r="113" spans="1:18" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="22"/>
       <c r="B113" s="22"/>
       <c r="C113" s="20"/>
@@ -44278,9 +44391,10 @@
       <c r="L113" s="15"/>
       <c r="M113" s="15"/>
       <c r="N113" s="15"/>
-      <c r="P113" s="20"/>
-    </row>
-    <row r="114" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O113" s="15"/>
+      <c r="Q113" s="20"/>
+    </row>
+    <row r="114" spans="1:18" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="22"/>
       <c r="B114" s="22"/>
       <c r="C114" s="20"/>
@@ -44292,9 +44406,10 @@
       <c r="L114" s="15"/>
       <c r="M114" s="15"/>
       <c r="N114" s="15"/>
-      <c r="P114" s="20"/>
-    </row>
-    <row r="115" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O114" s="15"/>
+      <c r="Q114" s="20"/>
+    </row>
+    <row r="115" spans="1:18" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="22"/>
       <c r="B115" s="22"/>
       <c r="C115" s="20"/>
@@ -44306,9 +44421,10 @@
       <c r="L115" s="15"/>
       <c r="M115" s="15"/>
       <c r="N115" s="15"/>
-      <c r="P115" s="20"/>
-    </row>
-    <row r="116" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O115" s="15"/>
+      <c r="Q115" s="20"/>
+    </row>
+    <row r="116" spans="1:18" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="22"/>
       <c r="B116" s="22"/>
       <c r="C116" s="20"/>
@@ -44320,9 +44436,10 @@
       <c r="L116" s="15"/>
       <c r="M116" s="15"/>
       <c r="N116" s="15"/>
-      <c r="P116" s="20"/>
-    </row>
-    <row r="117" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O116" s="15"/>
+      <c r="Q116" s="20"/>
+    </row>
+    <row r="117" spans="1:18" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="22"/>
       <c r="B117" s="22"/>
       <c r="C117" s="20"/>
@@ -44334,9 +44451,10 @@
       <c r="L117" s="15"/>
       <c r="M117" s="15"/>
       <c r="N117" s="15"/>
-      <c r="P117" s="20"/>
-    </row>
-    <row r="118" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O117" s="15"/>
+      <c r="Q117" s="20"/>
+    </row>
+    <row r="118" spans="1:18" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="22"/>
       <c r="B118" s="22"/>
       <c r="C118" s="20"/>
@@ -44348,9 +44466,10 @@
       <c r="L118" s="15"/>
       <c r="M118" s="15"/>
       <c r="N118" s="15"/>
-      <c r="P118" s="20"/>
-    </row>
-    <row r="119" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O118" s="15"/>
+      <c r="Q118" s="20"/>
+    </row>
+    <row r="119" spans="1:18" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="22"/>
       <c r="B119" s="22"/>
       <c r="C119" s="20"/>
@@ -44362,9 +44481,10 @@
       <c r="L119" s="15"/>
       <c r="M119" s="15"/>
       <c r="N119" s="15"/>
-      <c r="P119" s="20"/>
-    </row>
-    <row r="120" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O119" s="15"/>
+      <c r="Q119" s="20"/>
+    </row>
+    <row r="120" spans="1:18" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="22"/>
       <c r="B120" s="22"/>
       <c r="C120" s="20"/>
@@ -44376,9 +44496,10 @@
       <c r="L120" s="15"/>
       <c r="M120" s="15"/>
       <c r="N120" s="15"/>
-      <c r="P120" s="20"/>
-    </row>
-    <row r="121" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O120" s="15"/>
+      <c r="Q120" s="20"/>
+    </row>
+    <row r="121" spans="1:18" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="22"/>
       <c r="B121" s="22"/>
       <c r="C121" s="20"/>
@@ -44390,9 +44511,10 @@
       <c r="L121" s="15"/>
       <c r="M121" s="15"/>
       <c r="N121" s="15"/>
-      <c r="P121" s="20"/>
-    </row>
-    <row r="122" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O121" s="15"/>
+      <c r="Q121" s="20"/>
+    </row>
+    <row r="122" spans="1:18" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="22"/>
       <c r="B122" s="22"/>
       <c r="C122" s="20"/>
@@ -44404,9 +44526,10 @@
       <c r="L122" s="15"/>
       <c r="M122" s="15"/>
       <c r="N122" s="15"/>
-      <c r="P122" s="20"/>
-    </row>
-    <row r="123" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O122" s="15"/>
+      <c r="Q122" s="20"/>
+    </row>
+    <row r="123" spans="1:18" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="22"/>
       <c r="B123" s="22"/>
       <c r="C123" s="20"/>
@@ -44418,9 +44541,10 @@
       <c r="L123" s="15"/>
       <c r="M123" s="15"/>
       <c r="N123" s="15"/>
-      <c r="P123" s="20"/>
-    </row>
-    <row r="124" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O123" s="15"/>
+      <c r="Q123" s="20"/>
+    </row>
+    <row r="124" spans="1:18" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="22"/>
       <c r="B124" s="22"/>
       <c r="C124" s="20"/>
@@ -44432,9 +44556,10 @@
       <c r="L124" s="15"/>
       <c r="M124" s="15"/>
       <c r="N124" s="15"/>
-      <c r="P124" s="20"/>
-    </row>
-    <row r="125" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O124" s="15"/>
+      <c r="Q124" s="20"/>
+    </row>
+    <row r="125" spans="1:18" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="22"/>
       <c r="B125" s="22"/>
       <c r="C125" s="20"/>
@@ -44446,9 +44571,10 @@
       <c r="L125" s="15"/>
       <c r="M125" s="15"/>
       <c r="N125" s="15"/>
-      <c r="P125" s="20"/>
-    </row>
-    <row r="126" spans="1:17" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O125" s="15"/>
+      <c r="Q125" s="20"/>
+    </row>
+    <row r="126" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="22"/>
       <c r="B126" s="22"/>
       <c r="C126" s="30"/>
@@ -44462,14 +44588,15 @@
       <c r="M126" s="128"/>
       <c r="N126" s="128"/>
       <c r="O126" s="128"/>
-      <c r="Q126" s="127"/>
-    </row>
-    <row r="127" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P126" s="128"/>
+      <c r="R126" s="127"/>
+    </row>
+    <row r="127" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="22"/>
       <c r="B127" s="22"/>
-      <c r="P127" s="20"/>
-    </row>
-    <row r="128" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q127" s="20"/>
+    </row>
+    <row r="128" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="22"/>
       <c r="B128" s="22"/>
     </row>
@@ -44794,7 +44921,7 @@
       <c r="B208" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:T110" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
+  <autoFilter ref="A3:U110" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <conditionalFormatting sqref="I76">
     <cfRule type="duplicateValues" dxfId="70" priority="2"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added note and interlocReferralReason to response reviewed event (#612)
* added note and interlocReferralReason to response reviewed event

* fixed addNote

* changed appealNote to tempNoteDetail

* resolved conflicts

* resolved conflicts

* resolved conflicts

* changed inteloc referral reason naming

Co-authored-by: gokul <69240498+gokul-sol@users.noreply.github.com>
Co-authored-by: srochani <sunil.rochani@hotmail.com>
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jason.Hart/Downloads/projects/sscs-ccd-definitions/benefit/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jason.Hart/Downloads/ProjectsTools/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D2BA38-A676-7046-A52C-F763C0BF16A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5820EA4E-D33D-B645-BD12-9D9F908A5413}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="197">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -728,6 +728,18 @@
   <si>
     <t>Shuttered</t>
   </si>
+  <si>
+    <t>This is a string value overrides label from CaseField tab</t>
+  </si>
+  <si>
+    <t>This is a string value overrides hint from CaseField tab</t>
+  </si>
+  <si>
+    <t>CaseEventFieldLabel</t>
+  </si>
+  <si>
+    <t>CaseEventFieldHint</t>
+  </si>
 </sst>
 </file>
 
@@ -1324,7 +1336,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1636,6 +1648,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2795,7 +2811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -44810,8 +44826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMK229"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D324" sqref="D324"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -44828,10 +44844,12 @@
     <col min="10" max="15" width="8.83203125" style="18" customWidth="1"/>
     <col min="16" max="16" width="8.83203125" style="45" customWidth="1"/>
     <col min="17" max="17" width="24" style="45" customWidth="1"/>
-    <col min="18" max="1025" width="8.83203125" style="18" customWidth="1"/>
+    <col min="18" max="18" width="20.1640625" style="18" customWidth="1"/>
+    <col min="19" max="19" width="17" style="18" customWidth="1"/>
+    <col min="20" max="1025" width="8.83203125" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>114</v>
       </c>
@@ -44858,7 +44876,7 @@
       <c r="P1" s="185"/>
       <c r="Q1" s="185"/>
     </row>
-    <row r="2" spans="1:17" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="160" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>4</v>
       </c>
@@ -44910,8 +44928,14 @@
       <c r="Q2" s="187" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R2" s="221" t="s">
+        <v>193</v>
+      </c>
+      <c r="S2" s="221" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>9</v>
       </c>
@@ -44963,8 +44987,14 @@
       <c r="Q3" s="188" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R3" s="222" t="s">
+        <v>195</v>
+      </c>
+      <c r="S3" s="222" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
       <c r="C4" s="9"/>
@@ -44983,7 +45013,7 @@
       <c r="P4" s="58"/>
       <c r="Q4" s="58"/>
     </row>
-    <row r="5" spans="1:17" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
       <c r="B5" s="22"/>
       <c r="C5" s="9"/>
@@ -45002,7 +45032,7 @@
       <c r="P5" s="58"/>
       <c r="Q5" s="58"/>
     </row>
-    <row r="6" spans="1:17" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="9"/>
@@ -45021,7 +45051,7 @@
       <c r="P6" s="58"/>
       <c r="Q6" s="58"/>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -45036,7 +45066,7 @@
       <c r="N7" s="45"/>
       <c r="O7" s="189"/>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
@@ -45051,7 +45081,7 @@
       <c r="N8" s="45"/>
       <c r="O8" s="189"/>
     </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -45066,7 +45096,7 @@
       <c r="N9" s="45"/>
       <c r="O9" s="189"/>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -45081,7 +45111,7 @@
       <c r="N10" s="45"/>
       <c r="O10" s="189"/>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
@@ -45096,7 +45126,7 @@
       <c r="N11" s="45"/>
       <c r="O11" s="189"/>
     </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
@@ -45111,7 +45141,7 @@
       <c r="N12" s="45"/>
       <c r="O12" s="189"/>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
@@ -45126,7 +45156,7 @@
       <c r="N13" s="45"/>
       <c r="O13" s="189"/>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
@@ -45141,7 +45171,7 @@
       <c r="N14" s="45"/>
       <c r="O14" s="189"/>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
@@ -45156,7 +45186,7 @@
       <c r="N15" s="45"/>
       <c r="O15" s="189"/>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>

</xml_diff>

<commit_message>
sscs 9885 updated template
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherdavidson/Documents/Dev/hmcts/sscs/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4E88C3-91FE-C744-9BDD-FD7193CF81DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A67DA8A-0382-244B-98EA-84CF2302BAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="18960" windowHeight="11780" tabRatio="500" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="15980" tabRatio="500" firstSheet="15" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -23,21 +23,23 @@
     <sheet name="CaseEvent" sheetId="8" r:id="rId8"/>
     <sheet name="CaseEventToFields" sheetId="9" r:id="rId9"/>
     <sheet name="EventToComplexTypes" sheetId="10" r:id="rId10"/>
-    <sheet name="SearchInputFields" sheetId="11" r:id="rId11"/>
-    <sheet name="SearchResultFields" sheetId="12" r:id="rId12"/>
-    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId13"/>
-    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId14"/>
-    <sheet name="UserProfile" sheetId="15" r:id="rId15"/>
-    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId16"/>
-    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId17"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId18"/>
-    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId19"/>
-    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId20"/>
+    <sheet name="RoleToAccessProfiles" sheetId="21" r:id="rId11"/>
+    <sheet name="SearchParty" sheetId="22" r:id="rId12"/>
+    <sheet name="SearchInputFields" sheetId="11" r:id="rId13"/>
+    <sheet name="SearchResultFields" sheetId="12" r:id="rId14"/>
+    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId15"/>
+    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId16"/>
+    <sheet name="UserProfile" sheetId="15" r:id="rId17"/>
+    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId18"/>
+    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId19"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId20"/>
+    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId21"/>
+    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId22"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$U$110</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$2:$L$98</definedName>
@@ -45,9 +47,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ComplexTypes!$A$3:$M$232</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">FixedLists!$A$1:$E$702</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">State!$A$3:$H$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="16">AuthorisationCaseField!$J$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="18">AuthorisationCaseField!$J$5</definedName>
     <definedName name="_xlnm.Extract" localSheetId="5">CaseTypeTab!$K$61</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="215">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -753,12 +755,54 @@
   <si>
     <t>Yes or No to send a hidden value as part of the payload</t>
   </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>Authorisation</t>
+  </si>
+  <si>
+    <t>ReadOnly</t>
+  </si>
+  <si>
+    <t>AccessProfiles</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>SearchPartyName</t>
+  </si>
+  <si>
+    <t>SearchPartyEmailAddress</t>
+  </si>
+  <si>
+    <t>SearchPartyAddressLine1</t>
+  </si>
+  <si>
+    <t>SearchPartyPostCode</t>
+  </si>
+  <si>
+    <t>SearchPartyDoB</t>
+  </si>
+  <si>
+    <t>SearchPartyDoD</t>
+  </si>
+  <si>
+    <t>RoleToAccessProfiles</t>
+  </si>
+  <si>
+    <t>SearchParty</t>
+  </si>
+  <si>
+    <t>AccessProfile</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1009,6 +1053,24 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF172B4D"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1337,7 +1399,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="229">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1661,6 +1723,10 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2943,8 +3009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3071,11 +3137,126 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA006C0-1036-B948-9B6C-CC8E639AABDE}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="228"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="226" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2"/>
+    </row>
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="225" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="225" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="225" t="s">
+        <v>202</v>
+      </c>
+      <c r="E3" s="225" t="s">
+        <v>203</v>
+      </c>
+      <c r="F3" s="225" t="s">
+        <v>204</v>
+      </c>
+      <c r="G3" s="225" t="s">
+        <v>205</v>
+      </c>
+      <c r="H3" s="225"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F097FA-C043-D54B-950C-F25A8CB79016}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="228"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="226" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I573"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3140,7 +3321,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>74</v>
+        <v>214</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>78</v>
@@ -5187,12 +5368,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5257,7 +5438,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>74</v>
+        <v>214</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>78</v>
@@ -5490,12 +5671,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I91"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5560,7 +5741,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>74</v>
+        <v>214</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>78</v>
@@ -6162,12 +6343,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6236,7 +6417,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>74</v>
+        <v>214</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>78</v>
@@ -6633,11 +6814,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -7300,12 +7481,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:IV35"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7359,8 +7540,8 @@
       <c r="C3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>74</v>
+      <c r="D3" s="227" t="s">
+        <v>214</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>186</v>
@@ -7524,12 +7705,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMJ1015"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A801" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7590,8 +7771,8 @@
       <c r="D3" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>74</v>
+      <c r="E3" s="227" t="s">
+        <v>214</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>186</v>
@@ -21544,12 +21725,193 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="32" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="92.33203125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AMJ696"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A663" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21630,8 +21992,8 @@
       <c r="D3" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>74</v>
+      <c r="E3" s="227" t="s">
+        <v>214</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>186</v>
@@ -27591,12 +27953,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:IV151"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27657,8 +28019,8 @@
       <c r="D3" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>74</v>
+      <c r="E3" s="227" t="s">
+        <v>214</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>186</v>
@@ -28641,193 +29003,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="3" width="8.83203125" style="1"/>
-    <col min="4" max="4" width="32" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="1"/>
-    <col min="7" max="7" width="92.33203125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:AMJ38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28894,8 +29075,8 @@
       <c r="E3" s="222" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="221" t="s">
-        <v>74</v>
+      <c r="F3" s="227" t="s">
+        <v>214</v>
       </c>
       <c r="G3" s="221" t="s">
         <v>186</v>
@@ -41701,7 +41882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AMJ208"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="I2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -45035,7 +45216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMJ229"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T2" sqref="T2:T3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added changes from worked example
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherdavidson/Documents/Dev/hmcts/sscs/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E126649C-9346-DA4C-9B51-7A6147388A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD24B35-04DF-B240-A5C3-FB2AB3038703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="2840" windowWidth="24460" windowHeight="13900" tabRatio="500" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="2840" windowWidth="24460" windowHeight="13900" tabRatio="500" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -25,20 +25,21 @@
     <sheet name="SearchParty" sheetId="21" r:id="rId10"/>
     <sheet name="EventToComplexTypes" sheetId="10" r:id="rId11"/>
     <sheet name="SearchInputFields" sheetId="11" r:id="rId12"/>
-    <sheet name="SearchResultFields" sheetId="12" r:id="rId13"/>
-    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId14"/>
-    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId15"/>
-    <sheet name="UserProfile" sheetId="15" r:id="rId16"/>
-    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId17"/>
-    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId18"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId19"/>
-    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId20"/>
-    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId21"/>
+    <sheet name="RoleToAccessProfiles" sheetId="22" r:id="rId13"/>
+    <sheet name="SearchResultFields" sheetId="12" r:id="rId14"/>
+    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId15"/>
+    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId16"/>
+    <sheet name="UserProfile" sheetId="15" r:id="rId17"/>
+    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId18"/>
+    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId19"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId20"/>
+    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId21"/>
+    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId22"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$V$110</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$2:$L$98</definedName>
@@ -46,9 +47,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ComplexTypes!$A$3:$M$232</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">FixedLists!$A$1:$E$702</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">State!$A$3:$H$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="17">AuthorisationCaseField!$J$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="18">AuthorisationCaseField!$J$5</definedName>
     <definedName name="_xlnm.Extract" localSheetId="5">CaseTypeTab!$K$61</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="222">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -796,12 +797,33 @@
   <si>
     <t>SearchPartyDoD</t>
   </si>
+  <si>
+    <t>AccessProfile</t>
+  </si>
+  <si>
+    <t>RoleToAccessProfiles</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>Authorisation</t>
+  </si>
+  <si>
+    <t>ReadOnly</t>
+  </si>
+  <si>
+    <t>AccessProfiles</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1052,6 +1074,12 @@
       <sz val="14"/>
       <color rgb="FF172B4D"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1381,7 +1409,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="226">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1706,6 +1734,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2988,7 +3017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FC5E5D-C2A1-6040-955C-8FE864F39FBA}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -5301,6 +5330,55 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C78A949-D428-3D49-A8A3-A7455BA3C545}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="225"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="226" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F3" t="s">
+        <v>220</v>
+      </c>
+      <c r="G3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
@@ -5603,7 +5681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I91"/>
   <sheetViews>
@@ -6275,7 +6353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
@@ -6746,7 +6824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
@@ -7413,7 +7491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:IV35"/>
   <sheetViews>
@@ -7473,7 +7551,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="224" t="s">
-        <v>74</v>
+        <v>215</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>195</v>
@@ -7637,7 +7715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMJ1015"/>
   <sheetViews>
@@ -7704,7 +7782,7 @@
         <v>78</v>
       </c>
       <c r="E3" s="224" t="s">
-        <v>74</v>
+        <v>215</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>195</v>
@@ -21657,12 +21735,193 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="32" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="92.33203125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AMJ696"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21744,7 +22003,7 @@
         <v>138</v>
       </c>
       <c r="E3" s="224" t="s">
-        <v>74</v>
+        <v>215</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>195</v>
@@ -27704,188 +27963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I10"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="3" width="8.83203125" style="1"/>
-    <col min="4" max="4" width="32" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="1"/>
-    <col min="7" max="7" width="92.33203125" style="1" customWidth="1"/>
-    <col min="8" max="9" width="8.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:IV151"/>
   <sheetViews>
@@ -27952,7 +28030,7 @@
         <v>203</v>
       </c>
       <c r="E3" s="224" t="s">
-        <v>74</v>
+        <v>215</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>195</v>
@@ -28935,7 +29013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:AMJ38"/>
   <sheetViews>
@@ -29008,7 +29086,7 @@
         <v>57</v>
       </c>
       <c r="F3" s="224" t="s">
-        <v>74</v>
+        <v>215</v>
       </c>
       <c r="G3" s="220" t="s">
         <v>195</v>

</xml_diff>

<commit_message>
sscs 10317 added filters
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherdavidson/Documents/Dev/hmcts/sscs/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FEFE98-FC85-2E44-A096-A457F592A88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B71218-6DAC-204F-9BF8-31F4764791D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="2840" windowWidth="24460" windowHeight="13900" tabRatio="500" firstSheet="17" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="2840" windowWidth="24460" windowHeight="13900" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -22,35 +22,36 @@
     <sheet name="State" sheetId="7" r:id="rId7"/>
     <sheet name="CaseEvent" sheetId="8" r:id="rId8"/>
     <sheet name="CaseRoles" sheetId="23" r:id="rId9"/>
-    <sheet name="RoleToAccessProfiles" sheetId="22" r:id="rId10"/>
-    <sheet name="CaseEventToFields" sheetId="9" r:id="rId11"/>
-    <sheet name="SearchParty" sheetId="21" r:id="rId12"/>
-    <sheet name="EventToComplexTypes" sheetId="10" r:id="rId13"/>
-    <sheet name="SearchInputFields" sheetId="11" r:id="rId14"/>
-    <sheet name="SearchResultFields" sheetId="12" r:id="rId15"/>
-    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId16"/>
-    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId17"/>
-    <sheet name="UserProfile" sheetId="15" r:id="rId18"/>
-    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId19"/>
-    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId20"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId21"/>
-    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId22"/>
-    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId23"/>
+    <sheet name="RoleAccess" sheetId="24" r:id="rId10"/>
+    <sheet name="RoleToAccessProfiles" sheetId="22" r:id="rId11"/>
+    <sheet name="CaseEventToFields" sheetId="9" r:id="rId12"/>
+    <sheet name="SearchParty" sheetId="21" r:id="rId13"/>
+    <sheet name="EventToComplexTypes" sheetId="10" r:id="rId14"/>
+    <sheet name="SearchInputFields" sheetId="11" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="12" r:id="rId16"/>
+    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId17"/>
+    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId18"/>
+    <sheet name="UserProfile" sheetId="15" r:id="rId19"/>
+    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId20"/>
+    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId21"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId22"/>
+    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId23"/>
+    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$V$110</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$2:$L$98</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">CaseTypeTab!$H$58:$H$70</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ComplexTypes!$A$3:$M$232</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">FixedLists!$A$1:$E$702</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">State!$A$3:$H$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="19">AuthorisationCaseField!$J$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="20">AuthorisationCaseField!$J$5</definedName>
     <definedName name="_xlnm.Extract" localSheetId="5">CaseTypeTab!$K$61</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="225">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -822,12 +823,18 @@
   <si>
     <t>AccessProfile</t>
   </si>
+  <si>
+    <t>CaseAccessCategory</t>
+  </si>
+  <si>
+    <t>RoleAccess</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1078,6 +1085,11 @@
       <sz val="14"/>
       <color rgb="FF172B4D"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1407,7 +1419,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="226">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1732,6 +1744,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3011,10 +3024,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC9A68F-9D85-C640-9E0E-68D94EA93DB9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0DA8B8-A74A-274B-AB87-18953DC1F7CC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -3024,8 +3037,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>215</v>
+      <c r="A1" s="226" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3045,13 +3058,13 @@
         <v>217</v>
       </c>
       <c r="E3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F3" t="s">
         <v>218</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>219</v>
-      </c>
-      <c r="G3" t="s">
-        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3060,6 +3073,61 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC9A68F-9D85-C640-9E0E-68D94EA93DB9}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="225"/>
+    <col min="3" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F3" t="s">
+        <v>218</v>
+      </c>
+      <c r="G3" t="s">
+        <v>219</v>
+      </c>
+      <c r="H3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMJ229"/>
   <sheetViews>
@@ -5596,7 +5664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FC5E5D-C2A1-6040-955C-8FE864F39FBA}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -5648,7 +5716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
@@ -5795,7 +5863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I573"/>
   <sheetViews>
@@ -7912,7 +7980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
@@ -8215,7 +8283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I91"/>
   <sheetViews>
@@ -8887,7 +8955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
@@ -9358,7 +9426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
@@ -10025,230 +10093,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:IV35"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="1"/>
-    <col min="3" max="3" width="24.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" style="1" customWidth="1"/>
-    <col min="5" max="256" width="8.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="224" t="s">
-        <v>222</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-    </row>
-    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-    </row>
-    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
-    </row>
-    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-    </row>
-    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
-    </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-    </row>
-    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-    </row>
-    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
-    </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-    </row>
-    <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-    </row>
-    <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
-    </row>
-    <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24"/>
-      <c r="B27" s="24"/>
-    </row>
-    <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24"/>
-    </row>
-    <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-    </row>
-    <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-    </row>
-    <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
-    </row>
-    <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
-    </row>
-    <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-    </row>
-    <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
-    </row>
-    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I10"/>
@@ -10431,6 +10275,230 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:IV35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="24.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" style="1" customWidth="1"/>
+    <col min="5" max="256" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="224" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+    </row>
+    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+    </row>
+    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+    </row>
+    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+    </row>
+    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+    </row>
+    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+    </row>
+    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+    </row>
+    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+    </row>
+    <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+    </row>
+    <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+    </row>
+    <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+    </row>
+    <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+    </row>
+    <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+    </row>
+    <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+    </row>
+    <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+    </row>
+    <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+    </row>
+    <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+    </row>
+    <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="24"/>
+      <c r="B34" s="24"/>
+    </row>
+    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="24"/>
+      <c r="B35" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMJ1015"/>
   <sheetViews>
@@ -24450,7 +24518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AMJ696"/>
   <sheetViews>
@@ -30497,7 +30565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:IV151"/>
   <sheetViews>
@@ -31547,11 +31615,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:AMJ38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sscs 10317 working config
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherdavidson/Documents/Dev/hmcts/sscs/sscs-ccd-definitions/benefit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B71218-6DAC-204F-9BF8-31F4764791D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC90A1FE-6398-1E49-BAE5-EE01353010BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="2840" windowWidth="24460" windowHeight="13900" tabRatio="500" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,36 +22,35 @@
     <sheet name="State" sheetId="7" r:id="rId7"/>
     <sheet name="CaseEvent" sheetId="8" r:id="rId8"/>
     <sheet name="CaseRoles" sheetId="23" r:id="rId9"/>
-    <sheet name="RoleAccess" sheetId="24" r:id="rId10"/>
-    <sheet name="RoleToAccessProfiles" sheetId="22" r:id="rId11"/>
-    <sheet name="CaseEventToFields" sheetId="9" r:id="rId12"/>
-    <sheet name="SearchParty" sheetId="21" r:id="rId13"/>
-    <sheet name="EventToComplexTypes" sheetId="10" r:id="rId14"/>
-    <sheet name="SearchInputFields" sheetId="11" r:id="rId15"/>
-    <sheet name="SearchResultFields" sheetId="12" r:id="rId16"/>
-    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId17"/>
-    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId18"/>
-    <sheet name="UserProfile" sheetId="15" r:id="rId19"/>
-    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId20"/>
-    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId21"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId22"/>
-    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId23"/>
-    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId24"/>
+    <sheet name="RoleToAccessProfiles" sheetId="22" r:id="rId10"/>
+    <sheet name="CaseEventToFields" sheetId="9" r:id="rId11"/>
+    <sheet name="SearchParty" sheetId="21" r:id="rId12"/>
+    <sheet name="EventToComplexTypes" sheetId="10" r:id="rId13"/>
+    <sheet name="SearchInputFields" sheetId="11" r:id="rId14"/>
+    <sheet name="SearchResultFields" sheetId="12" r:id="rId15"/>
+    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId16"/>
+    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId17"/>
+    <sheet name="UserProfile" sheetId="15" r:id="rId18"/>
+    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId19"/>
+    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId20"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId21"/>
+    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId22"/>
+    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId23"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$V$110</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$2:$L$98</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">CaseTypeTab!$H$58:$H$70</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ComplexTypes!$A$3:$M$232</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">FixedLists!$A$1:$E$702</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">State!$A$3:$H$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="20">AuthorisationCaseField!$J$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="19">AuthorisationCaseField!$J$5</definedName>
     <definedName name="_xlnm.Extract" localSheetId="5">CaseTypeTab!$K$61</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
@@ -64,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="224">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -824,10 +823,7 @@
     <t>AccessProfile</t>
   </si>
   <si>
-    <t>CaseAccessCategory</t>
-  </si>
-  <si>
-    <t>RoleAccess</t>
+    <t>CaseAccessCategories</t>
   </si>
 </sst>
 </file>
@@ -3024,59 +3020,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0DA8B8-A74A-274B-AB87-18953DC1F7CC}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="225"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="226" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F3" t="s">
-        <v>218</v>
-      </c>
-      <c r="G3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC9A68F-9D85-C640-9E0E-68D94EA93DB9}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -3106,7 +3053,7 @@
       <c r="C3" t="s">
         <v>216</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="226" t="s">
         <v>223</v>
       </c>
       <c r="E3" t="s">
@@ -3127,7 +3074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMJ229"/>
   <sheetViews>
@@ -5664,7 +5611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FC5E5D-C2A1-6040-955C-8FE864F39FBA}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -5716,7 +5663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
@@ -5863,7 +5810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I573"/>
   <sheetViews>
@@ -7980,7 +7927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
@@ -8283,7 +8230,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I91"/>
   <sheetViews>
@@ -8955,7 +8902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
@@ -9426,7 +9373,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
@@ -10093,6 +10040,230 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:IV35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="24.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" style="1" customWidth="1"/>
+    <col min="5" max="256" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="224" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+    </row>
+    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+    </row>
+    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+    </row>
+    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+    </row>
+    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+    </row>
+    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+    </row>
+    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+    </row>
+    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+    </row>
+    <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+    </row>
+    <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+    </row>
+    <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+    </row>
+    <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+    </row>
+    <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+    </row>
+    <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+    </row>
+    <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+    </row>
+    <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+    </row>
+    <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+    </row>
+    <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="24"/>
+      <c r="B34" s="24"/>
+    </row>
+    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="24"/>
+      <c r="B35" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I10"/>
@@ -10275,230 +10446,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:IV35"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="1"/>
-    <col min="3" max="3" width="24.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" style="1" customWidth="1"/>
-    <col min="5" max="256" width="8.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="224" t="s">
-        <v>222</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-    </row>
-    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-    </row>
-    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
-    </row>
-    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-    </row>
-    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
-    </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-    </row>
-    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-    </row>
-    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
-    </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-    </row>
-    <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-    </row>
-    <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
-    </row>
-    <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="24"/>
-      <c r="B27" s="24"/>
-    </row>
-    <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24"/>
-    </row>
-    <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-    </row>
-    <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-    </row>
-    <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
-    </row>
-    <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
-    </row>
-    <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-    </row>
-    <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
-    </row>
-    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMJ1015"/>
   <sheetViews>
@@ -24518,7 +24465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AMJ696"/>
   <sheetViews>
@@ -30565,7 +30512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:IV151"/>
   <sheetViews>
@@ -31615,7 +31562,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:AMJ38"/>
   <sheetViews>

</xml_diff>

<commit_message>
SSCS-9939 - Ensure AccessProfile replacing all instances of UserRole
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\gordond\hmcts\sscs-ccd-definitions\benefit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C257CCDB-C376-4AD6-874E-B16AFA0C59BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E177FC6-0E21-43FB-A71B-57C68C1DDFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="791" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="791" firstSheet="10" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="223">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -816,9 +816,6 @@
   </si>
   <si>
     <t>AccessProfile</t>
-  </si>
-  <si>
-    <t>UserRole</t>
   </si>
 </sst>
 </file>
@@ -3007,7 +3004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62122A5-518A-4E9D-8EA5-3552B28CB978}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -3351,7 +3348,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>77</v>
@@ -3651,7 +3648,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>77</v>
@@ -5703,7 +5700,7 @@
   <dimension ref="A1:I91"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -5765,7 +5762,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>77</v>
@@ -6371,8 +6368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -6438,7 +6435,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
SSCS-11324 - Update ccd-template to use correct formatting date type
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\gordond\hmcts\sscs-ccd-definitions\benefit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36724BB5-C72A-4FE1-8E19-955F00B921F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C558668-988E-4968-8D45-E474B29035F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="785" firstSheet="19" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="785" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -3133,8 +3133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
@@ -3283,13 +3283,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I573"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="1" max="1" width="34" style="7" customWidth="1"/>
     <col min="4" max="4" width="32.44140625" customWidth="1"/>
     <col min="5" max="6" width="36.109375" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
@@ -5386,7 +5386,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
@@ -5397,13 +5397,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="15" style="7" customWidth="1"/>
     <col min="4" max="4" width="32.44140625" customWidth="1"/>
     <col min="5" max="6" width="41.44140625" customWidth="1"/>
     <col min="7" max="7" width="29.109375" customWidth="1"/>
@@ -5695,10 +5695,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" topLeftCell="A104" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91:B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -6351,6 +6351,166 @@
     <row r="91" spans="1:2" ht="15" customHeight="1">
       <c r="A91" s="12"/>
       <c r="B91" s="12"/>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="12"/>
+      <c r="B92" s="12"/>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="12"/>
+      <c r="B93" s="12"/>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="12"/>
+      <c r="B94" s="12"/>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="12"/>
+      <c r="B95" s="12"/>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="12"/>
+      <c r="B96" s="12"/>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="12"/>
+      <c r="B97" s="12"/>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="12"/>
+      <c r="B98" s="12"/>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="12"/>
+      <c r="B99" s="12"/>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="12"/>
+      <c r="B100" s="12"/>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="12"/>
+      <c r="B101" s="12"/>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="12"/>
+      <c r="B102" s="12"/>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="12"/>
+      <c r="B103" s="12"/>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="12"/>
+      <c r="B104" s="12"/>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="12"/>
+      <c r="B105" s="12"/>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="12"/>
+      <c r="B106" s="12"/>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="12"/>
+      <c r="B107" s="12"/>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="12"/>
+      <c r="B108" s="12"/>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="12"/>
+      <c r="B109" s="12"/>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="12"/>
+      <c r="B110" s="12"/>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="12"/>
+      <c r="B111" s="12"/>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="12"/>
+      <c r="B112" s="12"/>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="12"/>
+      <c r="B113" s="12"/>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="12"/>
+      <c r="B114" s="12"/>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="12"/>
+      <c r="B115" s="12"/>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="12"/>
+      <c r="B116" s="12"/>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="12"/>
+      <c r="B117" s="12"/>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="12"/>
+      <c r="B118" s="12"/>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="12"/>
+      <c r="B119" s="12"/>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="12"/>
+      <c r="B120" s="12"/>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="12"/>
+      <c r="B121" s="12"/>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="12"/>
+      <c r="B122" s="12"/>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="12"/>
+      <c r="B123" s="12"/>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="12"/>
+      <c r="B124" s="12"/>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="12"/>
+      <c r="B125" s="12"/>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="12"/>
+      <c r="B126" s="12"/>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="12"/>
+      <c r="B127" s="12"/>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="12"/>
+      <c r="B128" s="12"/>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="12"/>
+      <c r="B129" s="12"/>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="12"/>
+      <c r="B130" s="12"/>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="12"/>
+      <c r="B131" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:H30" xr:uid="{00000000-0009-0000-0000-00000C000000}"/>
@@ -20656,7 +20816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AMJ696"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
SSCS-11531 - Update template for merged rows in AuthCaseField sheet
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\gordond\hmcts\sscs-ccd-definitions\benefit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C558668-988E-4968-8D45-E474B29035F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1545CE49-7BAE-4A67-BAD6-BC61197D77A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="785" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="785" firstSheet="13" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -1407,7 +1407,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1681,9 +1681,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -2975,24 +2973,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="177" t="s">
+      <c r="A1" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="177" t="s">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="177" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="177" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="177" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3025,46 +3020,30 @@
       <c r="A1" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="B2" s="175"/>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="175" t="s">
+      <c r="B3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="175" t="s">
+      <c r="C3" t="s">
         <v>216</v>
       </c>
-      <c r="D3" s="176" t="s">
+      <c r="D3" s="175" t="s">
         <v>217</v>
       </c>
-      <c r="E3" s="175" t="s">
+      <c r="E3" t="s">
         <v>218</v>
       </c>
-      <c r="F3" s="175" t="s">
+      <c r="F3" t="s">
         <v>219</v>
       </c>
-      <c r="G3" s="175" t="s">
+      <c r="G3" t="s">
         <v>220</v>
       </c>
-      <c r="H3" s="175" t="s">
+      <c r="H3" t="s">
         <v>221</v>
       </c>
     </row>
@@ -3283,7 +3262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I573"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
@@ -7712,7 +7691,7 @@
       <c r="C3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="178" t="s">
+      <c r="D3" s="176" t="s">
         <v>214</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -8057,10 +8036,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:AMJ1015"/>
+  <dimension ref="A1:AMJ1109"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1072" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1015" sqref="A999:XFD1109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -8121,7 +8100,7 @@
       <c r="D3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="178" t="s">
+      <c r="E3" s="176" t="s">
         <v>214</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -20579,54 +20558,724 @@
       <c r="D1008" s="11"/>
       <c r="E1008" s="9"/>
     </row>
-    <row r="1009" spans="1:5" ht="15" customHeight="1">
+    <row r="1009" spans="1:6" ht="15" customHeight="1">
       <c r="A1009" s="12"/>
       <c r="B1009" s="11"/>
       <c r="C1009" s="9"/>
       <c r="D1009" s="11"/>
       <c r="E1009" s="9"/>
     </row>
-    <row r="1010" spans="1:5" ht="15" customHeight="1">
+    <row r="1010" spans="1:6" ht="15" customHeight="1">
       <c r="A1010" s="12"/>
       <c r="B1010" s="11"/>
       <c r="C1010" s="9"/>
       <c r="D1010" s="11"/>
       <c r="E1010" s="9"/>
     </row>
-    <row r="1011" spans="1:5" ht="15" customHeight="1">
+    <row r="1011" spans="1:6" ht="15" customHeight="1">
       <c r="A1011" s="12"/>
       <c r="B1011" s="11"/>
       <c r="C1011" s="9"/>
       <c r="D1011" s="11"/>
       <c r="E1011" s="9"/>
     </row>
-    <row r="1012" spans="1:5" ht="15" customHeight="1">
+    <row r="1012" spans="1:6" ht="15" customHeight="1">
       <c r="A1012" s="11"/>
       <c r="B1012" s="11"/>
       <c r="C1012" s="11"/>
       <c r="D1012" s="12"/>
       <c r="E1012" s="9"/>
     </row>
-    <row r="1013" spans="1:5" ht="15" customHeight="1">
+    <row r="1013" spans="1:6" ht="15" customHeight="1">
       <c r="A1013" s="11"/>
       <c r="B1013" s="11"/>
       <c r="C1013" s="11"/>
       <c r="D1013" s="9"/>
       <c r="E1013" s="9"/>
     </row>
-    <row r="1014" spans="1:5" ht="15" customHeight="1">
+    <row r="1014" spans="1:6" ht="15" customHeight="1">
       <c r="A1014" s="11"/>
       <c r="B1014" s="11"/>
       <c r="C1014" s="11"/>
       <c r="D1014" s="11"/>
       <c r="E1014" s="9"/>
     </row>
-    <row r="1015" spans="1:5" ht="15" customHeight="1">
+    <row r="1015" spans="1:6" ht="15" customHeight="1">
       <c r="A1015" s="11"/>
       <c r="B1015" s="11"/>
       <c r="C1015" s="11"/>
       <c r="D1015" s="12"/>
       <c r="E1015" s="9"/>
+    </row>
+    <row r="1016" spans="1:6" ht="15" customHeight="1">
+      <c r="A1016" s="12"/>
+      <c r="B1016" s="11"/>
+      <c r="C1016" s="9"/>
+      <c r="D1016" s="11"/>
+      <c r="E1016" s="9"/>
+    </row>
+    <row r="1017" spans="1:6" ht="15" customHeight="1">
+      <c r="A1017" s="12"/>
+      <c r="B1017" s="11"/>
+      <c r="C1017" s="9"/>
+      <c r="D1017" s="11"/>
+      <c r="E1017" s="9"/>
+    </row>
+    <row r="1018" spans="1:6" ht="15" customHeight="1">
+      <c r="A1018" s="12"/>
+      <c r="B1018" s="11"/>
+      <c r="C1018" s="9"/>
+      <c r="D1018" s="9"/>
+      <c r="E1018" s="9"/>
+      <c r="F1018" s="15"/>
+    </row>
+    <row r="1019" spans="1:6" ht="15" customHeight="1">
+      <c r="A1019" s="12"/>
+      <c r="B1019" s="11"/>
+      <c r="C1019" s="9"/>
+      <c r="D1019" s="11"/>
+      <c r="E1019" s="9"/>
+    </row>
+    <row r="1020" spans="1:6" ht="15" customHeight="1">
+      <c r="A1020" s="12"/>
+      <c r="B1020" s="11"/>
+      <c r="C1020" s="9"/>
+      <c r="D1020" s="11"/>
+      <c r="E1020" s="9"/>
+    </row>
+    <row r="1021" spans="1:6" ht="15" customHeight="1">
+      <c r="A1021" s="12"/>
+      <c r="B1021" s="11"/>
+      <c r="C1021" s="9"/>
+      <c r="D1021" s="11"/>
+      <c r="E1021" s="9"/>
+    </row>
+    <row r="1022" spans="1:6" ht="15" customHeight="1">
+      <c r="A1022" s="12"/>
+      <c r="B1022" s="11"/>
+      <c r="C1022" s="9"/>
+      <c r="D1022" s="156"/>
+      <c r="E1022" s="9"/>
+      <c r="F1022" s="149"/>
+    </row>
+    <row r="1023" spans="1:6" ht="15" customHeight="1">
+      <c r="A1023" s="12"/>
+      <c r="B1023" s="11"/>
+      <c r="C1023" s="9"/>
+      <c r="D1023" s="11"/>
+      <c r="E1023" s="9"/>
+    </row>
+    <row r="1024" spans="1:6" ht="15" customHeight="1">
+      <c r="A1024" s="12"/>
+      <c r="B1024" s="11"/>
+      <c r="C1024" s="9"/>
+      <c r="D1024" s="11"/>
+      <c r="E1024" s="9"/>
+    </row>
+    <row r="1025" spans="1:6" ht="15" customHeight="1">
+      <c r="A1025" s="12"/>
+      <c r="B1025" s="11"/>
+      <c r="C1025" s="9"/>
+      <c r="D1025" s="11"/>
+      <c r="E1025" s="9"/>
+    </row>
+    <row r="1026" spans="1:6" ht="15" customHeight="1">
+      <c r="A1026" s="12"/>
+      <c r="B1026" s="11"/>
+      <c r="C1026" s="9"/>
+      <c r="D1026" s="11"/>
+      <c r="E1026" s="9"/>
+    </row>
+    <row r="1027" spans="1:6" ht="15" customHeight="1">
+      <c r="A1027" s="12"/>
+      <c r="B1027" s="11"/>
+      <c r="C1027" s="9"/>
+      <c r="D1027" s="11"/>
+      <c r="E1027" s="9"/>
+    </row>
+    <row r="1028" spans="1:6" ht="15" customHeight="1">
+      <c r="A1028" s="12"/>
+      <c r="B1028" s="11"/>
+      <c r="C1028" s="9"/>
+      <c r="D1028" s="11"/>
+      <c r="E1028" s="9"/>
+    </row>
+    <row r="1029" spans="1:6" ht="15" customHeight="1">
+      <c r="A1029" s="11"/>
+      <c r="B1029" s="11"/>
+      <c r="C1029" s="11"/>
+      <c r="D1029" s="12"/>
+      <c r="E1029" s="9"/>
+    </row>
+    <row r="1030" spans="1:6" ht="15" customHeight="1">
+      <c r="A1030" s="11"/>
+      <c r="B1030" s="11"/>
+      <c r="C1030" s="11"/>
+      <c r="D1030" s="9"/>
+      <c r="E1030" s="9"/>
+    </row>
+    <row r="1031" spans="1:6" ht="15" customHeight="1">
+      <c r="A1031" s="11"/>
+      <c r="B1031" s="11"/>
+      <c r="C1031" s="11"/>
+      <c r="D1031" s="11"/>
+      <c r="E1031" s="9"/>
+    </row>
+    <row r="1032" spans="1:6" ht="15" customHeight="1">
+      <c r="A1032" s="11"/>
+      <c r="B1032" s="11"/>
+      <c r="C1032" s="11"/>
+      <c r="D1032" s="12"/>
+      <c r="E1032" s="9"/>
+    </row>
+    <row r="1033" spans="1:6" ht="15" customHeight="1">
+      <c r="A1033" s="12"/>
+      <c r="B1033" s="11"/>
+      <c r="C1033" s="9"/>
+      <c r="D1033" s="11"/>
+      <c r="E1033" s="9"/>
+    </row>
+    <row r="1034" spans="1:6" ht="15" customHeight="1">
+      <c r="A1034" s="12"/>
+      <c r="B1034" s="11"/>
+      <c r="C1034" s="9"/>
+      <c r="D1034" s="11"/>
+      <c r="E1034" s="9"/>
+    </row>
+    <row r="1035" spans="1:6" ht="15" customHeight="1">
+      <c r="A1035" s="12"/>
+      <c r="B1035" s="11"/>
+      <c r="C1035" s="9"/>
+      <c r="D1035" s="9"/>
+      <c r="E1035" s="9"/>
+      <c r="F1035" s="15"/>
+    </row>
+    <row r="1036" spans="1:6" ht="15" customHeight="1">
+      <c r="A1036" s="12"/>
+      <c r="B1036" s="11"/>
+      <c r="C1036" s="9"/>
+      <c r="D1036" s="11"/>
+      <c r="E1036" s="9"/>
+    </row>
+    <row r="1037" spans="1:6" ht="15" customHeight="1">
+      <c r="A1037" s="12"/>
+      <c r="B1037" s="11"/>
+      <c r="C1037" s="9"/>
+      <c r="D1037" s="11"/>
+      <c r="E1037" s="9"/>
+    </row>
+    <row r="1038" spans="1:6" ht="15" customHeight="1">
+      <c r="A1038" s="12"/>
+      <c r="B1038" s="11"/>
+      <c r="C1038" s="9"/>
+      <c r="D1038" s="11"/>
+      <c r="E1038" s="9"/>
+    </row>
+    <row r="1039" spans="1:6" ht="15" customHeight="1">
+      <c r="A1039" s="12"/>
+      <c r="B1039" s="11"/>
+      <c r="C1039" s="9"/>
+      <c r="D1039" s="156"/>
+      <c r="E1039" s="9"/>
+      <c r="F1039" s="149"/>
+    </row>
+    <row r="1040" spans="1:6" ht="15" customHeight="1">
+      <c r="A1040" s="12"/>
+      <c r="B1040" s="11"/>
+      <c r="C1040" s="9"/>
+      <c r="D1040" s="11"/>
+      <c r="E1040" s="9"/>
+    </row>
+    <row r="1041" spans="1:6" ht="15" customHeight="1">
+      <c r="A1041" s="12"/>
+      <c r="B1041" s="11"/>
+      <c r="C1041" s="9"/>
+      <c r="D1041" s="11"/>
+      <c r="E1041" s="9"/>
+    </row>
+    <row r="1042" spans="1:6" ht="15" customHeight="1">
+      <c r="A1042" s="12"/>
+      <c r="B1042" s="11"/>
+      <c r="C1042" s="9"/>
+      <c r="D1042" s="11"/>
+      <c r="E1042" s="9"/>
+    </row>
+    <row r="1043" spans="1:6" ht="15" customHeight="1">
+      <c r="A1043" s="12"/>
+      <c r="B1043" s="11"/>
+      <c r="C1043" s="9"/>
+      <c r="D1043" s="11"/>
+      <c r="E1043" s="9"/>
+    </row>
+    <row r="1044" spans="1:6" ht="15" customHeight="1">
+      <c r="A1044" s="12"/>
+      <c r="B1044" s="11"/>
+      <c r="C1044" s="9"/>
+      <c r="D1044" s="11"/>
+      <c r="E1044" s="9"/>
+    </row>
+    <row r="1045" spans="1:6" ht="15" customHeight="1">
+      <c r="A1045" s="12"/>
+      <c r="B1045" s="11"/>
+      <c r="C1045" s="9"/>
+      <c r="D1045" s="11"/>
+      <c r="E1045" s="9"/>
+    </row>
+    <row r="1046" spans="1:6" ht="15" customHeight="1">
+      <c r="A1046" s="11"/>
+      <c r="B1046" s="11"/>
+      <c r="C1046" s="11"/>
+      <c r="D1046" s="12"/>
+      <c r="E1046" s="9"/>
+    </row>
+    <row r="1047" spans="1:6" ht="15" customHeight="1">
+      <c r="A1047" s="11"/>
+      <c r="B1047" s="11"/>
+      <c r="C1047" s="11"/>
+      <c r="D1047" s="9"/>
+      <c r="E1047" s="9"/>
+    </row>
+    <row r="1048" spans="1:6" ht="15" customHeight="1">
+      <c r="A1048" s="11"/>
+      <c r="B1048" s="11"/>
+      <c r="C1048" s="11"/>
+      <c r="D1048" s="11"/>
+      <c r="E1048" s="9"/>
+    </row>
+    <row r="1049" spans="1:6" ht="15" customHeight="1">
+      <c r="A1049" s="11"/>
+      <c r="B1049" s="11"/>
+      <c r="C1049" s="11"/>
+      <c r="D1049" s="12"/>
+      <c r="E1049" s="9"/>
+    </row>
+    <row r="1050" spans="1:6" ht="15" customHeight="1">
+      <c r="A1050" s="12"/>
+      <c r="B1050" s="11"/>
+      <c r="C1050" s="9"/>
+      <c r="D1050" s="11"/>
+      <c r="E1050" s="9"/>
+    </row>
+    <row r="1051" spans="1:6" ht="15" customHeight="1">
+      <c r="A1051" s="12"/>
+      <c r="B1051" s="11"/>
+      <c r="C1051" s="9"/>
+      <c r="D1051" s="11"/>
+      <c r="E1051" s="9"/>
+    </row>
+    <row r="1052" spans="1:6" ht="15" customHeight="1">
+      <c r="A1052" s="12"/>
+      <c r="B1052" s="11"/>
+      <c r="C1052" s="9"/>
+      <c r="D1052" s="9"/>
+      <c r="E1052" s="9"/>
+      <c r="F1052" s="15"/>
+    </row>
+    <row r="1053" spans="1:6" ht="15" customHeight="1">
+      <c r="A1053" s="12"/>
+      <c r="B1053" s="11"/>
+      <c r="C1053" s="9"/>
+      <c r="D1053" s="11"/>
+      <c r="E1053" s="9"/>
+    </row>
+    <row r="1054" spans="1:6" ht="15" customHeight="1">
+      <c r="A1054" s="12"/>
+      <c r="B1054" s="11"/>
+      <c r="C1054" s="9"/>
+      <c r="D1054" s="11"/>
+      <c r="E1054" s="9"/>
+    </row>
+    <row r="1055" spans="1:6" ht="15" customHeight="1">
+      <c r="A1055" s="12"/>
+      <c r="B1055" s="11"/>
+      <c r="C1055" s="9"/>
+      <c r="D1055" s="11"/>
+      <c r="E1055" s="9"/>
+    </row>
+    <row r="1056" spans="1:6" ht="15" customHeight="1">
+      <c r="A1056" s="12"/>
+      <c r="B1056" s="11"/>
+      <c r="C1056" s="9"/>
+      <c r="D1056" s="156"/>
+      <c r="E1056" s="9"/>
+      <c r="F1056" s="149"/>
+    </row>
+    <row r="1057" spans="1:6" ht="15" customHeight="1">
+      <c r="A1057" s="12"/>
+      <c r="B1057" s="11"/>
+      <c r="C1057" s="9"/>
+      <c r="D1057" s="11"/>
+      <c r="E1057" s="9"/>
+    </row>
+    <row r="1058" spans="1:6" ht="15" customHeight="1">
+      <c r="A1058" s="12"/>
+      <c r="B1058" s="11"/>
+      <c r="C1058" s="9"/>
+      <c r="D1058" s="11"/>
+      <c r="E1058" s="9"/>
+    </row>
+    <row r="1059" spans="1:6" ht="15" customHeight="1">
+      <c r="A1059" s="12"/>
+      <c r="B1059" s="11"/>
+      <c r="C1059" s="9"/>
+      <c r="D1059" s="11"/>
+      <c r="E1059" s="9"/>
+    </row>
+    <row r="1060" spans="1:6" ht="15" customHeight="1">
+      <c r="A1060" s="12"/>
+      <c r="B1060" s="11"/>
+      <c r="C1060" s="9"/>
+      <c r="D1060" s="11"/>
+      <c r="E1060" s="9"/>
+    </row>
+    <row r="1061" spans="1:6" ht="15" customHeight="1">
+      <c r="A1061" s="12"/>
+      <c r="B1061" s="11"/>
+      <c r="C1061" s="9"/>
+      <c r="D1061" s="11"/>
+      <c r="E1061" s="9"/>
+    </row>
+    <row r="1062" spans="1:6" ht="15" customHeight="1">
+      <c r="A1062" s="12"/>
+      <c r="B1062" s="11"/>
+      <c r="C1062" s="9"/>
+      <c r="D1062" s="11"/>
+      <c r="E1062" s="9"/>
+    </row>
+    <row r="1063" spans="1:6" ht="15" customHeight="1">
+      <c r="A1063" s="11"/>
+      <c r="B1063" s="11"/>
+      <c r="C1063" s="11"/>
+      <c r="D1063" s="12"/>
+      <c r="E1063" s="9"/>
+    </row>
+    <row r="1064" spans="1:6" ht="15" customHeight="1">
+      <c r="A1064" s="11"/>
+      <c r="B1064" s="11"/>
+      <c r="C1064" s="11"/>
+      <c r="D1064" s="9"/>
+      <c r="E1064" s="9"/>
+    </row>
+    <row r="1065" spans="1:6" ht="15" customHeight="1">
+      <c r="A1065" s="11"/>
+      <c r="B1065" s="11"/>
+      <c r="C1065" s="11"/>
+      <c r="D1065" s="11"/>
+      <c r="E1065" s="9"/>
+    </row>
+    <row r="1066" spans="1:6" ht="15" customHeight="1">
+      <c r="A1066" s="11"/>
+      <c r="B1066" s="11"/>
+      <c r="C1066" s="11"/>
+      <c r="D1066" s="12"/>
+      <c r="E1066" s="9"/>
+    </row>
+    <row r="1067" spans="1:6" ht="15" customHeight="1">
+      <c r="A1067" s="12"/>
+      <c r="B1067" s="11"/>
+      <c r="C1067" s="9"/>
+      <c r="D1067" s="11"/>
+      <c r="E1067" s="9"/>
+    </row>
+    <row r="1068" spans="1:6" ht="15" customHeight="1">
+      <c r="A1068" s="12"/>
+      <c r="B1068" s="11"/>
+      <c r="C1068" s="9"/>
+      <c r="D1068" s="11"/>
+      <c r="E1068" s="9"/>
+    </row>
+    <row r="1069" spans="1:6" ht="15" customHeight="1">
+      <c r="A1069" s="12"/>
+      <c r="B1069" s="11"/>
+      <c r="C1069" s="9"/>
+      <c r="D1069" s="9"/>
+      <c r="E1069" s="9"/>
+      <c r="F1069" s="15"/>
+    </row>
+    <row r="1070" spans="1:6" ht="15" customHeight="1">
+      <c r="A1070" s="12"/>
+      <c r="B1070" s="11"/>
+      <c r="C1070" s="9"/>
+      <c r="D1070" s="11"/>
+      <c r="E1070" s="9"/>
+    </row>
+    <row r="1071" spans="1:6" ht="15" customHeight="1">
+      <c r="A1071" s="12"/>
+      <c r="B1071" s="11"/>
+      <c r="C1071" s="9"/>
+      <c r="D1071" s="11"/>
+      <c r="E1071" s="9"/>
+    </row>
+    <row r="1072" spans="1:6" ht="15" customHeight="1">
+      <c r="A1072" s="12"/>
+      <c r="B1072" s="11"/>
+      <c r="C1072" s="9"/>
+      <c r="D1072" s="11"/>
+      <c r="E1072" s="9"/>
+    </row>
+    <row r="1073" spans="1:6" ht="15" customHeight="1">
+      <c r="A1073" s="12"/>
+      <c r="B1073" s="11"/>
+      <c r="C1073" s="9"/>
+      <c r="D1073" s="156"/>
+      <c r="E1073" s="9"/>
+      <c r="F1073" s="149"/>
+    </row>
+    <row r="1074" spans="1:6" ht="15" customHeight="1">
+      <c r="A1074" s="12"/>
+      <c r="B1074" s="11"/>
+      <c r="C1074" s="9"/>
+      <c r="D1074" s="11"/>
+      <c r="E1074" s="9"/>
+    </row>
+    <row r="1075" spans="1:6" ht="15" customHeight="1">
+      <c r="A1075" s="12"/>
+      <c r="B1075" s="11"/>
+      <c r="C1075" s="9"/>
+      <c r="D1075" s="11"/>
+      <c r="E1075" s="9"/>
+    </row>
+    <row r="1076" spans="1:6" ht="15" customHeight="1">
+      <c r="A1076" s="12"/>
+      <c r="B1076" s="11"/>
+      <c r="C1076" s="9"/>
+      <c r="D1076" s="11"/>
+      <c r="E1076" s="9"/>
+    </row>
+    <row r="1077" spans="1:6" ht="15" customHeight="1">
+      <c r="A1077" s="12"/>
+      <c r="B1077" s="11"/>
+      <c r="C1077" s="9"/>
+      <c r="D1077" s="11"/>
+      <c r="E1077" s="9"/>
+    </row>
+    <row r="1078" spans="1:6" ht="15" customHeight="1">
+      <c r="A1078" s="12"/>
+      <c r="B1078" s="11"/>
+      <c r="C1078" s="9"/>
+      <c r="D1078" s="11"/>
+      <c r="E1078" s="9"/>
+    </row>
+    <row r="1079" spans="1:6" ht="15" customHeight="1">
+      <c r="A1079" s="12"/>
+      <c r="B1079" s="11"/>
+      <c r="C1079" s="9"/>
+      <c r="D1079" s="11"/>
+      <c r="E1079" s="9"/>
+    </row>
+    <row r="1080" spans="1:6" ht="15" customHeight="1">
+      <c r="A1080" s="11"/>
+      <c r="B1080" s="11"/>
+      <c r="C1080" s="11"/>
+      <c r="D1080" s="12"/>
+      <c r="E1080" s="9"/>
+    </row>
+    <row r="1081" spans="1:6" ht="15" customHeight="1">
+      <c r="A1081" s="12"/>
+      <c r="B1081" s="11"/>
+      <c r="C1081" s="9"/>
+      <c r="D1081" s="11"/>
+      <c r="E1081" s="9"/>
+    </row>
+    <row r="1082" spans="1:6" ht="15" customHeight="1">
+      <c r="A1082" s="12"/>
+      <c r="B1082" s="11"/>
+      <c r="C1082" s="9"/>
+      <c r="D1082" s="11"/>
+      <c r="E1082" s="9"/>
+    </row>
+    <row r="1083" spans="1:6" ht="15" customHeight="1">
+      <c r="A1083" s="12"/>
+      <c r="B1083" s="11"/>
+      <c r="C1083" s="9"/>
+      <c r="D1083" s="9"/>
+      <c r="E1083" s="9"/>
+      <c r="F1083" s="15"/>
+    </row>
+    <row r="1084" spans="1:6" ht="15" customHeight="1">
+      <c r="A1084" s="12"/>
+      <c r="B1084" s="11"/>
+      <c r="C1084" s="9"/>
+      <c r="D1084" s="11"/>
+      <c r="E1084" s="9"/>
+    </row>
+    <row r="1085" spans="1:6" ht="15" customHeight="1">
+      <c r="A1085" s="12"/>
+      <c r="B1085" s="11"/>
+      <c r="C1085" s="9"/>
+      <c r="D1085" s="11"/>
+      <c r="E1085" s="9"/>
+    </row>
+    <row r="1086" spans="1:6" ht="15" customHeight="1">
+      <c r="A1086" s="12"/>
+      <c r="B1086" s="11"/>
+      <c r="C1086" s="9"/>
+      <c r="D1086" s="11"/>
+      <c r="E1086" s="9"/>
+    </row>
+    <row r="1087" spans="1:6" ht="15" customHeight="1">
+      <c r="A1087" s="12"/>
+      <c r="B1087" s="11"/>
+      <c r="C1087" s="9"/>
+      <c r="D1087" s="156"/>
+      <c r="E1087" s="9"/>
+      <c r="F1087" s="149"/>
+    </row>
+    <row r="1088" spans="1:6" ht="15" customHeight="1">
+      <c r="A1088" s="12"/>
+      <c r="B1088" s="11"/>
+      <c r="C1088" s="9"/>
+      <c r="D1088" s="11"/>
+      <c r="E1088" s="9"/>
+    </row>
+    <row r="1089" spans="1:6" ht="15" customHeight="1">
+      <c r="A1089" s="12"/>
+      <c r="B1089" s="11"/>
+      <c r="C1089" s="9"/>
+      <c r="D1089" s="11"/>
+      <c r="E1089" s="9"/>
+    </row>
+    <row r="1090" spans="1:6" ht="15" customHeight="1">
+      <c r="A1090" s="12"/>
+      <c r="B1090" s="11"/>
+      <c r="C1090" s="9"/>
+      <c r="D1090" s="11"/>
+      <c r="E1090" s="9"/>
+    </row>
+    <row r="1091" spans="1:6" ht="15" customHeight="1">
+      <c r="A1091" s="12"/>
+      <c r="B1091" s="11"/>
+      <c r="C1091" s="9"/>
+      <c r="D1091" s="11"/>
+      <c r="E1091" s="9"/>
+    </row>
+    <row r="1092" spans="1:6" ht="15" customHeight="1">
+      <c r="A1092" s="12"/>
+      <c r="B1092" s="11"/>
+      <c r="C1092" s="9"/>
+      <c r="D1092" s="11"/>
+      <c r="E1092" s="9"/>
+    </row>
+    <row r="1093" spans="1:6" ht="15" customHeight="1">
+      <c r="A1093" s="12"/>
+      <c r="B1093" s="11"/>
+      <c r="C1093" s="9"/>
+      <c r="D1093" s="11"/>
+      <c r="E1093" s="9"/>
+    </row>
+    <row r="1094" spans="1:6" ht="15" customHeight="1">
+      <c r="A1094" s="11"/>
+      <c r="B1094" s="11"/>
+      <c r="C1094" s="11"/>
+      <c r="D1094" s="12"/>
+      <c r="E1094" s="9"/>
+    </row>
+    <row r="1095" spans="1:6" ht="15" customHeight="1">
+      <c r="A1095" s="11"/>
+      <c r="B1095" s="11"/>
+      <c r="C1095" s="11"/>
+      <c r="D1095" s="9"/>
+      <c r="E1095" s="9"/>
+    </row>
+    <row r="1096" spans="1:6" ht="15" customHeight="1">
+      <c r="A1096" s="11"/>
+      <c r="B1096" s="11"/>
+      <c r="C1096" s="11"/>
+      <c r="D1096" s="11"/>
+      <c r="E1096" s="9"/>
+    </row>
+    <row r="1097" spans="1:6" ht="15" customHeight="1">
+      <c r="A1097" s="11"/>
+      <c r="B1097" s="11"/>
+      <c r="C1097" s="11"/>
+      <c r="D1097" s="12"/>
+      <c r="E1097" s="9"/>
+    </row>
+    <row r="1098" spans="1:6" ht="15" customHeight="1">
+      <c r="A1098" s="12"/>
+      <c r="B1098" s="11"/>
+      <c r="C1098" s="9"/>
+      <c r="D1098" s="11"/>
+      <c r="E1098" s="9"/>
+    </row>
+    <row r="1099" spans="1:6" ht="15" customHeight="1">
+      <c r="A1099" s="12"/>
+      <c r="B1099" s="11"/>
+      <c r="C1099" s="9"/>
+      <c r="D1099" s="11"/>
+      <c r="E1099" s="9"/>
+    </row>
+    <row r="1100" spans="1:6" ht="15" customHeight="1">
+      <c r="A1100" s="12"/>
+      <c r="B1100" s="11"/>
+      <c r="C1100" s="9"/>
+      <c r="D1100" s="9"/>
+      <c r="E1100" s="9"/>
+      <c r="F1100" s="15"/>
+    </row>
+    <row r="1101" spans="1:6" ht="15" customHeight="1">
+      <c r="A1101" s="12"/>
+      <c r="B1101" s="11"/>
+      <c r="C1101" s="9"/>
+      <c r="D1101" s="11"/>
+      <c r="E1101" s="9"/>
+    </row>
+    <row r="1102" spans="1:6" ht="15" customHeight="1">
+      <c r="A1102" s="12"/>
+      <c r="B1102" s="11"/>
+      <c r="C1102" s="9"/>
+      <c r="D1102" s="11"/>
+      <c r="E1102" s="9"/>
+    </row>
+    <row r="1103" spans="1:6" ht="15" customHeight="1">
+      <c r="A1103" s="12"/>
+      <c r="B1103" s="11"/>
+      <c r="C1103" s="9"/>
+      <c r="D1103" s="11"/>
+      <c r="E1103" s="9"/>
+    </row>
+    <row r="1104" spans="1:6" ht="15" customHeight="1">
+      <c r="A1104" s="12"/>
+      <c r="B1104" s="11"/>
+      <c r="C1104" s="9"/>
+      <c r="D1104" s="156"/>
+      <c r="E1104" s="9"/>
+      <c r="F1104" s="149"/>
+    </row>
+    <row r="1105" spans="1:5" ht="15" customHeight="1">
+      <c r="A1105" s="12"/>
+      <c r="B1105" s="11"/>
+      <c r="C1105" s="9"/>
+      <c r="D1105" s="11"/>
+      <c r="E1105" s="9"/>
+    </row>
+    <row r="1106" spans="1:5" ht="15" customHeight="1">
+      <c r="A1106" s="12"/>
+      <c r="B1106" s="11"/>
+      <c r="C1106" s="9"/>
+      <c r="D1106" s="11"/>
+      <c r="E1106" s="9"/>
+    </row>
+    <row r="1107" spans="1:5" ht="15" customHeight="1">
+      <c r="A1107" s="12"/>
+      <c r="B1107" s="11"/>
+      <c r="C1107" s="9"/>
+      <c r="D1107" s="11"/>
+      <c r="E1107" s="9"/>
+    </row>
+    <row r="1108" spans="1:5" ht="15" customHeight="1">
+      <c r="A1108" s="12"/>
+      <c r="B1108" s="11"/>
+      <c r="C1108" s="9"/>
+      <c r="D1108" s="11"/>
+      <c r="E1108" s="9"/>
+    </row>
+    <row r="1109" spans="1:5" ht="15" customHeight="1">
+      <c r="A1109" s="12"/>
+      <c r="B1109" s="11"/>
+      <c r="C1109" s="9"/>
+      <c r="D1109" s="11"/>
+      <c r="E1109" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:F618" xr:uid="{00000000-0009-0000-0000-000010000000}"/>
@@ -20642,7 +21291,7 @@
   <conditionalFormatting sqref="D823:D912">
     <cfRule type="duplicateValues" dxfId="55" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D913:D1001">
+  <conditionalFormatting sqref="D913:D1001 D1016:D1018 D1033:D1035 D1050:D1052 D1067:D1069 D1081:D1083 D1098:D1100">
     <cfRule type="duplicateValues" dxfId="54" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D8">
@@ -20898,7 +21547,7 @@
       <c r="D3" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="E3" s="178" t="s">
+      <c r="E3" s="176" t="s">
         <v>214</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -26809,7 +27458,7 @@
       <c r="D3" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="178" t="s">
+      <c r="E3" s="176" t="s">
         <v>214</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -27856,7 +28505,7 @@
       <c r="E3" s="170" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="178" t="s">
+      <c r="F3" s="176" t="s">
         <v>214</v>
       </c>
       <c r="G3" s="169" t="s">

</xml_diff>

<commit_message>
update CCD template SSCS-12257
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\gordond\hmcts\sscs-ccd-definitions\benefit\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\nickhill111\sscs-ccd-definitions\benefit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1545CE49-7BAE-4A67-BAD6-BC61197D77A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E709F0-7072-46F2-B55C-D81C8540DF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="785" firstSheet="13" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="785" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -26,21 +26,22 @@
     <sheet name="RoleToAccessProfiles" sheetId="22" r:id="rId11"/>
     <sheet name="SearchParty" sheetId="21" r:id="rId12"/>
     <sheet name="EventToComplexTypes" sheetId="10" r:id="rId13"/>
-    <sheet name="SearchInputFields" sheetId="11" r:id="rId14"/>
-    <sheet name="SearchResultFields" sheetId="12" r:id="rId15"/>
-    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId16"/>
-    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId17"/>
-    <sheet name="UserProfile" sheetId="15" r:id="rId18"/>
-    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId19"/>
-    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId20"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId21"/>
-    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId22"/>
-    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId23"/>
+    <sheet name="SearchCriteria" sheetId="24" r:id="rId14"/>
+    <sheet name="SearchInputFields" sheetId="11" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="12" r:id="rId16"/>
+    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId17"/>
+    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId18"/>
+    <sheet name="UserProfile" sheetId="15" r:id="rId19"/>
+    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId20"/>
+    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId21"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId22"/>
+    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId23"/>
+    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$V$110</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$2:$L$98</definedName>
@@ -48,9 +49,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ComplexTypes!$A$3:$M$232</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">FixedLists!$A$1:$E$702</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">State!$A$3:$H$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="19">AuthorisationCaseField!$J$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="20">AuthorisationCaseField!$J$5</definedName>
     <definedName name="_xlnm.Extract" localSheetId="5">CaseTypeTab!$K$61</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="225">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -816,6 +817,12 @@
   </si>
   <si>
     <t>CaseRoles</t>
+  </si>
+  <si>
+    <t>SearchCriteria</t>
+  </si>
+  <si>
+    <t>OtherCaseReference</t>
   </si>
 </sst>
 </file>
@@ -2846,7 +2853,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -2966,10 +2973,10 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3004,16 +3011,16 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3047,7 +3054,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="29" ht="13.8" customHeight="1"/>
+    <row r="29" ht="13.9" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3058,12 +3065,12 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A1048576"/>
+      <selection sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="7"/>
+    <col min="1" max="1" width="10.85546875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3116,11 +3123,11 @@
       <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="126" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="127" customWidth="1"/>
-    <col min="13" max="13" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="126" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="127" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -3259,6 +3266,47 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5C8F2F-DDA6-4EEE-B95B-A1EF1BFC6D3A}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="175" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="175" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="175" t="s">
+        <v>224</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I573"/>
   <sheetViews>
@@ -3266,11 +3314,11 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34" style="7" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
-    <col min="5" max="6" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="6" width="36.140625" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5372,7 +5420,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
@@ -5380,12 +5428,12 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" style="7" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
-    <col min="5" max="6" width="41.44140625" customWidth="1"/>
-    <col min="7" max="7" width="29.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="6" width="41.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
@@ -5672,7 +5720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I131"/>
   <sheetViews>
@@ -5680,11 +5728,11 @@
       <selection activeCell="A91" sqref="A91:B131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
-    <col min="5" max="6" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="6" width="36.140625" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6501,7 +6549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
@@ -6509,11 +6557,11 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="6" width="54" customWidth="1"/>
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
@@ -6969,7 +7017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
@@ -6977,10 +7025,10 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -7634,228 +7682,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:E35"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="27" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="176" t="s">
-        <v>214</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-    </row>
-    <row r="17" spans="1:2" ht="15" customHeight="1">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-    </row>
-    <row r="18" spans="1:2" ht="15" customHeight="1">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-    </row>
-    <row r="19" spans="1:2" ht="15" customHeight="1">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-    </row>
-    <row r="20" spans="1:2" ht="15" customHeight="1">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-    </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-    </row>
-    <row r="22" spans="1:2" ht="15" customHeight="1">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-    </row>
-    <row r="23" spans="1:2" ht="15" customHeight="1">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-    </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-    </row>
-    <row r="25" spans="1:2" ht="15" customHeight="1">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-    </row>
-    <row r="26" spans="1:2" ht="15" customHeight="1">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-    </row>
-    <row r="27" spans="1:2" ht="15" customHeight="1">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-    </row>
-    <row r="28" spans="1:2" ht="15" customHeight="1">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-    </row>
-    <row r="29" spans="1:2" ht="15" customHeight="1">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-    </row>
-    <row r="30" spans="1:2" ht="15" customHeight="1">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-    </row>
-    <row r="31" spans="1:2" ht="15" customHeight="1">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-    </row>
-    <row r="32" spans="1:2" ht="15" customHeight="1">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-    </row>
-    <row r="33" spans="1:2" ht="15" customHeight="1">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-    </row>
-    <row r="34" spans="1:2" ht="15" customHeight="1">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-    </row>
-    <row r="35" spans="1:2" ht="15" customHeight="1">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I10"/>
@@ -7864,11 +7690,11 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
-    <col min="7" max="7" width="92.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="92.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1">
@@ -8035,20 +7861,242 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="27" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="176" t="s">
+        <v>214</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" s="20" customFormat="1" ht="15" customHeight="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+    </row>
+    <row r="17" spans="1:2" ht="15" customHeight="1">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+    </row>
+    <row r="19" spans="1:2" ht="15" customHeight="1">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:2" ht="15" customHeight="1">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+    </row>
+    <row r="21" spans="1:2" ht="15" customHeight="1">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+    </row>
+    <row r="22" spans="1:2" ht="15" customHeight="1">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+    </row>
+    <row r="23" spans="1:2" ht="15" customHeight="1">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+    </row>
+    <row r="24" spans="1:2" ht="15" customHeight="1">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+    </row>
+    <row r="25" spans="1:2" ht="15" customHeight="1">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+    </row>
+    <row r="26" spans="1:2" ht="15" customHeight="1">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+    </row>
+    <row r="27" spans="1:2" ht="15" customHeight="1">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+    </row>
+    <row r="28" spans="1:2" ht="15" customHeight="1">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+    </row>
+    <row r="29" spans="1:2" ht="15" customHeight="1">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+    </row>
+    <row r="30" spans="1:2" ht="15" customHeight="1">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+    </row>
+    <row r="31" spans="1:2" ht="15" customHeight="1">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+    </row>
+    <row r="32" spans="1:2" ht="15" customHeight="1">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+    </row>
+    <row r="33" spans="1:2" ht="15" customHeight="1">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+    </row>
+    <row r="34" spans="1:2" ht="15" customHeight="1">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+    </row>
+    <row r="35" spans="1:2" ht="15" customHeight="1">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMJ1109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1072" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A952" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1015" sqref="A999:XFD1109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="14" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="14"/>
-    <col min="4" max="4" width="37.6640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="75.44140625" style="14" customWidth="1"/>
-    <col min="6" max="1024" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="10.42578125" style="14" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="14"/>
+    <col min="4" max="4" width="37.7109375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="75.42578125" style="14" customWidth="1"/>
+    <col min="6" max="1024" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1">
@@ -21279,179 +21327,179 @@
     </row>
   </sheetData>
   <autoFilter ref="A3:F618" xr:uid="{00000000-0009-0000-0000-000010000000}"/>
+  <conditionalFormatting sqref="D4:D8">
+    <cfRule type="duplicateValues" dxfId="58" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D466">
+    <cfRule type="duplicateValues" dxfId="57" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D467">
+    <cfRule type="duplicateValues" dxfId="56" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D468">
+    <cfRule type="duplicateValues" dxfId="55" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D469">
+    <cfRule type="duplicateValues" dxfId="54" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D470">
+    <cfRule type="duplicateValues" dxfId="53" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D471">
+    <cfRule type="duplicateValues" dxfId="52" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D472">
+    <cfRule type="duplicateValues" dxfId="51" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D473">
+    <cfRule type="duplicateValues" dxfId="50" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D474">
+    <cfRule type="duplicateValues" dxfId="49" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D475">
+    <cfRule type="duplicateValues" dxfId="48" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D476">
+    <cfRule type="duplicateValues" dxfId="47" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D477">
+    <cfRule type="duplicateValues" dxfId="46" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D478">
+    <cfRule type="duplicateValues" dxfId="45" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D479">
+    <cfRule type="duplicateValues" dxfId="44" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D480">
+    <cfRule type="duplicateValues" dxfId="43" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D481">
+    <cfRule type="duplicateValues" dxfId="42" priority="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D482">
+    <cfRule type="duplicateValues" dxfId="41" priority="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D483">
+    <cfRule type="duplicateValues" dxfId="40" priority="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D486">
+    <cfRule type="duplicateValues" dxfId="39" priority="26"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D487">
+    <cfRule type="duplicateValues" dxfId="38" priority="27"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D488">
+    <cfRule type="duplicateValues" dxfId="37" priority="28"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D489">
+    <cfRule type="duplicateValues" dxfId="36" priority="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D490">
+    <cfRule type="duplicateValues" dxfId="35" priority="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D491">
+    <cfRule type="duplicateValues" dxfId="34" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D494">
+    <cfRule type="duplicateValues" dxfId="33" priority="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D495">
+    <cfRule type="duplicateValues" dxfId="32" priority="33"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D496">
+    <cfRule type="duplicateValues" dxfId="31" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D497">
+    <cfRule type="duplicateValues" dxfId="30" priority="35"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D498">
+    <cfRule type="duplicateValues" dxfId="29" priority="36"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D499">
+    <cfRule type="duplicateValues" dxfId="28" priority="37"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D524">
+    <cfRule type="duplicateValues" dxfId="27" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D530">
+    <cfRule type="duplicateValues" dxfId="26" priority="39"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D531">
+    <cfRule type="duplicateValues" dxfId="25" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D532">
+    <cfRule type="duplicateValues" dxfId="24" priority="41"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D533">
+    <cfRule type="duplicateValues" dxfId="23" priority="42"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D534">
+    <cfRule type="duplicateValues" dxfId="22" priority="43"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D535">
+    <cfRule type="duplicateValues" dxfId="21" priority="44"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D536">
+    <cfRule type="duplicateValues" dxfId="20" priority="45"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D537">
+    <cfRule type="duplicateValues" dxfId="19" priority="46"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D538">
+    <cfRule type="duplicateValues" dxfId="18" priority="47"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D539">
+    <cfRule type="duplicateValues" dxfId="17" priority="48"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D541">
+    <cfRule type="duplicateValues" dxfId="16" priority="49"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D542">
+    <cfRule type="duplicateValues" dxfId="15" priority="50"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D543">
+    <cfRule type="duplicateValues" dxfId="14" priority="51"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D544">
+    <cfRule type="duplicateValues" dxfId="13" priority="52"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D546">
+    <cfRule type="duplicateValues" dxfId="12" priority="53"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D547">
+    <cfRule type="duplicateValues" dxfId="11" priority="54"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D548">
+    <cfRule type="duplicateValues" dxfId="10" priority="55"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D549">
+    <cfRule type="duplicateValues" dxfId="9" priority="56"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D550">
+    <cfRule type="duplicateValues" dxfId="8" priority="57"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D551">
+    <cfRule type="duplicateValues" dxfId="7" priority="58"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D617">
+    <cfRule type="duplicateValues" dxfId="6" priority="59"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D619:D642 D606">
-    <cfRule type="duplicateValues" dxfId="58" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D643:D732">
-    <cfRule type="duplicateValues" dxfId="57" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D733:D822">
-    <cfRule type="duplicateValues" dxfId="56" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D823:D912">
-    <cfRule type="duplicateValues" dxfId="55" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D913:D1001 D1016:D1018 D1033:D1035 D1050:D1052 D1067:D1069 D1081:D1083 D1098:D1100">
-    <cfRule type="duplicateValues" dxfId="54" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8">
-    <cfRule type="duplicateValues" dxfId="53" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D466">
-    <cfRule type="duplicateValues" dxfId="52" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D467">
-    <cfRule type="duplicateValues" dxfId="51" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D468">
-    <cfRule type="duplicateValues" dxfId="50" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D469">
-    <cfRule type="duplicateValues" dxfId="49" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D470">
-    <cfRule type="duplicateValues" dxfId="48" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D471">
-    <cfRule type="duplicateValues" dxfId="47" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D472">
-    <cfRule type="duplicateValues" dxfId="46" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D473">
-    <cfRule type="duplicateValues" dxfId="45" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D474">
-    <cfRule type="duplicateValues" dxfId="44" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D475">
-    <cfRule type="duplicateValues" dxfId="43" priority="17"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D476">
-    <cfRule type="duplicateValues" dxfId="42" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D477">
-    <cfRule type="duplicateValues" dxfId="41" priority="19"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D478">
-    <cfRule type="duplicateValues" dxfId="40" priority="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D479">
-    <cfRule type="duplicateValues" dxfId="39" priority="21"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D480">
-    <cfRule type="duplicateValues" dxfId="38" priority="22"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D481">
-    <cfRule type="duplicateValues" dxfId="37" priority="23"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D482">
-    <cfRule type="duplicateValues" dxfId="36" priority="24"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D483">
-    <cfRule type="duplicateValues" dxfId="35" priority="25"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D486">
-    <cfRule type="duplicateValues" dxfId="34" priority="26"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D487">
-    <cfRule type="duplicateValues" dxfId="33" priority="27"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D488">
-    <cfRule type="duplicateValues" dxfId="32" priority="28"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D489">
-    <cfRule type="duplicateValues" dxfId="31" priority="29"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D490">
-    <cfRule type="duplicateValues" dxfId="30" priority="30"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D491">
-    <cfRule type="duplicateValues" dxfId="29" priority="31"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D494">
-    <cfRule type="duplicateValues" dxfId="28" priority="32"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D495">
-    <cfRule type="duplicateValues" dxfId="27" priority="33"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D496">
-    <cfRule type="duplicateValues" dxfId="26" priority="34"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D497">
-    <cfRule type="duplicateValues" dxfId="25" priority="35"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D498">
-    <cfRule type="duplicateValues" dxfId="24" priority="36"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D499">
-    <cfRule type="duplicateValues" dxfId="23" priority="37"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D524">
-    <cfRule type="duplicateValues" dxfId="22" priority="38"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D530">
-    <cfRule type="duplicateValues" dxfId="21" priority="39"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D531">
-    <cfRule type="duplicateValues" dxfId="20" priority="40"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D532">
-    <cfRule type="duplicateValues" dxfId="19" priority="41"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D533">
-    <cfRule type="duplicateValues" dxfId="18" priority="42"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D534">
-    <cfRule type="duplicateValues" dxfId="17" priority="43"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D535">
-    <cfRule type="duplicateValues" dxfId="16" priority="44"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D536">
-    <cfRule type="duplicateValues" dxfId="15" priority="45"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D537">
-    <cfRule type="duplicateValues" dxfId="14" priority="46"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D538">
-    <cfRule type="duplicateValues" dxfId="13" priority="47"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D539">
-    <cfRule type="duplicateValues" dxfId="12" priority="48"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D541">
-    <cfRule type="duplicateValues" dxfId="11" priority="49"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D542">
-    <cfRule type="duplicateValues" dxfId="10" priority="50"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D543">
-    <cfRule type="duplicateValues" dxfId="9" priority="51"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D544">
-    <cfRule type="duplicateValues" dxfId="8" priority="52"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D546">
-    <cfRule type="duplicateValues" dxfId="7" priority="53"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D547">
-    <cfRule type="duplicateValues" dxfId="6" priority="54"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D548">
-    <cfRule type="duplicateValues" dxfId="5" priority="55"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D549">
-    <cfRule type="duplicateValues" dxfId="4" priority="56"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D550">
-    <cfRule type="duplicateValues" dxfId="3" priority="57"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D551">
-    <cfRule type="duplicateValues" dxfId="2" priority="58"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D617">
-    <cfRule type="duplicateValues" dxfId="1" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -21461,7 +21509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AMJ696"/>
   <sheetViews>
@@ -21469,13 +21517,13 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="14" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="14"/>
-    <col min="4" max="4" width="41.88671875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="75.44140625" style="14" customWidth="1"/>
-    <col min="6" max="1024" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="10.42578125" style="14" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="14"/>
+    <col min="4" max="4" width="41.85546875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="75.42578125" style="14" customWidth="1"/>
+    <col min="6" max="1024" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1">
@@ -27394,7 +27442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:G151"/>
   <sheetViews>
@@ -27402,11 +27450,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" customWidth="1"/>
-    <col min="5" max="5" width="37.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
@@ -28433,7 +28481,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:AMJ38"/>
   <sheetViews>
@@ -28441,19 +28489,19 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.109375" style="161" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="161" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" style="161" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="161" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="161" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="161" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="161" customWidth="1"/>
-    <col min="8" max="1024" width="10.88671875" style="161"/>
+    <col min="1" max="1" width="33.140625" style="161" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="161" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="161" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="161" customWidth="1"/>
+    <col min="5" max="5" width="57.7109375" style="161" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="161" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="161" customWidth="1"/>
+    <col min="8" max="1024" width="10.85546875" style="161"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999">
+    <row r="1" spans="1:7" ht="18">
       <c r="A1" s="162" t="s">
         <v>203</v>
       </c>
@@ -28470,7 +28518,7 @@
       <c r="F1" s="166"/>
       <c r="G1" s="166"/>
     </row>
-    <row r="2" spans="1:7" ht="66.599999999999994">
+    <row r="2" spans="1:7" ht="64.5">
       <c r="A2" s="167"/>
       <c r="B2" s="167"/>
       <c r="C2" s="168" t="s">
@@ -28489,7 +28537,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.399999999999999">
+    <row r="3" spans="1:7" ht="18">
       <c r="A3" s="169" t="s">
         <v>9</v>
       </c>
@@ -28749,15 +28797,15 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="7"/>
-    <col min="4" max="4" width="28.44140625" customWidth="1"/>
-    <col min="5" max="5" width="30.44140625" customWidth="1"/>
-    <col min="6" max="6" width="46.109375" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
-    <col min="8" max="8" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="7"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+    <col min="6" max="6" width="46.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
@@ -30163,7 +30211,7 @@
       <c r="H109" s="33"/>
       <c r="J109" s="10"/>
     </row>
-    <row r="110" spans="1:12" s="14" customFormat="1" ht="45.9" customHeight="1">
+    <row r="110" spans="1:12" s="14" customFormat="1" ht="45.95" customHeight="1">
       <c r="A110" s="17"/>
       <c r="B110" s="17"/>
       <c r="C110" s="10"/>
@@ -30193,7 +30241,7 @@
       <c r="H112" s="35"/>
       <c r="J112" s="10"/>
     </row>
-    <row r="113" spans="1:10" s="14" customFormat="1" ht="48.9" customHeight="1">
+    <row r="113" spans="1:10" s="14" customFormat="1" ht="48.95" customHeight="1">
       <c r="A113" s="17"/>
       <c r="B113" s="17"/>
       <c r="C113" s="10"/>
@@ -30233,7 +30281,7 @@
       <c r="H116" s="15"/>
       <c r="J116" s="10"/>
     </row>
-    <row r="117" spans="1:10" s="14" customFormat="1" ht="54.9" customHeight="1">
+    <row r="117" spans="1:10" s="14" customFormat="1" ht="54.95" customHeight="1">
       <c r="A117" s="17"/>
       <c r="B117" s="17"/>
       <c r="C117" s="10"/>
@@ -30243,7 +30291,7 @@
       <c r="H117" s="15"/>
       <c r="J117" s="10"/>
     </row>
-    <row r="118" spans="1:10" s="14" customFormat="1" ht="48.9" customHeight="1">
+    <row r="118" spans="1:10" s="14" customFormat="1" ht="48.95" customHeight="1">
       <c r="A118" s="17"/>
       <c r="B118" s="17"/>
       <c r="C118" s="10"/>
@@ -30733,15 +30781,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="14"/>
-    <col min="3" max="3" width="74.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="14"/>
+    <col min="3" max="3" width="74.7109375" style="14" customWidth="1"/>
     <col min="4" max="4" width="117" style="14" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" style="14"/>
-    <col min="7" max="7" width="15.44140625" style="14" customWidth="1"/>
-    <col min="8" max="1024" width="8.88671875" style="14"/>
+    <col min="5" max="6" width="8.85546875" style="14"/>
+    <col min="7" max="7" width="15.42578125" style="14" customWidth="1"/>
+    <col min="8" max="1024" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="11" customFormat="1" ht="15" customHeight="1">
@@ -33230,14 +33278,14 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="18"/>
-    <col min="3" max="3" width="40.88671875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="28.109375" style="20" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="18"/>
+    <col min="3" max="3" width="40.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="20" customWidth="1"/>
     <col min="5" max="5" width="62" style="20" customWidth="1"/>
-    <col min="6" max="1024" width="8.88671875" style="20"/>
+    <col min="6" max="1024" width="8.85546875" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="49" customFormat="1" ht="15" customHeight="1">
@@ -39453,15 +39501,15 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
@@ -41255,17 +41303,17 @@
       <c r="B263" s="11"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H39">
+    <cfRule type="duplicateValues" dxfId="75" priority="3"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H54:H56">
-    <cfRule type="duplicateValues" dxfId="75" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
-    <cfRule type="duplicateValues" dxfId="74" priority="3"/>
+  <conditionalFormatting sqref="H86">
+    <cfRule type="duplicateValues" dxfId="73" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87:H88">
-    <cfRule type="duplicateValues" dxfId="73" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H86">
-    <cfRule type="duplicateValues" dxfId="72" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -41283,12 +41331,12 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="36.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -41442,7 +41490,7 @@
       <c r="G11" s="11"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" ht="15.9" customHeight="1">
+    <row r="12" spans="1:8" s="14" customFormat="1" ht="15.95" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
@@ -41643,24 +41691,24 @@
       <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="20"/>
-    <col min="4" max="4" width="30.6640625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="76.88671875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="20" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="20"/>
+    <col min="4" max="4" width="30.7109375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="76.85546875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="20" customWidth="1"/>
     <col min="7" max="7" width="34" style="20" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="20"/>
-    <col min="9" max="9" width="78.33203125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="36.6640625" style="20" customWidth="1"/>
-    <col min="11" max="11" width="40.88671875" customWidth="1"/>
-    <col min="12" max="12" width="63.44140625" style="20" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="20"/>
-    <col min="14" max="14" width="59.44140625" style="14" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="20"/>
-    <col min="16" max="16" width="65.33203125" style="14" customWidth="1"/>
-    <col min="17" max="1024" width="8.88671875" style="20"/>
+    <col min="8" max="8" width="8.85546875" style="20"/>
+    <col min="9" max="9" width="78.28515625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="36.7109375" style="20" customWidth="1"/>
+    <col min="11" max="11" width="40.85546875" customWidth="1"/>
+    <col min="12" max="12" width="63.42578125" style="20" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="20"/>
+    <col min="14" max="14" width="59.42578125" style="14" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" style="20"/>
+    <col min="16" max="16" width="65.28515625" style="14" customWidth="1"/>
+    <col min="17" max="1024" width="8.85546875" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
@@ -41695,7 +41743,7 @@
       <c r="U1" s="11"/>
       <c r="V1" s="11"/>
     </row>
-    <row r="2" spans="1:23" ht="63.9" customHeight="1">
+    <row r="2" spans="1:23" ht="63.95" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -50624,23 +50672,23 @@
       <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="12"/>
-    <col min="3" max="3" width="8.88671875" style="14"/>
-    <col min="4" max="4" width="77.109375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="12"/>
+    <col min="3" max="3" width="8.85546875" style="14"/>
+    <col min="4" max="4" width="77.140625" style="14" customWidth="1"/>
     <col min="5" max="5" width="66" style="14" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="14"/>
-    <col min="7" max="7" width="39.88671875" style="14" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="14"/>
-    <col min="9" max="9" width="27.33203125" style="14" customWidth="1"/>
-    <col min="10" max="15" width="8.88671875" style="14"/>
-    <col min="16" max="16" width="8.88671875" style="11"/>
+    <col min="6" max="6" width="8.85546875" style="14"/>
+    <col min="7" max="7" width="39.85546875" style="14" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="14"/>
+    <col min="9" max="9" width="27.28515625" style="14" customWidth="1"/>
+    <col min="10" max="15" width="8.85546875" style="14"/>
+    <col min="16" max="16" width="8.85546875" style="11"/>
     <col min="17" max="17" width="24" style="11" customWidth="1"/>
-    <col min="18" max="18" width="20.109375" style="14" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" style="14" customWidth="1"/>
     <col min="19" max="19" width="17" style="14" customWidth="1"/>
-    <col min="20" max="1024" width="8.88671875" style="14"/>
+    <col min="20" max="1024" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1">
@@ -50668,7 +50716,7 @@
       <c r="N1" s="11"/>
       <c r="O1" s="102"/>
     </row>
-    <row r="2" spans="1:22" ht="159.9" customHeight="1">
+    <row r="2" spans="1:22" ht="159.94999999999999" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -52952,38 +53000,38 @@
     <row r="229" ht="15" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A3:O161" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
-  <conditionalFormatting sqref="E120">
-    <cfRule type="duplicateValues" dxfId="69" priority="2"/>
+  <conditionalFormatting sqref="D91:D92 D156">
+    <cfRule type="duplicateValues" dxfId="69" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D142">
+    <cfRule type="duplicateValues" dxfId="68" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E73">
-    <cfRule type="duplicateValues" dxfId="68" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76">
-    <cfRule type="duplicateValues" dxfId="67" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="duplicateValues" dxfId="66" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E120">
+    <cfRule type="duplicateValues" dxfId="64" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E121:E128">
-    <cfRule type="duplicateValues" dxfId="65" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E136">
-    <cfRule type="duplicateValues" dxfId="64" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D142">
-    <cfRule type="duplicateValues" dxfId="63" priority="8"/>
+  <conditionalFormatting sqref="E144">
+    <cfRule type="duplicateValues" dxfId="61" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D91:D92 D156">
-    <cfRule type="duplicateValues" dxfId="62" priority="9"/>
+  <conditionalFormatting sqref="E155">
+    <cfRule type="duplicateValues" dxfId="60" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E158">
-    <cfRule type="duplicateValues" dxfId="61" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E144">
-    <cfRule type="duplicateValues" dxfId="60" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E155">
-    <cfRule type="duplicateValues" dxfId="59" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
fix ccd template SSCS-12257
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\nickhill111\sscs-ccd-definitions\benefit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF83B6F-9554-4438-A593-F7E73C2DE108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB151DCA-2BD8-4177-B673-855A54A1FA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="785" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="225">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -3268,66 +3268,77 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5C8F2F-DDA6-4EEE-B95B-A1EF1BFC6D3A}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
+    <col min="2" max="2" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="177" t="s">
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="177" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="177" t="s">
+      <c r="D3" s="177" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added SearchCriteria sheet in template
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\gordond\hmcts\sscs-ccd-definitions\benefit\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\andrei\sscs_dev\sscs-ccd-definitions\benefit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1545CE49-7BAE-4A67-BAD6-BC61197D77A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D58D6A-5CB9-4A27-88E0-0722CA1DFB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="785" firstSheet="13" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="785" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -25,22 +25,23 @@
     <sheet name="CaseRoles" sheetId="23" r:id="rId10"/>
     <sheet name="RoleToAccessProfiles" sheetId="22" r:id="rId11"/>
     <sheet name="SearchParty" sheetId="21" r:id="rId12"/>
-    <sheet name="EventToComplexTypes" sheetId="10" r:id="rId13"/>
-    <sheet name="SearchInputFields" sheetId="11" r:id="rId14"/>
-    <sheet name="SearchResultFields" sheetId="12" r:id="rId15"/>
-    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId16"/>
-    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId17"/>
-    <sheet name="UserProfile" sheetId="15" r:id="rId18"/>
-    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId19"/>
-    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId20"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId21"/>
-    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId22"/>
-    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId23"/>
+    <sheet name="SearchCriteria" sheetId="24" r:id="rId13"/>
+    <sheet name="EventToComplexTypes" sheetId="10" r:id="rId14"/>
+    <sheet name="SearchInputFields" sheetId="11" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="12" r:id="rId16"/>
+    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId17"/>
+    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId18"/>
+    <sheet name="UserProfile" sheetId="15" r:id="rId19"/>
+    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId20"/>
+    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId21"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId22"/>
+    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId23"/>
+    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$V$110</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$2:$L$98</definedName>
@@ -48,17 +49,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ComplexTypes!$A$3:$M$232</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">FixedLists!$A$1:$E$702</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">State!$A$3:$H$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="19">AuthorisationCaseField!$J$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="20">AuthorisationCaseField!$J$5</definedName>
     <definedName name="_xlnm.Extract" localSheetId="5">CaseTypeTab!$K$61</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="229">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -817,12 +818,32 @@
   <si>
     <t>CaseRoles</t>
   </si>
+  <si>
+    <t>OtherCaseReference</t>
+  </si>
+  <si>
+    <t>A complex types that make up the Other Case Reference.
+Max Length: 200</t>
+  </si>
+  <si>
+    <t>The Case Type for which the configuration applies
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Not used - but retained to be consistent with other CCD config</t>
+  </si>
+  <si>
+    <t>From when the configuration is valid</t>
+  </si>
+  <si>
+    <t>SearchCriteria</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="37">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1079,6 +1100,20 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333399"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1400,14 +1435,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1683,13 +1719,29 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal 2 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 4" xfId="5" xr:uid="{33532DE7-3164-4A94-8265-C1B9E588DC41}"/>
   </cellStyles>
   <dxfs count="77">
     <dxf>
@@ -2846,7 +2898,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -2953,7 +3005,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2966,10 +3018,10 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3004,16 +3056,16 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3047,7 +3099,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="29" ht="13.8" customHeight="1"/>
+    <row r="29" ht="13.9" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3061,9 +3113,9 @@
       <selection activeCell="A4" sqref="A4:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="7"/>
+    <col min="1" max="1" width="10.85546875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3102,13 +3154,66 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB591878-B3FF-41B4-AE48-D7E884A650BD}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="2" width="12.28515625" style="178" customWidth="1"/>
+    <col min="3" max="16384" width="12.85546875" style="177"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18">
+      <c r="A1" s="185" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" s="184"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="182"/>
+    </row>
+    <row r="2" spans="1:4" ht="90">
+      <c r="A2" s="181" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="181" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="181" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" s="181" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="179" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="180" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="179" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="179" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
@@ -3116,11 +3221,11 @@
       <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="126" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="127" customWidth="1"/>
-    <col min="13" max="13" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="126" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="127" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -3252,13 +3357,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I573"/>
   <sheetViews>
@@ -3266,11 +3368,11 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34" style="7" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
-    <col min="5" max="6" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="6" width="36.140625" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5367,12 +5469,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
@@ -5380,12 +5482,12 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" style="7" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
-    <col min="5" max="6" width="41.44140625" customWidth="1"/>
-    <col min="7" max="7" width="29.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="6" width="41.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
@@ -5667,24 +5769,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A104" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A91" sqref="A91:B131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
-    <col min="5" max="6" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="6" width="36.140625" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6496,12 +6598,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
@@ -6509,11 +6611,11 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="6" width="54" customWidth="1"/>
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
@@ -6964,12 +7066,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
@@ -6977,10 +7079,10 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -7629,229 +7731,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:E35"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="27" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="176" t="s">
-        <v>214</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-    </row>
-    <row r="17" spans="1:2" ht="15" customHeight="1">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-    </row>
-    <row r="18" spans="1:2" ht="15" customHeight="1">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-    </row>
-    <row r="19" spans="1:2" ht="15" customHeight="1">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-    </row>
-    <row r="20" spans="1:2" ht="15" customHeight="1">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-    </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-    </row>
-    <row r="22" spans="1:2" ht="15" customHeight="1">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-    </row>
-    <row r="23" spans="1:2" ht="15" customHeight="1">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-    </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-    </row>
-    <row r="25" spans="1:2" ht="15" customHeight="1">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-    </row>
-    <row r="26" spans="1:2" ht="15" customHeight="1">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-    </row>
-    <row r="27" spans="1:2" ht="15" customHeight="1">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-    </row>
-    <row r="28" spans="1:2" ht="15" customHeight="1">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-    </row>
-    <row r="29" spans="1:2" ht="15" customHeight="1">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-    </row>
-    <row r="30" spans="1:2" ht="15" customHeight="1">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-    </row>
-    <row r="31" spans="1:2" ht="15" customHeight="1">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-    </row>
-    <row r="32" spans="1:2" ht="15" customHeight="1">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-    </row>
-    <row r="33" spans="1:2" ht="15" customHeight="1">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-    </row>
-    <row r="34" spans="1:2" ht="15" customHeight="1">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-    </row>
-    <row r="35" spans="1:2" ht="15" customHeight="1">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -7864,11 +7744,11 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
-    <col min="7" max="7" width="92.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="92.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1">
@@ -8029,26 +7909,248 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="27" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="176" t="s">
+        <v>214</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" s="20" customFormat="1" ht="15" customHeight="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+    </row>
+    <row r="17" spans="1:2" ht="15" customHeight="1">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+    </row>
+    <row r="19" spans="1:2" ht="15" customHeight="1">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:2" ht="15" customHeight="1">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+    </row>
+    <row r="21" spans="1:2" ht="15" customHeight="1">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+    </row>
+    <row r="22" spans="1:2" ht="15" customHeight="1">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+    </row>
+    <row r="23" spans="1:2" ht="15" customHeight="1">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+    </row>
+    <row r="24" spans="1:2" ht="15" customHeight="1">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+    </row>
+    <row r="25" spans="1:2" ht="15" customHeight="1">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+    </row>
+    <row r="26" spans="1:2" ht="15" customHeight="1">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+    </row>
+    <row r="27" spans="1:2" ht="15" customHeight="1">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+    </row>
+    <row r="28" spans="1:2" ht="15" customHeight="1">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+    </row>
+    <row r="29" spans="1:2" ht="15" customHeight="1">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+    </row>
+    <row r="30" spans="1:2" ht="15" customHeight="1">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+    </row>
+    <row r="31" spans="1:2" ht="15" customHeight="1">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+    </row>
+    <row r="32" spans="1:2" ht="15" customHeight="1">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+    </row>
+    <row r="33" spans="1:2" ht="15" customHeight="1">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+    </row>
+    <row r="34" spans="1:2" ht="15" customHeight="1">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+    </row>
+    <row r="35" spans="1:2" ht="15" customHeight="1">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMJ1109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1072" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="ALF1081" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1015" sqref="A999:XFD1109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="14" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="14"/>
-    <col min="4" max="4" width="37.6640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="75.44140625" style="14" customWidth="1"/>
-    <col min="6" max="1024" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="10.42578125" style="14" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="14"/>
+    <col min="4" max="4" width="37.7109375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="75.42578125" style="14" customWidth="1"/>
+    <col min="6" max="1024" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1">
@@ -21279,189 +21381,189 @@
     </row>
   </sheetData>
   <autoFilter ref="A3:F618" xr:uid="{00000000-0009-0000-0000-000010000000}"/>
+  <conditionalFormatting sqref="D4:D8">
+    <cfRule type="duplicateValues" dxfId="58" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D466">
+    <cfRule type="duplicateValues" dxfId="57" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D467">
+    <cfRule type="duplicateValues" dxfId="56" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D468">
+    <cfRule type="duplicateValues" dxfId="55" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D469">
+    <cfRule type="duplicateValues" dxfId="54" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D470">
+    <cfRule type="duplicateValues" dxfId="53" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D471">
+    <cfRule type="duplicateValues" dxfId="52" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D472">
+    <cfRule type="duplicateValues" dxfId="51" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D473">
+    <cfRule type="duplicateValues" dxfId="50" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D474">
+    <cfRule type="duplicateValues" dxfId="49" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D475">
+    <cfRule type="duplicateValues" dxfId="48" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D476">
+    <cfRule type="duplicateValues" dxfId="47" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D477">
+    <cfRule type="duplicateValues" dxfId="46" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D478">
+    <cfRule type="duplicateValues" dxfId="45" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D479">
+    <cfRule type="duplicateValues" dxfId="44" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D480">
+    <cfRule type="duplicateValues" dxfId="43" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D481">
+    <cfRule type="duplicateValues" dxfId="42" priority="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D482">
+    <cfRule type="duplicateValues" dxfId="41" priority="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D483">
+    <cfRule type="duplicateValues" dxfId="40" priority="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D486">
+    <cfRule type="duplicateValues" dxfId="39" priority="26"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D487">
+    <cfRule type="duplicateValues" dxfId="38" priority="27"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D488">
+    <cfRule type="duplicateValues" dxfId="37" priority="28"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D489">
+    <cfRule type="duplicateValues" dxfId="36" priority="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D490">
+    <cfRule type="duplicateValues" dxfId="35" priority="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D491">
+    <cfRule type="duplicateValues" dxfId="34" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D494">
+    <cfRule type="duplicateValues" dxfId="33" priority="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D495">
+    <cfRule type="duplicateValues" dxfId="32" priority="33"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D496">
+    <cfRule type="duplicateValues" dxfId="31" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D497">
+    <cfRule type="duplicateValues" dxfId="30" priority="35"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D498">
+    <cfRule type="duplicateValues" dxfId="29" priority="36"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D499">
+    <cfRule type="duplicateValues" dxfId="28" priority="37"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D524">
+    <cfRule type="duplicateValues" dxfId="27" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D530">
+    <cfRule type="duplicateValues" dxfId="26" priority="39"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D531">
+    <cfRule type="duplicateValues" dxfId="25" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D532">
+    <cfRule type="duplicateValues" dxfId="24" priority="41"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D533">
+    <cfRule type="duplicateValues" dxfId="23" priority="42"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D534">
+    <cfRule type="duplicateValues" dxfId="22" priority="43"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D535">
+    <cfRule type="duplicateValues" dxfId="21" priority="44"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D536">
+    <cfRule type="duplicateValues" dxfId="20" priority="45"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D537">
+    <cfRule type="duplicateValues" dxfId="19" priority="46"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D538">
+    <cfRule type="duplicateValues" dxfId="18" priority="47"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D539">
+    <cfRule type="duplicateValues" dxfId="17" priority="48"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D541">
+    <cfRule type="duplicateValues" dxfId="16" priority="49"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D542">
+    <cfRule type="duplicateValues" dxfId="15" priority="50"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D543">
+    <cfRule type="duplicateValues" dxfId="14" priority="51"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D544">
+    <cfRule type="duplicateValues" dxfId="13" priority="52"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D546">
+    <cfRule type="duplicateValues" dxfId="12" priority="53"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D547">
+    <cfRule type="duplicateValues" dxfId="11" priority="54"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D548">
+    <cfRule type="duplicateValues" dxfId="10" priority="55"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D549">
+    <cfRule type="duplicateValues" dxfId="9" priority="56"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D550">
+    <cfRule type="duplicateValues" dxfId="8" priority="57"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D551">
+    <cfRule type="duplicateValues" dxfId="7" priority="58"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D617">
+    <cfRule type="duplicateValues" dxfId="6" priority="59"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D619:D642 D606">
-    <cfRule type="duplicateValues" dxfId="58" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D643:D732">
-    <cfRule type="duplicateValues" dxfId="57" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D733:D822">
-    <cfRule type="duplicateValues" dxfId="56" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D823:D912">
-    <cfRule type="duplicateValues" dxfId="55" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D913:D1001 D1016:D1018 D1033:D1035 D1050:D1052 D1067:D1069 D1081:D1083 D1098:D1100">
-    <cfRule type="duplicateValues" dxfId="54" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8">
-    <cfRule type="duplicateValues" dxfId="53" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D466">
-    <cfRule type="duplicateValues" dxfId="52" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D467">
-    <cfRule type="duplicateValues" dxfId="51" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D468">
-    <cfRule type="duplicateValues" dxfId="50" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D469">
-    <cfRule type="duplicateValues" dxfId="49" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D470">
-    <cfRule type="duplicateValues" dxfId="48" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D471">
-    <cfRule type="duplicateValues" dxfId="47" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D472">
-    <cfRule type="duplicateValues" dxfId="46" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D473">
-    <cfRule type="duplicateValues" dxfId="45" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D474">
-    <cfRule type="duplicateValues" dxfId="44" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D475">
-    <cfRule type="duplicateValues" dxfId="43" priority="17"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D476">
-    <cfRule type="duplicateValues" dxfId="42" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D477">
-    <cfRule type="duplicateValues" dxfId="41" priority="19"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D478">
-    <cfRule type="duplicateValues" dxfId="40" priority="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D479">
-    <cfRule type="duplicateValues" dxfId="39" priority="21"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D480">
-    <cfRule type="duplicateValues" dxfId="38" priority="22"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D481">
-    <cfRule type="duplicateValues" dxfId="37" priority="23"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D482">
-    <cfRule type="duplicateValues" dxfId="36" priority="24"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D483">
-    <cfRule type="duplicateValues" dxfId="35" priority="25"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D486">
-    <cfRule type="duplicateValues" dxfId="34" priority="26"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D487">
-    <cfRule type="duplicateValues" dxfId="33" priority="27"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D488">
-    <cfRule type="duplicateValues" dxfId="32" priority="28"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D489">
-    <cfRule type="duplicateValues" dxfId="31" priority="29"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D490">
-    <cfRule type="duplicateValues" dxfId="30" priority="30"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D491">
-    <cfRule type="duplicateValues" dxfId="29" priority="31"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D494">
-    <cfRule type="duplicateValues" dxfId="28" priority="32"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D495">
-    <cfRule type="duplicateValues" dxfId="27" priority="33"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D496">
-    <cfRule type="duplicateValues" dxfId="26" priority="34"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D497">
-    <cfRule type="duplicateValues" dxfId="25" priority="35"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D498">
-    <cfRule type="duplicateValues" dxfId="24" priority="36"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D499">
-    <cfRule type="duplicateValues" dxfId="23" priority="37"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D524">
-    <cfRule type="duplicateValues" dxfId="22" priority="38"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D530">
-    <cfRule type="duplicateValues" dxfId="21" priority="39"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D531">
-    <cfRule type="duplicateValues" dxfId="20" priority="40"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D532">
-    <cfRule type="duplicateValues" dxfId="19" priority="41"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D533">
-    <cfRule type="duplicateValues" dxfId="18" priority="42"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D534">
-    <cfRule type="duplicateValues" dxfId="17" priority="43"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D535">
-    <cfRule type="duplicateValues" dxfId="16" priority="44"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D536">
-    <cfRule type="duplicateValues" dxfId="15" priority="45"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D537">
-    <cfRule type="duplicateValues" dxfId="14" priority="46"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D538">
-    <cfRule type="duplicateValues" dxfId="13" priority="47"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D539">
-    <cfRule type="duplicateValues" dxfId="12" priority="48"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D541">
-    <cfRule type="duplicateValues" dxfId="11" priority="49"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D542">
-    <cfRule type="duplicateValues" dxfId="10" priority="50"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D543">
-    <cfRule type="duplicateValues" dxfId="9" priority="51"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D544">
-    <cfRule type="duplicateValues" dxfId="8" priority="52"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D546">
-    <cfRule type="duplicateValues" dxfId="7" priority="53"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D547">
-    <cfRule type="duplicateValues" dxfId="6" priority="54"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D548">
-    <cfRule type="duplicateValues" dxfId="5" priority="55"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D549">
-    <cfRule type="duplicateValues" dxfId="4" priority="56"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D550">
-    <cfRule type="duplicateValues" dxfId="3" priority="57"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D551">
-    <cfRule type="duplicateValues" dxfId="2" priority="58"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D617">
-    <cfRule type="duplicateValues" dxfId="1" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AMJ696"/>
   <sheetViews>
@@ -21469,13 +21571,13 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="14" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="14"/>
-    <col min="4" max="4" width="41.88671875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="75.44140625" style="14" customWidth="1"/>
-    <col min="6" max="1024" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="10.42578125" style="14" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="14"/>
+    <col min="4" max="4" width="41.85546875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="75.42578125" style="14" customWidth="1"/>
+    <col min="6" max="1024" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1">
@@ -27389,12 +27491,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:G151"/>
   <sheetViews>
@@ -27402,11 +27504,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" customWidth="1"/>
-    <col min="5" max="5" width="37.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
@@ -28428,12 +28530,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:AMJ38"/>
   <sheetViews>
@@ -28441,19 +28543,19 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.109375" style="161" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="161" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" style="161" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="161" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="161" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="161" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="161" customWidth="1"/>
-    <col min="8" max="1024" width="10.88671875" style="161"/>
+    <col min="1" max="1" width="33.140625" style="161" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="161" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="161" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="161" customWidth="1"/>
+    <col min="5" max="5" width="57.7109375" style="161" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="161" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="161" customWidth="1"/>
+    <col min="8" max="1024" width="10.85546875" style="161"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999">
+    <row r="1" spans="1:7" ht="18">
       <c r="A1" s="162" t="s">
         <v>203</v>
       </c>
@@ -28470,7 +28572,7 @@
       <c r="F1" s="166"/>
       <c r="G1" s="166"/>
     </row>
-    <row r="2" spans="1:7" ht="66.599999999999994">
+    <row r="2" spans="1:7" ht="64.5">
       <c r="A2" s="167"/>
       <c r="B2" s="167"/>
       <c r="C2" s="168" t="s">
@@ -28489,7 +28591,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.399999999999999">
+    <row r="3" spans="1:7" ht="18">
       <c r="A3" s="169" t="s">
         <v>9</v>
       </c>
@@ -28735,9 +28837,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -28749,15 +28848,15 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="7"/>
-    <col min="4" max="4" width="28.44140625" customWidth="1"/>
-    <col min="5" max="5" width="30.44140625" customWidth="1"/>
-    <col min="6" max="6" width="46.109375" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
-    <col min="8" max="8" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="7"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+    <col min="6" max="6" width="46.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
@@ -30163,7 +30262,7 @@
       <c r="H109" s="33"/>
       <c r="J109" s="10"/>
     </row>
-    <row r="110" spans="1:12" s="14" customFormat="1" ht="45.9" customHeight="1">
+    <row r="110" spans="1:12" s="14" customFormat="1" ht="45.95" customHeight="1">
       <c r="A110" s="17"/>
       <c r="B110" s="17"/>
       <c r="C110" s="10"/>
@@ -30193,7 +30292,7 @@
       <c r="H112" s="35"/>
       <c r="J112" s="10"/>
     </row>
-    <row r="113" spans="1:10" s="14" customFormat="1" ht="48.9" customHeight="1">
+    <row r="113" spans="1:10" s="14" customFormat="1" ht="48.95" customHeight="1">
       <c r="A113" s="17"/>
       <c r="B113" s="17"/>
       <c r="C113" s="10"/>
@@ -30233,7 +30332,7 @@
       <c r="H116" s="15"/>
       <c r="J116" s="10"/>
     </row>
-    <row r="117" spans="1:10" s="14" customFormat="1" ht="54.9" customHeight="1">
+    <row r="117" spans="1:10" s="14" customFormat="1" ht="54.95" customHeight="1">
       <c r="A117" s="17"/>
       <c r="B117" s="17"/>
       <c r="C117" s="10"/>
@@ -30243,7 +30342,7 @@
       <c r="H117" s="15"/>
       <c r="J117" s="10"/>
     </row>
-    <row r="118" spans="1:10" s="14" customFormat="1" ht="48.9" customHeight="1">
+    <row r="118" spans="1:10" s="14" customFormat="1" ht="48.95" customHeight="1">
       <c r="A118" s="17"/>
       <c r="B118" s="17"/>
       <c r="C118" s="10"/>
@@ -30720,7 +30819,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -30733,15 +30832,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="14"/>
-    <col min="3" max="3" width="74.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="14"/>
+    <col min="3" max="3" width="74.7109375" style="14" customWidth="1"/>
     <col min="4" max="4" width="117" style="14" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" style="14"/>
-    <col min="7" max="7" width="15.44140625" style="14" customWidth="1"/>
-    <col min="8" max="1024" width="8.88671875" style="14"/>
+    <col min="5" max="6" width="8.85546875" style="14"/>
+    <col min="7" max="7" width="15.42578125" style="14" customWidth="1"/>
+    <col min="8" max="1024" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="11" customFormat="1" ht="15" customHeight="1">
@@ -33217,7 +33316,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -33230,14 +33329,14 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="18"/>
-    <col min="3" max="3" width="40.88671875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="28.109375" style="20" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="18"/>
+    <col min="3" max="3" width="40.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="20" customWidth="1"/>
     <col min="5" max="5" width="62" style="20" customWidth="1"/>
-    <col min="6" max="1024" width="8.88671875" style="20"/>
+    <col min="6" max="1024" width="8.85546875" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="49" customFormat="1" ht="15" customHeight="1">
@@ -39440,7 +39539,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -39453,15 +39552,15 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
@@ -41255,22 +41354,22 @@
       <c r="B263" s="11"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H39">
+    <cfRule type="duplicateValues" dxfId="75" priority="3"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H54:H56">
-    <cfRule type="duplicateValues" dxfId="75" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
-    <cfRule type="duplicateValues" dxfId="74" priority="3"/>
+  <conditionalFormatting sqref="H86">
+    <cfRule type="duplicateValues" dxfId="73" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87:H88">
-    <cfRule type="duplicateValues" dxfId="73" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H86">
-    <cfRule type="duplicateValues" dxfId="72" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -41283,12 +41382,12 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="36.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -41442,7 +41541,7 @@
       <c r="G11" s="11"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" ht="15.9" customHeight="1">
+    <row r="12" spans="1:8" s="14" customFormat="1" ht="15.95" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
@@ -41630,7 +41729,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -41643,24 +41742,24 @@
       <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="20"/>
-    <col min="4" max="4" width="30.6640625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="76.88671875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="20" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="20"/>
+    <col min="4" max="4" width="30.7109375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="76.85546875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="20" customWidth="1"/>
     <col min="7" max="7" width="34" style="20" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="20"/>
-    <col min="9" max="9" width="78.33203125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="36.6640625" style="20" customWidth="1"/>
-    <col min="11" max="11" width="40.88671875" customWidth="1"/>
-    <col min="12" max="12" width="63.44140625" style="20" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="20"/>
-    <col min="14" max="14" width="59.44140625" style="14" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="20"/>
-    <col min="16" max="16" width="65.33203125" style="14" customWidth="1"/>
-    <col min="17" max="1024" width="8.88671875" style="20"/>
+    <col min="8" max="8" width="8.85546875" style="20"/>
+    <col min="9" max="9" width="78.28515625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="36.7109375" style="20" customWidth="1"/>
+    <col min="11" max="11" width="40.85546875" customWidth="1"/>
+    <col min="12" max="12" width="63.42578125" style="20" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="20"/>
+    <col min="14" max="14" width="59.42578125" style="14" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" style="20"/>
+    <col min="16" max="16" width="65.28515625" style="14" customWidth="1"/>
+    <col min="17" max="1024" width="8.85546875" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
@@ -41695,7 +41794,7 @@
       <c r="U1" s="11"/>
       <c r="V1" s="11"/>
     </row>
-    <row r="2" spans="1:23" ht="63.9" customHeight="1">
+    <row r="2" spans="1:23" ht="63.95" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -50611,7 +50710,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -50624,23 +50723,23 @@
       <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="12"/>
-    <col min="3" max="3" width="8.88671875" style="14"/>
-    <col min="4" max="4" width="77.109375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="12"/>
+    <col min="3" max="3" width="8.85546875" style="14"/>
+    <col min="4" max="4" width="77.140625" style="14" customWidth="1"/>
     <col min="5" max="5" width="66" style="14" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="14"/>
-    <col min="7" max="7" width="39.88671875" style="14" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="14"/>
-    <col min="9" max="9" width="27.33203125" style="14" customWidth="1"/>
-    <col min="10" max="15" width="8.88671875" style="14"/>
-    <col min="16" max="16" width="8.88671875" style="11"/>
+    <col min="6" max="6" width="8.85546875" style="14"/>
+    <col min="7" max="7" width="39.85546875" style="14" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="14"/>
+    <col min="9" max="9" width="27.28515625" style="14" customWidth="1"/>
+    <col min="10" max="15" width="8.85546875" style="14"/>
+    <col min="16" max="16" width="8.85546875" style="11"/>
     <col min="17" max="17" width="24" style="11" customWidth="1"/>
-    <col min="18" max="18" width="20.109375" style="14" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" style="14" customWidth="1"/>
     <col min="19" max="19" width="17" style="14" customWidth="1"/>
-    <col min="20" max="1024" width="8.88671875" style="14"/>
+    <col min="20" max="1024" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1">
@@ -50668,7 +50767,7 @@
       <c r="N1" s="11"/>
       <c r="O1" s="102"/>
     </row>
-    <row r="2" spans="1:22" ht="159.9" customHeight="1">
+    <row r="2" spans="1:22" ht="159.94999999999999" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -52952,49 +53051,49 @@
     <row r="229" ht="15" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A3:O161" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
-  <conditionalFormatting sqref="E120">
-    <cfRule type="duplicateValues" dxfId="69" priority="2"/>
+  <conditionalFormatting sqref="D91:D92 D156">
+    <cfRule type="duplicateValues" dxfId="69" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D142">
+    <cfRule type="duplicateValues" dxfId="68" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E73">
-    <cfRule type="duplicateValues" dxfId="68" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76">
-    <cfRule type="duplicateValues" dxfId="67" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="duplicateValues" dxfId="66" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E120">
+    <cfRule type="duplicateValues" dxfId="64" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E121:E128">
-    <cfRule type="duplicateValues" dxfId="65" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E136">
-    <cfRule type="duplicateValues" dxfId="64" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D142">
-    <cfRule type="duplicateValues" dxfId="63" priority="8"/>
+  <conditionalFormatting sqref="E144">
+    <cfRule type="duplicateValues" dxfId="61" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D91:D92 D156">
-    <cfRule type="duplicateValues" dxfId="62" priority="9"/>
+  <conditionalFormatting sqref="E155">
+    <cfRule type="duplicateValues" dxfId="60" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E158">
-    <cfRule type="duplicateValues" dxfId="61" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E144">
-    <cfRule type="duplicateValues" dxfId="60" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E155">
-    <cfRule type="duplicateValues" dxfId="59" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{95c71a0f-75e1-4c8f-90e2-641c9351dd98}" enabled="1" method="Standard" siteId="{3e0088dc-0629-4ae6-aa8c-813e7a296f50}" contentBits="2" removed="0"/>
+  <clbl:label id="{fa22dce2-39a9-4bf4-a557-7a50b593b56a}" enabled="1" method="Privileged" siteId="{3e0088dc-0629-4ae6-aa8c-813e7a296f50}" contentBits="0" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>

<commit_message>
SSCS-12361 Prepare for global search / work allocation data migration (#1522)
* Add field preWorkAllocation and migration event

* Add NINO to global search

* Add CaseReference to global search

* Update SearchCriteria

* suppress cves

* added SearchCriteria sheet in template

* new version

* Updated waCaseMigration event

* Remove superuser permission

* Tag 6.3.11

* Moved changes from nonProd sheets

---------

Co-authored-by: Nicholas Hill <nicholas.hill@HMCTS.net>
Co-authored-by: Andrei Trushkov <andrei.trushkov@hmcts.net>
</commit_message>
<xml_diff>
--- a/benefit/data/ccd-template.xlsx
+++ b/benefit/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\gordond\hmcts\sscs-ccd-definitions\benefit\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\andrei\sscs_dev\sscs-ccd-definitions\benefit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1545CE49-7BAE-4A67-BAD6-BC61197D77A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D58D6A-5CB9-4A27-88E0-0722CA1DFB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="785" firstSheet="13" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="785" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -25,22 +25,23 @@
     <sheet name="CaseRoles" sheetId="23" r:id="rId10"/>
     <sheet name="RoleToAccessProfiles" sheetId="22" r:id="rId11"/>
     <sheet name="SearchParty" sheetId="21" r:id="rId12"/>
-    <sheet name="EventToComplexTypes" sheetId="10" r:id="rId13"/>
-    <sheet name="SearchInputFields" sheetId="11" r:id="rId14"/>
-    <sheet name="SearchResultFields" sheetId="12" r:id="rId15"/>
-    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId16"/>
-    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId17"/>
-    <sheet name="UserProfile" sheetId="15" r:id="rId18"/>
-    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId19"/>
-    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId20"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId21"/>
-    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId22"/>
-    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId23"/>
+    <sheet name="SearchCriteria" sheetId="24" r:id="rId13"/>
+    <sheet name="EventToComplexTypes" sheetId="10" r:id="rId14"/>
+    <sheet name="SearchInputFields" sheetId="11" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="12" r:id="rId16"/>
+    <sheet name="WorkBasketInputFields" sheetId="13" r:id="rId17"/>
+    <sheet name="WorkBasketResultFields" sheetId="14" r:id="rId18"/>
+    <sheet name="UserProfile" sheetId="15" r:id="rId19"/>
+    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId20"/>
+    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId21"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId22"/>
+    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId23"/>
+    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">AuthorisationCaseEvent!$A$3:$F$452</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">AuthorisationCaseField!$A$3:$F$618</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AuthorisationCaseState!$A$3:$G$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CaseEvent!$A$3:$V$110</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CaseEventToFields!$A$3:$O$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$2:$L$98</definedName>
@@ -48,17 +49,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ComplexTypes!$A$3:$M$232</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">FixedLists!$A$1:$E$702</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">State!$A$3:$H$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="19">AuthorisationCaseField!$J$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">WorkBasketInputFields!$A$3:$H$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">WorkBasketResultFields!$A$3:$H$3</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="20">AuthorisationCaseField!$J$5</definedName>
     <definedName name="_xlnm.Extract" localSheetId="5">CaseTypeTab!$K$61</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="229">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -817,12 +818,32 @@
   <si>
     <t>CaseRoles</t>
   </si>
+  <si>
+    <t>OtherCaseReference</t>
+  </si>
+  <si>
+    <t>A complex types that make up the Other Case Reference.
+Max Length: 200</t>
+  </si>
+  <si>
+    <t>The Case Type for which the configuration applies
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Not used - but retained to be consistent with other CCD config</t>
+  </si>
+  <si>
+    <t>From when the configuration is valid</t>
+  </si>
+  <si>
+    <t>SearchCriteria</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="37">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1079,6 +1100,20 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333399"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1400,14 +1435,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1683,13 +1719,29 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal 2 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 4" xfId="5" xr:uid="{33532DE7-3164-4A94-8265-C1B9E588DC41}"/>
   </cellStyles>
   <dxfs count="77">
     <dxf>
@@ -2846,7 +2898,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -2953,7 +3005,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2966,10 +3018,10 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3004,16 +3056,16 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3047,7 +3099,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="29" ht="13.8" customHeight="1"/>
+    <row r="29" ht="13.9" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3061,9 +3113,9 @@
       <selection activeCell="A4" sqref="A4:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="7"/>
+    <col min="1" max="1" width="10.85546875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3102,13 +3154,66 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB591878-B3FF-41B4-AE48-D7E884A650BD}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="2" width="12.28515625" style="178" customWidth="1"/>
+    <col min="3" max="16384" width="12.85546875" style="177"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18">
+      <c r="A1" s="185" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" s="184"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="182"/>
+    </row>
+    <row r="2" spans="1:4" ht="90">
+      <c r="A2" s="181" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="181" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="181" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" s="181" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="179" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="180" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="179" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="179" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
@@ -3116,11 +3221,11 @@
       <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="126" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" style="127" customWidth="1"/>
-    <col min="13" max="13" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="126" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="127" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -3252,13 +3357,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I573"/>
   <sheetViews>
@@ -3266,11 +3368,11 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34" style="7" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
-    <col min="5" max="6" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="6" width="36.140625" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5367,12 +5469,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
@@ -5380,12 +5482,12 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" style="7" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
-    <col min="5" max="6" width="41.44140625" customWidth="1"/>
-    <col min="7" max="7" width="29.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="6" width="41.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
@@ -5667,24 +5769,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A104" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A91" sqref="A91:B131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
-    <col min="5" max="6" width="36.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="6" width="36.140625" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6496,12 +6598,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I1048576"/>
   <sheetViews>
@@ -6509,11 +6611,11 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="6" width="54" customWidth="1"/>
     <col min="7" max="7" width="32" customWidth="1"/>
   </cols>
@@ -6964,12 +7066,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
@@ -6977,10 +7079,10 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -7629,229 +7731,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:E35"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="27.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="27" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="176" t="s">
-        <v>214</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-    </row>
-    <row r="17" spans="1:2" ht="15" customHeight="1">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-    </row>
-    <row r="18" spans="1:2" ht="15" customHeight="1">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-    </row>
-    <row r="19" spans="1:2" ht="15" customHeight="1">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-    </row>
-    <row r="20" spans="1:2" ht="15" customHeight="1">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-    </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-    </row>
-    <row r="22" spans="1:2" ht="15" customHeight="1">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-    </row>
-    <row r="23" spans="1:2" ht="15" customHeight="1">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-    </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-    </row>
-    <row r="25" spans="1:2" ht="15" customHeight="1">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-    </row>
-    <row r="26" spans="1:2" ht="15" customHeight="1">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-    </row>
-    <row r="27" spans="1:2" ht="15" customHeight="1">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-    </row>
-    <row r="28" spans="1:2" ht="15" customHeight="1">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-    </row>
-    <row r="29" spans="1:2" ht="15" customHeight="1">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-    </row>
-    <row r="30" spans="1:2" ht="15" customHeight="1">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-    </row>
-    <row r="31" spans="1:2" ht="15" customHeight="1">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-    </row>
-    <row r="32" spans="1:2" ht="15" customHeight="1">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-    </row>
-    <row r="33" spans="1:2" ht="15" customHeight="1">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-    </row>
-    <row r="34" spans="1:2" ht="15" customHeight="1">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-    </row>
-    <row r="35" spans="1:2" ht="15" customHeight="1">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -7864,11 +7744,11 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
-    <col min="7" max="7" width="92.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="92.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1">
@@ -8029,26 +7909,248 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="27" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="176" t="s">
+        <v>214</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" s="20" customFormat="1" ht="15" customHeight="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+    </row>
+    <row r="17" spans="1:2" ht="15" customHeight="1">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="1:2" ht="15" customHeight="1">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+    </row>
+    <row r="19" spans="1:2" ht="15" customHeight="1">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="1:2" ht="15" customHeight="1">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+    </row>
+    <row r="21" spans="1:2" ht="15" customHeight="1">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+    </row>
+    <row r="22" spans="1:2" ht="15" customHeight="1">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+    </row>
+    <row r="23" spans="1:2" ht="15" customHeight="1">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+    </row>
+    <row r="24" spans="1:2" ht="15" customHeight="1">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+    </row>
+    <row r="25" spans="1:2" ht="15" customHeight="1">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+    </row>
+    <row r="26" spans="1:2" ht="15" customHeight="1">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+    </row>
+    <row r="27" spans="1:2" ht="15" customHeight="1">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+    </row>
+    <row r="28" spans="1:2" ht="15" customHeight="1">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+    </row>
+    <row r="29" spans="1:2" ht="15" customHeight="1">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+    </row>
+    <row r="30" spans="1:2" ht="15" customHeight="1">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+    </row>
+    <row r="31" spans="1:2" ht="15" customHeight="1">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+    </row>
+    <row r="32" spans="1:2" ht="15" customHeight="1">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+    </row>
+    <row r="33" spans="1:2" ht="15" customHeight="1">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+    </row>
+    <row r="34" spans="1:2" ht="15" customHeight="1">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+    </row>
+    <row r="35" spans="1:2" ht="15" customHeight="1">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMJ1109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A1072" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="ALF1081" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1015" sqref="A999:XFD1109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="14" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="14"/>
-    <col min="4" max="4" width="37.6640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="75.44140625" style="14" customWidth="1"/>
-    <col min="6" max="1024" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="10.42578125" style="14" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="14"/>
+    <col min="4" max="4" width="37.7109375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="75.42578125" style="14" customWidth="1"/>
+    <col min="6" max="1024" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1">
@@ -21279,189 +21381,189 @@
     </row>
   </sheetData>
   <autoFilter ref="A3:F618" xr:uid="{00000000-0009-0000-0000-000010000000}"/>
+  <conditionalFormatting sqref="D4:D8">
+    <cfRule type="duplicateValues" dxfId="58" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D466">
+    <cfRule type="duplicateValues" dxfId="57" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D467">
+    <cfRule type="duplicateValues" dxfId="56" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D468">
+    <cfRule type="duplicateValues" dxfId="55" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D469">
+    <cfRule type="duplicateValues" dxfId="54" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D470">
+    <cfRule type="duplicateValues" dxfId="53" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D471">
+    <cfRule type="duplicateValues" dxfId="52" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D472">
+    <cfRule type="duplicateValues" dxfId="51" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D473">
+    <cfRule type="duplicateValues" dxfId="50" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D474">
+    <cfRule type="duplicateValues" dxfId="49" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D475">
+    <cfRule type="duplicateValues" dxfId="48" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D476">
+    <cfRule type="duplicateValues" dxfId="47" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D477">
+    <cfRule type="duplicateValues" dxfId="46" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D478">
+    <cfRule type="duplicateValues" dxfId="45" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D479">
+    <cfRule type="duplicateValues" dxfId="44" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D480">
+    <cfRule type="duplicateValues" dxfId="43" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D481">
+    <cfRule type="duplicateValues" dxfId="42" priority="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D482">
+    <cfRule type="duplicateValues" dxfId="41" priority="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D483">
+    <cfRule type="duplicateValues" dxfId="40" priority="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D486">
+    <cfRule type="duplicateValues" dxfId="39" priority="26"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D487">
+    <cfRule type="duplicateValues" dxfId="38" priority="27"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D488">
+    <cfRule type="duplicateValues" dxfId="37" priority="28"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D489">
+    <cfRule type="duplicateValues" dxfId="36" priority="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D490">
+    <cfRule type="duplicateValues" dxfId="35" priority="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D491">
+    <cfRule type="duplicateValues" dxfId="34" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D494">
+    <cfRule type="duplicateValues" dxfId="33" priority="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D495">
+    <cfRule type="duplicateValues" dxfId="32" priority="33"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D496">
+    <cfRule type="duplicateValues" dxfId="31" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D497">
+    <cfRule type="duplicateValues" dxfId="30" priority="35"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D498">
+    <cfRule type="duplicateValues" dxfId="29" priority="36"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D499">
+    <cfRule type="duplicateValues" dxfId="28" priority="37"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D524">
+    <cfRule type="duplicateValues" dxfId="27" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D530">
+    <cfRule type="duplicateValues" dxfId="26" priority="39"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D531">
+    <cfRule type="duplicateValues" dxfId="25" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D532">
+    <cfRule type="duplicateValues" dxfId="24" priority="41"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D533">
+    <cfRule type="duplicateValues" dxfId="23" priority="42"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D534">
+    <cfRule type="duplicateValues" dxfId="22" priority="43"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D535">
+    <cfRule type="duplicateValues" dxfId="21" priority="44"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D536">
+    <cfRule type="duplicateValues" dxfId="20" priority="45"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D537">
+    <cfRule type="duplicateValues" dxfId="19" priority="46"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D538">
+    <cfRule type="duplicateValues" dxfId="18" priority="47"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D539">
+    <cfRule type="duplicateValues" dxfId="17" priority="48"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D541">
+    <cfRule type="duplicateValues" dxfId="16" priority="49"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D542">
+    <cfRule type="duplicateValues" dxfId="15" priority="50"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D543">
+    <cfRule type="duplicateValues" dxfId="14" priority="51"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D544">
+    <cfRule type="duplicateValues" dxfId="13" priority="52"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D546">
+    <cfRule type="duplicateValues" dxfId="12" priority="53"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D547">
+    <cfRule type="duplicateValues" dxfId="11" priority="54"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D548">
+    <cfRule type="duplicateValues" dxfId="10" priority="55"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D549">
+    <cfRule type="duplicateValues" dxfId="9" priority="56"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D550">
+    <cfRule type="duplicateValues" dxfId="8" priority="57"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D551">
+    <cfRule type="duplicateValues" dxfId="7" priority="58"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D617">
+    <cfRule type="duplicateValues" dxfId="6" priority="59"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D619:D642 D606">
-    <cfRule type="duplicateValues" dxfId="58" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D643:D732">
-    <cfRule type="duplicateValues" dxfId="57" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D733:D822">
-    <cfRule type="duplicateValues" dxfId="56" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D823:D912">
-    <cfRule type="duplicateValues" dxfId="55" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D913:D1001 D1016:D1018 D1033:D1035 D1050:D1052 D1067:D1069 D1081:D1083 D1098:D1100">
-    <cfRule type="duplicateValues" dxfId="54" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D8">
-    <cfRule type="duplicateValues" dxfId="53" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D466">
-    <cfRule type="duplicateValues" dxfId="52" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D467">
-    <cfRule type="duplicateValues" dxfId="51" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D468">
-    <cfRule type="duplicateValues" dxfId="50" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D469">
-    <cfRule type="duplicateValues" dxfId="49" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D470">
-    <cfRule type="duplicateValues" dxfId="48" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D471">
-    <cfRule type="duplicateValues" dxfId="47" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D472">
-    <cfRule type="duplicateValues" dxfId="46" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D473">
-    <cfRule type="duplicateValues" dxfId="45" priority="15"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D474">
-    <cfRule type="duplicateValues" dxfId="44" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D475">
-    <cfRule type="duplicateValues" dxfId="43" priority="17"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D476">
-    <cfRule type="duplicateValues" dxfId="42" priority="18"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D477">
-    <cfRule type="duplicateValues" dxfId="41" priority="19"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D478">
-    <cfRule type="duplicateValues" dxfId="40" priority="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D479">
-    <cfRule type="duplicateValues" dxfId="39" priority="21"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D480">
-    <cfRule type="duplicateValues" dxfId="38" priority="22"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D481">
-    <cfRule type="duplicateValues" dxfId="37" priority="23"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D482">
-    <cfRule type="duplicateValues" dxfId="36" priority="24"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D483">
-    <cfRule type="duplicateValues" dxfId="35" priority="25"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D486">
-    <cfRule type="duplicateValues" dxfId="34" priority="26"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D487">
-    <cfRule type="duplicateValues" dxfId="33" priority="27"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D488">
-    <cfRule type="duplicateValues" dxfId="32" priority="28"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D489">
-    <cfRule type="duplicateValues" dxfId="31" priority="29"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D490">
-    <cfRule type="duplicateValues" dxfId="30" priority="30"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D491">
-    <cfRule type="duplicateValues" dxfId="29" priority="31"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D494">
-    <cfRule type="duplicateValues" dxfId="28" priority="32"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D495">
-    <cfRule type="duplicateValues" dxfId="27" priority="33"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D496">
-    <cfRule type="duplicateValues" dxfId="26" priority="34"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D497">
-    <cfRule type="duplicateValues" dxfId="25" priority="35"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D498">
-    <cfRule type="duplicateValues" dxfId="24" priority="36"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D499">
-    <cfRule type="duplicateValues" dxfId="23" priority="37"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D524">
-    <cfRule type="duplicateValues" dxfId="22" priority="38"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D530">
-    <cfRule type="duplicateValues" dxfId="21" priority="39"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D531">
-    <cfRule type="duplicateValues" dxfId="20" priority="40"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D532">
-    <cfRule type="duplicateValues" dxfId="19" priority="41"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D533">
-    <cfRule type="duplicateValues" dxfId="18" priority="42"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D534">
-    <cfRule type="duplicateValues" dxfId="17" priority="43"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D535">
-    <cfRule type="duplicateValues" dxfId="16" priority="44"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D536">
-    <cfRule type="duplicateValues" dxfId="15" priority="45"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D537">
-    <cfRule type="duplicateValues" dxfId="14" priority="46"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D538">
-    <cfRule type="duplicateValues" dxfId="13" priority="47"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D539">
-    <cfRule type="duplicateValues" dxfId="12" priority="48"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D541">
-    <cfRule type="duplicateValues" dxfId="11" priority="49"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D542">
-    <cfRule type="duplicateValues" dxfId="10" priority="50"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D543">
-    <cfRule type="duplicateValues" dxfId="9" priority="51"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D544">
-    <cfRule type="duplicateValues" dxfId="8" priority="52"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D546">
-    <cfRule type="duplicateValues" dxfId="7" priority="53"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D547">
-    <cfRule type="duplicateValues" dxfId="6" priority="54"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D548">
-    <cfRule type="duplicateValues" dxfId="5" priority="55"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D549">
-    <cfRule type="duplicateValues" dxfId="4" priority="56"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D550">
-    <cfRule type="duplicateValues" dxfId="3" priority="57"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D551">
-    <cfRule type="duplicateValues" dxfId="2" priority="58"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D617">
-    <cfRule type="duplicateValues" dxfId="1" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AMJ696"/>
   <sheetViews>
@@ -21469,13 +21571,13 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="14" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="14"/>
-    <col min="4" max="4" width="41.88671875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="75.44140625" style="14" customWidth="1"/>
-    <col min="6" max="1024" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="10.42578125" style="14" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="14"/>
+    <col min="4" max="4" width="41.85546875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="75.42578125" style="14" customWidth="1"/>
+    <col min="6" max="1024" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1">
@@ -27389,12 +27491,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:G151"/>
   <sheetViews>
@@ -27402,11 +27504,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" customWidth="1"/>
-    <col min="5" max="5" width="37.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
@@ -28428,12 +28530,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:AMJ38"/>
   <sheetViews>
@@ -28441,19 +28543,19 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.109375" style="161" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" style="161" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" style="161" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="161" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="161" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="161" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="161" customWidth="1"/>
-    <col min="8" max="1024" width="10.88671875" style="161"/>
+    <col min="1" max="1" width="33.140625" style="161" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="161" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="161" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="161" customWidth="1"/>
+    <col min="5" max="5" width="57.7109375" style="161" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="161" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="161" customWidth="1"/>
+    <col min="8" max="1024" width="10.85546875" style="161"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999">
+    <row r="1" spans="1:7" ht="18">
       <c r="A1" s="162" t="s">
         <v>203</v>
       </c>
@@ -28470,7 +28572,7 @@
       <c r="F1" s="166"/>
       <c r="G1" s="166"/>
     </row>
-    <row r="2" spans="1:7" ht="66.599999999999994">
+    <row r="2" spans="1:7" ht="64.5">
       <c r="A2" s="167"/>
       <c r="B2" s="167"/>
       <c r="C2" s="168" t="s">
@@ -28489,7 +28591,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.399999999999999">
+    <row r="3" spans="1:7" ht="18">
       <c r="A3" s="169" t="s">
         <v>9</v>
       </c>
@@ -28735,9 +28837,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -28749,15 +28848,15 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="7"/>
-    <col min="4" max="4" width="28.44140625" customWidth="1"/>
-    <col min="5" max="5" width="30.44140625" customWidth="1"/>
-    <col min="6" max="6" width="46.109375" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
-    <col min="8" max="8" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="7"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+    <col min="6" max="6" width="46.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
@@ -30163,7 +30262,7 @@
       <c r="H109" s="33"/>
       <c r="J109" s="10"/>
     </row>
-    <row r="110" spans="1:12" s="14" customFormat="1" ht="45.9" customHeight="1">
+    <row r="110" spans="1:12" s="14" customFormat="1" ht="45.95" customHeight="1">
       <c r="A110" s="17"/>
       <c r="B110" s="17"/>
       <c r="C110" s="10"/>
@@ -30193,7 +30292,7 @@
       <c r="H112" s="35"/>
       <c r="J112" s="10"/>
     </row>
-    <row r="113" spans="1:10" s="14" customFormat="1" ht="48.9" customHeight="1">
+    <row r="113" spans="1:10" s="14" customFormat="1" ht="48.95" customHeight="1">
       <c r="A113" s="17"/>
       <c r="B113" s="17"/>
       <c r="C113" s="10"/>
@@ -30233,7 +30332,7 @@
       <c r="H116" s="15"/>
       <c r="J116" s="10"/>
     </row>
-    <row r="117" spans="1:10" s="14" customFormat="1" ht="54.9" customHeight="1">
+    <row r="117" spans="1:10" s="14" customFormat="1" ht="54.95" customHeight="1">
       <c r="A117" s="17"/>
       <c r="B117" s="17"/>
       <c r="C117" s="10"/>
@@ -30243,7 +30342,7 @@
       <c r="H117" s="15"/>
       <c r="J117" s="10"/>
     </row>
-    <row r="118" spans="1:10" s="14" customFormat="1" ht="48.9" customHeight="1">
+    <row r="118" spans="1:10" s="14" customFormat="1" ht="48.95" customHeight="1">
       <c r="A118" s="17"/>
       <c r="B118" s="17"/>
       <c r="C118" s="10"/>
@@ -30720,7 +30819,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -30733,15 +30832,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="14"/>
-    <col min="3" max="3" width="74.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="14"/>
+    <col min="3" max="3" width="74.7109375" style="14" customWidth="1"/>
     <col min="4" max="4" width="117" style="14" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" style="14"/>
-    <col min="7" max="7" width="15.44140625" style="14" customWidth="1"/>
-    <col min="8" max="1024" width="8.88671875" style="14"/>
+    <col min="5" max="6" width="8.85546875" style="14"/>
+    <col min="7" max="7" width="15.42578125" style="14" customWidth="1"/>
+    <col min="8" max="1024" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="11" customFormat="1" ht="15" customHeight="1">
@@ -33217,7 +33316,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -33230,14 +33329,14 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="18"/>
-    <col min="3" max="3" width="40.88671875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="28.109375" style="20" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="18"/>
+    <col min="3" max="3" width="40.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="20" customWidth="1"/>
     <col min="5" max="5" width="62" style="20" customWidth="1"/>
-    <col min="6" max="1024" width="8.88671875" style="20"/>
+    <col min="6" max="1024" width="8.85546875" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="49" customFormat="1" ht="15" customHeight="1">
@@ -39440,7 +39539,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -39453,15 +39552,15 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1">
@@ -41255,22 +41354,22 @@
       <c r="B263" s="11"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H39">
+    <cfRule type="duplicateValues" dxfId="75" priority="3"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H54:H56">
-    <cfRule type="duplicateValues" dxfId="75" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
-    <cfRule type="duplicateValues" dxfId="74" priority="3"/>
+  <conditionalFormatting sqref="H86">
+    <cfRule type="duplicateValues" dxfId="73" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87:H88">
-    <cfRule type="duplicateValues" dxfId="73" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H86">
-    <cfRule type="duplicateValues" dxfId="72" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -41283,12 +41382,12 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.44140625" customWidth="1"/>
-    <col min="6" max="6" width="36.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -41442,7 +41541,7 @@
       <c r="G11" s="11"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" s="14" customFormat="1" ht="15.9" customHeight="1">
+    <row r="12" spans="1:8" s="14" customFormat="1" ht="15.95" customHeight="1">
       <c r="A12" s="5"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
@@ -41630,7 +41729,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -41643,24 +41742,24 @@
       <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" style="20"/>
-    <col min="4" max="4" width="30.6640625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="76.88671875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="20" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.85546875" style="20"/>
+    <col min="4" max="4" width="30.7109375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="76.85546875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="20" customWidth="1"/>
     <col min="7" max="7" width="34" style="20" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="20"/>
-    <col min="9" max="9" width="78.33203125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="36.6640625" style="20" customWidth="1"/>
-    <col min="11" max="11" width="40.88671875" customWidth="1"/>
-    <col min="12" max="12" width="63.44140625" style="20" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="20"/>
-    <col min="14" max="14" width="59.44140625" style="14" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="20"/>
-    <col min="16" max="16" width="65.33203125" style="14" customWidth="1"/>
-    <col min="17" max="1024" width="8.88671875" style="20"/>
+    <col min="8" max="8" width="8.85546875" style="20"/>
+    <col min="9" max="9" width="78.28515625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="36.7109375" style="20" customWidth="1"/>
+    <col min="11" max="11" width="40.85546875" customWidth="1"/>
+    <col min="12" max="12" width="63.42578125" style="20" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="20"/>
+    <col min="14" max="14" width="59.42578125" style="14" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" style="20"/>
+    <col min="16" max="16" width="65.28515625" style="14" customWidth="1"/>
+    <col min="17" max="1024" width="8.85546875" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
@@ -41695,7 +41794,7 @@
       <c r="U1" s="11"/>
       <c r="V1" s="11"/>
     </row>
-    <row r="2" spans="1:23" ht="63.9" customHeight="1">
+    <row r="2" spans="1:23" ht="63.95" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -50611,7 +50710,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -50624,23 +50723,23 @@
       <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="12"/>
-    <col min="3" max="3" width="8.88671875" style="14"/>
-    <col min="4" max="4" width="77.109375" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="12"/>
+    <col min="3" max="3" width="8.85546875" style="14"/>
+    <col min="4" max="4" width="77.140625" style="14" customWidth="1"/>
     <col min="5" max="5" width="66" style="14" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="14"/>
-    <col min="7" max="7" width="39.88671875" style="14" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="14"/>
-    <col min="9" max="9" width="27.33203125" style="14" customWidth="1"/>
-    <col min="10" max="15" width="8.88671875" style="14"/>
-    <col min="16" max="16" width="8.88671875" style="11"/>
+    <col min="6" max="6" width="8.85546875" style="14"/>
+    <col min="7" max="7" width="39.85546875" style="14" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="14"/>
+    <col min="9" max="9" width="27.28515625" style="14" customWidth="1"/>
+    <col min="10" max="15" width="8.85546875" style="14"/>
+    <col min="16" max="16" width="8.85546875" style="11"/>
     <col min="17" max="17" width="24" style="11" customWidth="1"/>
-    <col min="18" max="18" width="20.109375" style="14" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" style="14" customWidth="1"/>
     <col min="19" max="19" width="17" style="14" customWidth="1"/>
-    <col min="20" max="1024" width="8.88671875" style="14"/>
+    <col min="20" max="1024" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1">
@@ -50668,7 +50767,7 @@
       <c r="N1" s="11"/>
       <c r="O1" s="102"/>
     </row>
-    <row r="2" spans="1:22" ht="159.9" customHeight="1">
+    <row r="2" spans="1:22" ht="159.94999999999999" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -52952,49 +53051,49 @@
     <row r="229" ht="15" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A3:O161" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
-  <conditionalFormatting sqref="E120">
-    <cfRule type="duplicateValues" dxfId="69" priority="2"/>
+  <conditionalFormatting sqref="D91:D92 D156">
+    <cfRule type="duplicateValues" dxfId="69" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D142">
+    <cfRule type="duplicateValues" dxfId="68" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E73">
-    <cfRule type="duplicateValues" dxfId="68" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E76">
-    <cfRule type="duplicateValues" dxfId="67" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E81">
-    <cfRule type="duplicateValues" dxfId="66" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E120">
+    <cfRule type="duplicateValues" dxfId="64" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E121:E128">
-    <cfRule type="duplicateValues" dxfId="65" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E136">
-    <cfRule type="duplicateValues" dxfId="64" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D142">
-    <cfRule type="duplicateValues" dxfId="63" priority="8"/>
+  <conditionalFormatting sqref="E144">
+    <cfRule type="duplicateValues" dxfId="61" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D91:D92 D156">
-    <cfRule type="duplicateValues" dxfId="62" priority="9"/>
+  <conditionalFormatting sqref="E155">
+    <cfRule type="duplicateValues" dxfId="60" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E158">
-    <cfRule type="duplicateValues" dxfId="61" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E144">
-    <cfRule type="duplicateValues" dxfId="60" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E155">
-    <cfRule type="duplicateValues" dxfId="59" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{95c71a0f-75e1-4c8f-90e2-641c9351dd98}" enabled="1" method="Standard" siteId="{3e0088dc-0629-4ae6-aa8c-813e7a296f50}" contentBits="2" removed="0"/>
+  <clbl:label id="{fa22dce2-39a9-4bf4-a557-7a50b593b56a}" enabled="1" method="Privileged" siteId="{3e0088dc-0629-4ae6-aa8c-813e7a296f50}" contentBits="0" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>